<commit_message>
Update remaining statistic files for April, 2025
</commit_message>
<xml_diff>
--- a/statistics_files/2025/2025_99_g_net_borrower_lender.xlsx
+++ b/statistics_files/2025/2025_99_g_net_borrower_lender.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\github\next_statistics\statistics_files\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F90E0CA-FD52-4435-8BCC-0538498BA7A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3B335E-B0CB-4F18-94E4-6E1A3E1DDCC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="673" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="199">
   <si>
     <t>NET</t>
   </si>
@@ -586,6 +586,78 @@
   </si>
   <si>
     <t>1.97 : 1</t>
+  </si>
+  <si>
+    <t>1.15 : 1</t>
+  </si>
+  <si>
+    <t>1.09 : 1</t>
+  </si>
+  <si>
+    <t>0.19 : 1</t>
+  </si>
+  <si>
+    <t>1.57 : 1</t>
+  </si>
+  <si>
+    <t>0.66 : 1</t>
+  </si>
+  <si>
+    <t>0.00 : 1</t>
+  </si>
+  <si>
+    <t>0.46 : 1</t>
+  </si>
+  <si>
+    <t>0.47 : 1</t>
+  </si>
+  <si>
+    <t>0.74 : 1</t>
+  </si>
+  <si>
+    <t>1.18 : 1</t>
+  </si>
+  <si>
+    <t>1.48 : 1</t>
+  </si>
+  <si>
+    <t>1.26 : 1</t>
+  </si>
+  <si>
+    <t>1.49 : 1</t>
+  </si>
+  <si>
+    <t>1.20 : 1</t>
+  </si>
+  <si>
+    <t>0.64 : 1</t>
+  </si>
+  <si>
+    <t>1.06 : 1</t>
+  </si>
+  <si>
+    <t>0.32 : 1</t>
+  </si>
+  <si>
+    <t>1.79 : 1</t>
+  </si>
+  <si>
+    <t>0.81 : 1</t>
+  </si>
+  <si>
+    <t>0.13 : 1</t>
+  </si>
+  <si>
+    <t>1.74 : 1</t>
+  </si>
+  <si>
+    <t>0.41 : 1</t>
+  </si>
+  <si>
+    <t>2.85 : 1</t>
+  </si>
+  <si>
+    <t>1.65 : 1</t>
   </si>
 </sst>
 </file>
@@ -5226,15 +5298,15 @@
       </c>
       <c r="B2" s="2">
         <f>January!B2+February!B2+March!B2+April!B2+May!B2+June!B2+July!B2+August!B2+September!B2+October!B2+November!B2+December!B2</f>
-        <v>4717</v>
+        <v>6107</v>
       </c>
       <c r="C2" s="2">
         <f>January!C2+February!C2+March!C2+April!C2+May!C2+June!C2+July!C2+August!C2+September!C2+October!C2+November!C2+December!C2</f>
-        <v>3941</v>
+        <v>5185</v>
       </c>
       <c r="D2" s="2">
         <f>January!D2+February!D2+March!D2+April!D2+May!D2+June!D2+July!D2+August!D2+September!D2+October!D2+November!D2+December!D2</f>
-        <v>776</v>
+        <v>922</v>
       </c>
       <c r="E2" s="28" t="str">
         <f t="shared" ref="E2:E33" si="0">IF(D2 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -5246,7 +5318,7 @@
       </c>
       <c r="G2" s="3" t="str">
         <f t="shared" ref="G2:G33" si="2">IF(ISERROR(ROUND(B2/C2,2)&amp;" : 1"), "", ROUND(B2/C2,2)&amp;" : 1")</f>
-        <v>1.2 : 1</v>
+        <v>1.18 : 1</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5255,15 +5327,15 @@
       </c>
       <c r="B3" s="4">
         <f>January!B3+February!B3+March!B3+April!B3+May!B3+June!B3+July!B3+August!B3+September!B3+October!B3+November!B3+December!B3</f>
-        <v>1777</v>
+        <v>2301</v>
       </c>
       <c r="C3" s="4">
         <f>January!C3+February!C3+March!C3+April!C3+May!C3+June!C3+July!C3+August!C3+September!C3+October!C3+November!C3+December!C3</f>
-        <v>1094</v>
+        <v>1550</v>
       </c>
       <c r="D3" s="4">
         <f>January!D3+February!D3+March!D3+April!D3+May!D3+June!D3+July!D3+August!D3+September!D3+October!D3+November!D3+December!D3</f>
-        <v>683</v>
+        <v>751</v>
       </c>
       <c r="E3" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5275,7 +5347,7 @@
       </c>
       <c r="G3" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.62 : 1</v>
+        <v>1.48 : 1</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5284,15 +5356,15 @@
       </c>
       <c r="B4" s="2">
         <f>January!B4+February!B4+March!B4+April!B4+May!B4+June!B4+July!B4+August!B4+September!B4+October!B4+November!B4+December!B4</f>
-        <v>3251</v>
+        <v>4380</v>
       </c>
       <c r="C4" s="2">
         <f>January!C4+February!C4+March!C4+April!C4+May!C4+June!C4+July!C4+August!C4+September!C4+October!C4+November!C4+December!C4</f>
-        <v>2975</v>
+        <v>4008</v>
       </c>
       <c r="D4" s="2">
         <f>January!D4+February!D4+March!D4+April!D4+May!D4+June!D4+July!D4+August!D4+September!D4+October!D4+November!D4+December!D4</f>
-        <v>276</v>
+        <v>372</v>
       </c>
       <c r="E4" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5313,15 +5385,15 @@
       </c>
       <c r="B5" s="4">
         <f>January!B5+February!B5+March!B5+April!B5+May!B5+June!B5+July!B5+August!B5+September!B5+October!B5+November!B5+December!B5</f>
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="C5" s="4">
         <f>January!C5+February!C5+March!C5+April!C5+May!C5+June!C5+July!C5+August!C5+September!C5+October!C5+November!C5+December!C5</f>
-        <v>360</v>
+        <v>521</v>
       </c>
       <c r="D5" s="4">
         <f>January!D5+February!D5+March!D5+April!D5+May!D5+June!D5+July!D5+August!D5+September!D5+October!D5+November!D5+December!D5</f>
-        <v>-281</v>
+        <v>-412</v>
       </c>
       <c r="E5" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5333,7 +5405,7 @@
       </c>
       <c r="G5" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.22 : 1</v>
+        <v>0.21 : 1</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5342,15 +5414,15 @@
       </c>
       <c r="B6" s="2">
         <f>January!B6+February!B6+March!B6+April!B6+May!B6+June!B6+July!B6+August!B6+September!B6+October!B6+November!B6+December!B6</f>
-        <v>3070</v>
+        <v>4202</v>
       </c>
       <c r="C6" s="2">
         <f>January!C6+February!C6+March!C6+April!C6+May!C6+June!C6+July!C6+August!C6+September!C6+October!C6+November!C6+December!C6</f>
-        <v>3404</v>
+        <v>4623</v>
       </c>
       <c r="D6" s="2">
         <f>January!D6+February!D6+March!D6+April!D6+May!D6+June!D6+July!D6+August!D6+September!D6+October!D6+November!D6+December!D6</f>
-        <v>-334</v>
+        <v>-421</v>
       </c>
       <c r="E6" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5362,7 +5434,7 @@
       </c>
       <c r="G6" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.9 : 1</v>
+        <v>0.91 : 1</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5371,15 +5443,15 @@
       </c>
       <c r="B7" s="4">
         <f>January!B7+February!B7+March!B7+April!B7+May!B7+June!B7+July!B7+August!B7+September!B7+October!B7+November!B7+December!B7</f>
-        <v>633</v>
+        <v>844</v>
       </c>
       <c r="C7" s="4">
         <f>January!C7+February!C7+March!C7+April!C7+May!C7+June!C7+July!C7+August!C7+September!C7+October!C7+November!C7+December!C7</f>
-        <v>413</v>
+        <v>547</v>
       </c>
       <c r="D7" s="4">
         <f>January!D7+February!D7+March!D7+April!D7+May!D7+June!D7+July!D7+August!D7+September!D7+October!D7+November!D7+December!D7</f>
-        <v>220</v>
+        <v>297</v>
       </c>
       <c r="E7" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5391,7 +5463,7 @@
       </c>
       <c r="G7" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.53 : 1</v>
+        <v>1.54 : 1</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5400,15 +5472,15 @@
       </c>
       <c r="B8" s="2">
         <f>January!B8+February!B8+March!B8+April!B8+May!B8+June!B8+July!B8+August!B8+September!B8+October!B8+November!B8+December!B8</f>
-        <v>533</v>
+        <v>650</v>
       </c>
       <c r="C8" s="2">
         <f>January!C8+February!C8+March!C8+April!C8+May!C8+June!C8+July!C8+August!C8+September!C8+October!C8+November!C8+December!C8</f>
-        <v>575</v>
+        <v>743</v>
       </c>
       <c r="D8" s="2">
         <f>January!D8+February!D8+March!D8+April!D8+May!D8+June!D8+July!D8+August!D8+September!D8+October!D8+November!D8+December!D8</f>
-        <v>-42</v>
+        <v>-93</v>
       </c>
       <c r="E8" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5420,7 +5492,7 @@
       </c>
       <c r="G8" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.93 : 1</v>
+        <v>0.87 : 1</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5429,15 +5501,15 @@
       </c>
       <c r="B9" s="4">
         <f>January!B9+February!B9+March!B9+April!B9+May!B9+June!B9+July!B9+August!B9+September!B9+October!B9+November!B9+December!B9</f>
-        <v>126</v>
+        <v>172</v>
       </c>
       <c r="C9" s="4">
         <f>January!C9+February!C9+March!C9+April!C9+May!C9+June!C9+July!C9+August!C9+September!C9+October!C9+November!C9+December!C9</f>
-        <v>234</v>
+        <v>304</v>
       </c>
       <c r="D9" s="4">
         <f>January!D9+February!D9+March!D9+April!D9+May!D9+June!D9+July!D9+August!D9+September!D9+October!D9+November!D9+December!D9</f>
-        <v>-108</v>
+        <v>-132</v>
       </c>
       <c r="E9" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5449,7 +5521,7 @@
       </c>
       <c r="G9" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.54 : 1</v>
+        <v>0.57 : 1</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5462,11 +5534,11 @@
       </c>
       <c r="C10" s="2">
         <f>January!C10+February!C10+March!C10+April!C10+May!C10+June!C10+July!C10+August!C10+September!C10+October!C10+November!C10+December!C10</f>
-        <v>138</v>
+        <v>184</v>
       </c>
       <c r="D10" s="2">
         <f>January!D10+February!D10+March!D10+April!D10+May!D10+June!D10+July!D10+August!D10+September!D10+October!D10+November!D10+December!D10</f>
-        <v>-135</v>
+        <v>-181</v>
       </c>
       <c r="E10" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5516,15 +5588,15 @@
       </c>
       <c r="B12" s="34">
         <f>January!B12+February!B12+March!B12+April!B12+May!B12+June!B12+July!B12+August!B12+September!B12+October!B12+November!B12+December!B12</f>
-        <v>111</v>
+        <v>131</v>
       </c>
       <c r="C12" s="34">
         <f>January!C12+February!C12+March!C12+April!C12+May!C12+June!C12+July!C12+August!C12+September!C12+October!C12+November!C12+December!C12</f>
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="D12" s="34">
         <f>January!D12+February!D12+March!D12+April!D12+May!D12+June!D12+July!D12+August!D12+September!D12+October!D12+November!D12+December!D12</f>
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="E12" s="35" t="str">
         <f t="shared" si="0"/>
@@ -5536,7 +5608,7 @@
       </c>
       <c r="G12" s="36" t="str">
         <f t="shared" si="2"/>
-        <v>2.47 : 1</v>
+        <v>2.38 : 1</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5545,27 +5617,27 @@
       </c>
       <c r="B13" s="6">
         <f>January!B13+February!B13+March!B13+April!B13+May!B13+June!B13+July!B13+August!B13+September!B13+October!B13+November!B13+December!B13</f>
-        <v>207</v>
+        <v>284</v>
       </c>
       <c r="C13" s="6">
         <f>January!C13+February!C13+March!C13+April!C13+May!C13+June!C13+July!C13+August!C13+September!C13+October!C13+November!C13+December!C13</f>
-        <v>214</v>
+        <v>271</v>
       </c>
       <c r="D13" s="6">
         <f>January!D13+February!D13+March!D13+April!D13+May!D13+June!D13+July!D13+August!D13+September!D13+October!D13+November!D13+December!D13</f>
-        <v>-7</v>
+        <v>13</v>
       </c>
       <c r="E13" s="30" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>We borrowed more than we lent this year</v>
       </c>
       <c r="F13" s="30" t="str">
         <f t="shared" si="1"/>
-        <v>We lent more than we borrowed this year</v>
+        <v/>
       </c>
       <c r="G13" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0.97 : 1</v>
+        <v>1.05 : 1</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5574,15 +5646,15 @@
       </c>
       <c r="B14" s="34">
         <f>January!B14+February!B14+March!B14+April!B14+May!B14+June!B14+July!B14+August!B14+September!B14+October!B14+November!B14+December!B14</f>
-        <v>480</v>
+        <v>734</v>
       </c>
       <c r="C14" s="34">
         <f>January!C14+February!C14+March!C14+April!C14+May!C14+June!C14+July!C14+August!C14+September!C14+October!C14+November!C14+December!C14</f>
-        <v>628</v>
+        <v>848</v>
       </c>
       <c r="D14" s="34">
         <f>January!D14+February!D14+March!D14+April!D14+May!D14+June!D14+July!D14+August!D14+September!D14+October!D14+November!D14+December!D14</f>
-        <v>-148</v>
+        <v>-114</v>
       </c>
       <c r="E14" s="35" t="str">
         <f t="shared" si="0"/>
@@ -5594,7 +5666,7 @@
       </c>
       <c r="G14" s="36" t="str">
         <f t="shared" si="2"/>
-        <v>0.76 : 1</v>
+        <v>0.87 : 1</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5603,15 +5675,15 @@
       </c>
       <c r="B15" s="6">
         <f>January!B15+February!B15+March!B15+April!B15+May!B15+June!B15+July!B15+August!B15+September!B15+October!B15+November!B15+December!B15</f>
-        <v>149</v>
+        <v>205</v>
       </c>
       <c r="C15" s="6">
         <f>January!C15+February!C15+March!C15+April!C15+May!C15+June!C15+July!C15+August!C15+September!C15+October!C15+November!C15+December!C15</f>
-        <v>498</v>
+        <v>619</v>
       </c>
       <c r="D15" s="6">
         <f>January!D15+February!D15+March!D15+April!D15+May!D15+June!D15+July!D15+August!D15+September!D15+October!D15+November!D15+December!D15</f>
-        <v>-349</v>
+        <v>-414</v>
       </c>
       <c r="E15" s="30" t="str">
         <f t="shared" si="0"/>
@@ -5623,7 +5695,7 @@
       </c>
       <c r="G15" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0.3 : 1</v>
+        <v>0.33 : 1</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5632,15 +5704,15 @@
       </c>
       <c r="B16" s="2">
         <f>January!B16+February!B16+March!B16+April!B16+May!B16+June!B16+July!B16+August!B16+September!B16+October!B16+November!B16+December!B16</f>
-        <v>160</v>
+        <v>226</v>
       </c>
       <c r="C16" s="2">
         <f>January!C16+February!C16+March!C16+April!C16+May!C16+June!C16+July!C16+August!C16+September!C16+October!C16+November!C16+December!C16</f>
-        <v>567</v>
+        <v>707</v>
       </c>
       <c r="D16" s="2">
         <f>January!D16+February!D16+March!D16+April!D16+May!D16+June!D16+July!D16+August!D16+September!D16+October!D16+November!D16+December!D16</f>
-        <v>-407</v>
+        <v>-481</v>
       </c>
       <c r="E16" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5652,7 +5724,7 @@
       </c>
       <c r="G16" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.28 : 1</v>
+        <v>0.32 : 1</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5661,15 +5733,15 @@
       </c>
       <c r="B17" s="4">
         <f>January!B17+February!B17+March!B17+April!B17+May!B17+June!B17+July!B17+August!B17+September!B17+October!B17+November!B17+December!B17</f>
-        <v>1821</v>
+        <v>2441</v>
       </c>
       <c r="C17" s="4">
         <f>January!C17+February!C17+March!C17+April!C17+May!C17+June!C17+July!C17+August!C17+September!C17+October!C17+November!C17+December!C17</f>
-        <v>1352</v>
+        <v>1821</v>
       </c>
       <c r="D17" s="4">
         <f>January!D17+February!D17+March!D17+April!D17+May!D17+June!D17+July!D17+August!D17+September!D17+October!D17+November!D17+December!D17</f>
-        <v>469</v>
+        <v>620</v>
       </c>
       <c r="E17" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5681,7 +5753,7 @@
       </c>
       <c r="G17" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.35 : 1</v>
+        <v>1.34 : 1</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5690,15 +5762,15 @@
       </c>
       <c r="B18" s="2">
         <f>January!B18+February!B18+March!B18+April!B18+May!B18+June!B18+July!B18+August!B18+September!B18+October!B18+November!B18+December!B18</f>
-        <v>152</v>
+        <v>223</v>
       </c>
       <c r="C18" s="2">
         <f>January!C18+February!C18+March!C18+April!C18+May!C18+June!C18+July!C18+August!C18+September!C18+October!C18+November!C18+December!C18</f>
-        <v>254</v>
+        <v>350</v>
       </c>
       <c r="D18" s="2">
         <f>January!D18+February!D18+March!D18+April!D18+May!D18+June!D18+July!D18+August!D18+September!D18+October!D18+November!D18+December!D18</f>
-        <v>-102</v>
+        <v>-127</v>
       </c>
       <c r="E18" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5710,7 +5782,7 @@
       </c>
       <c r="G18" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.6 : 1</v>
+        <v>0.64 : 1</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5719,15 +5791,15 @@
       </c>
       <c r="B19" s="4">
         <f>January!B19+February!B19+March!B19+April!B19+May!B19+June!B19+July!B19+August!B19+September!B19+October!B19+November!B19+December!B19</f>
-        <v>1249</v>
+        <v>1806</v>
       </c>
       <c r="C19" s="4">
         <f>January!C19+February!C19+March!C19+April!C19+May!C19+June!C19+July!C19+August!C19+September!C19+October!C19+November!C19+December!C19</f>
-        <v>1222</v>
+        <v>1694</v>
       </c>
       <c r="D19" s="4">
         <f>January!D19+February!D19+March!D19+April!D19+May!D19+June!D19+July!D19+August!D19+September!D19+October!D19+November!D19+December!D19</f>
-        <v>27</v>
+        <v>112</v>
       </c>
       <c r="E19" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5739,7 +5811,7 @@
       </c>
       <c r="G19" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.02 : 1</v>
+        <v>1.07 : 1</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5748,15 +5820,15 @@
       </c>
       <c r="B20" s="2">
         <f>January!B20+February!B20+March!B20+April!B20+May!B20+June!B20+July!B20+August!B20+September!B20+October!B20+November!B20+December!B20</f>
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="C20" s="2">
         <f>January!C20+February!C20+March!C20+April!C20+May!C20+June!C20+July!C20+August!C20+September!C20+October!C20+November!C20+December!C20</f>
-        <v>152</v>
+        <v>219</v>
       </c>
       <c r="D20" s="2">
         <f>January!D20+February!D20+March!D20+April!D20+May!D20+June!D20+July!D20+August!D20+September!D20+October!D20+November!D20+December!D20</f>
-        <v>-75</v>
+        <v>-109</v>
       </c>
       <c r="E20" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5768,7 +5840,7 @@
       </c>
       <c r="G20" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.51 : 1</v>
+        <v>0.5 : 1</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5777,15 +5849,15 @@
       </c>
       <c r="B21" s="4">
         <f>January!B21+February!B21+March!B21+April!B21+May!B21+June!B21+July!B21+August!B21+September!B21+October!B21+November!B21+December!B21</f>
-        <v>1449</v>
+        <v>1956</v>
       </c>
       <c r="C21" s="4">
         <f>January!C21+February!C21+March!C21+April!C21+May!C21+June!C21+July!C21+August!C21+September!C21+October!C21+November!C21+December!C21</f>
-        <v>935</v>
+        <v>1277</v>
       </c>
       <c r="D21" s="4">
         <f>January!D21+February!D21+March!D21+April!D21+May!D21+June!D21+July!D21+August!D21+September!D21+October!D21+November!D21+December!D21</f>
-        <v>514</v>
+        <v>679</v>
       </c>
       <c r="E21" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5797,7 +5869,7 @@
       </c>
       <c r="G21" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.55 : 1</v>
+        <v>1.53 : 1</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5806,15 +5878,15 @@
       </c>
       <c r="B22" s="2">
         <f>January!B22+February!B22+March!B22+April!B22+May!B22+June!B22+July!B22+August!B22+September!B22+October!B22+November!B22+December!B22</f>
-        <v>149</v>
+        <v>239</v>
       </c>
       <c r="C22" s="2">
         <f>January!C22+February!C22+March!C22+April!C22+May!C22+June!C22+July!C22+August!C22+September!C22+October!C22+November!C22+December!C22</f>
-        <v>751</v>
+        <v>984</v>
       </c>
       <c r="D22" s="2">
         <f>January!D22+February!D22+March!D22+April!D22+May!D22+June!D22+July!D22+August!D22+September!D22+October!D22+November!D22+December!D22</f>
-        <v>-602</v>
+        <v>-745</v>
       </c>
       <c r="E22" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5826,7 +5898,7 @@
       </c>
       <c r="G22" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.2 : 1</v>
+        <v>0.24 : 1</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5835,15 +5907,15 @@
       </c>
       <c r="B23" s="4">
         <f>January!B23+February!B23+March!B23+April!B23+May!B23+June!B23+July!B23+August!B23+September!B23+October!B23+November!B23+December!B23</f>
-        <v>1893</v>
+        <v>2509</v>
       </c>
       <c r="C23" s="4">
         <f>January!C23+February!C23+March!C23+April!C23+May!C23+June!C23+July!C23+August!C23+September!C23+October!C23+November!C23+December!C23</f>
-        <v>1152</v>
+        <v>1642</v>
       </c>
       <c r="D23" s="4">
         <f>January!D23+February!D23+March!D23+April!D23+May!D23+June!D23+July!D23+August!D23+September!D23+October!D23+November!D23+December!D23</f>
-        <v>741</v>
+        <v>867</v>
       </c>
       <c r="E23" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5855,7 +5927,7 @@
       </c>
       <c r="G23" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.64 : 1</v>
+        <v>1.53 : 1</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5864,15 +5936,15 @@
       </c>
       <c r="B24" s="2">
         <f>January!B24+February!B24+March!B24+April!B24+May!B24+June!B24+July!B24+August!B24+September!B24+October!B24+November!B24+December!B24</f>
-        <v>4400</v>
+        <v>6110</v>
       </c>
       <c r="C24" s="2">
         <f>January!C24+February!C24+March!C24+April!C24+May!C24+June!C24+July!C24+August!C24+September!C24+October!C24+November!C24+December!C24</f>
-        <v>3390</v>
+        <v>4534</v>
       </c>
       <c r="D24" s="2">
         <f>January!D24+February!D24+March!D24+April!D24+May!D24+June!D24+July!D24+August!D24+September!D24+October!D24+November!D24+December!D24</f>
-        <v>1010</v>
+        <v>1576</v>
       </c>
       <c r="E24" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5884,7 +5956,7 @@
       </c>
       <c r="G24" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.3 : 1</v>
+        <v>1.35 : 1</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5893,15 +5965,15 @@
       </c>
       <c r="B25" s="4">
         <f>January!B25+February!B25+March!B25+April!B25+May!B25+June!B25+July!B25+August!B25+September!B25+October!B25+November!B25+December!B25</f>
-        <v>451</v>
+        <v>654</v>
       </c>
       <c r="C25" s="4">
         <f>January!C25+February!C25+March!C25+April!C25+May!C25+June!C25+July!C25+August!C25+September!C25+October!C25+November!C25+December!C25</f>
-        <v>1299</v>
+        <v>1740</v>
       </c>
       <c r="D25" s="4">
         <f>January!D25+February!D25+March!D25+April!D25+May!D25+June!D25+July!D25+August!D25+September!D25+October!D25+November!D25+December!D25</f>
-        <v>-848</v>
+        <v>-1086</v>
       </c>
       <c r="E25" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5913,7 +5985,7 @@
       </c>
       <c r="G25" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.35 : 1</v>
+        <v>0.38 : 1</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5951,15 +6023,15 @@
       </c>
       <c r="B27" s="4">
         <f>January!B27+February!B27+March!B27+April!B27+May!B27+June!B27+July!B27+August!B27+September!B27+October!B27+November!B27+December!B27</f>
-        <v>547</v>
+        <v>748</v>
       </c>
       <c r="C27" s="4">
         <f>January!C27+February!C27+March!C27+April!C27+May!C27+June!C27+July!C27+August!C27+September!C27+October!C27+November!C27+December!C27</f>
-        <v>471</v>
+        <v>639</v>
       </c>
       <c r="D27" s="4">
         <f>January!D27+February!D27+March!D27+April!D27+May!D27+June!D27+July!D27+August!D27+September!D27+October!D27+November!D27+December!D27</f>
-        <v>76</v>
+        <v>109</v>
       </c>
       <c r="E27" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5971,7 +6043,7 @@
       </c>
       <c r="G27" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.16 : 1</v>
+        <v>1.17 : 1</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5980,15 +6052,15 @@
       </c>
       <c r="B28" s="2">
         <f>January!B28+February!B28+March!B28+April!B28+May!B28+June!B28+July!B28+August!B28+September!B28+October!B28+November!B28+December!B28</f>
-        <v>368</v>
+        <v>462</v>
       </c>
       <c r="C28" s="2">
         <f>January!C28+February!C28+March!C28+April!C28+May!C28+June!C28+July!C28+August!C28+September!C28+October!C28+November!C28+December!C28</f>
-        <v>354</v>
+        <v>446</v>
       </c>
       <c r="D28" s="2">
         <f>January!D28+February!D28+March!D28+April!D28+May!D28+June!D28+July!D28+August!D28+September!D28+October!D28+November!D28+December!D28</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E28" s="28" t="str">
         <f t="shared" si="0"/>
@@ -6009,15 +6081,15 @@
       </c>
       <c r="B29" s="4">
         <f>January!B29+February!B29+March!B29+April!B29+May!B29+June!B29+July!B29+August!B29+September!B29+October!B29+November!B29+December!B29</f>
-        <v>2359</v>
+        <v>2930</v>
       </c>
       <c r="C29" s="4">
         <f>January!C29+February!C29+March!C29+April!C29+May!C29+June!C29+July!C29+August!C29+September!C29+October!C29+November!C29+December!C29</f>
-        <v>1592</v>
+        <v>2017</v>
       </c>
       <c r="D29" s="4">
         <f>January!D29+February!D29+March!D29+April!D29+May!D29+June!D29+July!D29+August!D29+September!D29+October!D29+November!D29+December!D29</f>
-        <v>767</v>
+        <v>913</v>
       </c>
       <c r="E29" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6029,7 +6101,7 @@
       </c>
       <c r="G29" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.48 : 1</v>
+        <v>1.45 : 1</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6038,15 +6110,15 @@
       </c>
       <c r="B30" s="2">
         <f>January!B30+February!B30+March!B30+April!B30+May!B30+June!B30+July!B30+August!B30+September!B30+October!B30+November!B30+December!B30</f>
-        <v>109</v>
+        <v>147</v>
       </c>
       <c r="C30" s="2">
         <f>January!C30+February!C30+March!C30+April!C30+May!C30+June!C30+July!C30+August!C30+September!C30+October!C30+November!C30+December!C30</f>
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="D30" s="2">
         <f>January!D30+February!D30+March!D30+April!D30+May!D30+June!D30+July!D30+August!D30+September!D30+October!D30+November!D30+December!D30</f>
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="E30" s="28" t="str">
         <f t="shared" si="0"/>
@@ -6058,7 +6130,7 @@
       </c>
       <c r="G30" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.68 : 1</v>
+        <v>1.65 : 1</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6067,15 +6139,15 @@
       </c>
       <c r="B31" s="4">
         <f>January!B31+February!B31+March!B31+April!B31+May!B31+June!B31+July!B31+August!B31+September!B31+October!B31+November!B31+December!B31</f>
-        <v>147</v>
+        <v>225</v>
       </c>
       <c r="C31" s="4">
         <f>January!C31+February!C31+March!C31+April!C31+May!C31+June!C31+July!C31+August!C31+September!C31+October!C31+November!C31+December!C31</f>
-        <v>766</v>
+        <v>1019</v>
       </c>
       <c r="D31" s="4">
         <f>January!D31+February!D31+March!D31+April!D31+May!D31+June!D31+July!D31+August!D31+September!D31+October!D31+November!D31+December!D31</f>
-        <v>-619</v>
+        <v>-794</v>
       </c>
       <c r="E31" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6087,7 +6159,7 @@
       </c>
       <c r="G31" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.19 : 1</v>
+        <v>0.22 : 1</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6096,15 +6168,15 @@
       </c>
       <c r="B32" s="2">
         <f>January!B32+February!B32+March!B32+April!B32+May!B32+June!B32+July!B32+August!B32+September!B32+October!B32+November!B32+December!B32</f>
-        <v>1156</v>
+        <v>1527</v>
       </c>
       <c r="C32" s="2">
         <f>January!C32+February!C32+March!C32+April!C32+May!C32+June!C32+July!C32+August!C32+September!C32+October!C32+November!C32+December!C32</f>
-        <v>1606</v>
+        <v>2186</v>
       </c>
       <c r="D32" s="2">
         <f>January!D32+February!D32+March!D32+April!D32+May!D32+June!D32+July!D32+August!D32+September!D32+October!D32+November!D32+December!D32</f>
-        <v>-450</v>
+        <v>-659</v>
       </c>
       <c r="E32" s="28" t="str">
         <f t="shared" si="0"/>
@@ -6116,7 +6188,7 @@
       </c>
       <c r="G32" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.72 : 1</v>
+        <v>0.7 : 1</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6125,15 +6197,15 @@
       </c>
       <c r="B33" s="4">
         <f>January!B33+February!B33+March!B33+April!B33+May!B33+June!B33+July!B33+August!B33+September!B33+October!B33+November!B33+December!B33</f>
-        <v>1227</v>
+        <v>1670</v>
       </c>
       <c r="C33" s="4">
         <f>January!C33+February!C33+March!C33+April!C33+May!C33+June!C33+July!C33+August!C33+September!C33+October!C33+November!C33+December!C33</f>
-        <v>1426</v>
+        <v>1843</v>
       </c>
       <c r="D33" s="4">
         <f>January!D33+February!D33+March!D33+April!D33+May!D33+June!D33+July!D33+August!D33+September!D33+October!D33+November!D33+December!D33</f>
-        <v>-199</v>
+        <v>-173</v>
       </c>
       <c r="E33" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6145,7 +6217,7 @@
       </c>
       <c r="G33" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.86 : 1</v>
+        <v>0.91 : 1</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6154,15 +6226,15 @@
       </c>
       <c r="B34" s="2">
         <f>January!B34+February!B34+March!B34+April!B34+May!B34+June!B34+July!B34+August!B34+September!B34+October!B34+November!B34+December!B34</f>
-        <v>568</v>
+        <v>761</v>
       </c>
       <c r="C34" s="2">
         <f>January!C34+February!C34+March!C34+April!C34+May!C34+June!C34+July!C34+August!C34+September!C34+October!C34+November!C34+December!C34</f>
-        <v>504</v>
+        <v>653</v>
       </c>
       <c r="D34" s="2">
         <f>January!D34+February!D34+March!D34+April!D34+May!D34+June!D34+July!D34+August!D34+September!D34+October!D34+November!D34+December!D34</f>
-        <v>64</v>
+        <v>108</v>
       </c>
       <c r="E34" s="28" t="str">
         <f t="shared" ref="E34:E54" si="3">IF(D34 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -6174,7 +6246,7 @@
       </c>
       <c r="G34" s="3" t="str">
         <f t="shared" ref="G34:G54" si="5">IF(ISERROR(ROUND(B34/C34,2)&amp;" : 1"), "", ROUND(B34/C34,2)&amp;" : 1")</f>
-        <v>1.13 : 1</v>
+        <v>1.17 : 1</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6183,15 +6255,15 @@
       </c>
       <c r="B35" s="4">
         <f>January!B35+February!B35+March!B35+April!B35+May!B35+June!B35+July!B35+August!B35+September!B35+October!B35+November!B35+December!B35</f>
-        <v>2548</v>
+        <v>3335</v>
       </c>
       <c r="C35" s="4">
         <f>January!C35+February!C35+March!C35+April!C35+May!C35+June!C35+July!C35+August!C35+September!C35+October!C35+November!C35+December!C35</f>
-        <v>3635</v>
+        <v>4891</v>
       </c>
       <c r="D35" s="4">
         <f>January!D35+February!D35+March!D35+April!D35+May!D35+June!D35+July!D35+August!D35+September!D35+October!D35+November!D35+December!D35</f>
-        <v>-1087</v>
+        <v>-1556</v>
       </c>
       <c r="E35" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6203,7 +6275,7 @@
       </c>
       <c r="G35" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.7 : 1</v>
+        <v>0.68 : 1</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6212,15 +6284,15 @@
       </c>
       <c r="B36" s="2">
         <f>January!B36+February!B36+March!B36+April!B36+May!B36+June!B36+July!B36+August!B36+September!B36+October!B36+November!B36+December!B36</f>
-        <v>471</v>
+        <v>643</v>
       </c>
       <c r="C36" s="2">
         <f>January!C36+February!C36+March!C36+April!C36+May!C36+June!C36+July!C36+August!C36+September!C36+October!C36+November!C36+December!C36</f>
-        <v>1604</v>
+        <v>2145</v>
       </c>
       <c r="D36" s="2">
         <f>January!D36+February!D36+March!D36+April!D36+May!D36+June!D36+July!D36+August!D36+September!D36+October!D36+November!D36+December!D36</f>
-        <v>-1133</v>
+        <v>-1502</v>
       </c>
       <c r="E36" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6232,7 +6304,7 @@
       </c>
       <c r="G36" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.29 : 1</v>
+        <v>0.3 : 1</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6241,15 +6313,15 @@
       </c>
       <c r="B37" s="4">
         <f>January!B37+February!B37+March!B37+April!B37+May!B37+June!B37+July!B37+August!B37+September!B37+October!B37+November!B37+December!B37</f>
-        <v>1508</v>
+        <v>1993</v>
       </c>
       <c r="C37" s="4">
         <f>January!C37+February!C37+March!C37+April!C37+May!C37+June!C37+July!C37+August!C37+September!C37+October!C37+November!C37+December!C37</f>
-        <v>788</v>
+        <v>1059</v>
       </c>
       <c r="D37" s="4">
         <f>January!D37+February!D37+March!D37+April!D37+May!D37+June!D37+July!D37+August!D37+September!D37+October!D37+November!D37+December!D37</f>
-        <v>720</v>
+        <v>934</v>
       </c>
       <c r="E37" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6261,7 +6333,7 @@
       </c>
       <c r="G37" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>1.91 : 1</v>
+        <v>1.88 : 1</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6270,15 +6342,15 @@
       </c>
       <c r="B38" s="2">
         <f>January!B38+February!B38+March!B38+April!B38+May!B38+June!B38+July!B38+August!B38+September!B38+October!B38+November!B38+December!B38</f>
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="C38" s="2">
         <f>January!C38+February!C38+March!C38+April!C38+May!C38+June!C38+July!C38+August!C38+September!C38+October!C38+November!C38+December!C38</f>
-        <v>536</v>
+        <v>687</v>
       </c>
       <c r="D38" s="2">
         <f>January!D38+February!D38+March!D38+April!D38+May!D38+June!D38+July!D38+August!D38+September!D38+October!D38+November!D38+December!D38</f>
-        <v>-478</v>
+        <v>-613</v>
       </c>
       <c r="E38" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6299,15 +6371,15 @@
       </c>
       <c r="B39" s="4">
         <f>January!B39+February!B39+March!B39+April!B39+May!B39+June!B39+July!B39+August!B39+September!B39+October!B39+November!B39+December!B39</f>
-        <v>184</v>
+        <v>199</v>
       </c>
       <c r="C39" s="4">
         <f>January!C39+February!C39+March!C39+April!C39+May!C39+June!C39+July!C39+August!C39+September!C39+October!C39+November!C39+December!C39</f>
-        <v>329</v>
+        <v>429</v>
       </c>
       <c r="D39" s="4">
         <f>January!D39+February!D39+March!D39+April!D39+May!D39+June!D39+July!D39+August!D39+September!D39+October!D39+November!D39+December!D39</f>
-        <v>-145</v>
+        <v>-230</v>
       </c>
       <c r="E39" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6319,7 +6391,7 @@
       </c>
       <c r="G39" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.56 : 1</v>
+        <v>0.46 : 1</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6328,15 +6400,15 @@
       </c>
       <c r="B40" s="38">
         <f>January!B40+February!B40+March!B40+April!B40+May!B40+June!B40+July!B40+August!B40+September!B40+October!B40+November!B40+December!B40</f>
-        <v>139</v>
+        <v>211</v>
       </c>
       <c r="C40" s="38">
         <f>January!C40+February!C40+March!C40+April!C40+May!C40+June!C40+July!C40+August!C40+September!C40+October!C40+November!C40+December!C40</f>
-        <v>262</v>
+        <v>351</v>
       </c>
       <c r="D40" s="38">
         <f>January!D40+February!D40+March!D40+April!D40+May!D40+June!D40+July!D40+August!D40+September!D40+October!D40+November!D40+December!D40</f>
-        <v>-123</v>
+        <v>-140</v>
       </c>
       <c r="E40" s="39" t="str">
         <f t="shared" si="3"/>
@@ -6348,7 +6420,7 @@
       </c>
       <c r="G40" s="40" t="str">
         <f t="shared" si="5"/>
-        <v>0.53 : 1</v>
+        <v>0.6 : 1</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6357,27 +6429,27 @@
       </c>
       <c r="B41" s="8">
         <f>January!B41+February!B41+March!B41+April!B41+May!B41+June!B41+July!B41+August!B41+September!B41+October!B41+November!B41+December!B41</f>
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="C41" s="8">
         <f>January!C41+February!C41+March!C41+April!C41+May!C41+June!C41+July!C41+August!C41+September!C41+October!C41+November!C41+December!C41</f>
-        <v>216</v>
+        <v>238</v>
       </c>
       <c r="D41" s="8">
         <f>January!D41+February!D41+March!D41+April!D41+May!D41+June!D41+July!D41+August!D41+September!D41+October!D41+November!D41+December!D41</f>
-        <v>3</v>
+        <v>-9</v>
       </c>
       <c r="E41" s="31" t="str">
         <f t="shared" si="3"/>
-        <v>We borrowed more than we lent this year</v>
+        <v/>
       </c>
       <c r="F41" s="31" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>We lent more than we borrowed this year</v>
       </c>
       <c r="G41" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>1.01 : 1</v>
+        <v>0.96 : 1</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6386,15 +6458,15 @@
       </c>
       <c r="B42" s="38">
         <f>January!B42+February!B42+March!B42+April!B42+May!B42+June!B42+July!B42+August!B42+September!B42+October!B42+November!B42+December!B42</f>
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C42" s="38">
         <f>January!C42+February!C42+March!C42+April!C42+May!C42+June!C42+July!C42+August!C42+September!C42+October!C42+November!C42+December!C42</f>
-        <v>106</v>
+        <v>168</v>
       </c>
       <c r="D42" s="38">
         <f>January!D42+February!D42+March!D42+April!D42+May!D42+June!D42+July!D42+August!D42+September!D42+October!D42+November!D42+December!D42</f>
-        <v>-81</v>
+        <v>-135</v>
       </c>
       <c r="E42" s="39" t="str">
         <f t="shared" si="3"/>
@@ -6406,7 +6478,7 @@
       </c>
       <c r="G42" s="40" t="str">
         <f t="shared" si="5"/>
-        <v>0.24 : 1</v>
+        <v>0.2 : 1</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6415,15 +6487,15 @@
       </c>
       <c r="B43" s="8">
         <f>January!B43+February!B43+March!B43+April!B43+May!B43+June!B43+July!B43+August!B43+September!B43+October!B43+November!B43+December!B43</f>
-        <v>82</v>
+        <v>142</v>
       </c>
       <c r="C43" s="8">
         <f>January!C43+February!C43+March!C43+April!C43+May!C43+June!C43+July!C43+August!C43+September!C43+October!C43+November!C43+December!C43</f>
-        <v>153</v>
+        <v>239</v>
       </c>
       <c r="D43" s="8">
         <f>January!D43+February!D43+March!D43+April!D43+May!D43+June!D43+July!D43+August!D43+September!D43+October!D43+November!D43+December!D43</f>
-        <v>-71</v>
+        <v>-97</v>
       </c>
       <c r="E43" s="31" t="str">
         <f t="shared" si="3"/>
@@ -6435,7 +6507,7 @@
       </c>
       <c r="G43" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0.54 : 1</v>
+        <v>0.59 : 1</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6444,15 +6516,15 @@
       </c>
       <c r="B44" s="2">
         <f>January!B44+February!B44+March!B44+April!B44+May!B44+June!B44+July!B44+August!B44+September!B44+October!B44+November!B44+December!B44</f>
-        <v>127</v>
+        <v>202</v>
       </c>
       <c r="C44" s="2">
         <f>January!C44+February!C44+March!C44+April!C44+May!C44+June!C44+July!C44+August!C44+September!C44+October!C44+November!C44+December!C44</f>
-        <v>578</v>
+        <v>807</v>
       </c>
       <c r="D44" s="2">
         <f>January!D44+February!D44+March!D44+April!D44+May!D44+June!D44+July!D44+August!D44+September!D44+October!D44+November!D44+December!D44</f>
-        <v>-451</v>
+        <v>-605</v>
       </c>
       <c r="E44" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6464,7 +6536,7 @@
       </c>
       <c r="G44" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.22 : 1</v>
+        <v>0.25 : 1</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6473,15 +6545,15 @@
       </c>
       <c r="B45" s="4">
         <f>January!B45+February!B45+March!B45+April!B45+May!B45+June!B45+July!B45+August!B45+September!B45+October!B45+November!B45+December!B45</f>
-        <v>1690</v>
+        <v>2296</v>
       </c>
       <c r="C45" s="4">
         <f>January!C45+February!C45+March!C45+April!C45+May!C45+June!C45+July!C45+August!C45+September!C45+October!C45+November!C45+December!C45</f>
-        <v>1625</v>
+        <v>2166</v>
       </c>
       <c r="D45" s="4">
         <f>January!D45+February!D45+March!D45+April!D45+May!D45+June!D45+July!D45+August!D45+September!D45+October!D45+November!D45+December!D45</f>
-        <v>65</v>
+        <v>130</v>
       </c>
       <c r="E45" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6493,7 +6565,7 @@
       </c>
       <c r="G45" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>1.04 : 1</v>
+        <v>1.06 : 1</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6502,15 +6574,15 @@
       </c>
       <c r="B46" s="2">
         <f>January!B46+February!B46+March!B46+April!B46+May!B46+June!B46+July!B46+August!B46+September!B46+October!B46+November!B46+December!B46</f>
-        <v>3164</v>
+        <v>4286</v>
       </c>
       <c r="C46" s="2">
         <f>January!C46+February!C46+March!C46+April!C46+May!C46+June!C46+July!C46+August!C46+September!C46+October!C46+November!C46+December!C46</f>
-        <v>2151</v>
+        <v>2796</v>
       </c>
       <c r="D46" s="2">
         <f>January!D46+February!D46+March!D46+April!D46+May!D46+June!D46+July!D46+August!D46+September!D46+October!D46+November!D46+December!D46</f>
-        <v>1013</v>
+        <v>1490</v>
       </c>
       <c r="E46" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6522,7 +6594,7 @@
       </c>
       <c r="G46" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>1.47 : 1</v>
+        <v>1.53 : 1</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6531,15 +6603,15 @@
       </c>
       <c r="B47" s="4">
         <f>January!B47+February!B47+March!B47+April!B47+May!B47+June!B47+July!B47+August!B47+September!B47+October!B47+November!B47+December!B47</f>
-        <v>659</v>
+        <v>892</v>
       </c>
       <c r="C47" s="4">
         <f>January!C47+February!C47+March!C47+April!C47+May!C47+June!C47+July!C47+August!C47+September!C47+October!C47+November!C47+December!C47</f>
-        <v>1831</v>
+        <v>2401</v>
       </c>
       <c r="D47" s="4">
         <f>January!D47+February!D47+March!D47+April!D47+May!D47+June!D47+July!D47+August!D47+September!D47+October!D47+November!D47+December!D47</f>
-        <v>-1172</v>
+        <v>-1509</v>
       </c>
       <c r="E47" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6551,7 +6623,7 @@
       </c>
       <c r="G47" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.36 : 1</v>
+        <v>0.37 : 1</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6560,15 +6632,15 @@
       </c>
       <c r="B48" s="2">
         <f>January!B48+February!B48+March!B48+April!B48+May!B48+June!B48+July!B48+August!B48+September!B48+October!B48+November!B48+December!B48</f>
-        <v>2135</v>
+        <v>2793</v>
       </c>
       <c r="C48" s="2">
         <f>January!C48+February!C48+March!C48+April!C48+May!C48+June!C48+July!C48+August!C48+September!C48+October!C48+November!C48+December!C48</f>
-        <v>736</v>
+        <v>967</v>
       </c>
       <c r="D48" s="2">
         <f>January!D48+February!D48+March!D48+April!D48+May!D48+June!D48+July!D48+August!D48+September!D48+October!D48+November!D48+December!D48</f>
-        <v>1399</v>
+        <v>1826</v>
       </c>
       <c r="E48" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6580,7 +6652,7 @@
       </c>
       <c r="G48" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>2.9 : 1</v>
+        <v>2.89 : 1</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6589,15 +6661,15 @@
       </c>
       <c r="B49" s="4">
         <f>January!B49+February!B49+March!B49+April!B49+May!B49+June!B49+July!B49+August!B49+September!B49+October!B49+November!B49+December!B49</f>
-        <v>2485</v>
+        <v>3099</v>
       </c>
       <c r="C49" s="4">
         <f>January!C49+February!C49+March!C49+April!C49+May!C49+June!C49+July!C49+August!C49+September!C49+October!C49+November!C49+December!C49</f>
-        <v>1650</v>
+        <v>2192</v>
       </c>
       <c r="D49" s="4">
         <f>January!D49+February!D49+March!D49+April!D49+May!D49+June!D49+July!D49+August!D49+September!D49+October!D49+November!D49+December!D49</f>
-        <v>835</v>
+        <v>907</v>
       </c>
       <c r="E49" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6609,7 +6681,7 @@
       </c>
       <c r="G49" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>1.51 : 1</v>
+        <v>1.41 : 1</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6618,15 +6690,15 @@
       </c>
       <c r="B50" s="2">
         <f>January!B50+February!B50+March!B50+April!B50+May!B50+June!B50+July!B50+August!B50+September!B50+October!B50+November!B50+December!B50</f>
-        <v>636</v>
+        <v>799</v>
       </c>
       <c r="C50" s="2">
         <f>January!C50+February!C50+March!C50+April!C50+May!C50+June!C50+July!C50+August!C50+September!C50+October!C50+November!C50+December!C50</f>
-        <v>563</v>
+        <v>732</v>
       </c>
       <c r="D50" s="2">
         <f>January!D50+February!D50+March!D50+April!D50+May!D50+June!D50+July!D50+August!D50+September!D50+October!D50+November!D50+December!D50</f>
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E50" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6638,7 +6710,7 @@
       </c>
       <c r="G50" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>1.13 : 1</v>
+        <v>1.09 : 1</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6647,15 +6719,15 @@
       </c>
       <c r="B51" s="4">
         <f>January!B51+February!B51+March!B51+April!B51+May!B51+June!B51+July!B51+August!B51+September!B51+October!B51+November!B51+December!B51</f>
-        <v>1179</v>
+        <v>1550</v>
       </c>
       <c r="C51" s="4">
         <f>January!C51+February!C51+March!C51+April!C51+May!C51+June!C51+July!C51+August!C51+September!C51+October!C51+November!C51+December!C51</f>
-        <v>1215</v>
+        <v>1603</v>
       </c>
       <c r="D51" s="4">
         <f>January!D51+February!D51+March!D51+April!D51+May!D51+June!D51+July!D51+August!D51+September!D51+October!D51+November!D51+December!D51</f>
-        <v>-36</v>
+        <v>-53</v>
       </c>
       <c r="E51" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6676,15 +6748,15 @@
       </c>
       <c r="B52" s="2">
         <f>January!B52+February!B52+March!B52+April!B52+May!B52+June!B52+July!B52+August!B52+September!B52+October!B52+November!B52+December!B52</f>
-        <v>572</v>
+        <v>735</v>
       </c>
       <c r="C52" s="2">
         <f>January!C52+February!C52+March!C52+April!C52+May!C52+June!C52+July!C52+August!C52+September!C52+October!C52+November!C52+December!C52</f>
-        <v>702</v>
+        <v>886</v>
       </c>
       <c r="D52" s="2">
         <f>January!D52+February!D52+March!D52+April!D52+May!D52+June!D52+July!D52+August!D52+September!D52+October!D52+November!D52+December!D52</f>
-        <v>-130</v>
+        <v>-151</v>
       </c>
       <c r="E52" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6696,7 +6768,7 @@
       </c>
       <c r="G52" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.81 : 1</v>
+        <v>0.83 : 1</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6705,15 +6777,15 @@
       </c>
       <c r="B53" s="4">
         <f>January!B53+February!B53+March!B53+April!B53+May!B53+June!B53+July!B53+August!B53+September!B53+October!B53+November!B53+December!B53</f>
-        <v>83</v>
+        <v>134</v>
       </c>
       <c r="C53" s="4">
         <f>January!C53+February!C53+March!C53+April!C53+May!C53+June!C53+July!C53+August!C53+September!C53+October!C53+November!C53+December!C53</f>
-        <v>761</v>
+        <v>1016</v>
       </c>
       <c r="D53" s="4">
         <f>January!D53+February!D53+March!D53+April!D53+May!D53+June!D53+July!D53+August!D53+September!D53+October!D53+November!D53+December!D53</f>
-        <v>-678</v>
+        <v>-882</v>
       </c>
       <c r="E53" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6725,7 +6797,7 @@
       </c>
       <c r="G53" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.11 : 1</v>
+        <v>0.13 : 1</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6734,15 +6806,15 @@
       </c>
       <c r="B54" s="10">
         <f>January!B54+February!B54+March!B54+April!B54+May!B54+June!B54+July!B54+August!B54+September!B54+October!B54+November!B54+December!B54</f>
-        <v>1082</v>
+        <v>1447</v>
       </c>
       <c r="C54" s="10">
         <f>January!C54+February!C54+March!C54+April!C54+May!C54+June!C54+July!C54+August!C54+September!C54+October!C54+November!C54+December!C54</f>
-        <v>646</v>
+        <v>867</v>
       </c>
       <c r="D54" s="10">
         <f>January!D54+February!D54+March!D54+April!D54+May!D54+June!D54+July!D54+August!D54+September!D54+October!D54+November!D54+December!D54</f>
-        <v>436</v>
+        <v>580</v>
       </c>
       <c r="E54" s="32" t="str">
         <f t="shared" si="3"/>
@@ -9179,7 +9251,7 @@
       <selection activeCell="A42" activeCellId="1" sqref="A40:G40 A42:G42"/>
       <selection pane="topRight" activeCell="A42" activeCellId="1" sqref="A40:G40 A42:G42"/>
       <selection pane="bottomLeft" activeCell="A42" activeCellId="1" sqref="A40:G40 A42:G42"/>
-      <selection pane="bottomRight" activeCell="A42" activeCellId="1" sqref="A40:G40 A42:G42"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9219,108 +9291,204 @@
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="28"/>
+      <c r="B2" s="18">
+        <v>1390</v>
+      </c>
+      <c r="C2" s="18">
+        <v>1244</v>
+      </c>
+      <c r="D2" s="18">
+        <v>146</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F2" s="28"/>
-      <c r="G2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="29"/>
+      <c r="B3" s="21">
+        <v>524</v>
+      </c>
+      <c r="C3" s="21">
+        <v>456</v>
+      </c>
+      <c r="D3" s="21">
+        <v>68</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F3" s="29"/>
-      <c r="G3" s="5"/>
+      <c r="G3" s="5" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="28"/>
+      <c r="B4" s="18">
+        <v>1129</v>
+      </c>
+      <c r="C4" s="18">
+        <v>1033</v>
+      </c>
+      <c r="D4" s="18">
+        <v>96</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F4" s="28"/>
-      <c r="G4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
+      <c r="B5" s="21">
+        <v>30</v>
+      </c>
+      <c r="C5" s="21">
+        <v>161</v>
+      </c>
+      <c r="D5" s="21">
+        <v>-131</v>
+      </c>
       <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="5"/>
+      <c r="F5" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
+      <c r="B6" s="18">
+        <v>1132</v>
+      </c>
+      <c r="C6" s="18">
+        <v>1219</v>
+      </c>
+      <c r="D6" s="18">
+        <v>-87</v>
+      </c>
       <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="3"/>
+      <c r="F6" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="29"/>
+      <c r="B7" s="21">
+        <v>211</v>
+      </c>
+      <c r="C7" s="21">
+        <v>134</v>
+      </c>
+      <c r="D7" s="21">
+        <v>77</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F7" s="29"/>
-      <c r="G7" s="5"/>
+      <c r="G7" s="5" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
+      <c r="B8" s="18">
+        <v>117</v>
+      </c>
+      <c r="C8" s="18">
+        <v>168</v>
+      </c>
+      <c r="D8" s="18">
+        <v>-51</v>
+      </c>
       <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="3"/>
+      <c r="F8" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
+      <c r="B9" s="21">
+        <v>46</v>
+      </c>
+      <c r="C9" s="21">
+        <v>70</v>
+      </c>
+      <c r="D9" s="21">
+        <v>-24</v>
+      </c>
       <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="5"/>
+      <c r="F9" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
+      <c r="B10" s="18">
+        <v>0</v>
+      </c>
+      <c r="C10" s="18">
+        <v>46</v>
+      </c>
+      <c r="D10" s="18">
+        <v>-46</v>
+      </c>
       <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="3"/>
+      <c r="F10" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
+      <c r="B11" s="21">
+        <v>0</v>
+      </c>
+      <c r="C11" s="21">
+        <v>0</v>
+      </c>
+      <c r="D11" s="21">
+        <v>0</v>
+      </c>
       <c r="E11" s="29"/>
       <c r="F11" s="29"/>
       <c r="G11" s="5"/>
@@ -9329,163 +9497,309 @@
       <c r="A12" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="35"/>
+      <c r="B12" s="41">
+        <v>20</v>
+      </c>
+      <c r="C12" s="41">
+        <v>10</v>
+      </c>
+      <c r="D12" s="41">
+        <v>10</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>60</v>
+      </c>
       <c r="F12" s="35"/>
-      <c r="G12" s="36"/>
+      <c r="G12" s="36" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="30"/>
+      <c r="B13" s="23">
+        <v>77</v>
+      </c>
+      <c r="C13" s="23">
+        <v>57</v>
+      </c>
+      <c r="D13" s="23">
+        <v>20</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>60</v>
+      </c>
       <c r="F13" s="30"/>
-      <c r="G13" s="7"/>
+      <c r="G13" s="7" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="35"/>
+      <c r="B14" s="41">
+        <v>254</v>
+      </c>
+      <c r="C14" s="41">
+        <v>220</v>
+      </c>
+      <c r="D14" s="41">
+        <v>34</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>60</v>
+      </c>
       <c r="F14" s="35"/>
-      <c r="G14" s="36"/>
+      <c r="G14" s="36" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
+      <c r="B15" s="23">
+        <v>56</v>
+      </c>
+      <c r="C15" s="23">
+        <v>121</v>
+      </c>
+      <c r="D15" s="23">
+        <v>-65</v>
+      </c>
       <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="7"/>
+      <c r="F15" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="B16" s="18">
+        <v>66</v>
+      </c>
+      <c r="C16" s="18">
+        <v>140</v>
+      </c>
+      <c r="D16" s="18">
+        <v>-74</v>
+      </c>
       <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="3"/>
+      <c r="F16" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="29"/>
+      <c r="B17" s="21">
+        <v>620</v>
+      </c>
+      <c r="C17" s="21">
+        <v>469</v>
+      </c>
+      <c r="D17" s="21">
+        <v>151</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F17" s="29"/>
-      <c r="G17" s="5"/>
+      <c r="G17" s="5" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
+      <c r="B18" s="18">
+        <v>71</v>
+      </c>
+      <c r="C18" s="18">
+        <v>96</v>
+      </c>
+      <c r="D18" s="18">
+        <v>-25</v>
+      </c>
       <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="3"/>
+      <c r="F18" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="29"/>
+      <c r="B19" s="21">
+        <v>557</v>
+      </c>
+      <c r="C19" s="21">
+        <v>472</v>
+      </c>
+      <c r="D19" s="21">
+        <v>85</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F19" s="29"/>
-      <c r="G19" s="5"/>
+      <c r="G19" s="5" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+      <c r="B20" s="18">
+        <v>33</v>
+      </c>
+      <c r="C20" s="18">
+        <v>67</v>
+      </c>
+      <c r="D20" s="18">
+        <v>-34</v>
+      </c>
       <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="3"/>
+      <c r="F20" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="29"/>
+      <c r="B21" s="21">
+        <v>507</v>
+      </c>
+      <c r="C21" s="21">
+        <v>342</v>
+      </c>
+      <c r="D21" s="21">
+        <v>165</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F21" s="29"/>
-      <c r="G21" s="5"/>
+      <c r="G21" s="5" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="B22" s="18">
+        <v>90</v>
+      </c>
+      <c r="C22" s="18">
+        <v>233</v>
+      </c>
+      <c r="D22" s="18">
+        <v>-143</v>
+      </c>
       <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="3"/>
+      <c r="F22" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="29"/>
+      <c r="B23" s="21">
+        <v>616</v>
+      </c>
+      <c r="C23" s="21">
+        <v>490</v>
+      </c>
+      <c r="D23" s="21">
+        <v>126</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F23" s="29"/>
-      <c r="G23" s="5"/>
+      <c r="G23" s="5" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="28"/>
+      <c r="B24" s="18">
+        <v>1710</v>
+      </c>
+      <c r="C24" s="18">
+        <v>1144</v>
+      </c>
+      <c r="D24" s="18">
+        <v>566</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F24" s="28"/>
-      <c r="G24" s="3"/>
+      <c r="G24" s="3" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
+      <c r="B25" s="21">
+        <v>203</v>
+      </c>
+      <c r="C25" s="21">
+        <v>441</v>
+      </c>
+      <c r="D25" s="21">
+        <v>-238</v>
+      </c>
       <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="5"/>
+      <c r="F25" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
+      <c r="B26" s="18">
+        <v>0</v>
+      </c>
+      <c r="C26" s="18">
+        <v>0</v>
+      </c>
+      <c r="D26" s="18">
+        <v>0</v>
+      </c>
       <c r="E26" s="28"/>
       <c r="F26" s="28"/>
       <c r="G26" s="3"/>
@@ -9494,309 +9808,589 @@
       <c r="A27" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="29"/>
+      <c r="B27" s="21">
+        <v>201</v>
+      </c>
+      <c r="C27" s="21">
+        <v>168</v>
+      </c>
+      <c r="D27" s="21">
+        <v>33</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F27" s="29"/>
-      <c r="G27" s="5"/>
+      <c r="G27" s="5" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="28"/>
+      <c r="B28" s="18">
+        <v>94</v>
+      </c>
+      <c r="C28" s="18">
+        <v>92</v>
+      </c>
+      <c r="D28" s="18">
+        <v>2</v>
+      </c>
+      <c r="E28" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F28" s="28"/>
-      <c r="G28" s="3"/>
+      <c r="G28" s="3" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="29"/>
+      <c r="B29" s="21">
+        <v>571</v>
+      </c>
+      <c r="C29" s="21">
+        <v>425</v>
+      </c>
+      <c r="D29" s="21">
+        <v>146</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F29" s="29"/>
-      <c r="G29" s="5"/>
+      <c r="G29" s="5" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="28"/>
+      <c r="B30" s="18">
+        <v>38</v>
+      </c>
+      <c r="C30" s="18">
+        <v>24</v>
+      </c>
+      <c r="D30" s="18">
+        <v>14</v>
+      </c>
+      <c r="E30" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F30" s="28"/>
-      <c r="G30" s="3"/>
+      <c r="G30" s="3" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
+      <c r="B31" s="21">
+        <v>78</v>
+      </c>
+      <c r="C31" s="21">
+        <v>253</v>
+      </c>
+      <c r="D31" s="21">
+        <v>-175</v>
+      </c>
       <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="5"/>
+      <c r="F31" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="B32" s="18">
+        <v>371</v>
+      </c>
+      <c r="C32" s="18">
+        <v>580</v>
+      </c>
+      <c r="D32" s="18">
+        <v>-209</v>
+      </c>
       <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="3"/>
+      <c r="F32" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="29"/>
+      <c r="B33" s="21">
+        <v>443</v>
+      </c>
+      <c r="C33" s="21">
+        <v>417</v>
+      </c>
+      <c r="D33" s="21">
+        <v>26</v>
+      </c>
+      <c r="E33" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F33" s="29"/>
-      <c r="G33" s="5"/>
+      <c r="G33" s="5" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="28"/>
+      <c r="B34" s="18">
+        <v>193</v>
+      </c>
+      <c r="C34" s="18">
+        <v>149</v>
+      </c>
+      <c r="D34" s="18">
+        <v>44</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F34" s="28"/>
-      <c r="G34" s="3"/>
+      <c r="G34" s="3" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
+      <c r="B35" s="21">
+        <v>787</v>
+      </c>
+      <c r="C35" s="21">
+        <v>1256</v>
+      </c>
+      <c r="D35" s="21">
+        <v>-469</v>
+      </c>
       <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="5"/>
+      <c r="F35" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="B36" s="18">
+        <v>172</v>
+      </c>
+      <c r="C36" s="18">
+        <v>541</v>
+      </c>
+      <c r="D36" s="18">
+        <v>-369</v>
+      </c>
       <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="3"/>
+      <c r="F36" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="29"/>
+      <c r="B37" s="21">
+        <v>485</v>
+      </c>
+      <c r="C37" s="21">
+        <v>271</v>
+      </c>
+      <c r="D37" s="21">
+        <v>214</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F37" s="29"/>
-      <c r="G37" s="5"/>
+      <c r="G37" s="5" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
+      <c r="B38" s="18">
+        <v>16</v>
+      </c>
+      <c r="C38" s="18">
+        <v>151</v>
+      </c>
+      <c r="D38" s="18">
+        <v>-135</v>
+      </c>
       <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="3"/>
+      <c r="F38" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="B39" s="21"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
+        <v>44</v>
+      </c>
+      <c r="B39" s="21">
+        <v>15</v>
+      </c>
+      <c r="C39" s="21">
+        <v>100</v>
+      </c>
+      <c r="D39" s="21">
+        <v>-85</v>
+      </c>
       <c r="E39" s="29"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="5"/>
+      <c r="F39" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="B40" s="42"/>
-      <c r="C40" s="42"/>
-      <c r="D40" s="42"/>
+        <v>45</v>
+      </c>
+      <c r="B40" s="42">
+        <v>72</v>
+      </c>
+      <c r="C40" s="42">
+        <v>89</v>
+      </c>
+      <c r="D40" s="42">
+        <v>-17</v>
+      </c>
       <c r="E40" s="39"/>
-      <c r="F40" s="39"/>
-      <c r="G40" s="40"/>
+      <c r="F40" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="G40" s="40" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
+        <v>46</v>
+      </c>
+      <c r="B41" s="25">
+        <v>10</v>
+      </c>
+      <c r="C41" s="25">
+        <v>22</v>
+      </c>
+      <c r="D41" s="25">
+        <v>-12</v>
+      </c>
       <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="9"/>
+      <c r="F41" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" s="42"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="42"/>
+        <v>47</v>
+      </c>
+      <c r="B42" s="42">
+        <v>8</v>
+      </c>
+      <c r="C42" s="42">
+        <v>62</v>
+      </c>
+      <c r="D42" s="42">
+        <v>-54</v>
+      </c>
       <c r="E42" s="39"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="40"/>
+      <c r="F42" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="G42" s="40" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
+        <v>48</v>
+      </c>
+      <c r="B43" s="25">
+        <v>60</v>
+      </c>
+      <c r="C43" s="25">
+        <v>86</v>
+      </c>
+      <c r="D43" s="25">
+        <v>-26</v>
+      </c>
       <c r="E43" s="31"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="9"/>
+      <c r="F43" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
+      <c r="B44" s="18">
+        <v>75</v>
+      </c>
+      <c r="C44" s="18">
+        <v>229</v>
+      </c>
+      <c r="D44" s="18">
+        <v>-154</v>
+      </c>
       <c r="E44" s="28"/>
-      <c r="F44" s="28"/>
-      <c r="G44" s="3"/>
+      <c r="F44" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="21"/>
-      <c r="C45" s="21"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="29"/>
+      <c r="B45" s="21">
+        <v>606</v>
+      </c>
+      <c r="C45" s="21">
+        <v>541</v>
+      </c>
+      <c r="D45" s="21">
+        <v>65</v>
+      </c>
+      <c r="E45" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F45" s="29"/>
-      <c r="G45" s="5"/>
+      <c r="G45" s="5" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="28"/>
+      <c r="B46" s="18">
+        <v>1122</v>
+      </c>
+      <c r="C46" s="18">
+        <v>645</v>
+      </c>
+      <c r="D46" s="18">
+        <v>477</v>
+      </c>
+      <c r="E46" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F46" s="28"/>
-      <c r="G46" s="3"/>
+      <c r="G46" s="3" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="21"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
+      <c r="B47" s="21">
+        <v>233</v>
+      </c>
+      <c r="C47" s="21">
+        <v>570</v>
+      </c>
+      <c r="D47" s="21">
+        <v>-337</v>
+      </c>
       <c r="E47" s="29"/>
-      <c r="F47" s="29"/>
-      <c r="G47" s="5"/>
+      <c r="F47" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="28"/>
+      <c r="B48" s="18">
+        <v>658</v>
+      </c>
+      <c r="C48" s="18">
+        <v>231</v>
+      </c>
+      <c r="D48" s="18">
+        <v>427</v>
+      </c>
+      <c r="E48" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F48" s="28"/>
-      <c r="G48" s="3"/>
+      <c r="G48" s="3" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="21"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="29"/>
+      <c r="B49" s="21">
+        <v>614</v>
+      </c>
+      <c r="C49" s="21">
+        <v>542</v>
+      </c>
+      <c r="D49" s="21">
+        <v>72</v>
+      </c>
+      <c r="E49" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F49" s="29"/>
-      <c r="G49" s="5"/>
+      <c r="G49" s="5" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="18"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
+      <c r="B50" s="18">
+        <v>163</v>
+      </c>
+      <c r="C50" s="18">
+        <v>169</v>
+      </c>
+      <c r="D50" s="18">
+        <v>-6</v>
+      </c>
       <c r="E50" s="28"/>
-      <c r="F50" s="28"/>
-      <c r="G50" s="3"/>
+      <c r="F50" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="21"/>
-      <c r="C51" s="21"/>
-      <c r="D51" s="21"/>
+      <c r="B51" s="21">
+        <v>371</v>
+      </c>
+      <c r="C51" s="21">
+        <v>388</v>
+      </c>
+      <c r="D51" s="21">
+        <v>-17</v>
+      </c>
       <c r="E51" s="29"/>
-      <c r="F51" s="29"/>
-      <c r="G51" s="5"/>
+      <c r="F51" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="18"/>
-      <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
+      <c r="B52" s="18">
+        <v>163</v>
+      </c>
+      <c r="C52" s="18">
+        <v>184</v>
+      </c>
+      <c r="D52" s="18">
+        <v>-21</v>
+      </c>
       <c r="E52" s="28"/>
-      <c r="F52" s="28"/>
-      <c r="G52" s="3"/>
+      <c r="F52" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="21"/>
-      <c r="C53" s="21"/>
-      <c r="D53" s="21"/>
+      <c r="B53" s="21">
+        <v>51</v>
+      </c>
+      <c r="C53" s="21">
+        <v>255</v>
+      </c>
+      <c r="D53" s="21">
+        <v>-204</v>
+      </c>
       <c r="E53" s="29"/>
-      <c r="F53" s="29"/>
-      <c r="G53" s="5"/>
+      <c r="F53" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="B54" s="27"/>
-      <c r="C54" s="27"/>
-      <c r="D54" s="27"/>
-      <c r="E54" s="32"/>
+      <c r="B54" s="27">
+        <v>365</v>
+      </c>
+      <c r="C54" s="27">
+        <v>221</v>
+      </c>
+      <c r="D54" s="27">
+        <v>144</v>
+      </c>
+      <c r="E54" s="32" t="s">
+        <v>60</v>
+      </c>
       <c r="F54" s="32"/>
-      <c r="G54" s="11"/>
+      <c r="G54" s="11" t="s">
+        <v>198</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G54" xr:uid="{00000000-0009-0000-0000-000004000000}"/>

</xml_diff>

<commit_message>
Update all remaining May statistics files
</commit_message>
<xml_diff>
--- a/statistics_files/2025/2025_99_g_net_borrower_lender.xlsx
+++ b/statistics_files/2025/2025_99_g_net_borrower_lender.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\github\next_statistics\statistics_files\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3B335E-B0CB-4F18-94E4-6E1A3E1DDCC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B1B5DB-9AA2-4500-95BE-F58651F238AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="673" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1291" uniqueCount="210">
   <si>
     <t>NET</t>
   </si>
@@ -658,6 +658,39 @@
   </si>
   <si>
     <t>1.65 : 1</t>
+  </si>
+  <si>
+    <t>1.61 : 1</t>
+  </si>
+  <si>
+    <t>1.51 : 1</t>
+  </si>
+  <si>
+    <t>0.69 : 1</t>
+  </si>
+  <si>
+    <t>2.21 : 1</t>
+  </si>
+  <si>
+    <t>0.14 : 1</t>
+  </si>
+  <si>
+    <t>1.93 : 1</t>
+  </si>
+  <si>
+    <t>3.37 : 1</t>
+  </si>
+  <si>
+    <t>1.62 : 1</t>
+  </si>
+  <si>
+    <t>0.80 : 1</t>
+  </si>
+  <si>
+    <t>0.71 : 1</t>
+  </si>
+  <si>
+    <t>1.89 : 1</t>
   </si>
 </sst>
 </file>
@@ -5298,15 +5331,15 @@
       </c>
       <c r="B2" s="2">
         <f>January!B2+February!B2+March!B2+April!B2+May!B2+June!B2+July!B2+August!B2+September!B2+October!B2+November!B2+December!B2</f>
-        <v>6107</v>
+        <v>7511</v>
       </c>
       <c r="C2" s="2">
         <f>January!C2+February!C2+March!C2+April!C2+May!C2+June!C2+July!C2+August!C2+September!C2+October!C2+November!C2+December!C2</f>
-        <v>5185</v>
+        <v>6352</v>
       </c>
       <c r="D2" s="2">
         <f>January!D2+February!D2+March!D2+April!D2+May!D2+June!D2+July!D2+August!D2+September!D2+October!D2+November!D2+December!D2</f>
-        <v>922</v>
+        <v>1159</v>
       </c>
       <c r="E2" s="28" t="str">
         <f t="shared" ref="E2:E33" si="0">IF(D2 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -5327,15 +5360,15 @@
       </c>
       <c r="B3" s="4">
         <f>January!B3+February!B3+March!B3+April!B3+May!B3+June!B3+July!B3+August!B3+September!B3+October!B3+November!B3+December!B3</f>
-        <v>2301</v>
+        <v>2880</v>
       </c>
       <c r="C3" s="4">
         <f>January!C3+February!C3+March!C3+April!C3+May!C3+June!C3+July!C3+August!C3+September!C3+October!C3+November!C3+December!C3</f>
-        <v>1550</v>
+        <v>1910</v>
       </c>
       <c r="D3" s="4">
         <f>January!D3+February!D3+March!D3+April!D3+May!D3+June!D3+July!D3+August!D3+September!D3+October!D3+November!D3+December!D3</f>
-        <v>751</v>
+        <v>970</v>
       </c>
       <c r="E3" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5347,7 +5380,7 @@
       </c>
       <c r="G3" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.48 : 1</v>
+        <v>1.51 : 1</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5356,15 +5389,15 @@
       </c>
       <c r="B4" s="2">
         <f>January!B4+February!B4+March!B4+April!B4+May!B4+June!B4+July!B4+August!B4+September!B4+October!B4+November!B4+December!B4</f>
-        <v>4380</v>
+        <v>5527</v>
       </c>
       <c r="C4" s="2">
         <f>January!C4+February!C4+March!C4+April!C4+May!C4+June!C4+July!C4+August!C4+September!C4+October!C4+November!C4+December!C4</f>
-        <v>4008</v>
+        <v>5085</v>
       </c>
       <c r="D4" s="2">
         <f>January!D4+February!D4+March!D4+April!D4+May!D4+June!D4+July!D4+August!D4+September!D4+October!D4+November!D4+December!D4</f>
-        <v>372</v>
+        <v>442</v>
       </c>
       <c r="E4" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5385,15 +5418,15 @@
       </c>
       <c r="B5" s="4">
         <f>January!B5+February!B5+March!B5+April!B5+May!B5+June!B5+July!B5+August!B5+September!B5+October!B5+November!B5+December!B5</f>
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="C5" s="4">
         <f>January!C5+February!C5+March!C5+April!C5+May!C5+June!C5+July!C5+August!C5+September!C5+October!C5+November!C5+December!C5</f>
-        <v>521</v>
+        <v>667</v>
       </c>
       <c r="D5" s="4">
         <f>January!D5+February!D5+March!D5+April!D5+May!D5+June!D5+July!D5+August!D5+September!D5+October!D5+November!D5+December!D5</f>
-        <v>-412</v>
+        <v>-543</v>
       </c>
       <c r="E5" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5405,7 +5438,7 @@
       </c>
       <c r="G5" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.21 : 1</v>
+        <v>0.19 : 1</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5414,15 +5447,15 @@
       </c>
       <c r="B6" s="2">
         <f>January!B6+February!B6+March!B6+April!B6+May!B6+June!B6+July!B6+August!B6+September!B6+October!B6+November!B6+December!B6</f>
-        <v>4202</v>
+        <v>5117</v>
       </c>
       <c r="C6" s="2">
         <f>January!C6+February!C6+March!C6+April!C6+May!C6+June!C6+July!C6+August!C6+September!C6+October!C6+November!C6+December!C6</f>
-        <v>4623</v>
+        <v>5800</v>
       </c>
       <c r="D6" s="2">
         <f>January!D6+February!D6+March!D6+April!D6+May!D6+June!D6+July!D6+August!D6+September!D6+October!D6+November!D6+December!D6</f>
-        <v>-421</v>
+        <v>-683</v>
       </c>
       <c r="E6" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5434,7 +5467,7 @@
       </c>
       <c r="G6" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.91 : 1</v>
+        <v>0.88 : 1</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5443,15 +5476,15 @@
       </c>
       <c r="B7" s="4">
         <f>January!B7+February!B7+March!B7+April!B7+May!B7+June!B7+July!B7+August!B7+September!B7+October!B7+November!B7+December!B7</f>
-        <v>844</v>
+        <v>1048</v>
       </c>
       <c r="C7" s="4">
         <f>January!C7+February!C7+March!C7+April!C7+May!C7+June!C7+July!C7+August!C7+September!C7+October!C7+November!C7+December!C7</f>
-        <v>547</v>
+        <v>703</v>
       </c>
       <c r="D7" s="4">
         <f>January!D7+February!D7+March!D7+April!D7+May!D7+June!D7+July!D7+August!D7+September!D7+October!D7+November!D7+December!D7</f>
-        <v>297</v>
+        <v>345</v>
       </c>
       <c r="E7" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5463,7 +5496,7 @@
       </c>
       <c r="G7" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.54 : 1</v>
+        <v>1.49 : 1</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5472,15 +5505,15 @@
       </c>
       <c r="B8" s="2">
         <f>January!B8+February!B8+March!B8+April!B8+May!B8+June!B8+July!B8+August!B8+September!B8+October!B8+November!B8+December!B8</f>
-        <v>650</v>
+        <v>826</v>
       </c>
       <c r="C8" s="2">
         <f>January!C8+February!C8+March!C8+April!C8+May!C8+June!C8+July!C8+August!C8+September!C8+October!C8+November!C8+December!C8</f>
-        <v>743</v>
+        <v>898</v>
       </c>
       <c r="D8" s="2">
         <f>January!D8+February!D8+March!D8+April!D8+May!D8+June!D8+July!D8+August!D8+September!D8+October!D8+November!D8+December!D8</f>
-        <v>-93</v>
+        <v>-72</v>
       </c>
       <c r="E8" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5492,7 +5525,7 @@
       </c>
       <c r="G8" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.87 : 1</v>
+        <v>0.92 : 1</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5501,15 +5534,15 @@
       </c>
       <c r="B9" s="4">
         <f>January!B9+February!B9+March!B9+April!B9+May!B9+June!B9+July!B9+August!B9+September!B9+October!B9+November!B9+December!B9</f>
-        <v>172</v>
+        <v>203</v>
       </c>
       <c r="C9" s="4">
         <f>January!C9+February!C9+March!C9+April!C9+May!C9+June!C9+July!C9+August!C9+September!C9+October!C9+November!C9+December!C9</f>
-        <v>304</v>
+        <v>347</v>
       </c>
       <c r="D9" s="4">
         <f>January!D9+February!D9+March!D9+April!D9+May!D9+June!D9+July!D9+August!D9+September!D9+October!D9+November!D9+December!D9</f>
-        <v>-132</v>
+        <v>-144</v>
       </c>
       <c r="E9" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5521,7 +5554,7 @@
       </c>
       <c r="G9" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.57 : 1</v>
+        <v>0.59 : 1</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5534,11 +5567,11 @@
       </c>
       <c r="C10" s="2">
         <f>January!C10+February!C10+March!C10+April!C10+May!C10+June!C10+July!C10+August!C10+September!C10+October!C10+November!C10+December!C10</f>
-        <v>184</v>
+        <v>206</v>
       </c>
       <c r="D10" s="2">
         <f>January!D10+February!D10+March!D10+April!D10+May!D10+June!D10+July!D10+August!D10+September!D10+October!D10+November!D10+December!D10</f>
-        <v>-181</v>
+        <v>-203</v>
       </c>
       <c r="E10" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5550,7 +5583,7 @@
       </c>
       <c r="G10" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.02 : 1</v>
+        <v>0.01 : 1</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5559,7 +5592,7 @@
       </c>
       <c r="B11" s="4">
         <f>January!B11+February!B11+March!B11+April!B11+May!B11+June!B11+July!B11+August!B11+September!B11+October!B11+November!B11+December!B11</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C11" s="4">
         <f>January!C11+February!C11+March!C11+April!C11+May!C11+June!C11+July!C11+August!C11+September!C11+October!C11+November!C11+December!C11</f>
@@ -5567,11 +5600,11 @@
       </c>
       <c r="D11" s="4">
         <f>January!D11+February!D11+March!D11+April!D11+May!D11+June!D11+July!D11+August!D11+September!D11+October!D11+November!D11+December!D11</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E11" s="29" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>We borrowed more than we lent this year</v>
       </c>
       <c r="F11" s="29" t="str">
         <f t="shared" si="1"/>
@@ -5588,15 +5621,15 @@
       </c>
       <c r="B12" s="34">
         <f>January!B12+February!B12+March!B12+April!B12+May!B12+June!B12+July!B12+August!B12+September!B12+October!B12+November!B12+December!B12</f>
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="C12" s="34">
         <f>January!C12+February!C12+March!C12+April!C12+May!C12+June!C12+July!C12+August!C12+September!C12+October!C12+November!C12+December!C12</f>
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="D12" s="34">
         <f>January!D12+February!D12+March!D12+April!D12+May!D12+June!D12+July!D12+August!D12+September!D12+October!D12+November!D12+December!D12</f>
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="E12" s="35" t="str">
         <f t="shared" si="0"/>
@@ -5608,7 +5641,7 @@
       </c>
       <c r="G12" s="36" t="str">
         <f t="shared" si="2"/>
-        <v>2.38 : 1</v>
+        <v>2.26 : 1</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5617,15 +5650,15 @@
       </c>
       <c r="B13" s="6">
         <f>January!B13+February!B13+March!B13+April!B13+May!B13+June!B13+July!B13+August!B13+September!B13+October!B13+November!B13+December!B13</f>
-        <v>284</v>
+        <v>370</v>
       </c>
       <c r="C13" s="6">
         <f>January!C13+February!C13+March!C13+April!C13+May!C13+June!C13+July!C13+August!C13+September!C13+October!C13+November!C13+December!C13</f>
-        <v>271</v>
+        <v>347</v>
       </c>
       <c r="D13" s="6">
         <f>January!D13+February!D13+March!D13+April!D13+May!D13+June!D13+July!D13+August!D13+September!D13+October!D13+November!D13+December!D13</f>
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="E13" s="30" t="str">
         <f t="shared" si="0"/>
@@ -5637,7 +5670,7 @@
       </c>
       <c r="G13" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>1.05 : 1</v>
+        <v>1.07 : 1</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5646,15 +5679,15 @@
       </c>
       <c r="B14" s="34">
         <f>January!B14+February!B14+March!B14+April!B14+May!B14+June!B14+July!B14+August!B14+September!B14+October!B14+November!B14+December!B14</f>
-        <v>734</v>
+        <v>867</v>
       </c>
       <c r="C14" s="34">
         <f>January!C14+February!C14+March!C14+April!C14+May!C14+June!C14+July!C14+August!C14+September!C14+October!C14+November!C14+December!C14</f>
-        <v>848</v>
+        <v>1039</v>
       </c>
       <c r="D14" s="34">
         <f>January!D14+February!D14+March!D14+April!D14+May!D14+June!D14+July!D14+August!D14+September!D14+October!D14+November!D14+December!D14</f>
-        <v>-114</v>
+        <v>-172</v>
       </c>
       <c r="E14" s="35" t="str">
         <f t="shared" si="0"/>
@@ -5666,7 +5699,7 @@
       </c>
       <c r="G14" s="36" t="str">
         <f t="shared" si="2"/>
-        <v>0.87 : 1</v>
+        <v>0.83 : 1</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5675,15 +5708,15 @@
       </c>
       <c r="B15" s="6">
         <f>January!B15+February!B15+March!B15+April!B15+May!B15+June!B15+July!B15+August!B15+September!B15+October!B15+November!B15+December!B15</f>
-        <v>205</v>
+        <v>268</v>
       </c>
       <c r="C15" s="6">
         <f>January!C15+February!C15+March!C15+April!C15+May!C15+June!C15+July!C15+August!C15+September!C15+October!C15+November!C15+December!C15</f>
-        <v>619</v>
+        <v>752</v>
       </c>
       <c r="D15" s="6">
         <f>January!D15+February!D15+March!D15+April!D15+May!D15+June!D15+July!D15+August!D15+September!D15+October!D15+November!D15+December!D15</f>
-        <v>-414</v>
+        <v>-484</v>
       </c>
       <c r="E15" s="30" t="str">
         <f t="shared" si="0"/>
@@ -5695,7 +5728,7 @@
       </c>
       <c r="G15" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0.33 : 1</v>
+        <v>0.36 : 1</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5704,15 +5737,15 @@
       </c>
       <c r="B16" s="2">
         <f>January!B16+February!B16+March!B16+April!B16+May!B16+June!B16+July!B16+August!B16+September!B16+October!B16+November!B16+December!B16</f>
-        <v>226</v>
+        <v>296</v>
       </c>
       <c r="C16" s="2">
         <f>January!C16+February!C16+March!C16+April!C16+May!C16+June!C16+July!C16+August!C16+September!C16+October!C16+November!C16+December!C16</f>
-        <v>707</v>
+        <v>884</v>
       </c>
       <c r="D16" s="2">
         <f>January!D16+February!D16+March!D16+April!D16+May!D16+June!D16+July!D16+August!D16+September!D16+October!D16+November!D16+December!D16</f>
-        <v>-481</v>
+        <v>-588</v>
       </c>
       <c r="E16" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5724,7 +5757,7 @@
       </c>
       <c r="G16" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.32 : 1</v>
+        <v>0.33 : 1</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5733,15 +5766,15 @@
       </c>
       <c r="B17" s="4">
         <f>January!B17+February!B17+March!B17+April!B17+May!B17+June!B17+July!B17+August!B17+September!B17+October!B17+November!B17+December!B17</f>
-        <v>2441</v>
+        <v>3086</v>
       </c>
       <c r="C17" s="4">
         <f>January!C17+February!C17+March!C17+April!C17+May!C17+June!C17+July!C17+August!C17+September!C17+October!C17+November!C17+December!C17</f>
-        <v>1821</v>
+        <v>2249</v>
       </c>
       <c r="D17" s="4">
         <f>January!D17+February!D17+March!D17+April!D17+May!D17+June!D17+July!D17+August!D17+September!D17+October!D17+November!D17+December!D17</f>
-        <v>620</v>
+        <v>837</v>
       </c>
       <c r="E17" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5753,7 +5786,7 @@
       </c>
       <c r="G17" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.34 : 1</v>
+        <v>1.37 : 1</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5762,15 +5795,15 @@
       </c>
       <c r="B18" s="2">
         <f>January!B18+February!B18+March!B18+April!B18+May!B18+June!B18+July!B18+August!B18+September!B18+October!B18+November!B18+December!B18</f>
-        <v>223</v>
+        <v>259</v>
       </c>
       <c r="C18" s="2">
         <f>January!C18+February!C18+March!C18+April!C18+May!C18+June!C18+July!C18+August!C18+September!C18+October!C18+November!C18+December!C18</f>
-        <v>350</v>
+        <v>422</v>
       </c>
       <c r="D18" s="2">
         <f>January!D18+February!D18+March!D18+April!D18+May!D18+June!D18+July!D18+August!D18+September!D18+October!D18+November!D18+December!D18</f>
-        <v>-127</v>
+        <v>-163</v>
       </c>
       <c r="E18" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5782,7 +5815,7 @@
       </c>
       <c r="G18" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.64 : 1</v>
+        <v>0.61 : 1</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5791,15 +5824,15 @@
       </c>
       <c r="B19" s="4">
         <f>January!B19+February!B19+March!B19+April!B19+May!B19+June!B19+July!B19+August!B19+September!B19+October!B19+November!B19+December!B19</f>
-        <v>1806</v>
+        <v>2194</v>
       </c>
       <c r="C19" s="4">
         <f>January!C19+February!C19+March!C19+April!C19+May!C19+June!C19+July!C19+August!C19+September!C19+October!C19+November!C19+December!C19</f>
-        <v>1694</v>
+        <v>2093</v>
       </c>
       <c r="D19" s="4">
         <f>January!D19+February!D19+March!D19+April!D19+May!D19+June!D19+July!D19+August!D19+September!D19+October!D19+November!D19+December!D19</f>
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="E19" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5811,7 +5844,7 @@
       </c>
       <c r="G19" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.07 : 1</v>
+        <v>1.05 : 1</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5820,15 +5853,15 @@
       </c>
       <c r="B20" s="2">
         <f>January!B20+February!B20+March!B20+April!B20+May!B20+June!B20+July!B20+August!B20+September!B20+October!B20+November!B20+December!B20</f>
-        <v>110</v>
+        <v>133</v>
       </c>
       <c r="C20" s="2">
         <f>January!C20+February!C20+March!C20+April!C20+May!C20+June!C20+July!C20+August!C20+September!C20+October!C20+November!C20+December!C20</f>
-        <v>219</v>
+        <v>267</v>
       </c>
       <c r="D20" s="2">
         <f>January!D20+February!D20+March!D20+April!D20+May!D20+June!D20+July!D20+August!D20+September!D20+October!D20+November!D20+December!D20</f>
-        <v>-109</v>
+        <v>-134</v>
       </c>
       <c r="E20" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5849,15 +5882,15 @@
       </c>
       <c r="B21" s="4">
         <f>January!B21+February!B21+March!B21+April!B21+May!B21+June!B21+July!B21+August!B21+September!B21+October!B21+November!B21+December!B21</f>
-        <v>1956</v>
+        <v>2434</v>
       </c>
       <c r="C21" s="4">
         <f>January!C21+February!C21+March!C21+April!C21+May!C21+June!C21+July!C21+August!C21+September!C21+October!C21+November!C21+December!C21</f>
-        <v>1277</v>
+        <v>1619</v>
       </c>
       <c r="D21" s="4">
         <f>January!D21+February!D21+March!D21+April!D21+May!D21+June!D21+July!D21+August!D21+September!D21+October!D21+November!D21+December!D21</f>
-        <v>679</v>
+        <v>815</v>
       </c>
       <c r="E21" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5869,7 +5902,7 @@
       </c>
       <c r="G21" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.53 : 1</v>
+        <v>1.5 : 1</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5878,15 +5911,15 @@
       </c>
       <c r="B22" s="2">
         <f>January!B22+February!B22+March!B22+April!B22+May!B22+June!B22+July!B22+August!B22+September!B22+October!B22+November!B22+December!B22</f>
-        <v>239</v>
+        <v>335</v>
       </c>
       <c r="C22" s="2">
         <f>January!C22+February!C22+March!C22+April!C22+May!C22+June!C22+July!C22+August!C22+September!C22+October!C22+November!C22+December!C22</f>
-        <v>984</v>
+        <v>1201</v>
       </c>
       <c r="D22" s="2">
         <f>January!D22+February!D22+March!D22+April!D22+May!D22+June!D22+July!D22+August!D22+September!D22+October!D22+November!D22+December!D22</f>
-        <v>-745</v>
+        <v>-866</v>
       </c>
       <c r="E22" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5898,7 +5931,7 @@
       </c>
       <c r="G22" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.24 : 1</v>
+        <v>0.28 : 1</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5907,15 +5940,15 @@
       </c>
       <c r="B23" s="4">
         <f>January!B23+February!B23+March!B23+April!B23+May!B23+June!B23+July!B23+August!B23+September!B23+October!B23+November!B23+December!B23</f>
-        <v>2509</v>
+        <v>3123</v>
       </c>
       <c r="C23" s="4">
         <f>January!C23+February!C23+March!C23+April!C23+May!C23+June!C23+July!C23+August!C23+September!C23+October!C23+November!C23+December!C23</f>
-        <v>1642</v>
+        <v>2304</v>
       </c>
       <c r="D23" s="4">
         <f>January!D23+February!D23+March!D23+April!D23+May!D23+June!D23+July!D23+August!D23+September!D23+October!D23+November!D23+December!D23</f>
-        <v>867</v>
+        <v>819</v>
       </c>
       <c r="E23" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5927,7 +5960,7 @@
       </c>
       <c r="G23" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.53 : 1</v>
+        <v>1.36 : 1</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5936,15 +5969,15 @@
       </c>
       <c r="B24" s="2">
         <f>January!B24+February!B24+March!B24+April!B24+May!B24+June!B24+July!B24+August!B24+September!B24+October!B24+November!B24+December!B24</f>
-        <v>6110</v>
+        <v>7678</v>
       </c>
       <c r="C24" s="2">
         <f>January!C24+February!C24+March!C24+April!C24+May!C24+June!C24+July!C24+August!C24+September!C24+October!C24+November!C24+December!C24</f>
-        <v>4534</v>
+        <v>5663</v>
       </c>
       <c r="D24" s="2">
         <f>January!D24+February!D24+March!D24+April!D24+May!D24+June!D24+July!D24+August!D24+September!D24+October!D24+November!D24+December!D24</f>
-        <v>1576</v>
+        <v>2015</v>
       </c>
       <c r="E24" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5956,7 +5989,7 @@
       </c>
       <c r="G24" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.35 : 1</v>
+        <v>1.36 : 1</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5965,15 +5998,15 @@
       </c>
       <c r="B25" s="4">
         <f>January!B25+February!B25+March!B25+April!B25+May!B25+June!B25+July!B25+August!B25+September!B25+October!B25+November!B25+December!B25</f>
-        <v>654</v>
+        <v>757</v>
       </c>
       <c r="C25" s="4">
         <f>January!C25+February!C25+March!C25+April!C25+May!C25+June!C25+July!C25+August!C25+September!C25+October!C25+November!C25+December!C25</f>
-        <v>1740</v>
+        <v>2190</v>
       </c>
       <c r="D25" s="4">
         <f>January!D25+February!D25+March!D25+April!D25+May!D25+June!D25+July!D25+August!D25+September!D25+October!D25+November!D25+December!D25</f>
-        <v>-1086</v>
+        <v>-1433</v>
       </c>
       <c r="E25" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5985,7 +6018,7 @@
       </c>
       <c r="G25" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.38 : 1</v>
+        <v>0.35 : 1</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6023,15 +6056,15 @@
       </c>
       <c r="B27" s="4">
         <f>January!B27+February!B27+March!B27+April!B27+May!B27+June!B27+July!B27+August!B27+September!B27+October!B27+November!B27+December!B27</f>
-        <v>748</v>
+        <v>923</v>
       </c>
       <c r="C27" s="4">
         <f>January!C27+February!C27+March!C27+April!C27+May!C27+June!C27+July!C27+August!C27+September!C27+October!C27+November!C27+December!C27</f>
-        <v>639</v>
+        <v>780</v>
       </c>
       <c r="D27" s="4">
         <f>January!D27+February!D27+March!D27+April!D27+May!D27+June!D27+July!D27+August!D27+September!D27+October!D27+November!D27+December!D27</f>
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="E27" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6043,7 +6076,7 @@
       </c>
       <c r="G27" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.17 : 1</v>
+        <v>1.18 : 1</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6052,15 +6085,15 @@
       </c>
       <c r="B28" s="2">
         <f>January!B28+February!B28+March!B28+April!B28+May!B28+June!B28+July!B28+August!B28+September!B28+October!B28+November!B28+December!B28</f>
-        <v>462</v>
+        <v>553</v>
       </c>
       <c r="C28" s="2">
         <f>January!C28+February!C28+March!C28+April!C28+May!C28+June!C28+July!C28+August!C28+September!C28+October!C28+November!C28+December!C28</f>
-        <v>446</v>
+        <v>527</v>
       </c>
       <c r="D28" s="2">
         <f>January!D28+February!D28+March!D28+April!D28+May!D28+June!D28+July!D28+August!D28+September!D28+October!D28+November!D28+December!D28</f>
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E28" s="28" t="str">
         <f t="shared" si="0"/>
@@ -6072,7 +6105,7 @@
       </c>
       <c r="G28" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.04 : 1</v>
+        <v>1.05 : 1</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6081,15 +6114,15 @@
       </c>
       <c r="B29" s="4">
         <f>January!B29+February!B29+March!B29+April!B29+May!B29+June!B29+July!B29+August!B29+September!B29+October!B29+November!B29+December!B29</f>
-        <v>2930</v>
+        <v>3441</v>
       </c>
       <c r="C29" s="4">
         <f>January!C29+February!C29+March!C29+April!C29+May!C29+June!C29+July!C29+August!C29+September!C29+October!C29+November!C29+December!C29</f>
-        <v>2017</v>
+        <v>2406</v>
       </c>
       <c r="D29" s="4">
         <f>January!D29+February!D29+March!D29+April!D29+May!D29+June!D29+July!D29+August!D29+September!D29+October!D29+November!D29+December!D29</f>
-        <v>913</v>
+        <v>1035</v>
       </c>
       <c r="E29" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6101,7 +6134,7 @@
       </c>
       <c r="G29" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.45 : 1</v>
+        <v>1.43 : 1</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6110,15 +6143,15 @@
       </c>
       <c r="B30" s="2">
         <f>January!B30+February!B30+March!B30+April!B30+May!B30+June!B30+July!B30+August!B30+September!B30+October!B30+November!B30+December!B30</f>
-        <v>147</v>
+        <v>174</v>
       </c>
       <c r="C30" s="2">
         <f>January!C30+February!C30+March!C30+April!C30+May!C30+June!C30+July!C30+August!C30+September!C30+October!C30+November!C30+December!C30</f>
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="D30" s="2">
         <f>January!D30+February!D30+March!D30+April!D30+May!D30+June!D30+July!D30+August!D30+September!D30+October!D30+November!D30+December!D30</f>
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E30" s="28" t="str">
         <f t="shared" si="0"/>
@@ -6130,7 +6163,7 @@
       </c>
       <c r="G30" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.65 : 1</v>
+        <v>1.51 : 1</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6139,15 +6172,15 @@
       </c>
       <c r="B31" s="4">
         <f>January!B31+February!B31+March!B31+April!B31+May!B31+June!B31+July!B31+August!B31+September!B31+October!B31+November!B31+December!B31</f>
-        <v>225</v>
+        <v>293</v>
       </c>
       <c r="C31" s="4">
         <f>January!C31+February!C31+March!C31+April!C31+May!C31+June!C31+July!C31+August!C31+September!C31+October!C31+November!C31+December!C31</f>
-        <v>1019</v>
+        <v>1269</v>
       </c>
       <c r="D31" s="4">
         <f>January!D31+February!D31+March!D31+April!D31+May!D31+June!D31+July!D31+August!D31+September!D31+October!D31+November!D31+December!D31</f>
-        <v>-794</v>
+        <v>-976</v>
       </c>
       <c r="E31" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6159,7 +6192,7 @@
       </c>
       <c r="G31" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.22 : 1</v>
+        <v>0.23 : 1</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6168,15 +6201,15 @@
       </c>
       <c r="B32" s="2">
         <f>January!B32+February!B32+March!B32+April!B32+May!B32+June!B32+July!B32+August!B32+September!B32+October!B32+November!B32+December!B32</f>
-        <v>1527</v>
+        <v>1986</v>
       </c>
       <c r="C32" s="2">
         <f>January!C32+February!C32+March!C32+April!C32+May!C32+June!C32+July!C32+August!C32+September!C32+October!C32+November!C32+December!C32</f>
-        <v>2186</v>
+        <v>2754</v>
       </c>
       <c r="D32" s="2">
         <f>January!D32+February!D32+March!D32+April!D32+May!D32+June!D32+July!D32+August!D32+September!D32+October!D32+November!D32+December!D32</f>
-        <v>-659</v>
+        <v>-768</v>
       </c>
       <c r="E32" s="28" t="str">
         <f t="shared" si="0"/>
@@ -6188,7 +6221,7 @@
       </c>
       <c r="G32" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.7 : 1</v>
+        <v>0.72 : 1</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6197,15 +6230,15 @@
       </c>
       <c r="B33" s="4">
         <f>January!B33+February!B33+March!B33+April!B33+May!B33+June!B33+July!B33+August!B33+September!B33+October!B33+November!B33+December!B33</f>
-        <v>1670</v>
+        <v>2138</v>
       </c>
       <c r="C33" s="4">
         <f>January!C33+February!C33+March!C33+April!C33+May!C33+June!C33+July!C33+August!C33+September!C33+October!C33+November!C33+December!C33</f>
-        <v>1843</v>
+        <v>2219</v>
       </c>
       <c r="D33" s="4">
         <f>January!D33+February!D33+March!D33+April!D33+May!D33+June!D33+July!D33+August!D33+September!D33+October!D33+November!D33+December!D33</f>
-        <v>-173</v>
+        <v>-81</v>
       </c>
       <c r="E33" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6217,7 +6250,7 @@
       </c>
       <c r="G33" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.91 : 1</v>
+        <v>0.96 : 1</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6226,15 +6259,15 @@
       </c>
       <c r="B34" s="2">
         <f>January!B34+February!B34+March!B34+April!B34+May!B34+June!B34+July!B34+August!B34+September!B34+October!B34+November!B34+December!B34</f>
-        <v>761</v>
+        <v>968</v>
       </c>
       <c r="C34" s="2">
         <f>January!C34+February!C34+March!C34+April!C34+May!C34+June!C34+July!C34+August!C34+September!C34+October!C34+November!C34+December!C34</f>
-        <v>653</v>
+        <v>801</v>
       </c>
       <c r="D34" s="2">
         <f>January!D34+February!D34+March!D34+April!D34+May!D34+June!D34+July!D34+August!D34+September!D34+October!D34+November!D34+December!D34</f>
-        <v>108</v>
+        <v>167</v>
       </c>
       <c r="E34" s="28" t="str">
         <f t="shared" ref="E34:E54" si="3">IF(D34 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -6246,7 +6279,7 @@
       </c>
       <c r="G34" s="3" t="str">
         <f t="shared" ref="G34:G54" si="5">IF(ISERROR(ROUND(B34/C34,2)&amp;" : 1"), "", ROUND(B34/C34,2)&amp;" : 1")</f>
-        <v>1.17 : 1</v>
+        <v>1.21 : 1</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6255,15 +6288,15 @@
       </c>
       <c r="B35" s="4">
         <f>January!B35+February!B35+March!B35+April!B35+May!B35+June!B35+July!B35+August!B35+September!B35+October!B35+November!B35+December!B35</f>
-        <v>3335</v>
+        <v>4249</v>
       </c>
       <c r="C35" s="4">
         <f>January!C35+February!C35+March!C35+April!C35+May!C35+June!C35+July!C35+August!C35+September!C35+October!C35+November!C35+December!C35</f>
-        <v>4891</v>
+        <v>6224</v>
       </c>
       <c r="D35" s="4">
         <f>January!D35+February!D35+March!D35+April!D35+May!D35+June!D35+July!D35+August!D35+September!D35+October!D35+November!D35+December!D35</f>
-        <v>-1556</v>
+        <v>-1975</v>
       </c>
       <c r="E35" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6284,15 +6317,15 @@
       </c>
       <c r="B36" s="2">
         <f>January!B36+February!B36+March!B36+April!B36+May!B36+June!B36+July!B36+August!B36+September!B36+October!B36+November!B36+December!B36</f>
-        <v>643</v>
+        <v>788</v>
       </c>
       <c r="C36" s="2">
         <f>January!C36+February!C36+March!C36+April!C36+May!C36+June!C36+July!C36+August!C36+September!C36+October!C36+November!C36+December!C36</f>
-        <v>2145</v>
+        <v>2659</v>
       </c>
       <c r="D36" s="2">
         <f>January!D36+February!D36+March!D36+April!D36+May!D36+June!D36+July!D36+August!D36+September!D36+October!D36+November!D36+December!D36</f>
-        <v>-1502</v>
+        <v>-1871</v>
       </c>
       <c r="E36" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6313,15 +6346,15 @@
       </c>
       <c r="B37" s="4">
         <f>January!B37+February!B37+March!B37+April!B37+May!B37+June!B37+July!B37+August!B37+September!B37+October!B37+November!B37+December!B37</f>
-        <v>1993</v>
+        <v>2481</v>
       </c>
       <c r="C37" s="4">
         <f>January!C37+February!C37+March!C37+April!C37+May!C37+June!C37+July!C37+August!C37+September!C37+October!C37+November!C37+December!C37</f>
-        <v>1059</v>
+        <v>1280</v>
       </c>
       <c r="D37" s="4">
         <f>January!D37+February!D37+March!D37+April!D37+May!D37+June!D37+July!D37+August!D37+September!D37+October!D37+November!D37+December!D37</f>
-        <v>934</v>
+        <v>1201</v>
       </c>
       <c r="E37" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6333,7 +6366,7 @@
       </c>
       <c r="G37" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>1.88 : 1</v>
+        <v>1.94 : 1</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6342,15 +6375,15 @@
       </c>
       <c r="B38" s="2">
         <f>January!B38+February!B38+March!B38+April!B38+May!B38+June!B38+July!B38+August!B38+September!B38+October!B38+November!B38+December!B38</f>
-        <v>74</v>
+        <v>107</v>
       </c>
       <c r="C38" s="2">
         <f>January!C38+February!C38+March!C38+April!C38+May!C38+June!C38+July!C38+August!C38+September!C38+October!C38+November!C38+December!C38</f>
-        <v>687</v>
+        <v>821</v>
       </c>
       <c r="D38" s="2">
         <f>January!D38+February!D38+March!D38+April!D38+May!D38+June!D38+July!D38+August!D38+September!D38+October!D38+November!D38+December!D38</f>
-        <v>-613</v>
+        <v>-714</v>
       </c>
       <c r="E38" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6362,7 +6395,7 @@
       </c>
       <c r="G38" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.11 : 1</v>
+        <v>0.13 : 1</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6375,11 +6408,11 @@
       </c>
       <c r="C39" s="4">
         <f>January!C39+February!C39+March!C39+April!C39+May!C39+June!C39+July!C39+August!C39+September!C39+October!C39+November!C39+December!C39</f>
-        <v>429</v>
+        <v>487</v>
       </c>
       <c r="D39" s="4">
         <f>January!D39+February!D39+March!D39+April!D39+May!D39+June!D39+July!D39+August!D39+September!D39+October!D39+November!D39+December!D39</f>
-        <v>-230</v>
+        <v>-288</v>
       </c>
       <c r="E39" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6391,7 +6424,7 @@
       </c>
       <c r="G39" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.46 : 1</v>
+        <v>0.41 : 1</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6400,15 +6433,15 @@
       </c>
       <c r="B40" s="38">
         <f>January!B40+February!B40+March!B40+April!B40+May!B40+June!B40+July!B40+August!B40+September!B40+October!B40+November!B40+December!B40</f>
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="C40" s="38">
         <f>January!C40+February!C40+March!C40+April!C40+May!C40+June!C40+July!C40+August!C40+September!C40+October!C40+November!C40+December!C40</f>
-        <v>351</v>
+        <v>400</v>
       </c>
       <c r="D40" s="38">
         <f>January!D40+February!D40+March!D40+April!D40+May!D40+June!D40+July!D40+August!D40+September!D40+October!D40+November!D40+December!D40</f>
-        <v>-140</v>
+        <v>-181</v>
       </c>
       <c r="E40" s="39" t="str">
         <f t="shared" si="3"/>
@@ -6420,7 +6453,7 @@
       </c>
       <c r="G40" s="40" t="str">
         <f t="shared" si="5"/>
-        <v>0.6 : 1</v>
+        <v>0.55 : 1</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6429,15 +6462,15 @@
       </c>
       <c r="B41" s="8">
         <f>January!B41+February!B41+March!B41+April!B41+May!B41+June!B41+July!B41+August!B41+September!B41+October!B41+November!B41+December!B41</f>
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C41" s="8">
         <f>January!C41+February!C41+March!C41+April!C41+May!C41+June!C41+July!C41+August!C41+September!C41+October!C41+November!C41+December!C41</f>
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="D41" s="8">
         <f>January!D41+February!D41+March!D41+April!D41+May!D41+June!D41+July!D41+August!D41+September!D41+October!D41+November!D41+December!D41</f>
-        <v>-9</v>
+        <v>-15</v>
       </c>
       <c r="E41" s="31" t="str">
         <f t="shared" si="3"/>
@@ -6449,7 +6482,7 @@
       </c>
       <c r="G41" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0.96 : 1</v>
+        <v>0.94 : 1</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6462,11 +6495,11 @@
       </c>
       <c r="C42" s="38">
         <f>January!C42+February!C42+March!C42+April!C42+May!C42+June!C42+July!C42+August!C42+September!C42+October!C42+November!C42+December!C42</f>
-        <v>168</v>
+        <v>199</v>
       </c>
       <c r="D42" s="38">
         <f>January!D42+February!D42+March!D42+April!D42+May!D42+June!D42+July!D42+August!D42+September!D42+October!D42+November!D42+December!D42</f>
-        <v>-135</v>
+        <v>-166</v>
       </c>
       <c r="E42" s="39" t="str">
         <f t="shared" si="3"/>
@@ -6478,7 +6511,7 @@
       </c>
       <c r="G42" s="40" t="str">
         <f t="shared" si="5"/>
-        <v>0.2 : 1</v>
+        <v>0.17 : 1</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6487,15 +6520,15 @@
       </c>
       <c r="B43" s="8">
         <f>January!B43+February!B43+March!B43+April!B43+May!B43+June!B43+July!B43+August!B43+September!B43+October!B43+November!B43+December!B43</f>
-        <v>142</v>
+        <v>201</v>
       </c>
       <c r="C43" s="8">
         <f>January!C43+February!C43+March!C43+April!C43+May!C43+June!C43+July!C43+August!C43+September!C43+October!C43+November!C43+December!C43</f>
-        <v>239</v>
+        <v>312</v>
       </c>
       <c r="D43" s="8">
         <f>January!D43+February!D43+March!D43+April!D43+May!D43+June!D43+July!D43+August!D43+September!D43+October!D43+November!D43+December!D43</f>
-        <v>-97</v>
+        <v>-111</v>
       </c>
       <c r="E43" s="31" t="str">
         <f t="shared" si="3"/>
@@ -6507,7 +6540,7 @@
       </c>
       <c r="G43" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0.59 : 1</v>
+        <v>0.64 : 1</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6516,15 +6549,15 @@
       </c>
       <c r="B44" s="2">
         <f>January!B44+February!B44+March!B44+April!B44+May!B44+June!B44+July!B44+August!B44+September!B44+October!B44+November!B44+December!B44</f>
-        <v>202</v>
+        <v>247</v>
       </c>
       <c r="C44" s="2">
         <f>January!C44+February!C44+March!C44+April!C44+May!C44+June!C44+July!C44+August!C44+September!C44+October!C44+November!C44+December!C44</f>
-        <v>807</v>
+        <v>1010</v>
       </c>
       <c r="D44" s="2">
         <f>January!D44+February!D44+March!D44+April!D44+May!D44+June!D44+July!D44+August!D44+September!D44+October!D44+November!D44+December!D44</f>
-        <v>-605</v>
+        <v>-763</v>
       </c>
       <c r="E44" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6536,7 +6569,7 @@
       </c>
       <c r="G44" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.25 : 1</v>
+        <v>0.24 : 1</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6545,15 +6578,15 @@
       </c>
       <c r="B45" s="4">
         <f>January!B45+February!B45+March!B45+April!B45+May!B45+June!B45+July!B45+August!B45+September!B45+October!B45+November!B45+December!B45</f>
-        <v>2296</v>
+        <v>2823</v>
       </c>
       <c r="C45" s="4">
         <f>January!C45+February!C45+March!C45+April!C45+May!C45+June!C45+July!C45+August!C45+September!C45+October!C45+November!C45+December!C45</f>
-        <v>2166</v>
+        <v>2689</v>
       </c>
       <c r="D45" s="4">
         <f>January!D45+February!D45+March!D45+April!D45+May!D45+June!D45+July!D45+August!D45+September!D45+October!D45+November!D45+December!D45</f>
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="E45" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6565,7 +6598,7 @@
       </c>
       <c r="G45" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>1.06 : 1</v>
+        <v>1.05 : 1</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6574,15 +6607,15 @@
       </c>
       <c r="B46" s="2">
         <f>January!B46+February!B46+March!B46+April!B46+May!B46+June!B46+July!B46+August!B46+September!B46+October!B46+November!B46+December!B46</f>
-        <v>4286</v>
+        <v>5375</v>
       </c>
       <c r="C46" s="2">
         <f>January!C46+February!C46+March!C46+April!C46+May!C46+June!C46+July!C46+August!C46+September!C46+October!C46+November!C46+December!C46</f>
-        <v>2796</v>
+        <v>3359</v>
       </c>
       <c r="D46" s="2">
         <f>January!D46+February!D46+March!D46+April!D46+May!D46+June!D46+July!D46+August!D46+September!D46+October!D46+November!D46+December!D46</f>
-        <v>1490</v>
+        <v>2016</v>
       </c>
       <c r="E46" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6594,7 +6627,7 @@
       </c>
       <c r="G46" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>1.53 : 1</v>
+        <v>1.6 : 1</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6603,15 +6636,15 @@
       </c>
       <c r="B47" s="4">
         <f>January!B47+February!B47+March!B47+April!B47+May!B47+June!B47+July!B47+August!B47+September!B47+October!B47+November!B47+December!B47</f>
-        <v>892</v>
+        <v>1072</v>
       </c>
       <c r="C47" s="4">
         <f>January!C47+February!C47+March!C47+April!C47+May!C47+June!C47+July!C47+August!C47+September!C47+October!C47+November!C47+December!C47</f>
-        <v>2401</v>
+        <v>3007</v>
       </c>
       <c r="D47" s="4">
         <f>January!D47+February!D47+March!D47+April!D47+May!D47+June!D47+July!D47+August!D47+September!D47+October!D47+November!D47+December!D47</f>
-        <v>-1509</v>
+        <v>-1935</v>
       </c>
       <c r="E47" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6623,7 +6656,7 @@
       </c>
       <c r="G47" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.37 : 1</v>
+        <v>0.36 : 1</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6632,15 +6665,15 @@
       </c>
       <c r="B48" s="2">
         <f>January!B48+February!B48+March!B48+April!B48+May!B48+June!B48+July!B48+August!B48+September!B48+October!B48+November!B48+December!B48</f>
-        <v>2793</v>
+        <v>3429</v>
       </c>
       <c r="C48" s="2">
         <f>January!C48+February!C48+March!C48+April!C48+May!C48+June!C48+July!C48+August!C48+September!C48+October!C48+November!C48+December!C48</f>
-        <v>967</v>
+        <v>1156</v>
       </c>
       <c r="D48" s="2">
         <f>January!D48+February!D48+March!D48+April!D48+May!D48+June!D48+July!D48+August!D48+September!D48+October!D48+November!D48+December!D48</f>
-        <v>1826</v>
+        <v>2273</v>
       </c>
       <c r="E48" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6652,7 +6685,7 @@
       </c>
       <c r="G48" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>2.89 : 1</v>
+        <v>2.97 : 1</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6661,15 +6694,15 @@
       </c>
       <c r="B49" s="4">
         <f>January!B49+February!B49+March!B49+April!B49+May!B49+June!B49+July!B49+August!B49+September!B49+October!B49+November!B49+December!B49</f>
-        <v>3099</v>
+        <v>3943</v>
       </c>
       <c r="C49" s="4">
         <f>January!C49+February!C49+March!C49+April!C49+May!C49+June!C49+July!C49+August!C49+September!C49+October!C49+November!C49+December!C49</f>
-        <v>2192</v>
+        <v>2712</v>
       </c>
       <c r="D49" s="4">
         <f>January!D49+February!D49+March!D49+April!D49+May!D49+June!D49+July!D49+August!D49+September!D49+October!D49+November!D49+December!D49</f>
-        <v>907</v>
+        <v>1231</v>
       </c>
       <c r="E49" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6681,7 +6714,7 @@
       </c>
       <c r="G49" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>1.41 : 1</v>
+        <v>1.45 : 1</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6690,15 +6723,15 @@
       </c>
       <c r="B50" s="2">
         <f>January!B50+February!B50+March!B50+April!B50+May!B50+June!B50+July!B50+August!B50+September!B50+October!B50+November!B50+December!B50</f>
-        <v>799</v>
+        <v>947</v>
       </c>
       <c r="C50" s="2">
         <f>January!C50+February!C50+March!C50+April!C50+May!C50+June!C50+July!C50+August!C50+September!C50+October!C50+November!C50+December!C50</f>
-        <v>732</v>
+        <v>844</v>
       </c>
       <c r="D50" s="2">
         <f>January!D50+February!D50+March!D50+April!D50+May!D50+June!D50+July!D50+August!D50+September!D50+October!D50+November!D50+December!D50</f>
-        <v>67</v>
+        <v>103</v>
       </c>
       <c r="E50" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6710,7 +6743,7 @@
       </c>
       <c r="G50" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>1.09 : 1</v>
+        <v>1.12 : 1</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6719,15 +6752,15 @@
       </c>
       <c r="B51" s="4">
         <f>January!B51+February!B51+March!B51+April!B51+May!B51+June!B51+July!B51+August!B51+September!B51+October!B51+November!B51+December!B51</f>
-        <v>1550</v>
+        <v>1799</v>
       </c>
       <c r="C51" s="4">
         <f>January!C51+February!C51+March!C51+April!C51+May!C51+June!C51+July!C51+August!C51+September!C51+October!C51+November!C51+December!C51</f>
-        <v>1603</v>
+        <v>1916</v>
       </c>
       <c r="D51" s="4">
         <f>January!D51+February!D51+March!D51+April!D51+May!D51+June!D51+July!D51+August!D51+September!D51+October!D51+November!D51+December!D51</f>
-        <v>-53</v>
+        <v>-117</v>
       </c>
       <c r="E51" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6739,7 +6772,7 @@
       </c>
       <c r="G51" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.97 : 1</v>
+        <v>0.94 : 1</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6748,15 +6781,15 @@
       </c>
       <c r="B52" s="2">
         <f>January!B52+February!B52+March!B52+April!B52+May!B52+June!B52+July!B52+August!B52+September!B52+October!B52+November!B52+December!B52</f>
-        <v>735</v>
+        <v>869</v>
       </c>
       <c r="C52" s="2">
         <f>January!C52+February!C52+March!C52+April!C52+May!C52+June!C52+July!C52+August!C52+September!C52+October!C52+November!C52+December!C52</f>
-        <v>886</v>
+        <v>1074</v>
       </c>
       <c r="D52" s="2">
         <f>January!D52+February!D52+March!D52+April!D52+May!D52+June!D52+July!D52+August!D52+September!D52+October!D52+November!D52+December!D52</f>
-        <v>-151</v>
+        <v>-205</v>
       </c>
       <c r="E52" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6768,7 +6801,7 @@
       </c>
       <c r="G52" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.83 : 1</v>
+        <v>0.81 : 1</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6777,15 +6810,15 @@
       </c>
       <c r="B53" s="4">
         <f>January!B53+February!B53+March!B53+April!B53+May!B53+June!B53+July!B53+August!B53+September!B53+October!B53+November!B53+December!B53</f>
-        <v>134</v>
+        <v>163</v>
       </c>
       <c r="C53" s="4">
         <f>January!C53+February!C53+March!C53+April!C53+May!C53+June!C53+July!C53+August!C53+September!C53+October!C53+November!C53+December!C53</f>
-        <v>1016</v>
+        <v>1303</v>
       </c>
       <c r="D53" s="4">
         <f>January!D53+February!D53+March!D53+April!D53+May!D53+June!D53+July!D53+August!D53+September!D53+October!D53+November!D53+December!D53</f>
-        <v>-882</v>
+        <v>-1140</v>
       </c>
       <c r="E53" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6806,15 +6839,15 @@
       </c>
       <c r="B54" s="10">
         <f>January!B54+February!B54+March!B54+April!B54+May!B54+June!B54+July!B54+August!B54+September!B54+October!B54+November!B54+December!B54</f>
-        <v>1447</v>
+        <v>1880</v>
       </c>
       <c r="C54" s="10">
         <f>January!C54+February!C54+March!C54+April!C54+May!C54+June!C54+July!C54+August!C54+September!C54+October!C54+November!C54+December!C54</f>
-        <v>867</v>
+        <v>1096</v>
       </c>
       <c r="D54" s="10">
         <f>January!D54+February!D54+March!D54+April!D54+May!D54+June!D54+July!D54+August!D54+September!D54+October!D54+November!D54+December!D54</f>
-        <v>580</v>
+        <v>784</v>
       </c>
       <c r="E54" s="32" t="str">
         <f t="shared" si="3"/>
@@ -6826,7 +6859,7 @@
       </c>
       <c r="G54" s="11" t="str">
         <f t="shared" si="5"/>
-        <v>1.67 : 1</v>
+        <v>1.72 : 1</v>
       </c>
     </row>
   </sheetData>
@@ -10443,7 +10476,7 @@
       <selection activeCell="A42" activeCellId="1" sqref="A40:G40 A42:G42"/>
       <selection pane="topRight" activeCell="A42" activeCellId="1" sqref="A40:G40 A42:G42"/>
       <selection pane="bottomLeft" activeCell="A42" activeCellId="1" sqref="A40:G40 A42:G42"/>
-      <selection pane="bottomRight" activeCell="A42" activeCellId="1" sqref="A40:G40 A42:G42"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10483,109 +10516,207 @@
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="28"/>
+      <c r="B2" s="18">
+        <v>1404</v>
+      </c>
+      <c r="C2" s="18">
+        <v>1167</v>
+      </c>
+      <c r="D2" s="18">
+        <v>237</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F2" s="28"/>
-      <c r="G2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="29"/>
+      <c r="B3" s="21">
+        <v>579</v>
+      </c>
+      <c r="C3" s="21">
+        <v>360</v>
+      </c>
+      <c r="D3" s="21">
+        <v>219</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F3" s="29"/>
-      <c r="G3" s="5"/>
+      <c r="G3" s="5" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="28"/>
+      <c r="B4" s="18">
+        <v>1147</v>
+      </c>
+      <c r="C4" s="18">
+        <v>1077</v>
+      </c>
+      <c r="D4" s="18">
+        <v>70</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F4" s="28"/>
-      <c r="G4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
+      <c r="B5" s="21">
+        <v>15</v>
+      </c>
+      <c r="C5" s="21">
+        <v>146</v>
+      </c>
+      <c r="D5" s="21">
+        <v>-131</v>
+      </c>
       <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="5"/>
+      <c r="F5" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
+      <c r="B6" s="18">
+        <v>915</v>
+      </c>
+      <c r="C6" s="18">
+        <v>1177</v>
+      </c>
+      <c r="D6" s="18">
+        <v>-262</v>
+      </c>
       <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="3"/>
+      <c r="F6" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="29"/>
+      <c r="B7" s="21">
+        <v>204</v>
+      </c>
+      <c r="C7" s="21">
+        <v>156</v>
+      </c>
+      <c r="D7" s="21">
+        <v>48</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F7" s="29"/>
-      <c r="G7" s="5"/>
+      <c r="G7" s="5" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="28"/>
+      <c r="B8" s="18">
+        <v>176</v>
+      </c>
+      <c r="C8" s="18">
+        <v>155</v>
+      </c>
+      <c r="D8" s="18">
+        <v>21</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F8" s="28"/>
-      <c r="G8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
+      <c r="B9" s="21">
+        <v>31</v>
+      </c>
+      <c r="C9" s="21">
+        <v>43</v>
+      </c>
+      <c r="D9" s="21">
+        <v>-12</v>
+      </c>
       <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="5"/>
+      <c r="F9" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
+      <c r="B10" s="18">
+        <v>0</v>
+      </c>
+      <c r="C10" s="18">
+        <v>22</v>
+      </c>
+      <c r="D10" s="18">
+        <v>-22</v>
+      </c>
       <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="3"/>
+      <c r="F10" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="29"/>
+      <c r="B11" s="21">
+        <v>11</v>
+      </c>
+      <c r="C11" s="21">
+        <v>0</v>
+      </c>
+      <c r="D11" s="21">
+        <v>11</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F11" s="29"/>
       <c r="G11" s="5"/>
     </row>
@@ -10593,163 +10724,309 @@
       <c r="A12" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="35"/>
+      <c r="B12" s="41">
+        <v>16</v>
+      </c>
+      <c r="C12" s="41">
+        <v>10</v>
+      </c>
+      <c r="D12" s="41">
+        <v>6</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>60</v>
+      </c>
       <c r="F12" s="35"/>
-      <c r="G12" s="36"/>
+      <c r="G12" s="36" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="30"/>
+      <c r="B13" s="23">
+        <v>86</v>
+      </c>
+      <c r="C13" s="23">
+        <v>76</v>
+      </c>
+      <c r="D13" s="23">
+        <v>10</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>60</v>
+      </c>
       <c r="F13" s="30"/>
-      <c r="G13" s="7"/>
+      <c r="G13" s="7" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
+      <c r="B14" s="41">
+        <v>133</v>
+      </c>
+      <c r="C14" s="41">
+        <v>191</v>
+      </c>
+      <c r="D14" s="41">
+        <v>-58</v>
+      </c>
       <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="36"/>
+      <c r="F14" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="36" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
+      <c r="B15" s="23">
+        <v>63</v>
+      </c>
+      <c r="C15" s="23">
+        <v>133</v>
+      </c>
+      <c r="D15" s="23">
+        <v>-70</v>
+      </c>
       <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="7"/>
+      <c r="F15" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="B16" s="18">
+        <v>70</v>
+      </c>
+      <c r="C16" s="18">
+        <v>177</v>
+      </c>
+      <c r="D16" s="18">
+        <v>-107</v>
+      </c>
       <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="3"/>
+      <c r="F16" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="29"/>
+      <c r="B17" s="21">
+        <v>645</v>
+      </c>
+      <c r="C17" s="21">
+        <v>428</v>
+      </c>
+      <c r="D17" s="21">
+        <v>217</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F17" s="29"/>
-      <c r="G17" s="5"/>
+      <c r="G17" s="5" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
+      <c r="B18" s="18">
+        <v>36</v>
+      </c>
+      <c r="C18" s="18">
+        <v>72</v>
+      </c>
+      <c r="D18" s="18">
+        <v>-36</v>
+      </c>
       <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="3"/>
+      <c r="F18" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
+      <c r="B19" s="21">
+        <v>388</v>
+      </c>
+      <c r="C19" s="21">
+        <v>399</v>
+      </c>
+      <c r="D19" s="21">
+        <v>-11</v>
+      </c>
       <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="5"/>
+      <c r="F19" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+      <c r="B20" s="18">
+        <v>23</v>
+      </c>
+      <c r="C20" s="18">
+        <v>48</v>
+      </c>
+      <c r="D20" s="18">
+        <v>-25</v>
+      </c>
       <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="3"/>
+      <c r="F20" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="29"/>
+      <c r="B21" s="21">
+        <v>478</v>
+      </c>
+      <c r="C21" s="21">
+        <v>342</v>
+      </c>
+      <c r="D21" s="21">
+        <v>136</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F21" s="29"/>
-      <c r="G21" s="5"/>
+      <c r="G21" s="5" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="B22" s="18">
+        <v>96</v>
+      </c>
+      <c r="C22" s="18">
+        <v>217</v>
+      </c>
+      <c r="D22" s="18">
+        <v>-121</v>
+      </c>
       <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="3"/>
+      <c r="F22" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
+      <c r="B23" s="21">
+        <v>614</v>
+      </c>
+      <c r="C23" s="21">
+        <v>662</v>
+      </c>
+      <c r="D23" s="21">
+        <v>-48</v>
+      </c>
       <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="5"/>
+      <c r="F23" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="28"/>
+      <c r="B24" s="18">
+        <v>1568</v>
+      </c>
+      <c r="C24" s="18">
+        <v>1129</v>
+      </c>
+      <c r="D24" s="18">
+        <v>439</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F24" s="28"/>
-      <c r="G24" s="3"/>
+      <c r="G24" s="3" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
+      <c r="B25" s="21">
+        <v>103</v>
+      </c>
+      <c r="C25" s="21">
+        <v>450</v>
+      </c>
+      <c r="D25" s="21">
+        <v>-347</v>
+      </c>
       <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="5"/>
+      <c r="F25" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
+      <c r="B26" s="18">
+        <v>0</v>
+      </c>
+      <c r="C26" s="18">
+        <v>0</v>
+      </c>
+      <c r="D26" s="18">
+        <v>0</v>
+      </c>
       <c r="E26" s="28"/>
       <c r="F26" s="28"/>
       <c r="G26" s="3"/>
@@ -10758,309 +11035,589 @@
       <c r="A27" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="29"/>
+      <c r="B27" s="21">
+        <v>175</v>
+      </c>
+      <c r="C27" s="21">
+        <v>141</v>
+      </c>
+      <c r="D27" s="21">
+        <v>34</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F27" s="29"/>
-      <c r="G27" s="5"/>
+      <c r="G27" s="5" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="28"/>
+      <c r="B28" s="18">
+        <v>91</v>
+      </c>
+      <c r="C28" s="18">
+        <v>81</v>
+      </c>
+      <c r="D28" s="18">
+        <v>10</v>
+      </c>
+      <c r="E28" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F28" s="28"/>
-      <c r="G28" s="3"/>
+      <c r="G28" s="3" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="29"/>
+      <c r="B29" s="21">
+        <v>511</v>
+      </c>
+      <c r="C29" s="21">
+        <v>389</v>
+      </c>
+      <c r="D29" s="21">
+        <v>122</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F29" s="29"/>
-      <c r="G29" s="5"/>
+      <c r="G29" s="5" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="28"/>
+      <c r="B30" s="18">
+        <v>27</v>
+      </c>
+      <c r="C30" s="18">
+        <v>26</v>
+      </c>
+      <c r="D30" s="18">
+        <v>1</v>
+      </c>
+      <c r="E30" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F30" s="28"/>
-      <c r="G30" s="3"/>
+      <c r="G30" s="3" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
+      <c r="B31" s="21">
+        <v>68</v>
+      </c>
+      <c r="C31" s="21">
+        <v>250</v>
+      </c>
+      <c r="D31" s="21">
+        <v>-182</v>
+      </c>
       <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="5"/>
+      <c r="F31" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="B32" s="18">
+        <v>459</v>
+      </c>
+      <c r="C32" s="18">
+        <v>568</v>
+      </c>
+      <c r="D32" s="18">
+        <v>-109</v>
+      </c>
       <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="3"/>
+      <c r="F32" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="29"/>
+      <c r="B33" s="21">
+        <v>468</v>
+      </c>
+      <c r="C33" s="21">
+        <v>376</v>
+      </c>
+      <c r="D33" s="21">
+        <v>92</v>
+      </c>
+      <c r="E33" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F33" s="29"/>
-      <c r="G33" s="5"/>
+      <c r="G33" s="5" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="28"/>
+      <c r="B34" s="18">
+        <v>207</v>
+      </c>
+      <c r="C34" s="18">
+        <v>148</v>
+      </c>
+      <c r="D34" s="18">
+        <v>59</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F34" s="28"/>
-      <c r="G34" s="3"/>
+      <c r="G34" s="3" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
+      <c r="B35" s="21">
+        <v>914</v>
+      </c>
+      <c r="C35" s="21">
+        <v>1333</v>
+      </c>
+      <c r="D35" s="21">
+        <v>-419</v>
+      </c>
       <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="5"/>
+      <c r="F35" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="B36" s="18">
+        <v>145</v>
+      </c>
+      <c r="C36" s="18">
+        <v>514</v>
+      </c>
+      <c r="D36" s="18">
+        <v>-369</v>
+      </c>
       <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="3"/>
+      <c r="F36" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="29"/>
+      <c r="B37" s="21">
+        <v>488</v>
+      </c>
+      <c r="C37" s="21">
+        <v>221</v>
+      </c>
+      <c r="D37" s="21">
+        <v>267</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F37" s="29"/>
-      <c r="G37" s="5"/>
+      <c r="G37" s="5" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
+      <c r="B38" s="18">
+        <v>33</v>
+      </c>
+      <c r="C38" s="18">
+        <v>134</v>
+      </c>
+      <c r="D38" s="18">
+        <v>-101</v>
+      </c>
       <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="3"/>
+      <c r="F38" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="B39" s="21"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
+      <c r="B39" s="21">
+        <v>0</v>
+      </c>
+      <c r="C39" s="21">
+        <v>58</v>
+      </c>
+      <c r="D39" s="21">
+        <v>-58</v>
+      </c>
       <c r="E39" s="29"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="5"/>
+      <c r="F39" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="42"/>
-      <c r="C40" s="42"/>
-      <c r="D40" s="42"/>
+      <c r="B40" s="42">
+        <v>8</v>
+      </c>
+      <c r="C40" s="42">
+        <v>49</v>
+      </c>
+      <c r="D40" s="42">
+        <v>-41</v>
+      </c>
       <c r="E40" s="39"/>
-      <c r="F40" s="39"/>
-      <c r="G40" s="40"/>
+      <c r="F40" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="G40" s="40" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
+      <c r="B41" s="25">
+        <v>1</v>
+      </c>
+      <c r="C41" s="25">
+        <v>7</v>
+      </c>
+      <c r="D41" s="25">
+        <v>-6</v>
+      </c>
       <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="9"/>
+      <c r="F41" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="B42" s="42"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="42"/>
+      <c r="B42" s="42">
+        <v>0</v>
+      </c>
+      <c r="C42" s="42">
+        <v>31</v>
+      </c>
+      <c r="D42" s="42">
+        <v>-31</v>
+      </c>
       <c r="E42" s="39"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="40"/>
+      <c r="F42" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="G42" s="40" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
+      <c r="B43" s="25">
+        <v>59</v>
+      </c>
+      <c r="C43" s="25">
+        <v>73</v>
+      </c>
+      <c r="D43" s="25">
+        <v>-14</v>
+      </c>
       <c r="E43" s="31"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="9"/>
+      <c r="F43" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
+      <c r="B44" s="18">
+        <v>45</v>
+      </c>
+      <c r="C44" s="18">
+        <v>203</v>
+      </c>
+      <c r="D44" s="18">
+        <v>-158</v>
+      </c>
       <c r="E44" s="28"/>
-      <c r="F44" s="28"/>
-      <c r="G44" s="3"/>
+      <c r="F44" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="21"/>
-      <c r="C45" s="21"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="29"/>
+      <c r="B45" s="21">
+        <v>527</v>
+      </c>
+      <c r="C45" s="21">
+        <v>523</v>
+      </c>
+      <c r="D45" s="21">
+        <v>4</v>
+      </c>
+      <c r="E45" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F45" s="29"/>
-      <c r="G45" s="5"/>
+      <c r="G45" s="5" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="28"/>
+      <c r="B46" s="18">
+        <v>1089</v>
+      </c>
+      <c r="C46" s="18">
+        <v>563</v>
+      </c>
+      <c r="D46" s="18">
+        <v>526</v>
+      </c>
+      <c r="E46" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F46" s="28"/>
-      <c r="G46" s="3"/>
+      <c r="G46" s="3" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="21"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
+      <c r="B47" s="21">
+        <v>180</v>
+      </c>
+      <c r="C47" s="21">
+        <v>606</v>
+      </c>
+      <c r="D47" s="21">
+        <v>-426</v>
+      </c>
       <c r="E47" s="29"/>
-      <c r="F47" s="29"/>
-      <c r="G47" s="5"/>
+      <c r="F47" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="28"/>
+      <c r="B48" s="18">
+        <v>636</v>
+      </c>
+      <c r="C48" s="18">
+        <v>189</v>
+      </c>
+      <c r="D48" s="18">
+        <v>447</v>
+      </c>
+      <c r="E48" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F48" s="28"/>
-      <c r="G48" s="3"/>
+      <c r="G48" s="3" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="21"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="29"/>
+      <c r="B49" s="21">
+        <v>844</v>
+      </c>
+      <c r="C49" s="21">
+        <v>520</v>
+      </c>
+      <c r="D49" s="21">
+        <v>324</v>
+      </c>
+      <c r="E49" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F49" s="29"/>
-      <c r="G49" s="5"/>
+      <c r="G49" s="5" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="18"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="28"/>
+      <c r="B50" s="18">
+        <v>148</v>
+      </c>
+      <c r="C50" s="18">
+        <v>112</v>
+      </c>
+      <c r="D50" s="18">
+        <v>36</v>
+      </c>
+      <c r="E50" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F50" s="28"/>
-      <c r="G50" s="3"/>
+      <c r="G50" s="3" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="21"/>
-      <c r="C51" s="21"/>
-      <c r="D51" s="21"/>
+      <c r="B51" s="21">
+        <v>249</v>
+      </c>
+      <c r="C51" s="21">
+        <v>313</v>
+      </c>
+      <c r="D51" s="21">
+        <v>-64</v>
+      </c>
       <c r="E51" s="29"/>
-      <c r="F51" s="29"/>
-      <c r="G51" s="5"/>
+      <c r="F51" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="18"/>
-      <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
+      <c r="B52" s="18">
+        <v>134</v>
+      </c>
+      <c r="C52" s="18">
+        <v>188</v>
+      </c>
+      <c r="D52" s="18">
+        <v>-54</v>
+      </c>
       <c r="E52" s="28"/>
-      <c r="F52" s="28"/>
-      <c r="G52" s="3"/>
+      <c r="F52" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="21"/>
-      <c r="C53" s="21"/>
-      <c r="D53" s="21"/>
+      <c r="B53" s="21">
+        <v>29</v>
+      </c>
+      <c r="C53" s="21">
+        <v>287</v>
+      </c>
+      <c r="D53" s="21">
+        <v>-258</v>
+      </c>
       <c r="E53" s="29"/>
-      <c r="F53" s="29"/>
-      <c r="G53" s="5"/>
+      <c r="F53" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="B54" s="27"/>
-      <c r="C54" s="27"/>
-      <c r="D54" s="27"/>
-      <c r="E54" s="32"/>
+      <c r="B54" s="27">
+        <v>433</v>
+      </c>
+      <c r="C54" s="27">
+        <v>229</v>
+      </c>
+      <c r="D54" s="27">
+        <v>204</v>
+      </c>
+      <c r="E54" s="32" t="s">
+        <v>60</v>
+      </c>
       <c r="F54" s="32"/>
-      <c r="G54" s="11"/>
+      <c r="G54" s="11" t="s">
+        <v>209</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G54" xr:uid="{00000000-0009-0000-0000-000005000000}"/>

</xml_diff>

<commit_message>
Update all remaining files for June 2025
</commit_message>
<xml_diff>
--- a/statistics_files/2025/2025_99_g_net_borrower_lender.xlsx
+++ b/statistics_files/2025/2025_99_g_net_borrower_lender.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\github\next_statistics\statistics_files\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B1B5DB-9AA2-4500-95BE-F58651F238AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A680F80-DE8F-450E-87CA-52D219EF1B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="673" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1291" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1391" uniqueCount="222">
   <si>
     <t>NET</t>
   </si>
@@ -691,6 +691,42 @@
   </si>
   <si>
     <t>1.89 : 1</t>
+  </si>
+  <si>
+    <t>2.07 : 1</t>
+  </si>
+  <si>
+    <t>0.79 : 1</t>
+  </si>
+  <si>
+    <t>0.82 : 1</t>
+  </si>
+  <si>
+    <t>2.31 : 1</t>
+  </si>
+  <si>
+    <t>1.19 : 1</t>
+  </si>
+  <si>
+    <t>0.38 : 1</t>
+  </si>
+  <si>
+    <t>0.18 : 1</t>
+  </si>
+  <si>
+    <t>0.29 : 1</t>
+  </si>
+  <si>
+    <t>2.59 : 1</t>
+  </si>
+  <si>
+    <t>1.46 : 1</t>
+  </si>
+  <si>
+    <t>1.50 : 1</t>
+  </si>
+  <si>
+    <t>2.33 : 1</t>
   </si>
 </sst>
 </file>
@@ -5290,7 +5326,7 @@
       <selection activeCell="A40" sqref="A40"/>
       <selection pane="topRight" activeCell="A40" sqref="A40"/>
       <selection pane="bottomLeft" activeCell="A40" sqref="A40"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5331,15 +5367,15 @@
       </c>
       <c r="B2" s="2">
         <f>January!B2+February!B2+March!B2+April!B2+May!B2+June!B2+July!B2+August!B2+September!B2+October!B2+November!B2+December!B2</f>
-        <v>7511</v>
+        <v>8957</v>
       </c>
       <c r="C2" s="2">
         <f>January!C2+February!C2+March!C2+April!C2+May!C2+June!C2+July!C2+August!C2+September!C2+October!C2+November!C2+December!C2</f>
-        <v>6352</v>
+        <v>7393</v>
       </c>
       <c r="D2" s="2">
         <f>January!D2+February!D2+March!D2+April!D2+May!D2+June!D2+July!D2+August!D2+September!D2+October!D2+November!D2+December!D2</f>
-        <v>1159</v>
+        <v>1564</v>
       </c>
       <c r="E2" s="28" t="str">
         <f t="shared" ref="E2:E33" si="0">IF(D2 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -5351,7 +5387,7 @@
       </c>
       <c r="G2" s="3" t="str">
         <f t="shared" ref="G2:G33" si="2">IF(ISERROR(ROUND(B2/C2,2)&amp;" : 1"), "", ROUND(B2/C2,2)&amp;" : 1")</f>
-        <v>1.18 : 1</v>
+        <v>1.21 : 1</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5360,15 +5396,15 @@
       </c>
       <c r="B3" s="4">
         <f>January!B3+February!B3+March!B3+April!B3+May!B3+June!B3+July!B3+August!B3+September!B3+October!B3+November!B3+December!B3</f>
-        <v>2880</v>
+        <v>3556</v>
       </c>
       <c r="C3" s="4">
         <f>January!C3+February!C3+March!C3+April!C3+May!C3+June!C3+July!C3+August!C3+September!C3+October!C3+November!C3+December!C3</f>
-        <v>1910</v>
+        <v>2237</v>
       </c>
       <c r="D3" s="4">
         <f>January!D3+February!D3+March!D3+April!D3+May!D3+June!D3+July!D3+August!D3+September!D3+October!D3+November!D3+December!D3</f>
-        <v>970</v>
+        <v>1319</v>
       </c>
       <c r="E3" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5380,7 +5416,7 @@
       </c>
       <c r="G3" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.51 : 1</v>
+        <v>1.59 : 1</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5389,15 +5425,15 @@
       </c>
       <c r="B4" s="2">
         <f>January!B4+February!B4+March!B4+April!B4+May!B4+June!B4+July!B4+August!B4+September!B4+October!B4+November!B4+December!B4</f>
-        <v>5527</v>
+        <v>6785</v>
       </c>
       <c r="C4" s="2">
         <f>January!C4+February!C4+March!C4+April!C4+May!C4+June!C4+July!C4+August!C4+September!C4+October!C4+November!C4+December!C4</f>
-        <v>5085</v>
+        <v>6180</v>
       </c>
       <c r="D4" s="2">
         <f>January!D4+February!D4+March!D4+April!D4+May!D4+June!D4+July!D4+August!D4+September!D4+October!D4+November!D4+December!D4</f>
-        <v>442</v>
+        <v>605</v>
       </c>
       <c r="E4" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5409,7 +5445,7 @@
       </c>
       <c r="G4" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.09 : 1</v>
+        <v>1.1 : 1</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5418,15 +5454,15 @@
       </c>
       <c r="B5" s="4">
         <f>January!B5+February!B5+March!B5+April!B5+May!B5+June!B5+July!B5+August!B5+September!B5+October!B5+November!B5+December!B5</f>
-        <v>124</v>
+        <v>186</v>
       </c>
       <c r="C5" s="4">
         <f>January!C5+February!C5+March!C5+April!C5+May!C5+June!C5+July!C5+August!C5+September!C5+October!C5+November!C5+December!C5</f>
-        <v>667</v>
+        <v>790</v>
       </c>
       <c r="D5" s="4">
         <f>January!D5+February!D5+March!D5+April!D5+May!D5+June!D5+July!D5+August!D5+September!D5+October!D5+November!D5+December!D5</f>
-        <v>-543</v>
+        <v>-604</v>
       </c>
       <c r="E5" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5438,7 +5474,7 @@
       </c>
       <c r="G5" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.19 : 1</v>
+        <v>0.24 : 1</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5447,15 +5483,15 @@
       </c>
       <c r="B6" s="2">
         <f>January!B6+February!B6+March!B6+April!B6+May!B6+June!B6+July!B6+August!B6+September!B6+October!B6+November!B6+December!B6</f>
-        <v>5117</v>
+        <v>6119</v>
       </c>
       <c r="C6" s="2">
         <f>January!C6+February!C6+March!C6+April!C6+May!C6+June!C6+July!C6+August!C6+September!C6+October!C6+November!C6+December!C6</f>
-        <v>5800</v>
+        <v>6945</v>
       </c>
       <c r="D6" s="2">
         <f>January!D6+February!D6+March!D6+April!D6+May!D6+June!D6+July!D6+August!D6+September!D6+October!D6+November!D6+December!D6</f>
-        <v>-683</v>
+        <v>-826</v>
       </c>
       <c r="E6" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5476,15 +5512,15 @@
       </c>
       <c r="B7" s="4">
         <f>January!B7+February!B7+March!B7+April!B7+May!B7+June!B7+July!B7+August!B7+September!B7+October!B7+November!B7+December!B7</f>
-        <v>1048</v>
+        <v>1302</v>
       </c>
       <c r="C7" s="4">
         <f>January!C7+February!C7+March!C7+April!C7+May!C7+June!C7+July!C7+August!C7+September!C7+October!C7+November!C7+December!C7</f>
-        <v>703</v>
+        <v>886</v>
       </c>
       <c r="D7" s="4">
         <f>January!D7+February!D7+March!D7+April!D7+May!D7+June!D7+July!D7+August!D7+September!D7+October!D7+November!D7+December!D7</f>
-        <v>345</v>
+        <v>416</v>
       </c>
       <c r="E7" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5496,7 +5532,7 @@
       </c>
       <c r="G7" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.49 : 1</v>
+        <v>1.47 : 1</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5505,15 +5541,15 @@
       </c>
       <c r="B8" s="2">
         <f>January!B8+February!B8+March!B8+April!B8+May!B8+June!B8+July!B8+August!B8+September!B8+October!B8+November!B8+December!B8</f>
-        <v>826</v>
+        <v>954</v>
       </c>
       <c r="C8" s="2">
         <f>January!C8+February!C8+March!C8+April!C8+May!C8+June!C8+July!C8+August!C8+September!C8+October!C8+November!C8+December!C8</f>
-        <v>898</v>
+        <v>1061</v>
       </c>
       <c r="D8" s="2">
         <f>January!D8+February!D8+March!D8+April!D8+May!D8+June!D8+July!D8+August!D8+September!D8+October!D8+November!D8+December!D8</f>
-        <v>-72</v>
+        <v>-107</v>
       </c>
       <c r="E8" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5525,7 +5561,7 @@
       </c>
       <c r="G8" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.92 : 1</v>
+        <v>0.9 : 1</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5534,15 +5570,15 @@
       </c>
       <c r="B9" s="4">
         <f>January!B9+February!B9+March!B9+April!B9+May!B9+June!B9+July!B9+August!B9+September!B9+October!B9+November!B9+December!B9</f>
-        <v>203</v>
+        <v>253</v>
       </c>
       <c r="C9" s="4">
         <f>January!C9+February!C9+March!C9+April!C9+May!C9+June!C9+July!C9+August!C9+September!C9+October!C9+November!C9+December!C9</f>
-        <v>347</v>
+        <v>408</v>
       </c>
       <c r="D9" s="4">
         <f>January!D9+February!D9+March!D9+April!D9+May!D9+June!D9+July!D9+August!D9+September!D9+October!D9+November!D9+December!D9</f>
-        <v>-144</v>
+        <v>-155</v>
       </c>
       <c r="E9" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5554,7 +5590,7 @@
       </c>
       <c r="G9" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.59 : 1</v>
+        <v>0.62 : 1</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5567,11 +5603,11 @@
       </c>
       <c r="C10" s="2">
         <f>January!C10+February!C10+March!C10+April!C10+May!C10+June!C10+July!C10+August!C10+September!C10+October!C10+November!C10+December!C10</f>
-        <v>206</v>
+        <v>245</v>
       </c>
       <c r="D10" s="2">
         <f>January!D10+February!D10+March!D10+April!D10+May!D10+June!D10+July!D10+August!D10+September!D10+October!D10+November!D10+December!D10</f>
-        <v>-203</v>
+        <v>-242</v>
       </c>
       <c r="E10" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5621,15 +5657,15 @@
       </c>
       <c r="B12" s="34">
         <f>January!B12+February!B12+March!B12+April!B12+May!B12+June!B12+July!B12+August!B12+September!B12+October!B12+November!B12+December!B12</f>
-        <v>147</v>
+        <v>184</v>
       </c>
       <c r="C12" s="34">
         <f>January!C12+February!C12+March!C12+April!C12+May!C12+June!C12+July!C12+August!C12+September!C12+October!C12+November!C12+December!C12</f>
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="D12" s="34">
         <f>January!D12+February!D12+March!D12+April!D12+May!D12+June!D12+July!D12+August!D12+September!D12+October!D12+November!D12+December!D12</f>
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="E12" s="35" t="str">
         <f t="shared" si="0"/>
@@ -5641,7 +5677,7 @@
       </c>
       <c r="G12" s="36" t="str">
         <f t="shared" si="2"/>
-        <v>2.26 : 1</v>
+        <v>2.27 : 1</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5650,15 +5686,15 @@
       </c>
       <c r="B13" s="6">
         <f>January!B13+February!B13+March!B13+April!B13+May!B13+June!B13+July!B13+August!B13+September!B13+October!B13+November!B13+December!B13</f>
-        <v>370</v>
+        <v>477</v>
       </c>
       <c r="C13" s="6">
         <f>January!C13+February!C13+March!C13+April!C13+May!C13+June!C13+July!C13+August!C13+September!C13+October!C13+November!C13+December!C13</f>
-        <v>347</v>
+        <v>415</v>
       </c>
       <c r="D13" s="6">
         <f>January!D13+February!D13+March!D13+April!D13+May!D13+June!D13+July!D13+August!D13+September!D13+October!D13+November!D13+December!D13</f>
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="E13" s="30" t="str">
         <f t="shared" si="0"/>
@@ -5670,7 +5706,7 @@
       </c>
       <c r="G13" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>1.07 : 1</v>
+        <v>1.15 : 1</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5679,15 +5715,15 @@
       </c>
       <c r="B14" s="34">
         <f>January!B14+February!B14+March!B14+April!B14+May!B14+June!B14+July!B14+August!B14+September!B14+October!B14+November!B14+December!B14</f>
-        <v>867</v>
+        <v>1027</v>
       </c>
       <c r="C14" s="34">
         <f>January!C14+February!C14+March!C14+April!C14+May!C14+June!C14+July!C14+August!C14+September!C14+October!C14+November!C14+December!C14</f>
-        <v>1039</v>
+        <v>1267</v>
       </c>
       <c r="D14" s="34">
         <f>January!D14+February!D14+March!D14+April!D14+May!D14+June!D14+July!D14+August!D14+September!D14+October!D14+November!D14+December!D14</f>
-        <v>-172</v>
+        <v>-240</v>
       </c>
       <c r="E14" s="35" t="str">
         <f t="shared" si="0"/>
@@ -5699,7 +5735,7 @@
       </c>
       <c r="G14" s="36" t="str">
         <f t="shared" si="2"/>
-        <v>0.83 : 1</v>
+        <v>0.81 : 1</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5708,15 +5744,15 @@
       </c>
       <c r="B15" s="6">
         <f>January!B15+February!B15+March!B15+April!B15+May!B15+June!B15+July!B15+August!B15+September!B15+October!B15+November!B15+December!B15</f>
-        <v>268</v>
+        <v>332</v>
       </c>
       <c r="C15" s="6">
         <f>January!C15+February!C15+March!C15+April!C15+May!C15+June!C15+July!C15+August!C15+September!C15+October!C15+November!C15+December!C15</f>
-        <v>752</v>
+        <v>912</v>
       </c>
       <c r="D15" s="6">
         <f>January!D15+February!D15+March!D15+April!D15+May!D15+June!D15+July!D15+August!D15+September!D15+October!D15+November!D15+December!D15</f>
-        <v>-484</v>
+        <v>-580</v>
       </c>
       <c r="E15" s="30" t="str">
         <f t="shared" si="0"/>
@@ -5737,15 +5773,15 @@
       </c>
       <c r="B16" s="2">
         <f>January!B16+February!B16+March!B16+April!B16+May!B16+June!B16+July!B16+August!B16+September!B16+October!B16+November!B16+December!B16</f>
-        <v>296</v>
+        <v>379</v>
       </c>
       <c r="C16" s="2">
         <f>January!C16+February!C16+March!C16+April!C16+May!C16+June!C16+July!C16+August!C16+September!C16+October!C16+November!C16+December!C16</f>
-        <v>884</v>
+        <v>1050</v>
       </c>
       <c r="D16" s="2">
         <f>January!D16+February!D16+March!D16+April!D16+May!D16+June!D16+July!D16+August!D16+September!D16+October!D16+November!D16+December!D16</f>
-        <v>-588</v>
+        <v>-671</v>
       </c>
       <c r="E16" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5757,7 +5793,7 @@
       </c>
       <c r="G16" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.33 : 1</v>
+        <v>0.36 : 1</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5766,15 +5802,15 @@
       </c>
       <c r="B17" s="4">
         <f>January!B17+February!B17+March!B17+April!B17+May!B17+June!B17+July!B17+August!B17+September!B17+October!B17+November!B17+December!B17</f>
-        <v>3086</v>
+        <v>3677</v>
       </c>
       <c r="C17" s="4">
         <f>January!C17+February!C17+March!C17+April!C17+May!C17+June!C17+July!C17+August!C17+September!C17+October!C17+November!C17+December!C17</f>
-        <v>2249</v>
+        <v>2739</v>
       </c>
       <c r="D17" s="4">
         <f>January!D17+February!D17+March!D17+April!D17+May!D17+June!D17+July!D17+August!D17+September!D17+October!D17+November!D17+December!D17</f>
-        <v>837</v>
+        <v>938</v>
       </c>
       <c r="E17" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5786,7 +5822,7 @@
       </c>
       <c r="G17" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.37 : 1</v>
+        <v>1.34 : 1</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5795,15 +5831,15 @@
       </c>
       <c r="B18" s="2">
         <f>January!B18+February!B18+March!B18+April!B18+May!B18+June!B18+July!B18+August!B18+September!B18+October!B18+November!B18+December!B18</f>
-        <v>259</v>
+        <v>289</v>
       </c>
       <c r="C18" s="2">
         <f>January!C18+February!C18+March!C18+April!C18+May!C18+June!C18+July!C18+August!C18+September!C18+October!C18+November!C18+December!C18</f>
-        <v>422</v>
+        <v>514</v>
       </c>
       <c r="D18" s="2">
         <f>January!D18+February!D18+March!D18+April!D18+May!D18+June!D18+July!D18+August!D18+September!D18+October!D18+November!D18+December!D18</f>
-        <v>-163</v>
+        <v>-225</v>
       </c>
       <c r="E18" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5815,7 +5851,7 @@
       </c>
       <c r="G18" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.61 : 1</v>
+        <v>0.56 : 1</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5824,15 +5860,15 @@
       </c>
       <c r="B19" s="4">
         <f>January!B19+February!B19+March!B19+April!B19+May!B19+June!B19+July!B19+August!B19+September!B19+October!B19+November!B19+December!B19</f>
-        <v>2194</v>
+        <v>2535</v>
       </c>
       <c r="C19" s="4">
         <f>January!C19+February!C19+March!C19+April!C19+May!C19+June!C19+July!C19+August!C19+September!C19+October!C19+November!C19+December!C19</f>
-        <v>2093</v>
+        <v>2457</v>
       </c>
       <c r="D19" s="4">
         <f>January!D19+February!D19+March!D19+April!D19+May!D19+June!D19+July!D19+August!D19+September!D19+October!D19+November!D19+December!D19</f>
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="E19" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5844,7 +5880,7 @@
       </c>
       <c r="G19" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.05 : 1</v>
+        <v>1.03 : 1</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5853,15 +5889,15 @@
       </c>
       <c r="B20" s="2">
         <f>January!B20+February!B20+March!B20+April!B20+May!B20+June!B20+July!B20+August!B20+September!B20+October!B20+November!B20+December!B20</f>
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="C20" s="2">
         <f>January!C20+February!C20+March!C20+April!C20+May!C20+June!C20+July!C20+August!C20+September!C20+October!C20+November!C20+December!C20</f>
-        <v>267</v>
+        <v>314</v>
       </c>
       <c r="D20" s="2">
         <f>January!D20+February!D20+March!D20+April!D20+May!D20+June!D20+July!D20+August!D20+September!D20+October!D20+November!D20+December!D20</f>
-        <v>-134</v>
+        <v>-169</v>
       </c>
       <c r="E20" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5873,7 +5909,7 @@
       </c>
       <c r="G20" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.5 : 1</v>
+        <v>0.46 : 1</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5882,15 +5918,15 @@
       </c>
       <c r="B21" s="4">
         <f>January!B21+February!B21+March!B21+April!B21+May!B21+June!B21+July!B21+August!B21+September!B21+October!B21+November!B21+December!B21</f>
-        <v>2434</v>
+        <v>2965</v>
       </c>
       <c r="C21" s="4">
         <f>January!C21+February!C21+March!C21+April!C21+May!C21+June!C21+July!C21+August!C21+September!C21+October!C21+November!C21+December!C21</f>
-        <v>1619</v>
+        <v>1964</v>
       </c>
       <c r="D21" s="4">
         <f>January!D21+February!D21+March!D21+April!D21+May!D21+June!D21+July!D21+August!D21+September!D21+October!D21+November!D21+December!D21</f>
-        <v>815</v>
+        <v>1001</v>
       </c>
       <c r="E21" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5902,7 +5938,7 @@
       </c>
       <c r="G21" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.5 : 1</v>
+        <v>1.51 : 1</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5911,15 +5947,15 @@
       </c>
       <c r="B22" s="2">
         <f>January!B22+February!B22+March!B22+April!B22+May!B22+June!B22+July!B22+August!B22+September!B22+October!B22+November!B22+December!B22</f>
-        <v>335</v>
+        <v>399</v>
       </c>
       <c r="C22" s="2">
         <f>January!C22+February!C22+March!C22+April!C22+May!C22+June!C22+July!C22+August!C22+September!C22+October!C22+November!C22+December!C22</f>
-        <v>1201</v>
+        <v>1521</v>
       </c>
       <c r="D22" s="2">
         <f>January!D22+February!D22+March!D22+April!D22+May!D22+June!D22+July!D22+August!D22+September!D22+October!D22+November!D22+December!D22</f>
-        <v>-866</v>
+        <v>-1122</v>
       </c>
       <c r="E22" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5931,7 +5967,7 @@
       </c>
       <c r="G22" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.28 : 1</v>
+        <v>0.26 : 1</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5940,15 +5976,15 @@
       </c>
       <c r="B23" s="4">
         <f>January!B23+February!B23+March!B23+April!B23+May!B23+June!B23+July!B23+August!B23+September!B23+October!B23+November!B23+December!B23</f>
-        <v>3123</v>
+        <v>3659</v>
       </c>
       <c r="C23" s="4">
         <f>January!C23+February!C23+March!C23+April!C23+May!C23+June!C23+July!C23+August!C23+September!C23+October!C23+November!C23+December!C23</f>
-        <v>2304</v>
+        <v>2968</v>
       </c>
       <c r="D23" s="4">
         <f>January!D23+February!D23+March!D23+April!D23+May!D23+June!D23+July!D23+August!D23+September!D23+October!D23+November!D23+December!D23</f>
-        <v>819</v>
+        <v>691</v>
       </c>
       <c r="E23" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5960,7 +5996,7 @@
       </c>
       <c r="G23" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.36 : 1</v>
+        <v>1.23 : 1</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5969,15 +6005,15 @@
       </c>
       <c r="B24" s="2">
         <f>January!B24+February!B24+March!B24+April!B24+May!B24+June!B24+July!B24+August!B24+September!B24+October!B24+November!B24+December!B24</f>
-        <v>7678</v>
+        <v>9041</v>
       </c>
       <c r="C24" s="2">
         <f>January!C24+February!C24+March!C24+April!C24+May!C24+June!C24+July!C24+August!C24+September!C24+October!C24+November!C24+December!C24</f>
-        <v>5663</v>
+        <v>6809</v>
       </c>
       <c r="D24" s="2">
         <f>January!D24+February!D24+March!D24+April!D24+May!D24+June!D24+July!D24+August!D24+September!D24+October!D24+November!D24+December!D24</f>
-        <v>2015</v>
+        <v>2232</v>
       </c>
       <c r="E24" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5989,7 +6025,7 @@
       </c>
       <c r="G24" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.36 : 1</v>
+        <v>1.33 : 1</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5998,15 +6034,15 @@
       </c>
       <c r="B25" s="4">
         <f>January!B25+February!B25+March!B25+April!B25+May!B25+June!B25+July!B25+August!B25+September!B25+October!B25+November!B25+December!B25</f>
-        <v>757</v>
+        <v>901</v>
       </c>
       <c r="C25" s="4">
         <f>January!C25+February!C25+March!C25+April!C25+May!C25+June!C25+July!C25+August!C25+September!C25+October!C25+November!C25+December!C25</f>
-        <v>2190</v>
+        <v>2572</v>
       </c>
       <c r="D25" s="4">
         <f>January!D25+February!D25+March!D25+April!D25+May!D25+June!D25+July!D25+August!D25+September!D25+October!D25+November!D25+December!D25</f>
-        <v>-1433</v>
+        <v>-1671</v>
       </c>
       <c r="E25" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6056,15 +6092,15 @@
       </c>
       <c r="B27" s="4">
         <f>January!B27+February!B27+March!B27+April!B27+May!B27+June!B27+July!B27+August!B27+September!B27+October!B27+November!B27+December!B27</f>
-        <v>923</v>
+        <v>1126</v>
       </c>
       <c r="C27" s="4">
         <f>January!C27+February!C27+March!C27+April!C27+May!C27+June!C27+July!C27+August!C27+September!C27+October!C27+November!C27+December!C27</f>
-        <v>780</v>
+        <v>958</v>
       </c>
       <c r="D27" s="4">
         <f>January!D27+February!D27+March!D27+April!D27+May!D27+June!D27+July!D27+August!D27+September!D27+October!D27+November!D27+December!D27</f>
-        <v>143</v>
+        <v>168</v>
       </c>
       <c r="E27" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6085,15 +6121,15 @@
       </c>
       <c r="B28" s="2">
         <f>January!B28+February!B28+March!B28+April!B28+May!B28+June!B28+July!B28+August!B28+September!B28+October!B28+November!B28+December!B28</f>
-        <v>553</v>
+        <v>745</v>
       </c>
       <c r="C28" s="2">
         <f>January!C28+February!C28+March!C28+April!C28+May!C28+June!C28+July!C28+August!C28+September!C28+October!C28+November!C28+December!C28</f>
-        <v>527</v>
+        <v>649</v>
       </c>
       <c r="D28" s="2">
         <f>January!D28+February!D28+March!D28+April!D28+May!D28+June!D28+July!D28+August!D28+September!D28+October!D28+November!D28+December!D28</f>
-        <v>26</v>
+        <v>96</v>
       </c>
       <c r="E28" s="28" t="str">
         <f t="shared" si="0"/>
@@ -6105,7 +6141,7 @@
       </c>
       <c r="G28" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.05 : 1</v>
+        <v>1.15 : 1</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6114,15 +6150,15 @@
       </c>
       <c r="B29" s="4">
         <f>January!B29+February!B29+March!B29+April!B29+May!B29+June!B29+July!B29+August!B29+September!B29+October!B29+November!B29+December!B29</f>
-        <v>3441</v>
+        <v>4006</v>
       </c>
       <c r="C29" s="4">
         <f>January!C29+February!C29+March!C29+April!C29+May!C29+June!C29+July!C29+August!C29+September!C29+October!C29+November!C29+December!C29</f>
-        <v>2406</v>
+        <v>2756</v>
       </c>
       <c r="D29" s="4">
         <f>January!D29+February!D29+March!D29+April!D29+May!D29+June!D29+July!D29+August!D29+September!D29+October!D29+November!D29+December!D29</f>
-        <v>1035</v>
+        <v>1250</v>
       </c>
       <c r="E29" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6134,7 +6170,7 @@
       </c>
       <c r="G29" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.43 : 1</v>
+        <v>1.45 : 1</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6143,15 +6179,15 @@
       </c>
       <c r="B30" s="2">
         <f>January!B30+February!B30+March!B30+April!B30+May!B30+June!B30+July!B30+August!B30+September!B30+October!B30+November!B30+December!B30</f>
-        <v>174</v>
+        <v>194</v>
       </c>
       <c r="C30" s="2">
         <f>January!C30+February!C30+March!C30+April!C30+May!C30+June!C30+July!C30+August!C30+September!C30+October!C30+November!C30+December!C30</f>
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="D30" s="2">
         <f>January!D30+February!D30+March!D30+April!D30+May!D30+June!D30+July!D30+August!D30+September!D30+October!D30+November!D30+December!D30</f>
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E30" s="28" t="str">
         <f t="shared" si="0"/>
@@ -6163,7 +6199,7 @@
       </c>
       <c r="G30" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.51 : 1</v>
+        <v>1.36 : 1</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6172,15 +6208,15 @@
       </c>
       <c r="B31" s="4">
         <f>January!B31+February!B31+March!B31+April!B31+May!B31+June!B31+July!B31+August!B31+September!B31+October!B31+November!B31+December!B31</f>
-        <v>293</v>
+        <v>358</v>
       </c>
       <c r="C31" s="4">
         <f>January!C31+February!C31+March!C31+April!C31+May!C31+June!C31+July!C31+August!C31+September!C31+October!C31+November!C31+December!C31</f>
-        <v>1269</v>
+        <v>1521</v>
       </c>
       <c r="D31" s="4">
         <f>January!D31+February!D31+March!D31+April!D31+May!D31+June!D31+July!D31+August!D31+September!D31+October!D31+November!D31+December!D31</f>
-        <v>-976</v>
+        <v>-1163</v>
       </c>
       <c r="E31" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6192,7 +6228,7 @@
       </c>
       <c r="G31" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.23 : 1</v>
+        <v>0.24 : 1</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6201,15 +6237,15 @@
       </c>
       <c r="B32" s="2">
         <f>January!B32+February!B32+March!B32+April!B32+May!B32+June!B32+July!B32+August!B32+September!B32+October!B32+November!B32+December!B32</f>
-        <v>1986</v>
+        <v>2410</v>
       </c>
       <c r="C32" s="2">
         <f>January!C32+February!C32+March!C32+April!C32+May!C32+June!C32+July!C32+August!C32+September!C32+October!C32+November!C32+December!C32</f>
-        <v>2754</v>
+        <v>3287</v>
       </c>
       <c r="D32" s="2">
         <f>January!D32+February!D32+March!D32+April!D32+May!D32+June!D32+July!D32+August!D32+September!D32+October!D32+November!D32+December!D32</f>
-        <v>-768</v>
+        <v>-877</v>
       </c>
       <c r="E32" s="28" t="str">
         <f t="shared" si="0"/>
@@ -6221,7 +6257,7 @@
       </c>
       <c r="G32" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.72 : 1</v>
+        <v>0.73 : 1</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6230,15 +6266,15 @@
       </c>
       <c r="B33" s="4">
         <f>January!B33+February!B33+March!B33+April!B33+May!B33+June!B33+July!B33+August!B33+September!B33+October!B33+November!B33+December!B33</f>
-        <v>2138</v>
+        <v>2552</v>
       </c>
       <c r="C33" s="4">
         <f>January!C33+February!C33+March!C33+April!C33+May!C33+June!C33+July!C33+August!C33+September!C33+October!C33+November!C33+December!C33</f>
-        <v>2219</v>
+        <v>2609</v>
       </c>
       <c r="D33" s="4">
         <f>January!D33+February!D33+March!D33+April!D33+May!D33+June!D33+July!D33+August!D33+September!D33+October!D33+November!D33+December!D33</f>
-        <v>-81</v>
+        <v>-57</v>
       </c>
       <c r="E33" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6250,7 +6286,7 @@
       </c>
       <c r="G33" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.96 : 1</v>
+        <v>0.98 : 1</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6259,15 +6295,15 @@
       </c>
       <c r="B34" s="2">
         <f>January!B34+February!B34+March!B34+April!B34+May!B34+June!B34+July!B34+August!B34+September!B34+October!B34+November!B34+December!B34</f>
-        <v>968</v>
+        <v>1148</v>
       </c>
       <c r="C34" s="2">
         <f>January!C34+February!C34+March!C34+April!C34+May!C34+June!C34+July!C34+August!C34+September!C34+October!C34+November!C34+December!C34</f>
-        <v>801</v>
+        <v>937</v>
       </c>
       <c r="D34" s="2">
         <f>January!D34+February!D34+March!D34+April!D34+May!D34+June!D34+July!D34+August!D34+September!D34+October!D34+November!D34+December!D34</f>
-        <v>167</v>
+        <v>211</v>
       </c>
       <c r="E34" s="28" t="str">
         <f t="shared" ref="E34:E54" si="3">IF(D34 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -6279,7 +6315,7 @@
       </c>
       <c r="G34" s="3" t="str">
         <f t="shared" ref="G34:G54" si="5">IF(ISERROR(ROUND(B34/C34,2)&amp;" : 1"), "", ROUND(B34/C34,2)&amp;" : 1")</f>
-        <v>1.21 : 1</v>
+        <v>1.23 : 1</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6288,15 +6324,15 @@
       </c>
       <c r="B35" s="4">
         <f>January!B35+February!B35+March!B35+April!B35+May!B35+June!B35+July!B35+August!B35+September!B35+October!B35+November!B35+December!B35</f>
-        <v>4249</v>
+        <v>5144</v>
       </c>
       <c r="C35" s="4">
         <f>January!C35+February!C35+March!C35+April!C35+May!C35+June!C35+July!C35+August!C35+September!C35+October!C35+November!C35+December!C35</f>
-        <v>6224</v>
+        <v>7584</v>
       </c>
       <c r="D35" s="4">
         <f>January!D35+February!D35+March!D35+April!D35+May!D35+June!D35+July!D35+August!D35+September!D35+October!D35+November!D35+December!D35</f>
-        <v>-1975</v>
+        <v>-2440</v>
       </c>
       <c r="E35" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6317,15 +6353,15 @@
       </c>
       <c r="B36" s="2">
         <f>January!B36+February!B36+March!B36+April!B36+May!B36+June!B36+July!B36+August!B36+September!B36+October!B36+November!B36+December!B36</f>
-        <v>788</v>
+        <v>943</v>
       </c>
       <c r="C36" s="2">
         <f>January!C36+February!C36+March!C36+April!C36+May!C36+June!C36+July!C36+August!C36+September!C36+October!C36+November!C36+December!C36</f>
-        <v>2659</v>
+        <v>3123</v>
       </c>
       <c r="D36" s="2">
         <f>January!D36+February!D36+March!D36+April!D36+May!D36+June!D36+July!D36+August!D36+September!D36+October!D36+November!D36+December!D36</f>
-        <v>-1871</v>
+        <v>-2180</v>
       </c>
       <c r="E36" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6346,15 +6382,15 @@
       </c>
       <c r="B37" s="4">
         <f>January!B37+February!B37+March!B37+April!B37+May!B37+June!B37+July!B37+August!B37+September!B37+October!B37+November!B37+December!B37</f>
-        <v>2481</v>
+        <v>3077</v>
       </c>
       <c r="C37" s="4">
         <f>January!C37+February!C37+March!C37+April!C37+May!C37+June!C37+July!C37+August!C37+September!C37+October!C37+November!C37+December!C37</f>
-        <v>1280</v>
+        <v>1643</v>
       </c>
       <c r="D37" s="4">
         <f>January!D37+February!D37+March!D37+April!D37+May!D37+June!D37+July!D37+August!D37+September!D37+October!D37+November!D37+December!D37</f>
-        <v>1201</v>
+        <v>1434</v>
       </c>
       <c r="E37" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6366,7 +6402,7 @@
       </c>
       <c r="G37" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>1.94 : 1</v>
+        <v>1.87 : 1</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6375,15 +6411,15 @@
       </c>
       <c r="B38" s="2">
         <f>January!B38+February!B38+March!B38+April!B38+May!B38+June!B38+July!B38+August!B38+September!B38+October!B38+November!B38+December!B38</f>
-        <v>107</v>
+        <v>136</v>
       </c>
       <c r="C38" s="2">
         <f>January!C38+February!C38+March!C38+April!C38+May!C38+June!C38+July!C38+August!C38+September!C38+October!C38+November!C38+December!C38</f>
-        <v>821</v>
+        <v>985</v>
       </c>
       <c r="D38" s="2">
         <f>January!D38+February!D38+March!D38+April!D38+May!D38+June!D38+July!D38+August!D38+September!D38+October!D38+November!D38+December!D38</f>
-        <v>-714</v>
+        <v>-849</v>
       </c>
       <c r="E38" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6395,7 +6431,7 @@
       </c>
       <c r="G38" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.13 : 1</v>
+        <v>0.14 : 1</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6408,11 +6444,11 @@
       </c>
       <c r="C39" s="4">
         <f>January!C39+February!C39+March!C39+April!C39+May!C39+June!C39+July!C39+August!C39+September!C39+October!C39+November!C39+December!C39</f>
-        <v>487</v>
+        <v>494</v>
       </c>
       <c r="D39" s="4">
         <f>January!D39+February!D39+March!D39+April!D39+May!D39+June!D39+July!D39+August!D39+September!D39+October!D39+November!D39+December!D39</f>
-        <v>-288</v>
+        <v>-295</v>
       </c>
       <c r="E39" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6424,7 +6460,7 @@
       </c>
       <c r="G39" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.41 : 1</v>
+        <v>0.4 : 1</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6437,11 +6473,11 @@
       </c>
       <c r="C40" s="38">
         <f>January!C40+February!C40+March!C40+April!C40+May!C40+June!C40+July!C40+August!C40+September!C40+October!C40+November!C40+December!C40</f>
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="D40" s="38">
         <f>January!D40+February!D40+March!D40+April!D40+May!D40+June!D40+July!D40+August!D40+September!D40+October!D40+November!D40+December!D40</f>
-        <v>-181</v>
+        <v>-184</v>
       </c>
       <c r="E40" s="39" t="str">
         <f t="shared" si="3"/>
@@ -6453,7 +6489,7 @@
       </c>
       <c r="G40" s="40" t="str">
         <f t="shared" si="5"/>
-        <v>0.55 : 1</v>
+        <v>0.54 : 1</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6495,11 +6531,11 @@
       </c>
       <c r="C42" s="38">
         <f>January!C42+February!C42+March!C42+April!C42+May!C42+June!C42+July!C42+August!C42+September!C42+October!C42+November!C42+December!C42</f>
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="D42" s="38">
         <f>January!D42+February!D42+March!D42+April!D42+May!D42+June!D42+July!D42+August!D42+September!D42+October!D42+November!D42+December!D42</f>
-        <v>-166</v>
+        <v>-171</v>
       </c>
       <c r="E42" s="39" t="str">
         <f t="shared" si="3"/>
@@ -6511,7 +6547,7 @@
       </c>
       <c r="G42" s="40" t="str">
         <f t="shared" si="5"/>
-        <v>0.17 : 1</v>
+        <v>0.16 : 1</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6520,15 +6556,15 @@
       </c>
       <c r="B43" s="8">
         <f>January!B43+February!B43+March!B43+April!B43+May!B43+June!B43+July!B43+August!B43+September!B43+October!B43+November!B43+December!B43</f>
-        <v>201</v>
+        <v>305</v>
       </c>
       <c r="C43" s="8">
         <f>January!C43+February!C43+March!C43+April!C43+May!C43+June!C43+July!C43+August!C43+September!C43+October!C43+November!C43+December!C43</f>
-        <v>312</v>
+        <v>384</v>
       </c>
       <c r="D43" s="8">
         <f>January!D43+February!D43+March!D43+April!D43+May!D43+June!D43+July!D43+August!D43+September!D43+October!D43+November!D43+December!D43</f>
-        <v>-111</v>
+        <v>-79</v>
       </c>
       <c r="E43" s="31" t="str">
         <f t="shared" si="3"/>
@@ -6540,7 +6576,7 @@
       </c>
       <c r="G43" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0.64 : 1</v>
+        <v>0.79 : 1</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6549,15 +6585,15 @@
       </c>
       <c r="B44" s="2">
         <f>January!B44+February!B44+March!B44+April!B44+May!B44+June!B44+July!B44+August!B44+September!B44+October!B44+November!B44+December!B44</f>
-        <v>247</v>
+        <v>336</v>
       </c>
       <c r="C44" s="2">
         <f>January!C44+February!C44+March!C44+April!C44+May!C44+June!C44+July!C44+August!C44+September!C44+October!C44+November!C44+December!C44</f>
-        <v>1010</v>
+        <v>1204</v>
       </c>
       <c r="D44" s="2">
         <f>January!D44+February!D44+March!D44+April!D44+May!D44+June!D44+July!D44+August!D44+September!D44+October!D44+November!D44+December!D44</f>
-        <v>-763</v>
+        <v>-868</v>
       </c>
       <c r="E44" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6569,7 +6605,7 @@
       </c>
       <c r="G44" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.24 : 1</v>
+        <v>0.28 : 1</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6578,27 +6614,27 @@
       </c>
       <c r="B45" s="4">
         <f>January!B45+February!B45+March!B45+April!B45+May!B45+June!B45+July!B45+August!B45+September!B45+October!B45+November!B45+December!B45</f>
-        <v>2823</v>
+        <v>3301</v>
       </c>
       <c r="C45" s="4">
         <f>January!C45+February!C45+March!C45+April!C45+May!C45+June!C45+July!C45+August!C45+September!C45+October!C45+November!C45+December!C45</f>
-        <v>2689</v>
+        <v>3320</v>
       </c>
       <c r="D45" s="4">
         <f>January!D45+February!D45+March!D45+April!D45+May!D45+June!D45+July!D45+August!D45+September!D45+October!D45+November!D45+December!D45</f>
-        <v>134</v>
+        <v>-19</v>
       </c>
       <c r="E45" s="29" t="str">
         <f t="shared" si="3"/>
-        <v>We borrowed more than we lent this year</v>
+        <v/>
       </c>
       <c r="F45" s="29" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>We lent more than we borrowed this year</v>
       </c>
       <c r="G45" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>1.05 : 1</v>
+        <v>0.99 : 1</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6607,15 +6643,15 @@
       </c>
       <c r="B46" s="2">
         <f>January!B46+February!B46+March!B46+April!B46+May!B46+June!B46+July!B46+August!B46+September!B46+October!B46+November!B46+December!B46</f>
-        <v>5375</v>
+        <v>6448</v>
       </c>
       <c r="C46" s="2">
         <f>January!C46+February!C46+March!C46+April!C46+May!C46+June!C46+July!C46+August!C46+September!C46+October!C46+November!C46+December!C46</f>
-        <v>3359</v>
+        <v>3907</v>
       </c>
       <c r="D46" s="2">
         <f>January!D46+February!D46+March!D46+April!D46+May!D46+June!D46+July!D46+August!D46+September!D46+October!D46+November!D46+December!D46</f>
-        <v>2016</v>
+        <v>2541</v>
       </c>
       <c r="E46" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6627,7 +6663,7 @@
       </c>
       <c r="G46" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>1.6 : 1</v>
+        <v>1.65 : 1</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6636,15 +6672,15 @@
       </c>
       <c r="B47" s="4">
         <f>January!B47+February!B47+March!B47+April!B47+May!B47+June!B47+July!B47+August!B47+September!B47+October!B47+November!B47+December!B47</f>
-        <v>1072</v>
+        <v>1251</v>
       </c>
       <c r="C47" s="4">
         <f>January!C47+February!C47+March!C47+April!C47+May!C47+June!C47+July!C47+August!C47+September!C47+October!C47+November!C47+December!C47</f>
-        <v>3007</v>
+        <v>3628</v>
       </c>
       <c r="D47" s="4">
         <f>January!D47+February!D47+March!D47+April!D47+May!D47+June!D47+July!D47+August!D47+September!D47+October!D47+November!D47+December!D47</f>
-        <v>-1935</v>
+        <v>-2377</v>
       </c>
       <c r="E47" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6656,7 +6692,7 @@
       </c>
       <c r="G47" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.36 : 1</v>
+        <v>0.34 : 1</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6665,15 +6701,15 @@
       </c>
       <c r="B48" s="2">
         <f>January!B48+February!B48+March!B48+April!B48+May!B48+June!B48+July!B48+August!B48+September!B48+October!B48+November!B48+December!B48</f>
-        <v>3429</v>
+        <v>3986</v>
       </c>
       <c r="C48" s="2">
         <f>January!C48+February!C48+March!C48+April!C48+May!C48+June!C48+July!C48+August!C48+September!C48+October!C48+November!C48+December!C48</f>
-        <v>1156</v>
+        <v>1371</v>
       </c>
       <c r="D48" s="2">
         <f>January!D48+February!D48+March!D48+April!D48+May!D48+June!D48+July!D48+August!D48+September!D48+October!D48+November!D48+December!D48</f>
-        <v>2273</v>
+        <v>2615</v>
       </c>
       <c r="E48" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6685,7 +6721,7 @@
       </c>
       <c r="G48" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>2.97 : 1</v>
+        <v>2.91 : 1</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6694,15 +6730,15 @@
       </c>
       <c r="B49" s="4">
         <f>January!B49+February!B49+March!B49+April!B49+May!B49+June!B49+July!B49+August!B49+September!B49+October!B49+November!B49+December!B49</f>
-        <v>3943</v>
+        <v>4830</v>
       </c>
       <c r="C49" s="4">
         <f>January!C49+February!C49+March!C49+April!C49+May!C49+June!C49+July!C49+August!C49+September!C49+October!C49+November!C49+December!C49</f>
-        <v>2712</v>
+        <v>3319</v>
       </c>
       <c r="D49" s="4">
         <f>January!D49+February!D49+March!D49+April!D49+May!D49+June!D49+July!D49+August!D49+September!D49+October!D49+November!D49+December!D49</f>
-        <v>1231</v>
+        <v>1511</v>
       </c>
       <c r="E49" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6714,7 +6750,7 @@
       </c>
       <c r="G49" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>1.45 : 1</v>
+        <v>1.46 : 1</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6723,15 +6759,15 @@
       </c>
       <c r="B50" s="2">
         <f>January!B50+February!B50+March!B50+April!B50+May!B50+June!B50+July!B50+August!B50+September!B50+October!B50+November!B50+December!B50</f>
-        <v>947</v>
+        <v>1137</v>
       </c>
       <c r="C50" s="2">
         <f>January!C50+February!C50+March!C50+April!C50+May!C50+June!C50+July!C50+August!C50+September!C50+October!C50+November!C50+December!C50</f>
-        <v>844</v>
+        <v>971</v>
       </c>
       <c r="D50" s="2">
         <f>January!D50+February!D50+March!D50+April!D50+May!D50+June!D50+July!D50+August!D50+September!D50+October!D50+November!D50+December!D50</f>
-        <v>103</v>
+        <v>166</v>
       </c>
       <c r="E50" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6743,7 +6779,7 @@
       </c>
       <c r="G50" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>1.12 : 1</v>
+        <v>1.17 : 1</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6752,15 +6788,15 @@
       </c>
       <c r="B51" s="4">
         <f>January!B51+February!B51+March!B51+April!B51+May!B51+June!B51+July!B51+August!B51+September!B51+October!B51+November!B51+December!B51</f>
-        <v>1799</v>
+        <v>2096</v>
       </c>
       <c r="C51" s="4">
         <f>January!C51+February!C51+March!C51+April!C51+May!C51+June!C51+July!C51+August!C51+September!C51+October!C51+November!C51+December!C51</f>
-        <v>1916</v>
+        <v>2277</v>
       </c>
       <c r="D51" s="4">
         <f>January!D51+February!D51+March!D51+April!D51+May!D51+June!D51+July!D51+August!D51+September!D51+October!D51+November!D51+December!D51</f>
-        <v>-117</v>
+        <v>-181</v>
       </c>
       <c r="E51" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6772,7 +6808,7 @@
       </c>
       <c r="G51" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.94 : 1</v>
+        <v>0.92 : 1</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6781,15 +6817,15 @@
       </c>
       <c r="B52" s="2">
         <f>January!B52+February!B52+March!B52+April!B52+May!B52+June!B52+July!B52+August!B52+September!B52+October!B52+November!B52+December!B52</f>
-        <v>869</v>
+        <v>933</v>
       </c>
       <c r="C52" s="2">
         <f>January!C52+February!C52+March!C52+April!C52+May!C52+June!C52+July!C52+August!C52+September!C52+October!C52+November!C52+December!C52</f>
-        <v>1074</v>
+        <v>1296</v>
       </c>
       <c r="D52" s="2">
         <f>January!D52+February!D52+March!D52+April!D52+May!D52+June!D52+July!D52+August!D52+September!D52+October!D52+November!D52+December!D52</f>
-        <v>-205</v>
+        <v>-363</v>
       </c>
       <c r="E52" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6801,7 +6837,7 @@
       </c>
       <c r="G52" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.81 : 1</v>
+        <v>0.72 : 1</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6810,15 +6846,15 @@
       </c>
       <c r="B53" s="4">
         <f>January!B53+February!B53+March!B53+April!B53+May!B53+June!B53+July!B53+August!B53+September!B53+October!B53+November!B53+December!B53</f>
-        <v>163</v>
+        <v>189</v>
       </c>
       <c r="C53" s="4">
         <f>January!C53+February!C53+March!C53+April!C53+May!C53+June!C53+July!C53+August!C53+September!C53+October!C53+November!C53+December!C53</f>
-        <v>1303</v>
+        <v>1536</v>
       </c>
       <c r="D53" s="4">
         <f>January!D53+February!D53+March!D53+April!D53+May!D53+June!D53+July!D53+August!D53+September!D53+October!D53+November!D53+December!D53</f>
-        <v>-1140</v>
+        <v>-1347</v>
       </c>
       <c r="E53" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6830,7 +6866,7 @@
       </c>
       <c r="G53" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.13 : 1</v>
+        <v>0.12 : 1</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6839,15 +6875,15 @@
       </c>
       <c r="B54" s="10">
         <f>January!B54+February!B54+March!B54+April!B54+May!B54+June!B54+July!B54+August!B54+September!B54+October!B54+November!B54+December!B54</f>
-        <v>1880</v>
+        <v>2283</v>
       </c>
       <c r="C54" s="10">
         <f>January!C54+February!C54+March!C54+April!C54+May!C54+June!C54+July!C54+August!C54+September!C54+October!C54+November!C54+December!C54</f>
-        <v>1096</v>
+        <v>1269</v>
       </c>
       <c r="D54" s="10">
         <f>January!D54+February!D54+March!D54+April!D54+May!D54+June!D54+July!D54+August!D54+September!D54+October!D54+November!D54+December!D54</f>
-        <v>784</v>
+        <v>1014</v>
       </c>
       <c r="E54" s="32" t="str">
         <f t="shared" si="3"/>
@@ -6859,7 +6895,7 @@
       </c>
       <c r="G54" s="11" t="str">
         <f t="shared" si="5"/>
-        <v>1.72 : 1</v>
+        <v>1.8 : 1</v>
       </c>
     </row>
   </sheetData>
@@ -11670,7 +11706,7 @@
       <selection activeCell="A42" activeCellId="1" sqref="A40:G40 A42:G42"/>
       <selection pane="topRight" activeCell="A42" activeCellId="1" sqref="A40:G40 A42:G42"/>
       <selection pane="bottomLeft" activeCell="A42" activeCellId="1" sqref="A40:G40 A42:G42"/>
-      <selection pane="bottomRight" activeCell="A42" activeCellId="1" sqref="A40:G40 A42:G42"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11710,108 +11746,204 @@
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="28"/>
+      <c r="B2" s="18">
+        <v>1446</v>
+      </c>
+      <c r="C2" s="18">
+        <v>1041</v>
+      </c>
+      <c r="D2" s="18">
+        <v>405</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F2" s="28"/>
-      <c r="G2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="29"/>
+      <c r="B3" s="21">
+        <v>676</v>
+      </c>
+      <c r="C3" s="21">
+        <v>327</v>
+      </c>
+      <c r="D3" s="21">
+        <v>349</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F3" s="29"/>
-      <c r="G3" s="5"/>
+      <c r="G3" s="5" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="28"/>
+      <c r="B4" s="18">
+        <v>1258</v>
+      </c>
+      <c r="C4" s="18">
+        <v>1095</v>
+      </c>
+      <c r="D4" s="18">
+        <v>163</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F4" s="28"/>
-      <c r="G4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
+      <c r="B5" s="21">
+        <v>62</v>
+      </c>
+      <c r="C5" s="21">
+        <v>123</v>
+      </c>
+      <c r="D5" s="21">
+        <v>-61</v>
+      </c>
       <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="5"/>
+      <c r="F5" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
+      <c r="B6" s="18">
+        <v>1002</v>
+      </c>
+      <c r="C6" s="18">
+        <v>1145</v>
+      </c>
+      <c r="D6" s="18">
+        <v>-143</v>
+      </c>
       <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="3"/>
+      <c r="F6" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="29"/>
+      <c r="B7" s="21">
+        <v>254</v>
+      </c>
+      <c r="C7" s="21">
+        <v>183</v>
+      </c>
+      <c r="D7" s="21">
+        <v>71</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F7" s="29"/>
-      <c r="G7" s="5"/>
+      <c r="G7" s="5" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
+      <c r="B8" s="18">
+        <v>128</v>
+      </c>
+      <c r="C8" s="18">
+        <v>163</v>
+      </c>
+      <c r="D8" s="18">
+        <v>-35</v>
+      </c>
       <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="3"/>
+      <c r="F8" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
+      <c r="B9" s="21">
+        <v>50</v>
+      </c>
+      <c r="C9" s="21">
+        <v>61</v>
+      </c>
+      <c r="D9" s="21">
+        <v>-11</v>
+      </c>
       <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="5"/>
+      <c r="F9" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
+      <c r="B10" s="18">
+        <v>0</v>
+      </c>
+      <c r="C10" s="18">
+        <v>39</v>
+      </c>
+      <c r="D10" s="18">
+        <v>-39</v>
+      </c>
       <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="3"/>
+      <c r="F10" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
+      <c r="B11" s="21">
+        <v>0</v>
+      </c>
+      <c r="C11" s="21">
+        <v>0</v>
+      </c>
+      <c r="D11" s="21">
+        <v>0</v>
+      </c>
       <c r="E11" s="29"/>
       <c r="F11" s="29"/>
       <c r="G11" s="5"/>
@@ -11820,163 +11952,309 @@
       <c r="A12" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="35"/>
+      <c r="B12" s="41">
+        <v>37</v>
+      </c>
+      <c r="C12" s="41">
+        <v>16</v>
+      </c>
+      <c r="D12" s="41">
+        <v>21</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>60</v>
+      </c>
       <c r="F12" s="35"/>
-      <c r="G12" s="36"/>
+      <c r="G12" s="36" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="30"/>
+      <c r="B13" s="23">
+        <v>107</v>
+      </c>
+      <c r="C13" s="23">
+        <v>68</v>
+      </c>
+      <c r="D13" s="23">
+        <v>39</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>60</v>
+      </c>
       <c r="F13" s="30"/>
-      <c r="G13" s="7"/>
+      <c r="G13" s="7" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
+      <c r="B14" s="41">
+        <v>160</v>
+      </c>
+      <c r="C14" s="41">
+        <v>228</v>
+      </c>
+      <c r="D14" s="41">
+        <v>-68</v>
+      </c>
       <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="36"/>
+      <c r="F14" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="36" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
+      <c r="B15" s="23">
+        <v>64</v>
+      </c>
+      <c r="C15" s="23">
+        <v>160</v>
+      </c>
+      <c r="D15" s="23">
+        <v>-96</v>
+      </c>
       <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="7"/>
+      <c r="F15" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="B16" s="18">
+        <v>83</v>
+      </c>
+      <c r="C16" s="18">
+        <v>166</v>
+      </c>
+      <c r="D16" s="18">
+        <v>-83</v>
+      </c>
       <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="3"/>
+      <c r="F16" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="29"/>
+      <c r="B17" s="21">
+        <v>591</v>
+      </c>
+      <c r="C17" s="21">
+        <v>490</v>
+      </c>
+      <c r="D17" s="21">
+        <v>101</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F17" s="29"/>
-      <c r="G17" s="5"/>
+      <c r="G17" s="5" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
+      <c r="B18" s="18">
+        <v>30</v>
+      </c>
+      <c r="C18" s="18">
+        <v>92</v>
+      </c>
+      <c r="D18" s="18">
+        <v>-62</v>
+      </c>
       <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="3"/>
+      <c r="F18" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
+      <c r="B19" s="21">
+        <v>341</v>
+      </c>
+      <c r="C19" s="21">
+        <v>364</v>
+      </c>
+      <c r="D19" s="21">
+        <v>-23</v>
+      </c>
       <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="5"/>
+      <c r="F19" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+      <c r="B20" s="18">
+        <v>12</v>
+      </c>
+      <c r="C20" s="18">
+        <v>47</v>
+      </c>
+      <c r="D20" s="18">
+        <v>-35</v>
+      </c>
       <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="3"/>
+      <c r="F20" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="29"/>
+      <c r="B21" s="21">
+        <v>531</v>
+      </c>
+      <c r="C21" s="21">
+        <v>345</v>
+      </c>
+      <c r="D21" s="21">
+        <v>186</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F21" s="29"/>
-      <c r="G21" s="5"/>
+      <c r="G21" s="5" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="B22" s="18">
+        <v>64</v>
+      </c>
+      <c r="C22" s="18">
+        <v>320</v>
+      </c>
+      <c r="D22" s="18">
+        <v>-256</v>
+      </c>
       <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="3"/>
+      <c r="F22" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
+      <c r="B23" s="21">
+        <v>536</v>
+      </c>
+      <c r="C23" s="21">
+        <v>664</v>
+      </c>
+      <c r="D23" s="21">
+        <v>-128</v>
+      </c>
       <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="5"/>
+      <c r="F23" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="28"/>
+      <c r="B24" s="18">
+        <v>1363</v>
+      </c>
+      <c r="C24" s="18">
+        <v>1146</v>
+      </c>
+      <c r="D24" s="18">
+        <v>217</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F24" s="28"/>
-      <c r="G24" s="3"/>
+      <c r="G24" s="3" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
+      <c r="B25" s="21">
+        <v>144</v>
+      </c>
+      <c r="C25" s="21">
+        <v>382</v>
+      </c>
+      <c r="D25" s="21">
+        <v>-238</v>
+      </c>
       <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="5"/>
+      <c r="F25" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
+      <c r="B26" s="18">
+        <v>0</v>
+      </c>
+      <c r="C26" s="18">
+        <v>0</v>
+      </c>
+      <c r="D26" s="18">
+        <v>0</v>
+      </c>
       <c r="E26" s="28"/>
       <c r="F26" s="28"/>
       <c r="G26" s="3"/>
@@ -11985,309 +12263,585 @@
       <c r="A27" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="29"/>
+      <c r="B27" s="21">
+        <v>203</v>
+      </c>
+      <c r="C27" s="21">
+        <v>178</v>
+      </c>
+      <c r="D27" s="21">
+        <v>25</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F27" s="29"/>
-      <c r="G27" s="5"/>
+      <c r="G27" s="5" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="28"/>
+      <c r="B28" s="18">
+        <v>192</v>
+      </c>
+      <c r="C28" s="18">
+        <v>122</v>
+      </c>
+      <c r="D28" s="18">
+        <v>70</v>
+      </c>
+      <c r="E28" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F28" s="28"/>
-      <c r="G28" s="3"/>
+      <c r="G28" s="3" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="29"/>
+      <c r="B29" s="21">
+        <v>565</v>
+      </c>
+      <c r="C29" s="21">
+        <v>350</v>
+      </c>
+      <c r="D29" s="21">
+        <v>215</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F29" s="29"/>
-      <c r="G29" s="5"/>
+      <c r="G29" s="5" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
+      <c r="B30" s="18">
+        <v>20</v>
+      </c>
+      <c r="C30" s="18">
+        <v>28</v>
+      </c>
+      <c r="D30" s="18">
+        <v>-8</v>
+      </c>
       <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="3"/>
+      <c r="F30" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
+      <c r="B31" s="21">
+        <v>65</v>
+      </c>
+      <c r="C31" s="21">
+        <v>252</v>
+      </c>
+      <c r="D31" s="21">
+        <v>-187</v>
+      </c>
       <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="5"/>
+      <c r="F31" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="B32" s="18">
+        <v>424</v>
+      </c>
+      <c r="C32" s="18">
+        <v>533</v>
+      </c>
+      <c r="D32" s="18">
+        <v>-109</v>
+      </c>
       <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="3"/>
+      <c r="F32" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="29"/>
+      <c r="B33" s="21">
+        <v>414</v>
+      </c>
+      <c r="C33" s="21">
+        <v>390</v>
+      </c>
+      <c r="D33" s="21">
+        <v>24</v>
+      </c>
+      <c r="E33" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F33" s="29"/>
-      <c r="G33" s="5"/>
+      <c r="G33" s="5" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="28"/>
+      <c r="B34" s="18">
+        <v>180</v>
+      </c>
+      <c r="C34" s="18">
+        <v>136</v>
+      </c>
+      <c r="D34" s="18">
+        <v>44</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F34" s="28"/>
-      <c r="G34" s="3"/>
+      <c r="G34" s="3" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
+      <c r="B35" s="21">
+        <v>895</v>
+      </c>
+      <c r="C35" s="21">
+        <v>1360</v>
+      </c>
+      <c r="D35" s="21">
+        <v>-465</v>
+      </c>
       <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="5"/>
+      <c r="F35" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="B36" s="18">
+        <v>155</v>
+      </c>
+      <c r="C36" s="18">
+        <v>464</v>
+      </c>
+      <c r="D36" s="18">
+        <v>-309</v>
+      </c>
       <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="3"/>
+      <c r="F36" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="29"/>
+      <c r="B37" s="21">
+        <v>596</v>
+      </c>
+      <c r="C37" s="21">
+        <v>363</v>
+      </c>
+      <c r="D37" s="21">
+        <v>233</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F37" s="29"/>
-      <c r="G37" s="5"/>
+      <c r="G37" s="5" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
+      <c r="B38" s="18">
+        <v>29</v>
+      </c>
+      <c r="C38" s="18">
+        <v>164</v>
+      </c>
+      <c r="D38" s="18">
+        <v>-135</v>
+      </c>
       <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="3"/>
+      <c r="F38" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="B39" s="21"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
+        <v>44</v>
+      </c>
+      <c r="B39" s="21">
+        <v>0</v>
+      </c>
+      <c r="C39" s="21">
+        <v>7</v>
+      </c>
+      <c r="D39" s="21">
+        <v>-7</v>
+      </c>
       <c r="E39" s="29"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="5"/>
+      <c r="F39" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="B40" s="42"/>
-      <c r="C40" s="42"/>
-      <c r="D40" s="42"/>
+        <v>45</v>
+      </c>
+      <c r="B40" s="42">
+        <v>0</v>
+      </c>
+      <c r="C40" s="42">
+        <v>3</v>
+      </c>
+      <c r="D40" s="42">
+        <v>-3</v>
+      </c>
       <c r="E40" s="39"/>
-      <c r="F40" s="39"/>
-      <c r="G40" s="40"/>
+      <c r="F40" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="G40" s="40" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
+        <v>46</v>
+      </c>
+      <c r="B41" s="25">
+        <v>0</v>
+      </c>
+      <c r="C41" s="25">
+        <v>0</v>
+      </c>
+      <c r="D41" s="25">
+        <v>0</v>
+      </c>
       <c r="E41" s="31"/>
       <c r="F41" s="31"/>
       <c r="G41" s="9"/>
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" s="42"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="42"/>
+        <v>47</v>
+      </c>
+      <c r="B42" s="42">
+        <v>0</v>
+      </c>
+      <c r="C42" s="42">
+        <v>5</v>
+      </c>
+      <c r="D42" s="42">
+        <v>-5</v>
+      </c>
       <c r="E42" s="39"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="40"/>
+      <c r="F42" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="G42" s="40" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="31"/>
+        <v>48</v>
+      </c>
+      <c r="B43" s="25">
+        <v>104</v>
+      </c>
+      <c r="C43" s="25">
+        <v>72</v>
+      </c>
+      <c r="D43" s="25">
+        <v>32</v>
+      </c>
+      <c r="E43" s="31" t="s">
+        <v>60</v>
+      </c>
       <c r="F43" s="31"/>
-      <c r="G43" s="9"/>
+      <c r="G43" s="9" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
+      <c r="B44" s="18">
+        <v>89</v>
+      </c>
+      <c r="C44" s="18">
+        <v>194</v>
+      </c>
+      <c r="D44" s="18">
+        <v>-105</v>
+      </c>
       <c r="E44" s="28"/>
-      <c r="F44" s="28"/>
-      <c r="G44" s="3"/>
+      <c r="F44" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="21"/>
-      <c r="C45" s="21"/>
-      <c r="D45" s="21"/>
+      <c r="B45" s="21">
+        <v>478</v>
+      </c>
+      <c r="C45" s="21">
+        <v>631</v>
+      </c>
+      <c r="D45" s="21">
+        <v>-153</v>
+      </c>
       <c r="E45" s="29"/>
-      <c r="F45" s="29"/>
-      <c r="G45" s="5"/>
+      <c r="F45" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="28"/>
+      <c r="B46" s="18">
+        <v>1073</v>
+      </c>
+      <c r="C46" s="18">
+        <v>548</v>
+      </c>
+      <c r="D46" s="18">
+        <v>525</v>
+      </c>
+      <c r="E46" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F46" s="28"/>
-      <c r="G46" s="3"/>
+      <c r="G46" s="3" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="21"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
+      <c r="B47" s="21">
+        <v>179</v>
+      </c>
+      <c r="C47" s="21">
+        <v>621</v>
+      </c>
+      <c r="D47" s="21">
+        <v>-442</v>
+      </c>
       <c r="E47" s="29"/>
-      <c r="F47" s="29"/>
-      <c r="G47" s="5"/>
+      <c r="F47" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="28"/>
+      <c r="B48" s="18">
+        <v>557</v>
+      </c>
+      <c r="C48" s="18">
+        <v>215</v>
+      </c>
+      <c r="D48" s="18">
+        <v>342</v>
+      </c>
+      <c r="E48" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F48" s="28"/>
-      <c r="G48" s="3"/>
+      <c r="G48" s="3" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="21"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="29"/>
+      <c r="B49" s="21">
+        <v>887</v>
+      </c>
+      <c r="C49" s="21">
+        <v>607</v>
+      </c>
+      <c r="D49" s="21">
+        <v>280</v>
+      </c>
+      <c r="E49" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F49" s="29"/>
-      <c r="G49" s="5"/>
+      <c r="G49" s="5" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="18"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="28"/>
+      <c r="B50" s="18">
+        <v>190</v>
+      </c>
+      <c r="C50" s="18">
+        <v>127</v>
+      </c>
+      <c r="D50" s="18">
+        <v>63</v>
+      </c>
+      <c r="E50" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F50" s="28"/>
-      <c r="G50" s="3"/>
+      <c r="G50" s="3" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="21"/>
-      <c r="C51" s="21"/>
-      <c r="D51" s="21"/>
+      <c r="B51" s="21">
+        <v>297</v>
+      </c>
+      <c r="C51" s="21">
+        <v>361</v>
+      </c>
+      <c r="D51" s="21">
+        <v>-64</v>
+      </c>
       <c r="E51" s="29"/>
-      <c r="F51" s="29"/>
-      <c r="G51" s="5"/>
+      <c r="F51" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="18"/>
-      <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
+      <c r="B52" s="18">
+        <v>64</v>
+      </c>
+      <c r="C52" s="18">
+        <v>222</v>
+      </c>
+      <c r="D52" s="18">
+        <v>-158</v>
+      </c>
       <c r="E52" s="28"/>
-      <c r="F52" s="28"/>
-      <c r="G52" s="3"/>
+      <c r="F52" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="21"/>
-      <c r="C53" s="21"/>
-      <c r="D53" s="21"/>
+      <c r="B53" s="21">
+        <v>26</v>
+      </c>
+      <c r="C53" s="21">
+        <v>233</v>
+      </c>
+      <c r="D53" s="21">
+        <v>-207</v>
+      </c>
       <c r="E53" s="29"/>
-      <c r="F53" s="29"/>
-      <c r="G53" s="5"/>
+      <c r="F53" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="B54" s="27"/>
-      <c r="C54" s="27"/>
-      <c r="D54" s="27"/>
-      <c r="E54" s="32"/>
+      <c r="B54" s="27">
+        <v>403</v>
+      </c>
+      <c r="C54" s="27">
+        <v>173</v>
+      </c>
+      <c r="D54" s="27">
+        <v>230</v>
+      </c>
+      <c r="E54" s="32" t="s">
+        <v>60</v>
+      </c>
       <c r="F54" s="32"/>
-      <c r="G54" s="11"/>
+      <c r="G54" s="11" t="s">
+        <v>221</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G54" xr:uid="{00000000-0009-0000-0000-000006000000}"/>

</xml_diff>

<commit_message>
All files except itype files
</commit_message>
<xml_diff>
--- a/statistics_files/2025/2025_99_g_net_borrower_lender.xlsx
+++ b/statistics_files/2025/2025_99_g_net_borrower_lender.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\github\next_statistics\statistics_files\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A680F80-DE8F-450E-87CA-52D219EF1B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12DA758B-D999-413B-923B-74A2830475BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="673" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1391" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="230">
   <si>
     <t>NET</t>
   </si>
@@ -727,6 +727,30 @@
   </si>
   <si>
     <t>2.33 : 1</t>
+  </si>
+  <si>
+    <t>2.01 : 1</t>
+  </si>
+  <si>
+    <t>2.15 : 1</t>
+  </si>
+  <si>
+    <t>0.54 : 1</t>
+  </si>
+  <si>
+    <t>1.23 : 1</t>
+  </si>
+  <si>
+    <t>1.41 : 1</t>
+  </si>
+  <si>
+    <t>0.37 : 1</t>
+  </si>
+  <si>
+    <t>2.30 : 1</t>
+  </si>
+  <si>
+    <t>2.06 : 1</t>
   </si>
 </sst>
 </file>
@@ -5326,7 +5350,7 @@
       <selection activeCell="A40" sqref="A40"/>
       <selection pane="topRight" activeCell="A40" sqref="A40"/>
       <selection pane="bottomLeft" activeCell="A40" sqref="A40"/>
-      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5367,15 +5391,15 @@
       </c>
       <c r="B2" s="2">
         <f>January!B2+February!B2+March!B2+April!B2+May!B2+June!B2+July!B2+August!B2+September!B2+October!B2+November!B2+December!B2</f>
-        <v>8957</v>
+        <v>10497</v>
       </c>
       <c r="C2" s="2">
         <f>January!C2+February!C2+March!C2+April!C2+May!C2+June!C2+July!C2+August!C2+September!C2+October!C2+November!C2+December!C2</f>
-        <v>7393</v>
+        <v>8670</v>
       </c>
       <c r="D2" s="2">
         <f>January!D2+February!D2+March!D2+April!D2+May!D2+June!D2+July!D2+August!D2+September!D2+October!D2+November!D2+December!D2</f>
-        <v>1564</v>
+        <v>1827</v>
       </c>
       <c r="E2" s="28" t="str">
         <f t="shared" ref="E2:E33" si="0">IF(D2 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -5396,15 +5420,15 @@
       </c>
       <c r="B3" s="4">
         <f>January!B3+February!B3+March!B3+April!B3+May!B3+June!B3+July!B3+August!B3+September!B3+October!B3+November!B3+December!B3</f>
-        <v>3556</v>
+        <v>4306</v>
       </c>
       <c r="C3" s="4">
         <f>January!C3+February!C3+March!C3+April!C3+May!C3+June!C3+July!C3+August!C3+September!C3+October!C3+November!C3+December!C3</f>
-        <v>2237</v>
+        <v>2610</v>
       </c>
       <c r="D3" s="4">
         <f>January!D3+February!D3+March!D3+April!D3+May!D3+June!D3+July!D3+August!D3+September!D3+October!D3+November!D3+December!D3</f>
-        <v>1319</v>
+        <v>1696</v>
       </c>
       <c r="E3" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5416,7 +5440,7 @@
       </c>
       <c r="G3" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.59 : 1</v>
+        <v>1.65 : 1</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5425,15 +5449,15 @@
       </c>
       <c r="B4" s="2">
         <f>January!B4+February!B4+March!B4+April!B4+May!B4+June!B4+July!B4+August!B4+September!B4+October!B4+November!B4+December!B4</f>
-        <v>6785</v>
+        <v>8015</v>
       </c>
       <c r="C4" s="2">
         <f>January!C4+February!C4+March!C4+April!C4+May!C4+June!C4+July!C4+August!C4+September!C4+October!C4+November!C4+December!C4</f>
-        <v>6180</v>
+        <v>7578</v>
       </c>
       <c r="D4" s="2">
         <f>January!D4+February!D4+March!D4+April!D4+May!D4+June!D4+July!D4+August!D4+September!D4+October!D4+November!D4+December!D4</f>
-        <v>605</v>
+        <v>437</v>
       </c>
       <c r="E4" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5445,7 +5469,7 @@
       </c>
       <c r="G4" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.1 : 1</v>
+        <v>1.06 : 1</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5454,15 +5478,15 @@
       </c>
       <c r="B5" s="4">
         <f>January!B5+February!B5+March!B5+April!B5+May!B5+June!B5+July!B5+August!B5+September!B5+October!B5+November!B5+December!B5</f>
-        <v>186</v>
+        <v>232</v>
       </c>
       <c r="C5" s="4">
         <f>January!C5+February!C5+March!C5+April!C5+May!C5+June!C5+July!C5+August!C5+September!C5+October!C5+November!C5+December!C5</f>
-        <v>790</v>
+        <v>922</v>
       </c>
       <c r="D5" s="4">
         <f>January!D5+February!D5+March!D5+April!D5+May!D5+June!D5+July!D5+August!D5+September!D5+October!D5+November!D5+December!D5</f>
-        <v>-604</v>
+        <v>-690</v>
       </c>
       <c r="E5" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5474,7 +5498,7 @@
       </c>
       <c r="G5" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.24 : 1</v>
+        <v>0.25 : 1</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5483,15 +5507,15 @@
       </c>
       <c r="B6" s="2">
         <f>January!B6+February!B6+March!B6+April!B6+May!B6+June!B6+July!B6+August!B6+September!B6+October!B6+November!B6+December!B6</f>
-        <v>6119</v>
+        <v>7193</v>
       </c>
       <c r="C6" s="2">
         <f>January!C6+February!C6+March!C6+April!C6+May!C6+June!C6+July!C6+August!C6+September!C6+October!C6+November!C6+December!C6</f>
-        <v>6945</v>
+        <v>8109</v>
       </c>
       <c r="D6" s="2">
         <f>January!D6+February!D6+March!D6+April!D6+May!D6+June!D6+July!D6+August!D6+September!D6+October!D6+November!D6+December!D6</f>
-        <v>-826</v>
+        <v>-916</v>
       </c>
       <c r="E6" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5503,7 +5527,7 @@
       </c>
       <c r="G6" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.88 : 1</v>
+        <v>0.89 : 1</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5512,15 +5536,15 @@
       </c>
       <c r="B7" s="4">
         <f>January!B7+February!B7+March!B7+April!B7+May!B7+June!B7+July!B7+August!B7+September!B7+October!B7+November!B7+December!B7</f>
-        <v>1302</v>
+        <v>1633</v>
       </c>
       <c r="C7" s="4">
         <f>January!C7+February!C7+March!C7+April!C7+May!C7+June!C7+July!C7+August!C7+September!C7+October!C7+November!C7+December!C7</f>
-        <v>886</v>
+        <v>1118</v>
       </c>
       <c r="D7" s="4">
         <f>January!D7+February!D7+March!D7+April!D7+May!D7+June!D7+July!D7+August!D7+September!D7+October!D7+November!D7+December!D7</f>
-        <v>416</v>
+        <v>515</v>
       </c>
       <c r="E7" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5532,7 +5556,7 @@
       </c>
       <c r="G7" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.47 : 1</v>
+        <v>1.46 : 1</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5541,15 +5565,15 @@
       </c>
       <c r="B8" s="2">
         <f>January!B8+February!B8+March!B8+April!B8+May!B8+June!B8+July!B8+August!B8+September!B8+October!B8+November!B8+December!B8</f>
-        <v>954</v>
+        <v>1059</v>
       </c>
       <c r="C8" s="2">
         <f>January!C8+February!C8+March!C8+April!C8+May!C8+June!C8+July!C8+August!C8+September!C8+October!C8+November!C8+December!C8</f>
-        <v>1061</v>
+        <v>1221</v>
       </c>
       <c r="D8" s="2">
         <f>January!D8+February!D8+March!D8+April!D8+May!D8+June!D8+July!D8+August!D8+September!D8+October!D8+November!D8+December!D8</f>
-        <v>-107</v>
+        <v>-162</v>
       </c>
       <c r="E8" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5561,7 +5585,7 @@
       </c>
       <c r="G8" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.9 : 1</v>
+        <v>0.87 : 1</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5570,15 +5594,15 @@
       </c>
       <c r="B9" s="4">
         <f>January!B9+February!B9+March!B9+April!B9+May!B9+June!B9+July!B9+August!B9+September!B9+October!B9+November!B9+December!B9</f>
-        <v>253</v>
+        <v>335</v>
       </c>
       <c r="C9" s="4">
         <f>January!C9+February!C9+March!C9+April!C9+May!C9+June!C9+July!C9+August!C9+September!C9+October!C9+November!C9+December!C9</f>
-        <v>408</v>
+        <v>473</v>
       </c>
       <c r="D9" s="4">
         <f>January!D9+February!D9+March!D9+April!D9+May!D9+June!D9+July!D9+August!D9+September!D9+October!D9+November!D9+December!D9</f>
-        <v>-155</v>
+        <v>-138</v>
       </c>
       <c r="E9" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5590,7 +5614,7 @@
       </c>
       <c r="G9" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.62 : 1</v>
+        <v>0.71 : 1</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5603,11 +5627,11 @@
       </c>
       <c r="C10" s="2">
         <f>January!C10+February!C10+March!C10+April!C10+May!C10+June!C10+July!C10+August!C10+September!C10+October!C10+November!C10+December!C10</f>
-        <v>245</v>
+        <v>282</v>
       </c>
       <c r="D10" s="2">
         <f>January!D10+February!D10+March!D10+April!D10+May!D10+June!D10+July!D10+August!D10+September!D10+October!D10+November!D10+December!D10</f>
-        <v>-242</v>
+        <v>-279</v>
       </c>
       <c r="E10" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5657,15 +5681,15 @@
       </c>
       <c r="B12" s="34">
         <f>January!B12+February!B12+March!B12+April!B12+May!B12+June!B12+July!B12+August!B12+September!B12+October!B12+November!B12+December!B12</f>
-        <v>184</v>
+        <v>212</v>
       </c>
       <c r="C12" s="34">
         <f>January!C12+February!C12+March!C12+April!C12+May!C12+June!C12+July!C12+August!C12+September!C12+October!C12+November!C12+December!C12</f>
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="D12" s="34">
         <f>January!D12+February!D12+March!D12+April!D12+May!D12+June!D12+July!D12+August!D12+September!D12+October!D12+November!D12+December!D12</f>
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="E12" s="35" t="str">
         <f t="shared" si="0"/>
@@ -5677,7 +5701,7 @@
       </c>
       <c r="G12" s="36" t="str">
         <f t="shared" si="2"/>
-        <v>2.27 : 1</v>
+        <v>2.26 : 1</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5686,15 +5710,15 @@
       </c>
       <c r="B13" s="6">
         <f>January!B13+February!B13+March!B13+April!B13+May!B13+June!B13+July!B13+August!B13+September!B13+October!B13+November!B13+December!B13</f>
-        <v>477</v>
+        <v>566</v>
       </c>
       <c r="C13" s="6">
         <f>January!C13+February!C13+March!C13+April!C13+May!C13+June!C13+July!C13+August!C13+September!C13+October!C13+November!C13+December!C13</f>
-        <v>415</v>
+        <v>502</v>
       </c>
       <c r="D13" s="6">
         <f>January!D13+February!D13+March!D13+April!D13+May!D13+June!D13+July!D13+August!D13+September!D13+October!D13+November!D13+December!D13</f>
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E13" s="30" t="str">
         <f t="shared" si="0"/>
@@ -5706,7 +5730,7 @@
       </c>
       <c r="G13" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>1.15 : 1</v>
+        <v>1.13 : 1</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5715,15 +5739,15 @@
       </c>
       <c r="B14" s="34">
         <f>January!B14+February!B14+March!B14+April!B14+May!B14+June!B14+July!B14+August!B14+September!B14+October!B14+November!B14+December!B14</f>
-        <v>1027</v>
+        <v>1218</v>
       </c>
       <c r="C14" s="34">
         <f>January!C14+February!C14+March!C14+April!C14+May!C14+June!C14+July!C14+August!C14+September!C14+October!C14+November!C14+December!C14</f>
-        <v>1267</v>
+        <v>1507</v>
       </c>
       <c r="D14" s="34">
         <f>January!D14+February!D14+March!D14+April!D14+May!D14+June!D14+July!D14+August!D14+September!D14+October!D14+November!D14+December!D14</f>
-        <v>-240</v>
+        <v>-289</v>
       </c>
       <c r="E14" s="35" t="str">
         <f t="shared" si="0"/>
@@ -5744,15 +5768,15 @@
       </c>
       <c r="B15" s="6">
         <f>January!B15+February!B15+March!B15+April!B15+May!B15+June!B15+July!B15+August!B15+September!B15+October!B15+November!B15+December!B15</f>
-        <v>332</v>
+        <v>412</v>
       </c>
       <c r="C15" s="6">
         <f>January!C15+February!C15+March!C15+April!C15+May!C15+June!C15+July!C15+August!C15+September!C15+October!C15+November!C15+December!C15</f>
-        <v>912</v>
+        <v>1064</v>
       </c>
       <c r="D15" s="6">
         <f>January!D15+February!D15+March!D15+April!D15+May!D15+June!D15+July!D15+August!D15+September!D15+October!D15+November!D15+December!D15</f>
-        <v>-580</v>
+        <v>-652</v>
       </c>
       <c r="E15" s="30" t="str">
         <f t="shared" si="0"/>
@@ -5764,7 +5788,7 @@
       </c>
       <c r="G15" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0.36 : 1</v>
+        <v>0.39 : 1</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5773,15 +5797,15 @@
       </c>
       <c r="B16" s="2">
         <f>January!B16+February!B16+March!B16+April!B16+May!B16+June!B16+July!B16+August!B16+September!B16+October!B16+November!B16+December!B16</f>
-        <v>379</v>
+        <v>460</v>
       </c>
       <c r="C16" s="2">
         <f>January!C16+February!C16+March!C16+April!C16+May!C16+June!C16+July!C16+August!C16+September!C16+October!C16+November!C16+December!C16</f>
-        <v>1050</v>
+        <v>1200</v>
       </c>
       <c r="D16" s="2">
         <f>January!D16+February!D16+March!D16+April!D16+May!D16+June!D16+July!D16+August!D16+September!D16+October!D16+November!D16+December!D16</f>
-        <v>-671</v>
+        <v>-740</v>
       </c>
       <c r="E16" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5793,7 +5817,7 @@
       </c>
       <c r="G16" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.36 : 1</v>
+        <v>0.38 : 1</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5802,15 +5826,15 @@
       </c>
       <c r="B17" s="4">
         <f>January!B17+February!B17+March!B17+April!B17+May!B17+June!B17+July!B17+August!B17+September!B17+October!B17+November!B17+December!B17</f>
-        <v>3677</v>
+        <v>4330</v>
       </c>
       <c r="C17" s="4">
         <f>January!C17+February!C17+March!C17+April!C17+May!C17+June!C17+July!C17+August!C17+September!C17+October!C17+November!C17+December!C17</f>
-        <v>2739</v>
+        <v>3193</v>
       </c>
       <c r="D17" s="4">
         <f>January!D17+February!D17+March!D17+April!D17+May!D17+June!D17+July!D17+August!D17+September!D17+October!D17+November!D17+December!D17</f>
-        <v>938</v>
+        <v>1137</v>
       </c>
       <c r="E17" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5822,7 +5846,7 @@
       </c>
       <c r="G17" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.34 : 1</v>
+        <v>1.36 : 1</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5831,15 +5855,15 @@
       </c>
       <c r="B18" s="2">
         <f>January!B18+February!B18+March!B18+April!B18+May!B18+June!B18+July!B18+August!B18+September!B18+October!B18+November!B18+December!B18</f>
-        <v>289</v>
+        <v>314</v>
       </c>
       <c r="C18" s="2">
         <f>January!C18+February!C18+March!C18+April!C18+May!C18+June!C18+July!C18+August!C18+September!C18+October!C18+November!C18+December!C18</f>
-        <v>514</v>
+        <v>608</v>
       </c>
       <c r="D18" s="2">
         <f>January!D18+February!D18+March!D18+April!D18+May!D18+June!D18+July!D18+August!D18+September!D18+October!D18+November!D18+December!D18</f>
-        <v>-225</v>
+        <v>-294</v>
       </c>
       <c r="E18" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5851,7 +5875,7 @@
       </c>
       <c r="G18" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.56 : 1</v>
+        <v>0.52 : 1</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5860,15 +5884,15 @@
       </c>
       <c r="B19" s="4">
         <f>January!B19+February!B19+March!B19+April!B19+May!B19+June!B19+July!B19+August!B19+September!B19+October!B19+November!B19+December!B19</f>
-        <v>2535</v>
+        <v>3000</v>
       </c>
       <c r="C19" s="4">
         <f>January!C19+February!C19+March!C19+April!C19+May!C19+June!C19+July!C19+August!C19+September!C19+October!C19+November!C19+December!C19</f>
-        <v>2457</v>
+        <v>2962</v>
       </c>
       <c r="D19" s="4">
         <f>January!D19+February!D19+March!D19+April!D19+May!D19+June!D19+July!D19+August!D19+September!D19+October!D19+November!D19+December!D19</f>
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="E19" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5880,7 +5904,7 @@
       </c>
       <c r="G19" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.03 : 1</v>
+        <v>1.01 : 1</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5889,15 +5913,15 @@
       </c>
       <c r="B20" s="2">
         <f>January!B20+February!B20+March!B20+April!B20+May!B20+June!B20+July!B20+August!B20+September!B20+October!B20+November!B20+December!B20</f>
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="C20" s="2">
         <f>January!C20+February!C20+March!C20+April!C20+May!C20+June!C20+July!C20+August!C20+September!C20+October!C20+November!C20+December!C20</f>
-        <v>314</v>
+        <v>381</v>
       </c>
       <c r="D20" s="2">
         <f>January!D20+February!D20+March!D20+April!D20+May!D20+June!D20+July!D20+August!D20+September!D20+October!D20+November!D20+December!D20</f>
-        <v>-169</v>
+        <v>-224</v>
       </c>
       <c r="E20" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5909,7 +5933,7 @@
       </c>
       <c r="G20" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.46 : 1</v>
+        <v>0.41 : 1</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5918,15 +5942,15 @@
       </c>
       <c r="B21" s="4">
         <f>January!B21+February!B21+March!B21+April!B21+May!B21+June!B21+July!B21+August!B21+September!B21+October!B21+November!B21+December!B21</f>
-        <v>2965</v>
+        <v>3463</v>
       </c>
       <c r="C21" s="4">
         <f>January!C21+February!C21+March!C21+April!C21+May!C21+June!C21+July!C21+August!C21+September!C21+October!C21+November!C21+December!C21</f>
-        <v>1964</v>
+        <v>2303</v>
       </c>
       <c r="D21" s="4">
         <f>January!D21+February!D21+March!D21+April!D21+May!D21+June!D21+July!D21+August!D21+September!D21+October!D21+November!D21+December!D21</f>
-        <v>1001</v>
+        <v>1160</v>
       </c>
       <c r="E21" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5938,7 +5962,7 @@
       </c>
       <c r="G21" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.51 : 1</v>
+        <v>1.5 : 1</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5947,15 +5971,15 @@
       </c>
       <c r="B22" s="2">
         <f>January!B22+February!B22+March!B22+April!B22+May!B22+June!B22+July!B22+August!B22+September!B22+October!B22+November!B22+December!B22</f>
-        <v>399</v>
+        <v>474</v>
       </c>
       <c r="C22" s="2">
         <f>January!C22+February!C22+March!C22+April!C22+May!C22+June!C22+July!C22+August!C22+September!C22+October!C22+November!C22+December!C22</f>
-        <v>1521</v>
+        <v>1804</v>
       </c>
       <c r="D22" s="2">
         <f>January!D22+February!D22+March!D22+April!D22+May!D22+June!D22+July!D22+August!D22+September!D22+October!D22+November!D22+December!D22</f>
-        <v>-1122</v>
+        <v>-1330</v>
       </c>
       <c r="E22" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5976,15 +6000,15 @@
       </c>
       <c r="B23" s="4">
         <f>January!B23+February!B23+March!B23+April!B23+May!B23+June!B23+July!B23+August!B23+September!B23+October!B23+November!B23+December!B23</f>
-        <v>3659</v>
+        <v>4293</v>
       </c>
       <c r="C23" s="4">
         <f>January!C23+February!C23+March!C23+April!C23+May!C23+June!C23+July!C23+August!C23+September!C23+October!C23+November!C23+December!C23</f>
-        <v>2968</v>
+        <v>3604</v>
       </c>
       <c r="D23" s="4">
         <f>January!D23+February!D23+March!D23+April!D23+May!D23+June!D23+July!D23+August!D23+September!D23+October!D23+November!D23+December!D23</f>
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="E23" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5996,7 +6020,7 @@
       </c>
       <c r="G23" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.23 : 1</v>
+        <v>1.19 : 1</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6005,15 +6029,15 @@
       </c>
       <c r="B24" s="2">
         <f>January!B24+February!B24+March!B24+April!B24+May!B24+June!B24+July!B24+August!B24+September!B24+October!B24+November!B24+December!B24</f>
-        <v>9041</v>
+        <v>10750</v>
       </c>
       <c r="C24" s="2">
         <f>January!C24+February!C24+March!C24+April!C24+May!C24+June!C24+July!C24+August!C24+September!C24+October!C24+November!C24+December!C24</f>
-        <v>6809</v>
+        <v>7907</v>
       </c>
       <c r="D24" s="2">
         <f>January!D24+February!D24+March!D24+April!D24+May!D24+June!D24+July!D24+August!D24+September!D24+October!D24+November!D24+December!D24</f>
-        <v>2232</v>
+        <v>2843</v>
       </c>
       <c r="E24" s="28" t="str">
         <f t="shared" si="0"/>
@@ -6025,7 +6049,7 @@
       </c>
       <c r="G24" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.33 : 1</v>
+        <v>1.36 : 1</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6034,15 +6058,15 @@
       </c>
       <c r="B25" s="4">
         <f>January!B25+February!B25+March!B25+April!B25+May!B25+June!B25+July!B25+August!B25+September!B25+October!B25+November!B25+December!B25</f>
-        <v>901</v>
+        <v>1070</v>
       </c>
       <c r="C25" s="4">
         <f>January!C25+February!C25+March!C25+April!C25+May!C25+June!C25+July!C25+August!C25+September!C25+October!C25+November!C25+December!C25</f>
-        <v>2572</v>
+        <v>3001</v>
       </c>
       <c r="D25" s="4">
         <f>January!D25+February!D25+March!D25+April!D25+May!D25+June!D25+July!D25+August!D25+September!D25+October!D25+November!D25+December!D25</f>
-        <v>-1671</v>
+        <v>-1931</v>
       </c>
       <c r="E25" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6054,7 +6078,7 @@
       </c>
       <c r="G25" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.35 : 1</v>
+        <v>0.36 : 1</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6092,15 +6116,15 @@
       </c>
       <c r="B27" s="4">
         <f>January!B27+February!B27+March!B27+April!B27+May!B27+June!B27+July!B27+August!B27+September!B27+October!B27+November!B27+December!B27</f>
-        <v>1126</v>
+        <v>1345</v>
       </c>
       <c r="C27" s="4">
         <f>January!C27+February!C27+March!C27+April!C27+May!C27+June!C27+July!C27+August!C27+September!C27+October!C27+November!C27+December!C27</f>
-        <v>958</v>
+        <v>1135</v>
       </c>
       <c r="D27" s="4">
         <f>January!D27+February!D27+March!D27+April!D27+May!D27+June!D27+July!D27+August!D27+September!D27+October!D27+November!D27+December!D27</f>
-        <v>168</v>
+        <v>210</v>
       </c>
       <c r="E27" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6112,7 +6136,7 @@
       </c>
       <c r="G27" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.18 : 1</v>
+        <v>1.19 : 1</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6121,15 +6145,15 @@
       </c>
       <c r="B28" s="2">
         <f>January!B28+February!B28+March!B28+April!B28+May!B28+June!B28+July!B28+August!B28+September!B28+October!B28+November!B28+December!B28</f>
-        <v>745</v>
+        <v>864</v>
       </c>
       <c r="C28" s="2">
         <f>January!C28+February!C28+March!C28+April!C28+May!C28+June!C28+July!C28+August!C28+September!C28+October!C28+November!C28+December!C28</f>
-        <v>649</v>
+        <v>794</v>
       </c>
       <c r="D28" s="2">
         <f>January!D28+February!D28+March!D28+April!D28+May!D28+June!D28+July!D28+August!D28+September!D28+October!D28+November!D28+December!D28</f>
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="E28" s="28" t="str">
         <f t="shared" si="0"/>
@@ -6141,7 +6165,7 @@
       </c>
       <c r="G28" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.15 : 1</v>
+        <v>1.09 : 1</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6150,15 +6174,15 @@
       </c>
       <c r="B29" s="4">
         <f>January!B29+February!B29+March!B29+April!B29+May!B29+June!B29+July!B29+August!B29+September!B29+October!B29+November!B29+December!B29</f>
-        <v>4006</v>
+        <v>4530</v>
       </c>
       <c r="C29" s="4">
         <f>January!C29+February!C29+March!C29+April!C29+May!C29+June!C29+July!C29+August!C29+September!C29+October!C29+November!C29+December!C29</f>
-        <v>2756</v>
+        <v>3217</v>
       </c>
       <c r="D29" s="4">
         <f>January!D29+February!D29+March!D29+April!D29+May!D29+June!D29+July!D29+August!D29+September!D29+October!D29+November!D29+December!D29</f>
-        <v>1250</v>
+        <v>1313</v>
       </c>
       <c r="E29" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6170,7 +6194,7 @@
       </c>
       <c r="G29" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.45 : 1</v>
+        <v>1.41 : 1</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6179,15 +6203,15 @@
       </c>
       <c r="B30" s="2">
         <f>January!B30+February!B30+March!B30+April!B30+May!B30+June!B30+July!B30+August!B30+September!B30+October!B30+November!B30+December!B30</f>
-        <v>194</v>
+        <v>232</v>
       </c>
       <c r="C30" s="2">
         <f>January!C30+February!C30+March!C30+April!C30+May!C30+June!C30+July!C30+August!C30+September!C30+October!C30+November!C30+December!C30</f>
-        <v>143</v>
+        <v>174</v>
       </c>
       <c r="D30" s="2">
         <f>January!D30+February!D30+March!D30+April!D30+May!D30+June!D30+July!D30+August!D30+September!D30+October!D30+November!D30+December!D30</f>
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="E30" s="28" t="str">
         <f t="shared" si="0"/>
@@ -6199,7 +6223,7 @@
       </c>
       <c r="G30" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.36 : 1</v>
+        <v>1.33 : 1</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6208,15 +6232,15 @@
       </c>
       <c r="B31" s="4">
         <f>January!B31+February!B31+March!B31+April!B31+May!B31+June!B31+July!B31+August!B31+September!B31+October!B31+November!B31+December!B31</f>
-        <v>358</v>
+        <v>432</v>
       </c>
       <c r="C31" s="4">
         <f>January!C31+February!C31+March!C31+April!C31+May!C31+June!C31+July!C31+August!C31+September!C31+October!C31+November!C31+December!C31</f>
-        <v>1521</v>
+        <v>1742</v>
       </c>
       <c r="D31" s="4">
         <f>January!D31+February!D31+March!D31+April!D31+May!D31+June!D31+July!D31+August!D31+September!D31+October!D31+November!D31+December!D31</f>
-        <v>-1163</v>
+        <v>-1310</v>
       </c>
       <c r="E31" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6228,7 +6252,7 @@
       </c>
       <c r="G31" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.24 : 1</v>
+        <v>0.25 : 1</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6237,15 +6261,15 @@
       </c>
       <c r="B32" s="2">
         <f>January!B32+February!B32+March!B32+April!B32+May!B32+June!B32+July!B32+August!B32+September!B32+October!B32+November!B32+December!B32</f>
-        <v>2410</v>
+        <v>2876</v>
       </c>
       <c r="C32" s="2">
         <f>January!C32+February!C32+March!C32+April!C32+May!C32+June!C32+July!C32+August!C32+September!C32+October!C32+November!C32+December!C32</f>
-        <v>3287</v>
+        <v>3850</v>
       </c>
       <c r="D32" s="2">
         <f>January!D32+February!D32+March!D32+April!D32+May!D32+June!D32+July!D32+August!D32+September!D32+October!D32+November!D32+December!D32</f>
-        <v>-877</v>
+        <v>-974</v>
       </c>
       <c r="E32" s="28" t="str">
         <f t="shared" si="0"/>
@@ -6257,7 +6281,7 @@
       </c>
       <c r="G32" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.73 : 1</v>
+        <v>0.75 : 1</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6266,15 +6290,15 @@
       </c>
       <c r="B33" s="4">
         <f>January!B33+February!B33+March!B33+April!B33+May!B33+June!B33+July!B33+August!B33+September!B33+October!B33+November!B33+December!B33</f>
-        <v>2552</v>
+        <v>3029</v>
       </c>
       <c r="C33" s="4">
         <f>January!C33+February!C33+March!C33+April!C33+May!C33+June!C33+July!C33+August!C33+September!C33+October!C33+November!C33+December!C33</f>
-        <v>2609</v>
+        <v>3045</v>
       </c>
       <c r="D33" s="4">
         <f>January!D33+February!D33+March!D33+April!D33+May!D33+June!D33+July!D33+August!D33+September!D33+October!D33+November!D33+December!D33</f>
-        <v>-57</v>
+        <v>-16</v>
       </c>
       <c r="E33" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6286,7 +6310,7 @@
       </c>
       <c r="G33" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.98 : 1</v>
+        <v>0.99 : 1</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6295,15 +6319,15 @@
       </c>
       <c r="B34" s="2">
         <f>January!B34+February!B34+March!B34+April!B34+May!B34+June!B34+July!B34+August!B34+September!B34+October!B34+November!B34+December!B34</f>
-        <v>1148</v>
+        <v>1380</v>
       </c>
       <c r="C34" s="2">
         <f>January!C34+February!C34+March!C34+April!C34+May!C34+June!C34+July!C34+August!C34+September!C34+October!C34+November!C34+December!C34</f>
-        <v>937</v>
+        <v>1080</v>
       </c>
       <c r="D34" s="2">
         <f>January!D34+February!D34+March!D34+April!D34+May!D34+June!D34+July!D34+August!D34+September!D34+October!D34+November!D34+December!D34</f>
-        <v>211</v>
+        <v>300</v>
       </c>
       <c r="E34" s="28" t="str">
         <f t="shared" ref="E34:E54" si="3">IF(D34 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -6315,7 +6339,7 @@
       </c>
       <c r="G34" s="3" t="str">
         <f t="shared" ref="G34:G54" si="5">IF(ISERROR(ROUND(B34/C34,2)&amp;" : 1"), "", ROUND(B34/C34,2)&amp;" : 1")</f>
-        <v>1.23 : 1</v>
+        <v>1.28 : 1</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6324,15 +6348,15 @@
       </c>
       <c r="B35" s="4">
         <f>January!B35+February!B35+March!B35+April!B35+May!B35+June!B35+July!B35+August!B35+September!B35+October!B35+November!B35+December!B35</f>
-        <v>5144</v>
+        <v>6265</v>
       </c>
       <c r="C35" s="4">
         <f>January!C35+February!C35+March!C35+April!C35+May!C35+June!C35+July!C35+August!C35+September!C35+October!C35+November!C35+December!C35</f>
-        <v>7584</v>
+        <v>8938</v>
       </c>
       <c r="D35" s="4">
         <f>January!D35+February!D35+March!D35+April!D35+May!D35+June!D35+July!D35+August!D35+September!D35+October!D35+November!D35+December!D35</f>
-        <v>-2440</v>
+        <v>-2673</v>
       </c>
       <c r="E35" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6344,7 +6368,7 @@
       </c>
       <c r="G35" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.68 : 1</v>
+        <v>0.7 : 1</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6353,15 +6377,15 @@
       </c>
       <c r="B36" s="2">
         <f>January!B36+February!B36+March!B36+April!B36+May!B36+June!B36+July!B36+August!B36+September!B36+October!B36+November!B36+December!B36</f>
-        <v>943</v>
+        <v>1125</v>
       </c>
       <c r="C36" s="2">
         <f>January!C36+February!C36+March!C36+April!C36+May!C36+June!C36+July!C36+August!C36+September!C36+October!C36+November!C36+December!C36</f>
-        <v>3123</v>
+        <v>3586</v>
       </c>
       <c r="D36" s="2">
         <f>January!D36+February!D36+March!D36+April!D36+May!D36+June!D36+July!D36+August!D36+September!D36+October!D36+November!D36+December!D36</f>
-        <v>-2180</v>
+        <v>-2461</v>
       </c>
       <c r="E36" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6373,7 +6397,7 @@
       </c>
       <c r="G36" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.3 : 1</v>
+        <v>0.31 : 1</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6382,15 +6406,15 @@
       </c>
       <c r="B37" s="4">
         <f>January!B37+February!B37+March!B37+April!B37+May!B37+June!B37+July!B37+August!B37+September!B37+October!B37+November!B37+December!B37</f>
-        <v>3077</v>
+        <v>3634</v>
       </c>
       <c r="C37" s="4">
         <f>January!C37+February!C37+March!C37+April!C37+May!C37+June!C37+July!C37+August!C37+September!C37+October!C37+November!C37+December!C37</f>
-        <v>1643</v>
+        <v>2037</v>
       </c>
       <c r="D37" s="4">
         <f>January!D37+February!D37+March!D37+April!D37+May!D37+June!D37+July!D37+August!D37+September!D37+October!D37+November!D37+December!D37</f>
-        <v>1434</v>
+        <v>1597</v>
       </c>
       <c r="E37" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6402,7 +6426,7 @@
       </c>
       <c r="G37" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>1.87 : 1</v>
+        <v>1.78 : 1</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6411,15 +6435,15 @@
       </c>
       <c r="B38" s="2">
         <f>January!B38+February!B38+March!B38+April!B38+May!B38+June!B38+July!B38+August!B38+September!B38+October!B38+November!B38+December!B38</f>
-        <v>136</v>
+        <v>171</v>
       </c>
       <c r="C38" s="2">
         <f>January!C38+February!C38+March!C38+April!C38+May!C38+June!C38+July!C38+August!C38+September!C38+October!C38+November!C38+December!C38</f>
-        <v>985</v>
+        <v>1173</v>
       </c>
       <c r="D38" s="2">
         <f>January!D38+February!D38+March!D38+April!D38+May!D38+June!D38+July!D38+August!D38+September!D38+October!D38+November!D38+December!D38</f>
-        <v>-849</v>
+        <v>-1002</v>
       </c>
       <c r="E38" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6431,7 +6455,7 @@
       </c>
       <c r="G38" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.14 : 1</v>
+        <v>0.15 : 1</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6444,11 +6468,11 @@
       </c>
       <c r="C39" s="4">
         <f>January!C39+February!C39+March!C39+April!C39+May!C39+June!C39+July!C39+August!C39+September!C39+October!C39+November!C39+December!C39</f>
-        <v>494</v>
+        <v>502</v>
       </c>
       <c r="D39" s="4">
         <f>January!D39+February!D39+March!D39+April!D39+May!D39+June!D39+July!D39+August!D39+September!D39+October!D39+November!D39+December!D39</f>
-        <v>-295</v>
+        <v>-303</v>
       </c>
       <c r="E39" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6531,11 +6555,11 @@
       </c>
       <c r="C42" s="38">
         <f>January!C42+February!C42+March!C42+April!C42+May!C42+June!C42+July!C42+August!C42+September!C42+October!C42+November!C42+December!C42</f>
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D42" s="38">
         <f>January!D42+February!D42+March!D42+April!D42+May!D42+June!D42+July!D42+August!D42+September!D42+October!D42+November!D42+December!D42</f>
-        <v>-171</v>
+        <v>-172</v>
       </c>
       <c r="E42" s="39" t="str">
         <f t="shared" si="3"/>
@@ -6556,15 +6580,15 @@
       </c>
       <c r="B43" s="8">
         <f>January!B43+February!B43+March!B43+April!B43+May!B43+June!B43+July!B43+August!B43+September!B43+October!B43+November!B43+December!B43</f>
-        <v>305</v>
+        <v>383</v>
       </c>
       <c r="C43" s="8">
         <f>January!C43+February!C43+March!C43+April!C43+May!C43+June!C43+July!C43+August!C43+September!C43+October!C43+November!C43+December!C43</f>
-        <v>384</v>
+        <v>478</v>
       </c>
       <c r="D43" s="8">
         <f>January!D43+February!D43+March!D43+April!D43+May!D43+June!D43+July!D43+August!D43+September!D43+October!D43+November!D43+December!D43</f>
-        <v>-79</v>
+        <v>-95</v>
       </c>
       <c r="E43" s="31" t="str">
         <f t="shared" si="3"/>
@@ -6576,7 +6600,7 @@
       </c>
       <c r="G43" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0.79 : 1</v>
+        <v>0.8 : 1</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6585,15 +6609,15 @@
       </c>
       <c r="B44" s="2">
         <f>January!B44+February!B44+March!B44+April!B44+May!B44+June!B44+July!B44+August!B44+September!B44+October!B44+November!B44+December!B44</f>
-        <v>336</v>
+        <v>420</v>
       </c>
       <c r="C44" s="2">
         <f>January!C44+February!C44+March!C44+April!C44+May!C44+June!C44+July!C44+August!C44+September!C44+October!C44+November!C44+December!C44</f>
-        <v>1204</v>
+        <v>1429</v>
       </c>
       <c r="D44" s="2">
         <f>January!D44+February!D44+March!D44+April!D44+May!D44+June!D44+July!D44+August!D44+September!D44+October!D44+November!D44+December!D44</f>
-        <v>-868</v>
+        <v>-1009</v>
       </c>
       <c r="E44" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6605,7 +6629,7 @@
       </c>
       <c r="G44" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.28 : 1</v>
+        <v>0.29 : 1</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6614,15 +6638,15 @@
       </c>
       <c r="B45" s="4">
         <f>January!B45+February!B45+March!B45+April!B45+May!B45+June!B45+July!B45+August!B45+September!B45+October!B45+November!B45+December!B45</f>
-        <v>3301</v>
+        <v>3750</v>
       </c>
       <c r="C45" s="4">
         <f>January!C45+February!C45+March!C45+April!C45+May!C45+June!C45+July!C45+August!C45+September!C45+October!C45+November!C45+December!C45</f>
-        <v>3320</v>
+        <v>3922</v>
       </c>
       <c r="D45" s="4">
         <f>January!D45+February!D45+March!D45+April!D45+May!D45+June!D45+July!D45+August!D45+September!D45+October!D45+November!D45+December!D45</f>
-        <v>-19</v>
+        <v>-172</v>
       </c>
       <c r="E45" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6634,7 +6658,7 @@
       </c>
       <c r="G45" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.99 : 1</v>
+        <v>0.96 : 1</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6643,15 +6667,15 @@
       </c>
       <c r="B46" s="2">
         <f>January!B46+February!B46+March!B46+April!B46+May!B46+June!B46+July!B46+August!B46+September!B46+October!B46+November!B46+December!B46</f>
-        <v>6448</v>
+        <v>7458</v>
       </c>
       <c r="C46" s="2">
         <f>January!C46+February!C46+March!C46+April!C46+May!C46+June!C46+July!C46+August!C46+September!C46+October!C46+November!C46+December!C46</f>
-        <v>3907</v>
+        <v>4551</v>
       </c>
       <c r="D46" s="2">
         <f>January!D46+February!D46+March!D46+April!D46+May!D46+June!D46+July!D46+August!D46+September!D46+October!D46+November!D46+December!D46</f>
-        <v>2541</v>
+        <v>2907</v>
       </c>
       <c r="E46" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6663,7 +6687,7 @@
       </c>
       <c r="G46" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>1.65 : 1</v>
+        <v>1.64 : 1</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6672,15 +6696,15 @@
       </c>
       <c r="B47" s="4">
         <f>January!B47+February!B47+March!B47+April!B47+May!B47+June!B47+July!B47+August!B47+September!B47+October!B47+November!B47+December!B47</f>
-        <v>1251</v>
+        <v>1445</v>
       </c>
       <c r="C47" s="4">
         <f>January!C47+February!C47+March!C47+April!C47+May!C47+June!C47+July!C47+August!C47+September!C47+October!C47+November!C47+December!C47</f>
-        <v>3628</v>
+        <v>4293</v>
       </c>
       <c r="D47" s="4">
         <f>January!D47+February!D47+March!D47+April!D47+May!D47+June!D47+July!D47+August!D47+September!D47+October!D47+November!D47+December!D47</f>
-        <v>-2377</v>
+        <v>-2848</v>
       </c>
       <c r="E47" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6701,15 +6725,15 @@
       </c>
       <c r="B48" s="2">
         <f>January!B48+February!B48+March!B48+April!B48+May!B48+June!B48+July!B48+August!B48+September!B48+October!B48+November!B48+December!B48</f>
-        <v>3986</v>
+        <v>4496</v>
       </c>
       <c r="C48" s="2">
         <f>January!C48+February!C48+March!C48+April!C48+May!C48+June!C48+July!C48+August!C48+September!C48+October!C48+November!C48+December!C48</f>
-        <v>1371</v>
+        <v>1593</v>
       </c>
       <c r="D48" s="2">
         <f>January!D48+February!D48+March!D48+April!D48+May!D48+June!D48+July!D48+August!D48+September!D48+October!D48+November!D48+December!D48</f>
-        <v>2615</v>
+        <v>2903</v>
       </c>
       <c r="E48" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6721,7 +6745,7 @@
       </c>
       <c r="G48" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>2.91 : 1</v>
+        <v>2.82 : 1</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6730,15 +6754,15 @@
       </c>
       <c r="B49" s="4">
         <f>January!B49+February!B49+March!B49+April!B49+May!B49+June!B49+July!B49+August!B49+September!B49+October!B49+November!B49+December!B49</f>
-        <v>4830</v>
+        <v>5812</v>
       </c>
       <c r="C49" s="4">
         <f>January!C49+February!C49+March!C49+April!C49+May!C49+June!C49+July!C49+August!C49+September!C49+October!C49+November!C49+December!C49</f>
-        <v>3319</v>
+        <v>4053</v>
       </c>
       <c r="D49" s="4">
         <f>January!D49+February!D49+March!D49+April!D49+May!D49+June!D49+July!D49+August!D49+September!D49+October!D49+November!D49+December!D49</f>
-        <v>1511</v>
+        <v>1759</v>
       </c>
       <c r="E49" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6750,7 +6774,7 @@
       </c>
       <c r="G49" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>1.46 : 1</v>
+        <v>1.43 : 1</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6759,15 +6783,15 @@
       </c>
       <c r="B50" s="2">
         <f>January!B50+February!B50+March!B50+April!B50+May!B50+June!B50+July!B50+August!B50+September!B50+October!B50+November!B50+December!B50</f>
-        <v>1137</v>
+        <v>1267</v>
       </c>
       <c r="C50" s="2">
         <f>January!C50+February!C50+March!C50+April!C50+May!C50+June!C50+July!C50+August!C50+September!C50+October!C50+November!C50+December!C50</f>
-        <v>971</v>
+        <v>1135</v>
       </c>
       <c r="D50" s="2">
         <f>January!D50+February!D50+March!D50+April!D50+May!D50+June!D50+July!D50+August!D50+September!D50+October!D50+November!D50+December!D50</f>
-        <v>166</v>
+        <v>132</v>
       </c>
       <c r="E50" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6779,7 +6803,7 @@
       </c>
       <c r="G50" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>1.17 : 1</v>
+        <v>1.12 : 1</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6788,15 +6812,15 @@
       </c>
       <c r="B51" s="4">
         <f>January!B51+February!B51+March!B51+April!B51+May!B51+June!B51+July!B51+August!B51+September!B51+October!B51+November!B51+December!B51</f>
-        <v>2096</v>
+        <v>2456</v>
       </c>
       <c r="C51" s="4">
         <f>January!C51+February!C51+March!C51+April!C51+May!C51+June!C51+July!C51+August!C51+September!C51+October!C51+November!C51+December!C51</f>
-        <v>2277</v>
+        <v>2621</v>
       </c>
       <c r="D51" s="4">
         <f>January!D51+February!D51+March!D51+April!D51+May!D51+June!D51+July!D51+August!D51+September!D51+October!D51+November!D51+December!D51</f>
-        <v>-181</v>
+        <v>-165</v>
       </c>
       <c r="E51" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6808,7 +6832,7 @@
       </c>
       <c r="G51" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.92 : 1</v>
+        <v>0.94 : 1</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6817,15 +6841,15 @@
       </c>
       <c r="B52" s="2">
         <f>January!B52+February!B52+March!B52+April!B52+May!B52+June!B52+July!B52+August!B52+September!B52+October!B52+November!B52+December!B52</f>
-        <v>933</v>
+        <v>1029</v>
       </c>
       <c r="C52" s="2">
         <f>January!C52+February!C52+March!C52+April!C52+May!C52+June!C52+July!C52+August!C52+September!C52+October!C52+November!C52+December!C52</f>
-        <v>1296</v>
+        <v>1478</v>
       </c>
       <c r="D52" s="2">
         <f>January!D52+February!D52+March!D52+April!D52+May!D52+June!D52+July!D52+August!D52+September!D52+October!D52+November!D52+December!D52</f>
-        <v>-363</v>
+        <v>-449</v>
       </c>
       <c r="E52" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6837,7 +6861,7 @@
       </c>
       <c r="G52" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.72 : 1</v>
+        <v>0.7 : 1</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6846,15 +6870,15 @@
       </c>
       <c r="B53" s="4">
         <f>January!B53+February!B53+March!B53+April!B53+May!B53+June!B53+July!B53+August!B53+September!B53+October!B53+November!B53+December!B53</f>
-        <v>189</v>
+        <v>226</v>
       </c>
       <c r="C53" s="4">
         <f>January!C53+February!C53+March!C53+April!C53+May!C53+June!C53+July!C53+August!C53+September!C53+October!C53+November!C53+December!C53</f>
-        <v>1536</v>
+        <v>1733</v>
       </c>
       <c r="D53" s="4">
         <f>January!D53+February!D53+March!D53+April!D53+May!D53+June!D53+July!D53+August!D53+September!D53+October!D53+November!D53+December!D53</f>
-        <v>-1347</v>
+        <v>-1507</v>
       </c>
       <c r="E53" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6866,7 +6890,7 @@
       </c>
       <c r="G53" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.12 : 1</v>
+        <v>0.13 : 1</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6875,15 +6899,15 @@
       </c>
       <c r="B54" s="10">
         <f>January!B54+February!B54+March!B54+April!B54+May!B54+June!B54+July!B54+August!B54+September!B54+October!B54+November!B54+December!B54</f>
-        <v>2283</v>
+        <v>2676</v>
       </c>
       <c r="C54" s="10">
         <f>January!C54+February!C54+March!C54+April!C54+May!C54+June!C54+July!C54+August!C54+September!C54+October!C54+November!C54+December!C54</f>
-        <v>1269</v>
+        <v>1460</v>
       </c>
       <c r="D54" s="10">
         <f>January!D54+February!D54+March!D54+April!D54+May!D54+June!D54+July!D54+August!D54+September!D54+October!D54+November!D54+December!D54</f>
-        <v>1014</v>
+        <v>1216</v>
       </c>
       <c r="E54" s="32" t="str">
         <f t="shared" si="3"/>
@@ -6895,7 +6919,7 @@
       </c>
       <c r="G54" s="11" t="str">
         <f t="shared" si="5"/>
-        <v>1.8 : 1</v>
+        <v>1.83 : 1</v>
       </c>
     </row>
   </sheetData>
@@ -12894,7 +12918,7 @@
       <selection activeCell="A42" activeCellId="1" sqref="A40:G40 A42:G42"/>
       <selection pane="topRight" activeCell="A42" activeCellId="1" sqref="A40:G40 A42:G42"/>
       <selection pane="bottomLeft" activeCell="A42" activeCellId="1" sqref="A40:G40 A42:G42"/>
-      <selection pane="bottomRight" activeCell="A42" activeCellId="1" sqref="A40:G40 A42:G42"/>
+      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12934,108 +12958,204 @@
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="28"/>
+      <c r="B2" s="18">
+        <v>1540</v>
+      </c>
+      <c r="C2" s="18">
+        <v>1277</v>
+      </c>
+      <c r="D2" s="18">
+        <v>263</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F2" s="28"/>
-      <c r="G2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="29"/>
+      <c r="B3" s="21">
+        <v>750</v>
+      </c>
+      <c r="C3" s="21">
+        <v>373</v>
+      </c>
+      <c r="D3" s="21">
+        <v>377</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F3" s="29"/>
-      <c r="G3" s="5"/>
+      <c r="G3" s="5" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
+      <c r="B4" s="18">
+        <v>1230</v>
+      </c>
+      <c r="C4" s="18">
+        <v>1398</v>
+      </c>
+      <c r="D4" s="18">
+        <v>-168</v>
+      </c>
       <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="3"/>
+      <c r="F4" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
+      <c r="B5" s="21">
+        <v>46</v>
+      </c>
+      <c r="C5" s="21">
+        <v>132</v>
+      </c>
+      <c r="D5" s="21">
+        <v>-86</v>
+      </c>
       <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="5"/>
+      <c r="F5" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
+      <c r="B6" s="18">
+        <v>1074</v>
+      </c>
+      <c r="C6" s="18">
+        <v>1164</v>
+      </c>
+      <c r="D6" s="18">
+        <v>-90</v>
+      </c>
       <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="3"/>
+      <c r="F6" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="29"/>
+      <c r="B7" s="21">
+        <v>331</v>
+      </c>
+      <c r="C7" s="21">
+        <v>232</v>
+      </c>
+      <c r="D7" s="21">
+        <v>99</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F7" s="29"/>
-      <c r="G7" s="5"/>
+      <c r="G7" s="5" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
+      <c r="B8" s="18">
+        <v>105</v>
+      </c>
+      <c r="C8" s="18">
+        <v>160</v>
+      </c>
+      <c r="D8" s="18">
+        <v>-55</v>
+      </c>
       <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="3"/>
+      <c r="F8" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="29"/>
+      <c r="B9" s="21">
+        <v>82</v>
+      </c>
+      <c r="C9" s="21">
+        <v>65</v>
+      </c>
+      <c r="D9" s="21">
+        <v>17</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F9" s="29"/>
-      <c r="G9" s="5"/>
+      <c r="G9" s="5" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
+      <c r="B10" s="18">
+        <v>0</v>
+      </c>
+      <c r="C10" s="18">
+        <v>37</v>
+      </c>
+      <c r="D10" s="18">
+        <v>-37</v>
+      </c>
       <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="3"/>
+      <c r="F10" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
+      <c r="B11" s="21">
+        <v>0</v>
+      </c>
+      <c r="C11" s="21">
+        <v>0</v>
+      </c>
+      <c r="D11" s="21">
+        <v>0</v>
+      </c>
       <c r="E11" s="29"/>
       <c r="F11" s="29"/>
       <c r="G11" s="5"/>
@@ -13044,163 +13164,309 @@
       <c r="A12" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="35"/>
+      <c r="B12" s="41">
+        <v>28</v>
+      </c>
+      <c r="C12" s="41">
+        <v>13</v>
+      </c>
+      <c r="D12" s="41">
+        <v>15</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>60</v>
+      </c>
       <c r="F12" s="35"/>
-      <c r="G12" s="36"/>
+      <c r="G12" s="36" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="30"/>
+      <c r="B13" s="23">
+        <v>89</v>
+      </c>
+      <c r="C13" s="23">
+        <v>87</v>
+      </c>
+      <c r="D13" s="23">
+        <v>2</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>60</v>
+      </c>
       <c r="F13" s="30"/>
-      <c r="G13" s="7"/>
+      <c r="G13" s="7" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
+      <c r="B14" s="41">
+        <v>191</v>
+      </c>
+      <c r="C14" s="41">
+        <v>240</v>
+      </c>
+      <c r="D14" s="41">
+        <v>-49</v>
+      </c>
       <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="36"/>
+      <c r="F14" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="36" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
+      <c r="B15" s="23">
+        <v>80</v>
+      </c>
+      <c r="C15" s="23">
+        <v>152</v>
+      </c>
+      <c r="D15" s="23">
+        <v>-72</v>
+      </c>
       <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="7"/>
+      <c r="F15" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="B16" s="18">
+        <v>81</v>
+      </c>
+      <c r="C16" s="18">
+        <v>150</v>
+      </c>
+      <c r="D16" s="18">
+        <v>-69</v>
+      </c>
       <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="3"/>
+      <c r="F16" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="29"/>
+      <c r="B17" s="21">
+        <v>653</v>
+      </c>
+      <c r="C17" s="21">
+        <v>454</v>
+      </c>
+      <c r="D17" s="21">
+        <v>199</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F17" s="29"/>
-      <c r="G17" s="5"/>
+      <c r="G17" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
+      <c r="B18" s="18">
+        <v>25</v>
+      </c>
+      <c r="C18" s="18">
+        <v>94</v>
+      </c>
+      <c r="D18" s="18">
+        <v>-69</v>
+      </c>
       <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="3"/>
+      <c r="F18" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
+      <c r="B19" s="21">
+        <v>465</v>
+      </c>
+      <c r="C19" s="21">
+        <v>505</v>
+      </c>
+      <c r="D19" s="21">
+        <v>-40</v>
+      </c>
       <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="5"/>
+      <c r="F19" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+      <c r="B20" s="18">
+        <v>12</v>
+      </c>
+      <c r="C20" s="18">
+        <v>67</v>
+      </c>
+      <c r="D20" s="18">
+        <v>-55</v>
+      </c>
       <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="3"/>
+      <c r="F20" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="29"/>
+      <c r="B21" s="21">
+        <v>498</v>
+      </c>
+      <c r="C21" s="21">
+        <v>339</v>
+      </c>
+      <c r="D21" s="21">
+        <v>159</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F21" s="29"/>
-      <c r="G21" s="5"/>
+      <c r="G21" s="5" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="B22" s="18">
+        <v>75</v>
+      </c>
+      <c r="C22" s="18">
+        <v>283</v>
+      </c>
+      <c r="D22" s="18">
+        <v>-208</v>
+      </c>
       <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="3"/>
+      <c r="F22" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
+      <c r="B23" s="21">
+        <v>634</v>
+      </c>
+      <c r="C23" s="21">
+        <v>636</v>
+      </c>
+      <c r="D23" s="21">
+        <v>-2</v>
+      </c>
       <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="5"/>
+      <c r="F23" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="28"/>
+      <c r="B24" s="18">
+        <v>1709</v>
+      </c>
+      <c r="C24" s="18">
+        <v>1098</v>
+      </c>
+      <c r="D24" s="18">
+        <v>611</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F24" s="28"/>
-      <c r="G24" s="3"/>
+      <c r="G24" s="3" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
+      <c r="B25" s="21">
+        <v>169</v>
+      </c>
+      <c r="C25" s="21">
+        <v>429</v>
+      </c>
+      <c r="D25" s="21">
+        <v>-260</v>
+      </c>
       <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="5"/>
+      <c r="F25" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
+      <c r="B26" s="18">
+        <v>0</v>
+      </c>
+      <c r="C26" s="18">
+        <v>0</v>
+      </c>
+      <c r="D26" s="18">
+        <v>0</v>
+      </c>
       <c r="E26" s="28"/>
       <c r="F26" s="28"/>
       <c r="G26" s="3"/>
@@ -13209,152 +13475,288 @@
       <c r="A27" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="29"/>
+      <c r="B27" s="21">
+        <v>219</v>
+      </c>
+      <c r="C27" s="21">
+        <v>177</v>
+      </c>
+      <c r="D27" s="21">
+        <v>42</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F27" s="29"/>
-      <c r="G27" s="5"/>
+      <c r="G27" s="5" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
+      <c r="B28" s="18">
+        <v>119</v>
+      </c>
+      <c r="C28" s="18">
+        <v>145</v>
+      </c>
+      <c r="D28" s="18">
+        <v>-26</v>
+      </c>
       <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="3"/>
+      <c r="F28" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="29"/>
+      <c r="B29" s="21">
+        <v>524</v>
+      </c>
+      <c r="C29" s="21">
+        <v>461</v>
+      </c>
+      <c r="D29" s="21">
+        <v>63</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F29" s="29"/>
-      <c r="G29" s="5"/>
+      <c r="G29" s="5" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="28"/>
+      <c r="B30" s="18">
+        <v>38</v>
+      </c>
+      <c r="C30" s="18">
+        <v>31</v>
+      </c>
+      <c r="D30" s="18">
+        <v>7</v>
+      </c>
+      <c r="E30" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F30" s="28"/>
-      <c r="G30" s="3"/>
+      <c r="G30" s="3" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
+      <c r="B31" s="21">
+        <v>74</v>
+      </c>
+      <c r="C31" s="21">
+        <v>221</v>
+      </c>
+      <c r="D31" s="21">
+        <v>-147</v>
+      </c>
       <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="5"/>
+      <c r="F31" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="B32" s="18">
+        <v>466</v>
+      </c>
+      <c r="C32" s="18">
+        <v>563</v>
+      </c>
+      <c r="D32" s="18">
+        <v>-97</v>
+      </c>
       <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="3"/>
+      <c r="F32" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="29"/>
+      <c r="B33" s="21">
+        <v>477</v>
+      </c>
+      <c r="C33" s="21">
+        <v>436</v>
+      </c>
+      <c r="D33" s="21">
+        <v>41</v>
+      </c>
+      <c r="E33" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F33" s="29"/>
-      <c r="G33" s="5"/>
+      <c r="G33" s="5" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="28"/>
+      <c r="B34" s="18">
+        <v>232</v>
+      </c>
+      <c r="C34" s="18">
+        <v>143</v>
+      </c>
+      <c r="D34" s="18">
+        <v>89</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F34" s="28"/>
-      <c r="G34" s="3"/>
+      <c r="G34" s="3" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
+      <c r="B35" s="21">
+        <v>1121</v>
+      </c>
+      <c r="C35" s="21">
+        <v>1354</v>
+      </c>
+      <c r="D35" s="21">
+        <v>-233</v>
+      </c>
       <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="5"/>
+      <c r="F35" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="B36" s="18">
+        <v>182</v>
+      </c>
+      <c r="C36" s="18">
+        <v>463</v>
+      </c>
+      <c r="D36" s="18">
+        <v>-281</v>
+      </c>
       <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="3"/>
+      <c r="F36" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="29"/>
+      <c r="B37" s="21">
+        <v>557</v>
+      </c>
+      <c r="C37" s="21">
+        <v>394</v>
+      </c>
+      <c r="D37" s="21">
+        <v>163</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F37" s="29"/>
-      <c r="G37" s="5"/>
+      <c r="G37" s="5" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
+      <c r="B38" s="18">
+        <v>35</v>
+      </c>
+      <c r="C38" s="18">
+        <v>188</v>
+      </c>
+      <c r="D38" s="18">
+        <v>-153</v>
+      </c>
       <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="3"/>
+      <c r="F38" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="B39" s="21"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
+      <c r="B39" s="21">
+        <v>0</v>
+      </c>
+      <c r="C39" s="21">
+        <v>8</v>
+      </c>
+      <c r="D39" s="21">
+        <v>-8</v>
+      </c>
       <c r="E39" s="29"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="5"/>
+      <c r="F39" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="42"/>
-      <c r="C40" s="42"/>
-      <c r="D40" s="42"/>
+      <c r="B40" s="42">
+        <v>0</v>
+      </c>
+      <c r="C40" s="42">
+        <v>0</v>
+      </c>
+      <c r="D40" s="42">
+        <v>0</v>
+      </c>
       <c r="E40" s="39"/>
       <c r="F40" s="39"/>
       <c r="G40" s="40"/>
@@ -13363,9 +13765,15 @@
       <c r="A41" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
+      <c r="B41" s="25">
+        <v>0</v>
+      </c>
+      <c r="C41" s="25">
+        <v>0</v>
+      </c>
+      <c r="D41" s="25">
+        <v>0</v>
+      </c>
       <c r="E41" s="31"/>
       <c r="F41" s="31"/>
       <c r="G41" s="9"/>
@@ -13374,144 +13782,274 @@
       <c r="A42" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="B42" s="42"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="42"/>
+      <c r="B42" s="42">
+        <v>0</v>
+      </c>
+      <c r="C42" s="42">
+        <v>1</v>
+      </c>
+      <c r="D42" s="42">
+        <v>-1</v>
+      </c>
       <c r="E42" s="39"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="40"/>
+      <c r="F42" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="G42" s="40" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
+      <c r="B43" s="25">
+        <v>78</v>
+      </c>
+      <c r="C43" s="25">
+        <v>94</v>
+      </c>
+      <c r="D43" s="25">
+        <v>-16</v>
+      </c>
       <c r="E43" s="31"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="9"/>
+      <c r="F43" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
+      <c r="B44" s="18">
+        <v>84</v>
+      </c>
+      <c r="C44" s="18">
+        <v>225</v>
+      </c>
+      <c r="D44" s="18">
+        <v>-141</v>
+      </c>
       <c r="E44" s="28"/>
-      <c r="F44" s="28"/>
-      <c r="G44" s="3"/>
+      <c r="F44" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="21"/>
-      <c r="C45" s="21"/>
-      <c r="D45" s="21"/>
+      <c r="B45" s="21">
+        <v>449</v>
+      </c>
+      <c r="C45" s="21">
+        <v>602</v>
+      </c>
+      <c r="D45" s="21">
+        <v>-153</v>
+      </c>
       <c r="E45" s="29"/>
-      <c r="F45" s="29"/>
-      <c r="G45" s="5"/>
+      <c r="F45" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="28"/>
+      <c r="B46" s="18">
+        <v>1010</v>
+      </c>
+      <c r="C46" s="18">
+        <v>644</v>
+      </c>
+      <c r="D46" s="18">
+        <v>366</v>
+      </c>
+      <c r="E46" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F46" s="28"/>
-      <c r="G46" s="3"/>
+      <c r="G46" s="3" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="21"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
+      <c r="B47" s="21">
+        <v>194</v>
+      </c>
+      <c r="C47" s="21">
+        <v>665</v>
+      </c>
+      <c r="D47" s="21">
+        <v>-471</v>
+      </c>
       <c r="E47" s="29"/>
-      <c r="F47" s="29"/>
-      <c r="G47" s="5"/>
+      <c r="F47" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="28"/>
+      <c r="B48" s="18">
+        <v>510</v>
+      </c>
+      <c r="C48" s="18">
+        <v>222</v>
+      </c>
+      <c r="D48" s="18">
+        <v>288</v>
+      </c>
+      <c r="E48" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F48" s="28"/>
-      <c r="G48" s="3"/>
+      <c r="G48" s="3" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="21"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="29"/>
+      <c r="B49" s="21">
+        <v>982</v>
+      </c>
+      <c r="C49" s="21">
+        <v>734</v>
+      </c>
+      <c r="D49" s="21">
+        <v>248</v>
+      </c>
+      <c r="E49" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F49" s="29"/>
-      <c r="G49" s="5"/>
+      <c r="G49" s="5" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="18"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
+      <c r="B50" s="18">
+        <v>130</v>
+      </c>
+      <c r="C50" s="18">
+        <v>164</v>
+      </c>
+      <c r="D50" s="18">
+        <v>-34</v>
+      </c>
       <c r="E50" s="28"/>
-      <c r="F50" s="28"/>
-      <c r="G50" s="3"/>
+      <c r="F50" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="21"/>
-      <c r="C51" s="21"/>
-      <c r="D51" s="21"/>
-      <c r="E51" s="29"/>
+      <c r="B51" s="21">
+        <v>360</v>
+      </c>
+      <c r="C51" s="21">
+        <v>344</v>
+      </c>
+      <c r="D51" s="21">
+        <v>16</v>
+      </c>
+      <c r="E51" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F51" s="29"/>
-      <c r="G51" s="5"/>
+      <c r="G51" s="5" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="18"/>
-      <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
+      <c r="B52" s="18">
+        <v>96</v>
+      </c>
+      <c r="C52" s="18">
+        <v>182</v>
+      </c>
+      <c r="D52" s="18">
+        <v>-86</v>
+      </c>
       <c r="E52" s="28"/>
-      <c r="F52" s="28"/>
-      <c r="G52" s="3"/>
+      <c r="F52" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="21"/>
-      <c r="C53" s="21"/>
-      <c r="D53" s="21"/>
+      <c r="B53" s="21">
+        <v>37</v>
+      </c>
+      <c r="C53" s="21">
+        <v>197</v>
+      </c>
+      <c r="D53" s="21">
+        <v>-160</v>
+      </c>
       <c r="E53" s="29"/>
-      <c r="F53" s="29"/>
-      <c r="G53" s="5"/>
+      <c r="F53" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="B54" s="27"/>
-      <c r="C54" s="27"/>
-      <c r="D54" s="27"/>
-      <c r="E54" s="32"/>
+      <c r="B54" s="27">
+        <v>393</v>
+      </c>
+      <c r="C54" s="27">
+        <v>191</v>
+      </c>
+      <c r="D54" s="27">
+        <v>202</v>
+      </c>
+      <c r="E54" s="32" t="s">
+        <v>60</v>
+      </c>
       <c r="F54" s="32"/>
-      <c r="G54" s="11"/>
+      <c r="G54" s="11" t="s">
+        <v>229</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G54" xr:uid="{00000000-0009-0000-0000-000007000000}"/>

</xml_diff>

<commit_message>
Update all remaining September statistic files
</commit_message>
<xml_diff>
--- a/statistics_files/2025/2025_99_g_net_borrower_lender.xlsx
+++ b/statistics_files/2025/2025_99_g_net_borrower_lender.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\github\next_statistics\statistics_files\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2500806-0369-4011-8CD3-98E1C3666FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09807FBD-0A2A-4655-A8DB-5DB5BC19E211}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="673" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="673" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="January" sheetId="2" r:id="rId1"/>
@@ -47,15 +47,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
       <xlwcv:version setVersion="1"/>
     </ext>
@@ -64,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1692" uniqueCount="248">
   <si>
     <t>NET</t>
   </si>
@@ -778,6 +769,36 @@
   </si>
   <si>
     <t>2.03 : 1</t>
+  </si>
+  <si>
+    <t>1.91 : 1</t>
+  </si>
+  <si>
+    <t>0.87 : 1</t>
+  </si>
+  <si>
+    <t>1.11 : 1</t>
+  </si>
+  <si>
+    <t>1.37 : 1</t>
+  </si>
+  <si>
+    <t>1.42 : 1</t>
+  </si>
+  <si>
+    <t>0.55 : 1</t>
+  </si>
+  <si>
+    <t>2.27 : 1</t>
+  </si>
+  <si>
+    <t>1.22 : 1</t>
+  </si>
+  <si>
+    <t>0.57 : 1</t>
+  </si>
+  <si>
+    <t>1.72 : 1</t>
   </si>
 </sst>
 </file>
@@ -2171,7 +2192,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B40" sqref="B40"/>
       <selection pane="topRight" activeCell="B40" sqref="B40"/>
@@ -5418,15 +5439,15 @@
       </c>
       <c r="B2" s="2">
         <f>January!B2+February!B2+March!B2+April!B2+May!B2+June!B2+July!B2+August!B2+September!B2+October!B2+November!B2+December!B2</f>
-        <v>12044</v>
+        <v>13621</v>
       </c>
       <c r="C2" s="2">
         <f>January!C2+February!C2+March!C2+April!C2+May!C2+June!C2+July!C2+August!C2+September!C2+October!C2+November!C2+December!C2</f>
-        <v>9982</v>
+        <v>11327</v>
       </c>
       <c r="D2" s="2">
         <f>January!D2+February!D2+March!D2+April!D2+May!D2+June!D2+July!D2+August!D2+September!D2+October!D2+November!D2+December!D2</f>
-        <v>2062</v>
+        <v>2294</v>
       </c>
       <c r="E2" s="28" t="str">
         <f t="shared" ref="E2:E33" si="0">IF(D2 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -5438,7 +5459,7 @@
       </c>
       <c r="G2" s="3" t="str">
         <f t="shared" ref="G2:G33" si="2">IF(ISERROR(ROUND(B2/C2,2)&amp;" : 1"), "", ROUND(B2/C2,2)&amp;" : 1")</f>
-        <v>1.21 : 1</v>
+        <v>1.2 : 1</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5447,15 +5468,15 @@
       </c>
       <c r="B3" s="4">
         <f>January!B3+February!B3+March!B3+April!B3+May!B3+June!B3+July!B3+August!B3+September!B3+October!B3+November!B3+December!B3</f>
-        <v>5138</v>
+        <v>5808</v>
       </c>
       <c r="C3" s="4">
         <f>January!C3+February!C3+March!C3+April!C3+May!C3+June!C3+July!C3+August!C3+September!C3+October!C3+November!C3+December!C3</f>
-        <v>2942</v>
+        <v>3293</v>
       </c>
       <c r="D3" s="4">
         <f>January!D3+February!D3+March!D3+April!D3+May!D3+June!D3+July!D3+August!D3+September!D3+October!D3+November!D3+December!D3</f>
-        <v>2196</v>
+        <v>2515</v>
       </c>
       <c r="E3" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5467,7 +5488,7 @@
       </c>
       <c r="G3" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.75 : 1</v>
+        <v>1.76 : 1</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5476,15 +5497,15 @@
       </c>
       <c r="B4" s="2">
         <f>January!B4+February!B4+March!B4+April!B4+May!B4+June!B4+July!B4+August!B4+September!B4+October!B4+November!B4+December!B4</f>
-        <v>9167</v>
+        <v>10341</v>
       </c>
       <c r="C4" s="2">
         <f>January!C4+February!C4+March!C4+April!C4+May!C4+June!C4+July!C4+August!C4+September!C4+October!C4+November!C4+December!C4</f>
-        <v>8965</v>
+        <v>10314</v>
       </c>
       <c r="D4" s="2">
         <f>January!D4+February!D4+March!D4+April!D4+May!D4+June!D4+July!D4+August!D4+September!D4+October!D4+November!D4+December!D4</f>
-        <v>202</v>
+        <v>27</v>
       </c>
       <c r="E4" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5496,7 +5517,7 @@
       </c>
       <c r="G4" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.02 : 1</v>
+        <v>1 : 1</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5505,15 +5526,15 @@
       </c>
       <c r="B5" s="4">
         <f>January!B5+February!B5+March!B5+April!B5+May!B5+June!B5+July!B5+August!B5+September!B5+October!B5+November!B5+December!B5</f>
-        <v>266</v>
+        <v>290</v>
       </c>
       <c r="C5" s="4">
         <f>January!C5+February!C5+March!C5+April!C5+May!C5+June!C5+July!C5+August!C5+September!C5+October!C5+November!C5+December!C5</f>
-        <v>1022</v>
+        <v>1119</v>
       </c>
       <c r="D5" s="4">
         <f>January!D5+February!D5+March!D5+April!D5+May!D5+June!D5+July!D5+August!D5+September!D5+October!D5+November!D5+December!D5</f>
-        <v>-756</v>
+        <v>-829</v>
       </c>
       <c r="E5" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5534,15 +5555,15 @@
       </c>
       <c r="B6" s="2">
         <f>January!B6+February!B6+March!B6+April!B6+May!B6+June!B6+July!B6+August!B6+September!B6+October!B6+November!B6+December!B6</f>
-        <v>8307</v>
+        <v>9497</v>
       </c>
       <c r="C6" s="2">
         <f>January!C6+February!C6+March!C6+April!C6+May!C6+June!C6+July!C6+August!C6+September!C6+October!C6+November!C6+December!C6</f>
-        <v>9588</v>
+        <v>10783</v>
       </c>
       <c r="D6" s="2">
         <f>January!D6+February!D6+March!D6+April!D6+May!D6+June!D6+July!D6+August!D6+September!D6+October!D6+November!D6+December!D6</f>
-        <v>-1281</v>
+        <v>-1286</v>
       </c>
       <c r="E6" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5554,7 +5575,7 @@
       </c>
       <c r="G6" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.87 : 1</v>
+        <v>0.88 : 1</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5563,15 +5584,15 @@
       </c>
       <c r="B7" s="4">
         <f>January!B7+February!B7+March!B7+April!B7+May!B7+June!B7+July!B7+August!B7+September!B7+October!B7+November!B7+December!B7</f>
-        <v>1810</v>
+        <v>2034</v>
       </c>
       <c r="C7" s="4">
         <f>January!C7+February!C7+March!C7+April!C7+May!C7+June!C7+July!C7+August!C7+September!C7+October!C7+November!C7+December!C7</f>
-        <v>1343</v>
+        <v>1515</v>
       </c>
       <c r="D7" s="4">
         <f>January!D7+February!D7+March!D7+April!D7+May!D7+June!D7+July!D7+August!D7+September!D7+October!D7+November!D7+December!D7</f>
-        <v>467</v>
+        <v>519</v>
       </c>
       <c r="E7" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5583,7 +5604,7 @@
       </c>
       <c r="G7" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.35 : 1</v>
+        <v>1.34 : 1</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5592,15 +5613,15 @@
       </c>
       <c r="B8" s="2">
         <f>January!B8+February!B8+March!B8+April!B8+May!B8+June!B8+July!B8+August!B8+September!B8+October!B8+November!B8+December!B8</f>
-        <v>1186</v>
+        <v>1363</v>
       </c>
       <c r="C8" s="2">
         <f>January!C8+February!C8+March!C8+April!C8+May!C8+June!C8+July!C8+August!C8+September!C8+October!C8+November!C8+December!C8</f>
-        <v>1401</v>
+        <v>1564</v>
       </c>
       <c r="D8" s="2">
         <f>January!D8+February!D8+March!D8+April!D8+May!D8+June!D8+July!D8+August!D8+September!D8+October!D8+November!D8+December!D8</f>
-        <v>-215</v>
+        <v>-201</v>
       </c>
       <c r="E8" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5612,7 +5633,7 @@
       </c>
       <c r="G8" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.85 : 1</v>
+        <v>0.87 : 1</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5621,15 +5642,15 @@
       </c>
       <c r="B9" s="4">
         <f>January!B9+February!B9+March!B9+April!B9+May!B9+June!B9+July!B9+August!B9+September!B9+October!B9+November!B9+December!B9</f>
-        <v>419</v>
+        <v>507</v>
       </c>
       <c r="C9" s="4">
         <f>January!C9+February!C9+March!C9+April!C9+May!C9+June!C9+July!C9+August!C9+September!C9+October!C9+November!C9+December!C9</f>
-        <v>544</v>
+        <v>604</v>
       </c>
       <c r="D9" s="4">
         <f>January!D9+February!D9+March!D9+April!D9+May!D9+June!D9+July!D9+August!D9+September!D9+October!D9+November!D9+December!D9</f>
-        <v>-125</v>
+        <v>-97</v>
       </c>
       <c r="E9" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5641,7 +5662,7 @@
       </c>
       <c r="G9" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.77 : 1</v>
+        <v>0.84 : 1</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5650,15 +5671,15 @@
       </c>
       <c r="B10" s="2">
         <f>January!B10+February!B10+March!B10+April!B10+May!B10+June!B10+July!B10+August!B10+September!B10+October!B10+November!B10+December!B10</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C10" s="2">
         <f>January!C10+February!C10+March!C10+April!C10+May!C10+June!C10+July!C10+August!C10+September!C10+October!C10+November!C10+December!C10</f>
-        <v>315</v>
+        <v>351</v>
       </c>
       <c r="D10" s="2">
         <f>January!D10+February!D10+March!D10+April!D10+May!D10+June!D10+July!D10+August!D10+September!D10+October!D10+November!D10+December!D10</f>
-        <v>-312</v>
+        <v>-347</v>
       </c>
       <c r="E10" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5708,11 +5729,11 @@
       </c>
       <c r="B12" s="34">
         <f>January!B12+February!B12+March!B12+April!B12+May!B12+June!B12+July!B12+August!B12+September!B12+October!B12+November!B12+December!B12</f>
-        <v>246</v>
+        <v>268</v>
       </c>
       <c r="C12" s="34">
         <f>January!C12+February!C12+March!C12+April!C12+May!C12+June!C12+July!C12+August!C12+September!C12+October!C12+November!C12+December!C12</f>
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="D12" s="34">
         <f>January!D12+February!D12+March!D12+April!D12+May!D12+June!D12+July!D12+August!D12+September!D12+October!D12+November!D12+December!D12</f>
@@ -5728,7 +5749,7 @@
       </c>
       <c r="G12" s="36" t="str">
         <f t="shared" si="2"/>
-        <v>2.07 : 1</v>
+        <v>1.9 : 1</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5737,15 +5758,15 @@
       </c>
       <c r="B13" s="6">
         <f>January!B13+February!B13+March!B13+April!B13+May!B13+June!B13+July!B13+August!B13+September!B13+October!B13+November!B13+December!B13</f>
-        <v>650</v>
+        <v>744</v>
       </c>
       <c r="C13" s="6">
         <f>January!C13+February!C13+March!C13+April!C13+May!C13+June!C13+July!C13+August!C13+September!C13+October!C13+November!C13+December!C13</f>
-        <v>587</v>
+        <v>672</v>
       </c>
       <c r="D13" s="6">
         <f>January!D13+February!D13+March!D13+April!D13+May!D13+June!D13+July!D13+August!D13+September!D13+October!D13+November!D13+December!D13</f>
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="E13" s="30" t="str">
         <f t="shared" si="0"/>
@@ -5766,15 +5787,15 @@
       </c>
       <c r="B14" s="34">
         <f>January!B14+February!B14+March!B14+April!B14+May!B14+June!B14+July!B14+August!B14+September!B14+October!B14+November!B14+December!B14</f>
-        <v>1394</v>
+        <v>1611</v>
       </c>
       <c r="C14" s="34">
         <f>January!C14+February!C14+March!C14+April!C14+May!C14+June!C14+July!C14+August!C14+September!C14+October!C14+November!C14+December!C14</f>
-        <v>1771</v>
+        <v>2070</v>
       </c>
       <c r="D14" s="34">
         <f>January!D14+February!D14+March!D14+April!D14+May!D14+June!D14+July!D14+August!D14+September!D14+October!D14+November!D14+December!D14</f>
-        <v>-377</v>
+        <v>-459</v>
       </c>
       <c r="E14" s="35" t="str">
         <f t="shared" si="0"/>
@@ -5786,7 +5807,7 @@
       </c>
       <c r="G14" s="36" t="str">
         <f t="shared" si="2"/>
-        <v>0.79 : 1</v>
+        <v>0.78 : 1</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5795,15 +5816,15 @@
       </c>
       <c r="B15" s="6">
         <f>January!B15+February!B15+March!B15+April!B15+May!B15+June!B15+July!B15+August!B15+September!B15+October!B15+November!B15+December!B15</f>
-        <v>472</v>
+        <v>531</v>
       </c>
       <c r="C15" s="6">
         <f>January!C15+February!C15+March!C15+April!C15+May!C15+June!C15+July!C15+August!C15+September!C15+October!C15+November!C15+December!C15</f>
-        <v>1204</v>
+        <v>1321</v>
       </c>
       <c r="D15" s="6">
         <f>January!D15+February!D15+March!D15+April!D15+May!D15+June!D15+July!D15+August!D15+September!D15+October!D15+November!D15+December!D15</f>
-        <v>-732</v>
+        <v>-790</v>
       </c>
       <c r="E15" s="30" t="str">
         <f t="shared" si="0"/>
@@ -5815,7 +5836,7 @@
       </c>
       <c r="G15" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0.39 : 1</v>
+        <v>0.4 : 1</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5824,15 +5845,15 @@
       </c>
       <c r="B16" s="2">
         <f>January!B16+February!B16+March!B16+April!B16+May!B16+June!B16+July!B16+August!B16+September!B16+October!B16+November!B16+December!B16</f>
-        <v>553</v>
+        <v>635</v>
       </c>
       <c r="C16" s="2">
         <f>January!C16+February!C16+March!C16+April!C16+May!C16+June!C16+July!C16+August!C16+September!C16+October!C16+November!C16+December!C16</f>
-        <v>1358</v>
+        <v>1545</v>
       </c>
       <c r="D16" s="2">
         <f>January!D16+February!D16+March!D16+April!D16+May!D16+June!D16+July!D16+August!D16+September!D16+October!D16+November!D16+December!D16</f>
-        <v>-805</v>
+        <v>-910</v>
       </c>
       <c r="E16" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5853,15 +5874,15 @@
       </c>
       <c r="B17" s="4">
         <f>January!B17+February!B17+March!B17+April!B17+May!B17+June!B17+July!B17+August!B17+September!B17+October!B17+November!B17+December!B17</f>
-        <v>5031</v>
+        <v>5648</v>
       </c>
       <c r="C17" s="4">
         <f>January!C17+February!C17+March!C17+April!C17+May!C17+June!C17+July!C17+August!C17+September!C17+October!C17+November!C17+December!C17</f>
-        <v>3663</v>
+        <v>4179</v>
       </c>
       <c r="D17" s="4">
         <f>January!D17+February!D17+March!D17+April!D17+May!D17+June!D17+July!D17+August!D17+September!D17+October!D17+November!D17+December!D17</f>
-        <v>1368</v>
+        <v>1469</v>
       </c>
       <c r="E17" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5873,7 +5894,7 @@
       </c>
       <c r="G17" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.37 : 1</v>
+        <v>1.35 : 1</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5882,15 +5903,15 @@
       </c>
       <c r="B18" s="2">
         <f>January!B18+February!B18+March!B18+April!B18+May!B18+June!B18+July!B18+August!B18+September!B18+October!B18+November!B18+December!B18</f>
-        <v>332</v>
+        <v>413</v>
       </c>
       <c r="C18" s="2">
         <f>January!C18+February!C18+March!C18+April!C18+May!C18+June!C18+July!C18+August!C18+September!C18+October!C18+November!C18+December!C18</f>
-        <v>711</v>
+        <v>819</v>
       </c>
       <c r="D18" s="2">
         <f>January!D18+February!D18+March!D18+April!D18+May!D18+June!D18+July!D18+August!D18+September!D18+October!D18+November!D18+December!D18</f>
-        <v>-379</v>
+        <v>-406</v>
       </c>
       <c r="E18" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5902,7 +5923,7 @@
       </c>
       <c r="G18" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.47 : 1</v>
+        <v>0.5 : 1</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5911,15 +5932,15 @@
       </c>
       <c r="B19" s="4">
         <f>January!B19+February!B19+March!B19+April!B19+May!B19+June!B19+July!B19+August!B19+September!B19+October!B19+November!B19+December!B19</f>
-        <v>3488</v>
+        <v>4107</v>
       </c>
       <c r="C19" s="4">
         <f>January!C19+February!C19+March!C19+April!C19+May!C19+June!C19+July!C19+August!C19+September!C19+October!C19+November!C19+December!C19</f>
-        <v>3434</v>
+        <v>3900</v>
       </c>
       <c r="D19" s="4">
         <f>January!D19+February!D19+March!D19+April!D19+May!D19+June!D19+July!D19+August!D19+September!D19+October!D19+November!D19+December!D19</f>
-        <v>54</v>
+        <v>207</v>
       </c>
       <c r="E19" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5931,7 +5952,7 @@
       </c>
       <c r="G19" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.02 : 1</v>
+        <v>1.05 : 1</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5940,15 +5961,15 @@
       </c>
       <c r="B20" s="2">
         <f>January!B20+February!B20+March!B20+April!B20+May!B20+June!B20+July!B20+August!B20+September!B20+October!B20+November!B20+December!B20</f>
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="C20" s="2">
         <f>January!C20+February!C20+March!C20+April!C20+May!C20+June!C20+July!C20+August!C20+September!C20+October!C20+November!C20+December!C20</f>
-        <v>431</v>
+        <v>486</v>
       </c>
       <c r="D20" s="2">
         <f>January!D20+February!D20+March!D20+April!D20+May!D20+June!D20+July!D20+August!D20+September!D20+October!D20+November!D20+December!D20</f>
-        <v>-264</v>
+        <v>-303</v>
       </c>
       <c r="E20" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5960,7 +5981,7 @@
       </c>
       <c r="G20" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.39 : 1</v>
+        <v>0.38 : 1</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5969,15 +5990,15 @@
       </c>
       <c r="B21" s="4">
         <f>January!B21+February!B21+March!B21+April!B21+May!B21+June!B21+July!B21+August!B21+September!B21+October!B21+November!B21+December!B21</f>
-        <v>3956</v>
+        <v>4481</v>
       </c>
       <c r="C21" s="4">
         <f>January!C21+February!C21+March!C21+April!C21+May!C21+June!C21+July!C21+August!C21+September!C21+October!C21+November!C21+December!C21</f>
-        <v>2645</v>
+        <v>3024</v>
       </c>
       <c r="D21" s="4">
         <f>January!D21+February!D21+March!D21+April!D21+May!D21+June!D21+July!D21+August!D21+September!D21+October!D21+November!D21+December!D21</f>
-        <v>1311</v>
+        <v>1457</v>
       </c>
       <c r="E21" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5989,7 +6010,7 @@
       </c>
       <c r="G21" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.5 : 1</v>
+        <v>1.48 : 1</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5998,15 +6019,15 @@
       </c>
       <c r="B22" s="2">
         <f>January!B22+February!B22+March!B22+April!B22+May!B22+June!B22+July!B22+August!B22+September!B22+October!B22+November!B22+December!B22</f>
-        <v>538</v>
+        <v>600</v>
       </c>
       <c r="C22" s="2">
         <f>January!C22+February!C22+March!C22+April!C22+May!C22+June!C22+July!C22+August!C22+September!C22+October!C22+November!C22+December!C22</f>
-        <v>2028</v>
+        <v>2283</v>
       </c>
       <c r="D22" s="2">
         <f>January!D22+February!D22+March!D22+April!D22+May!D22+June!D22+July!D22+August!D22+September!D22+October!D22+November!D22+December!D22</f>
-        <v>-1490</v>
+        <v>-1683</v>
       </c>
       <c r="E22" s="28" t="str">
         <f t="shared" si="0"/>
@@ -6018,7 +6039,7 @@
       </c>
       <c r="G22" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.27 : 1</v>
+        <v>0.26 : 1</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6027,15 +6048,15 @@
       </c>
       <c r="B23" s="4">
         <f>January!B23+February!B23+March!B23+April!B23+May!B23+June!B23+July!B23+August!B23+September!B23+October!B23+November!B23+December!B23</f>
-        <v>4930</v>
+        <v>5700</v>
       </c>
       <c r="C23" s="4">
         <f>January!C23+February!C23+March!C23+April!C23+May!C23+June!C23+July!C23+August!C23+September!C23+October!C23+November!C23+December!C23</f>
-        <v>4285</v>
+        <v>4999</v>
       </c>
       <c r="D23" s="4">
         <f>January!D23+February!D23+March!D23+April!D23+May!D23+June!D23+July!D23+August!D23+September!D23+October!D23+November!D23+December!D23</f>
-        <v>645</v>
+        <v>701</v>
       </c>
       <c r="E23" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6047,7 +6068,7 @@
       </c>
       <c r="G23" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.15 : 1</v>
+        <v>1.14 : 1</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6056,15 +6077,15 @@
       </c>
       <c r="B24" s="2">
         <f>January!B24+February!B24+March!B24+April!B24+May!B24+June!B24+July!B24+August!B24+September!B24+October!B24+November!B24+December!B24</f>
-        <v>12421</v>
+        <v>14127</v>
       </c>
       <c r="C24" s="2">
         <f>January!C24+February!C24+March!C24+April!C24+May!C24+June!C24+July!C24+August!C24+September!C24+October!C24+November!C24+December!C24</f>
-        <v>9045</v>
+        <v>10197</v>
       </c>
       <c r="D24" s="2">
         <f>January!D24+February!D24+March!D24+April!D24+May!D24+June!D24+July!D24+August!D24+September!D24+October!D24+November!D24+December!D24</f>
-        <v>3376</v>
+        <v>3930</v>
       </c>
       <c r="E24" s="28" t="str">
         <f t="shared" si="0"/>
@@ -6076,7 +6097,7 @@
       </c>
       <c r="G24" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.37 : 1</v>
+        <v>1.39 : 1</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6085,15 +6106,15 @@
       </c>
       <c r="B25" s="4">
         <f>January!B25+February!B25+March!B25+April!B25+May!B25+June!B25+July!B25+August!B25+September!B25+October!B25+November!B25+December!B25</f>
-        <v>1212</v>
+        <v>1357</v>
       </c>
       <c r="C25" s="4">
         <f>January!C25+February!C25+March!C25+April!C25+May!C25+June!C25+July!C25+August!C25+September!C25+October!C25+November!C25+December!C25</f>
-        <v>3518</v>
+        <v>3923</v>
       </c>
       <c r="D25" s="4">
         <f>January!D25+February!D25+March!D25+April!D25+May!D25+June!D25+July!D25+August!D25+September!D25+October!D25+November!D25+December!D25</f>
-        <v>-2306</v>
+        <v>-2566</v>
       </c>
       <c r="E25" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6105,7 +6126,7 @@
       </c>
       <c r="G25" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.34 : 1</v>
+        <v>0.35 : 1</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6143,15 +6164,15 @@
       </c>
       <c r="B27" s="4">
         <f>January!B27+February!B27+March!B27+April!B27+May!B27+June!B27+July!B27+August!B27+September!B27+October!B27+November!B27+December!B27</f>
-        <v>1616</v>
+        <v>1882</v>
       </c>
       <c r="C27" s="4">
         <f>January!C27+February!C27+March!C27+April!C27+May!C27+June!C27+July!C27+August!C27+September!C27+October!C27+November!C27+December!C27</f>
-        <v>1317</v>
+        <v>1496</v>
       </c>
       <c r="D27" s="4">
         <f>January!D27+February!D27+March!D27+April!D27+May!D27+June!D27+July!D27+August!D27+September!D27+October!D27+November!D27+December!D27</f>
-        <v>299</v>
+        <v>386</v>
       </c>
       <c r="E27" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6163,7 +6184,7 @@
       </c>
       <c r="G27" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.23 : 1</v>
+        <v>1.26 : 1</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6172,15 +6193,15 @@
       </c>
       <c r="B28" s="2">
         <f>January!B28+February!B28+March!B28+April!B28+May!B28+June!B28+July!B28+August!B28+September!B28+October!B28+November!B28+December!B28</f>
-        <v>958</v>
+        <v>1077</v>
       </c>
       <c r="C28" s="2">
         <f>January!C28+February!C28+March!C28+April!C28+May!C28+June!C28+July!C28+August!C28+September!C28+October!C28+November!C28+December!C28</f>
-        <v>901</v>
+        <v>988</v>
       </c>
       <c r="D28" s="2">
         <f>January!D28+February!D28+March!D28+April!D28+May!D28+June!D28+July!D28+August!D28+September!D28+October!D28+November!D28+December!D28</f>
-        <v>57</v>
+        <v>89</v>
       </c>
       <c r="E28" s="28" t="str">
         <f t="shared" si="0"/>
@@ -6192,7 +6213,7 @@
       </c>
       <c r="G28" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.06 : 1</v>
+        <v>1.09 : 1</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6201,15 +6222,15 @@
       </c>
       <c r="B29" s="4">
         <f>January!B29+February!B29+March!B29+April!B29+May!B29+June!B29+July!B29+August!B29+September!B29+October!B29+November!B29+December!B29</f>
-        <v>5234</v>
+        <v>5804</v>
       </c>
       <c r="C29" s="4">
         <f>January!C29+February!C29+March!C29+April!C29+May!C29+June!C29+July!C29+August!C29+September!C29+October!C29+November!C29+December!C29</f>
-        <v>3678</v>
+        <v>4174</v>
       </c>
       <c r="D29" s="4">
         <f>January!D29+February!D29+March!D29+April!D29+May!D29+June!D29+July!D29+August!D29+September!D29+October!D29+November!D29+December!D29</f>
-        <v>1556</v>
+        <v>1630</v>
       </c>
       <c r="E29" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6221,7 +6242,7 @@
       </c>
       <c r="G29" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.42 : 1</v>
+        <v>1.39 : 1</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6230,15 +6251,15 @@
       </c>
       <c r="B30" s="2">
         <f>January!B30+February!B30+March!B30+April!B30+May!B30+June!B30+July!B30+August!B30+September!B30+October!B30+November!B30+December!B30</f>
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="C30" s="2">
         <f>January!C30+February!C30+March!C30+April!C30+May!C30+June!C30+July!C30+August!C30+September!C30+October!C30+November!C30+December!C30</f>
-        <v>198</v>
+        <v>226</v>
       </c>
       <c r="D30" s="2">
         <f>January!D30+February!D30+March!D30+April!D30+May!D30+June!D30+July!D30+August!D30+September!D30+October!D30+November!D30+December!D30</f>
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E30" s="28" t="str">
         <f t="shared" si="0"/>
@@ -6250,7 +6271,7 @@
       </c>
       <c r="G30" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.44 : 1</v>
+        <v>1.36 : 1</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6259,15 +6280,15 @@
       </c>
       <c r="B31" s="4">
         <f>January!B31+February!B31+March!B31+April!B31+May!B31+June!B31+July!B31+August!B31+September!B31+October!B31+November!B31+December!B31</f>
-        <v>540</v>
+        <v>634</v>
       </c>
       <c r="C31" s="4">
         <f>January!C31+February!C31+March!C31+April!C31+May!C31+June!C31+July!C31+August!C31+September!C31+October!C31+November!C31+December!C31</f>
-        <v>1993</v>
+        <v>2317</v>
       </c>
       <c r="D31" s="4">
         <f>January!D31+February!D31+March!D31+April!D31+May!D31+June!D31+July!D31+August!D31+September!D31+October!D31+November!D31+December!D31</f>
-        <v>-1453</v>
+        <v>-1683</v>
       </c>
       <c r="E31" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6288,15 +6309,15 @@
       </c>
       <c r="B32" s="2">
         <f>January!B32+February!B32+March!B32+April!B32+May!B32+June!B32+July!B32+August!B32+September!B32+October!B32+November!B32+December!B32</f>
-        <v>3288</v>
+        <v>3696</v>
       </c>
       <c r="C32" s="2">
         <f>January!C32+February!C32+March!C32+April!C32+May!C32+June!C32+July!C32+August!C32+September!C32+October!C32+November!C32+December!C32</f>
-        <v>4438</v>
+        <v>5034</v>
       </c>
       <c r="D32" s="2">
         <f>January!D32+February!D32+March!D32+April!D32+May!D32+June!D32+July!D32+August!D32+September!D32+October!D32+November!D32+December!D32</f>
-        <v>-1150</v>
+        <v>-1338</v>
       </c>
       <c r="E32" s="28" t="str">
         <f t="shared" si="0"/>
@@ -6308,7 +6329,7 @@
       </c>
       <c r="G32" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.74 : 1</v>
+        <v>0.73 : 1</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6317,27 +6338,27 @@
       </c>
       <c r="B33" s="4">
         <f>January!B33+February!B33+March!B33+April!B33+May!B33+June!B33+July!B33+August!B33+September!B33+October!B33+November!B33+December!B33</f>
-        <v>3462</v>
+        <v>3904</v>
       </c>
       <c r="C33" s="4">
         <f>January!C33+February!C33+March!C33+April!C33+May!C33+June!C33+July!C33+August!C33+September!C33+October!C33+November!C33+December!C33</f>
-        <v>3486</v>
+        <v>3855</v>
       </c>
       <c r="D33" s="4">
         <f>January!D33+February!D33+March!D33+April!D33+May!D33+June!D33+July!D33+August!D33+September!D33+October!D33+November!D33+December!D33</f>
-        <v>-24</v>
+        <v>49</v>
       </c>
       <c r="E33" s="29" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>We borrowed more than we lent this year</v>
       </c>
       <c r="F33" s="29" t="str">
         <f t="shared" si="1"/>
-        <v>We lent more than we borrowed this year</v>
+        <v/>
       </c>
       <c r="G33" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.99 : 1</v>
+        <v>1.01 : 1</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6346,15 +6367,15 @@
       </c>
       <c r="B34" s="2">
         <f>January!B34+February!B34+March!B34+April!B34+May!B34+June!B34+July!B34+August!B34+September!B34+October!B34+November!B34+December!B34</f>
-        <v>1572</v>
+        <v>1744</v>
       </c>
       <c r="C34" s="2">
         <f>January!C34+February!C34+March!C34+April!C34+May!C34+June!C34+July!C34+August!C34+September!C34+October!C34+November!C34+December!C34</f>
-        <v>1206</v>
+        <v>1327</v>
       </c>
       <c r="D34" s="2">
         <f>January!D34+February!D34+March!D34+April!D34+May!D34+June!D34+July!D34+August!D34+September!D34+October!D34+November!D34+December!D34</f>
-        <v>366</v>
+        <v>417</v>
       </c>
       <c r="E34" s="28" t="str">
         <f t="shared" ref="E34:E54" si="3">IF(D34 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -6366,7 +6387,7 @@
       </c>
       <c r="G34" s="3" t="str">
         <f t="shared" ref="G34:G54" si="5">IF(ISERROR(ROUND(B34/C34,2)&amp;" : 1"), "", ROUND(B34/C34,2)&amp;" : 1")</f>
-        <v>1.3 : 1</v>
+        <v>1.31 : 1</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6375,15 +6396,15 @@
       </c>
       <c r="B35" s="4">
         <f>January!B35+February!B35+March!B35+April!B35+May!B35+June!B35+July!B35+August!B35+September!B35+October!B35+November!B35+December!B35</f>
-        <v>7545</v>
+        <v>9076</v>
       </c>
       <c r="C35" s="4">
         <f>January!C35+February!C35+March!C35+April!C35+May!C35+June!C35+July!C35+August!C35+September!C35+October!C35+November!C35+December!C35</f>
-        <v>10333</v>
+        <v>11692</v>
       </c>
       <c r="D35" s="4">
         <f>January!D35+February!D35+March!D35+April!D35+May!D35+June!D35+July!D35+August!D35+September!D35+October!D35+November!D35+December!D35</f>
-        <v>-2788</v>
+        <v>-2616</v>
       </c>
       <c r="E35" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6395,7 +6416,7 @@
       </c>
       <c r="G35" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.73 : 1</v>
+        <v>0.78 : 1</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6404,15 +6425,15 @@
       </c>
       <c r="B36" s="2">
         <f>January!B36+February!B36+March!B36+April!B36+May!B36+June!B36+July!B36+August!B36+September!B36+October!B36+November!B36+December!B36</f>
-        <v>1268</v>
+        <v>1437</v>
       </c>
       <c r="C36" s="2">
         <f>January!C36+February!C36+March!C36+April!C36+May!C36+June!C36+July!C36+August!C36+September!C36+October!C36+November!C36+December!C36</f>
-        <v>4137</v>
+        <v>4747</v>
       </c>
       <c r="D36" s="2">
         <f>January!D36+February!D36+March!D36+April!D36+May!D36+June!D36+July!D36+August!D36+September!D36+October!D36+November!D36+December!D36</f>
-        <v>-2869</v>
+        <v>-3310</v>
       </c>
       <c r="E36" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6424,7 +6445,7 @@
       </c>
       <c r="G36" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.31 : 1</v>
+        <v>0.3 : 1</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6433,15 +6454,15 @@
       </c>
       <c r="B37" s="4">
         <f>January!B37+February!B37+March!B37+April!B37+May!B37+June!B37+July!B37+August!B37+September!B37+October!B37+November!B37+December!B37</f>
-        <v>4158</v>
+        <v>4638</v>
       </c>
       <c r="C37" s="4">
         <f>January!C37+February!C37+March!C37+April!C37+May!C37+June!C37+July!C37+August!C37+September!C37+October!C37+November!C37+December!C37</f>
-        <v>2369</v>
+        <v>2751</v>
       </c>
       <c r="D37" s="4">
         <f>January!D37+February!D37+March!D37+April!D37+May!D37+June!D37+July!D37+August!D37+September!D37+October!D37+November!D37+December!D37</f>
-        <v>1789</v>
+        <v>1887</v>
       </c>
       <c r="E37" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6453,7 +6474,7 @@
       </c>
       <c r="G37" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>1.76 : 1</v>
+        <v>1.69 : 1</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6462,15 +6483,15 @@
       </c>
       <c r="B38" s="2">
         <f>January!B38+February!B38+March!B38+April!B38+May!B38+June!B38+July!B38+August!B38+September!B38+October!B38+November!B38+December!B38</f>
-        <v>196</v>
+        <v>225</v>
       </c>
       <c r="C38" s="2">
         <f>January!C38+February!C38+March!C38+April!C38+May!C38+June!C38+July!C38+August!C38+September!C38+October!C38+November!C38+December!C38</f>
-        <v>1355</v>
+        <v>1584</v>
       </c>
       <c r="D38" s="2">
         <f>January!D38+February!D38+March!D38+April!D38+May!D38+June!D38+July!D38+August!D38+September!D38+October!D38+November!D38+December!D38</f>
-        <v>-1159</v>
+        <v>-1359</v>
       </c>
       <c r="E38" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6491,15 +6512,15 @@
       </c>
       <c r="B39" s="4">
         <f>January!B39+February!B39+March!B39+April!B39+May!B39+June!B39+July!B39+August!B39+September!B39+October!B39+November!B39+December!B39</f>
-        <v>215</v>
+        <v>306</v>
       </c>
       <c r="C39" s="4">
         <f>January!C39+February!C39+March!C39+April!C39+May!C39+June!C39+July!C39+August!C39+September!C39+October!C39+November!C39+December!C39</f>
-        <v>514</v>
+        <v>632</v>
       </c>
       <c r="D39" s="4">
         <f>January!D39+February!D39+March!D39+April!D39+May!D39+June!D39+July!D39+August!D39+September!D39+October!D39+November!D39+December!D39</f>
-        <v>-299</v>
+        <v>-326</v>
       </c>
       <c r="E39" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6511,7 +6532,7 @@
       </c>
       <c r="G39" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.42 : 1</v>
+        <v>0.48 : 1</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6520,15 +6541,15 @@
       </c>
       <c r="B40" s="38">
         <f>January!B40+February!B40+March!B40+April!B40+May!B40+June!B40+July!B40+August!B40+September!B40+October!B40+November!B40+December!B40</f>
-        <v>224</v>
+        <v>265</v>
       </c>
       <c r="C40" s="38">
         <f>January!C40+February!C40+March!C40+April!C40+May!C40+June!C40+July!C40+August!C40+September!C40+October!C40+November!C40+December!C40</f>
-        <v>424</v>
+        <v>498</v>
       </c>
       <c r="D40" s="38">
         <f>January!D40+February!D40+March!D40+April!D40+May!D40+June!D40+July!D40+August!D40+September!D40+October!D40+November!D40+December!D40</f>
-        <v>-200</v>
+        <v>-233</v>
       </c>
       <c r="E40" s="39" t="str">
         <f t="shared" si="3"/>
@@ -6549,15 +6570,15 @@
       </c>
       <c r="B41" s="8">
         <f>January!B41+February!B41+March!B41+April!B41+May!B41+June!B41+July!B41+August!B41+September!B41+October!B41+November!B41+December!B41</f>
-        <v>237</v>
+        <v>251</v>
       </c>
       <c r="C41" s="8">
         <f>January!C41+February!C41+March!C41+April!C41+May!C41+June!C41+July!C41+August!C41+September!C41+October!C41+November!C41+December!C41</f>
-        <v>253</v>
+        <v>281</v>
       </c>
       <c r="D41" s="8">
         <f>January!D41+February!D41+March!D41+April!D41+May!D41+June!D41+July!D41+August!D41+September!D41+October!D41+November!D41+December!D41</f>
-        <v>-16</v>
+        <v>-30</v>
       </c>
       <c r="E41" s="31" t="str">
         <f t="shared" si="3"/>
@@ -6569,7 +6590,7 @@
       </c>
       <c r="G41" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0.94 : 1</v>
+        <v>0.89 : 1</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6578,15 +6599,15 @@
       </c>
       <c r="B42" s="38">
         <f>January!B42+February!B42+March!B42+April!B42+May!B42+June!B42+July!B42+August!B42+September!B42+October!B42+November!B42+December!B42</f>
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C42" s="38">
         <f>January!C42+February!C42+March!C42+April!C42+May!C42+June!C42+July!C42+August!C42+September!C42+October!C42+November!C42+December!C42</f>
-        <v>216</v>
+        <v>239</v>
       </c>
       <c r="D42" s="38">
         <f>January!D42+February!D42+March!D42+April!D42+May!D42+June!D42+July!D42+August!D42+September!D42+October!D42+November!D42+December!D42</f>
-        <v>-178</v>
+        <v>-190</v>
       </c>
       <c r="E42" s="39" t="str">
         <f t="shared" si="3"/>
@@ -6598,7 +6619,7 @@
       </c>
       <c r="G42" s="40" t="str">
         <f t="shared" si="5"/>
-        <v>0.18 : 1</v>
+        <v>0.21 : 1</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6607,15 +6628,15 @@
       </c>
       <c r="B43" s="8">
         <f>January!B43+February!B43+March!B43+April!B43+May!B43+June!B43+July!B43+August!B43+September!B43+October!B43+November!B43+December!B43</f>
-        <v>451</v>
+        <v>542</v>
       </c>
       <c r="C43" s="8">
         <f>January!C43+February!C43+March!C43+April!C43+May!C43+June!C43+July!C43+August!C43+September!C43+October!C43+November!C43+December!C43</f>
-        <v>600</v>
+        <v>712</v>
       </c>
       <c r="D43" s="8">
         <f>January!D43+February!D43+March!D43+April!D43+May!D43+June!D43+July!D43+August!D43+September!D43+October!D43+November!D43+December!D43</f>
-        <v>-149</v>
+        <v>-170</v>
       </c>
       <c r="E43" s="31" t="str">
         <f t="shared" si="3"/>
@@ -6627,7 +6648,7 @@
       </c>
       <c r="G43" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0.75 : 1</v>
+        <v>0.76 : 1</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6636,15 +6657,15 @@
       </c>
       <c r="B44" s="2">
         <f>January!B44+February!B44+March!B44+April!B44+May!B44+June!B44+July!B44+August!B44+September!B44+October!B44+November!B44+December!B44</f>
-        <v>451</v>
+        <v>551</v>
       </c>
       <c r="C44" s="2">
         <f>January!C44+February!C44+March!C44+April!C44+May!C44+June!C44+July!C44+August!C44+September!C44+October!C44+November!C44+December!C44</f>
-        <v>1607</v>
+        <v>1796</v>
       </c>
       <c r="D44" s="2">
         <f>January!D44+February!D44+March!D44+April!D44+May!D44+June!D44+July!D44+August!D44+September!D44+October!D44+November!D44+December!D44</f>
-        <v>-1156</v>
+        <v>-1245</v>
       </c>
       <c r="E44" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6656,7 +6677,7 @@
       </c>
       <c r="G44" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.28 : 1</v>
+        <v>0.31 : 1</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6665,15 +6686,15 @@
       </c>
       <c r="B45" s="4">
         <f>January!B45+February!B45+March!B45+April!B45+May!B45+June!B45+July!B45+August!B45+September!B45+October!B45+November!B45+December!B45</f>
-        <v>4363</v>
+        <v>4946</v>
       </c>
       <c r="C45" s="4">
         <f>January!C45+February!C45+March!C45+April!C45+May!C45+June!C45+July!C45+August!C45+September!C45+October!C45+November!C45+December!C45</f>
-        <v>4446</v>
+        <v>4975</v>
       </c>
       <c r="D45" s="4">
         <f>January!D45+February!D45+March!D45+April!D45+May!D45+June!D45+July!D45+August!D45+September!D45+October!D45+November!D45+December!D45</f>
-        <v>-83</v>
+        <v>-29</v>
       </c>
       <c r="E45" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6685,7 +6706,7 @@
       </c>
       <c r="G45" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.98 : 1</v>
+        <v>0.99 : 1</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6694,15 +6715,15 @@
       </c>
       <c r="B46" s="2">
         <f>January!B46+February!B46+March!B46+April!B46+May!B46+June!B46+July!B46+August!B46+September!B46+October!B46+November!B46+December!B46</f>
-        <v>8295</v>
+        <v>9260</v>
       </c>
       <c r="C46" s="2">
         <f>January!C46+February!C46+March!C46+April!C46+May!C46+June!C46+July!C46+August!C46+September!C46+October!C46+November!C46+December!C46</f>
-        <v>5274</v>
+        <v>5983</v>
       </c>
       <c r="D46" s="2">
         <f>January!D46+February!D46+March!D46+April!D46+May!D46+June!D46+July!D46+August!D46+September!D46+October!D46+November!D46+December!D46</f>
-        <v>3021</v>
+        <v>3277</v>
       </c>
       <c r="E46" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6714,7 +6735,7 @@
       </c>
       <c r="G46" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>1.57 : 1</v>
+        <v>1.55 : 1</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6723,15 +6744,15 @@
       </c>
       <c r="B47" s="4">
         <f>January!B47+February!B47+March!B47+April!B47+May!B47+June!B47+July!B47+August!B47+September!B47+October!B47+November!B47+December!B47</f>
-        <v>1648</v>
+        <v>1883</v>
       </c>
       <c r="C47" s="4">
         <f>January!C47+February!C47+March!C47+April!C47+May!C47+June!C47+July!C47+August!C47+September!C47+October!C47+November!C47+December!C47</f>
-        <v>4909</v>
+        <v>5505</v>
       </c>
       <c r="D47" s="4">
         <f>January!D47+February!D47+March!D47+April!D47+May!D47+June!D47+July!D47+August!D47+September!D47+October!D47+November!D47+December!D47</f>
-        <v>-3261</v>
+        <v>-3622</v>
       </c>
       <c r="E47" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6752,15 +6773,15 @@
       </c>
       <c r="B48" s="2">
         <f>January!B48+February!B48+March!B48+April!B48+May!B48+June!B48+July!B48+August!B48+September!B48+October!B48+November!B48+December!B48</f>
-        <v>5094</v>
+        <v>5544</v>
       </c>
       <c r="C48" s="2">
         <f>January!C48+February!C48+March!C48+April!C48+May!C48+June!C48+July!C48+August!C48+September!C48+October!C48+November!C48+December!C48</f>
-        <v>1806</v>
+        <v>2004</v>
       </c>
       <c r="D48" s="2">
         <f>January!D48+February!D48+March!D48+April!D48+May!D48+June!D48+July!D48+August!D48+September!D48+October!D48+November!D48+December!D48</f>
-        <v>3288</v>
+        <v>3540</v>
       </c>
       <c r="E48" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6772,7 +6793,7 @@
       </c>
       <c r="G48" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>2.82 : 1</v>
+        <v>2.77 : 1</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6781,15 +6802,15 @@
       </c>
       <c r="B49" s="4">
         <f>January!B49+February!B49+March!B49+April!B49+May!B49+June!B49+July!B49+August!B49+September!B49+October!B49+November!B49+December!B49</f>
-        <v>7050</v>
+        <v>7919</v>
       </c>
       <c r="C49" s="4">
         <f>January!C49+February!C49+March!C49+April!C49+May!C49+June!C49+July!C49+August!C49+September!C49+October!C49+November!C49+December!C49</f>
-        <v>4663</v>
+        <v>5376</v>
       </c>
       <c r="D49" s="4">
         <f>January!D49+February!D49+March!D49+April!D49+May!D49+June!D49+July!D49+August!D49+September!D49+October!D49+November!D49+December!D49</f>
-        <v>2387</v>
+        <v>2543</v>
       </c>
       <c r="E49" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6801,7 +6822,7 @@
       </c>
       <c r="G49" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>1.51 : 1</v>
+        <v>1.47 : 1</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6810,15 +6831,15 @@
       </c>
       <c r="B50" s="2">
         <f>January!B50+February!B50+March!B50+April!B50+May!B50+June!B50+July!B50+August!B50+September!B50+October!B50+November!B50+December!B50</f>
-        <v>1393</v>
+        <v>1488</v>
       </c>
       <c r="C50" s="2">
         <f>January!C50+February!C50+March!C50+April!C50+May!C50+June!C50+July!C50+August!C50+September!C50+October!C50+November!C50+December!C50</f>
-        <v>1290</v>
+        <v>1457</v>
       </c>
       <c r="D50" s="2">
         <f>January!D50+February!D50+March!D50+April!D50+May!D50+June!D50+July!D50+August!D50+September!D50+October!D50+November!D50+December!D50</f>
-        <v>103</v>
+        <v>31</v>
       </c>
       <c r="E50" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6830,7 +6851,7 @@
       </c>
       <c r="G50" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>1.08 : 1</v>
+        <v>1.02 : 1</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6839,15 +6860,15 @@
       </c>
       <c r="B51" s="4">
         <f>January!B51+February!B51+March!B51+April!B51+May!B51+June!B51+July!B51+August!B51+September!B51+October!B51+November!B51+December!B51</f>
-        <v>2828</v>
+        <v>3145</v>
       </c>
       <c r="C51" s="4">
         <f>January!C51+February!C51+March!C51+April!C51+May!C51+June!C51+July!C51+August!C51+September!C51+October!C51+November!C51+December!C51</f>
-        <v>3000</v>
+        <v>3470</v>
       </c>
       <c r="D51" s="4">
         <f>January!D51+February!D51+March!D51+April!D51+May!D51+June!D51+July!D51+August!D51+September!D51+October!D51+November!D51+December!D51</f>
-        <v>-172</v>
+        <v>-325</v>
       </c>
       <c r="E51" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6859,7 +6880,7 @@
       </c>
       <c r="G51" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.94 : 1</v>
+        <v>0.91 : 1</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6868,15 +6889,15 @@
       </c>
       <c r="B52" s="2">
         <f>January!B52+February!B52+March!B52+April!B52+May!B52+June!B52+July!B52+August!B52+September!B52+October!B52+November!B52+December!B52</f>
-        <v>1146</v>
+        <v>1406</v>
       </c>
       <c r="C52" s="2">
         <f>January!C52+February!C52+March!C52+April!C52+May!C52+June!C52+July!C52+August!C52+September!C52+October!C52+November!C52+December!C52</f>
-        <v>1716</v>
+        <v>1933</v>
       </c>
       <c r="D52" s="2">
         <f>January!D52+February!D52+March!D52+April!D52+May!D52+June!D52+July!D52+August!D52+September!D52+October!D52+November!D52+December!D52</f>
-        <v>-570</v>
+        <v>-527</v>
       </c>
       <c r="E52" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6888,7 +6909,7 @@
       </c>
       <c r="G52" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.67 : 1</v>
+        <v>0.73 : 1</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6897,15 +6918,15 @@
       </c>
       <c r="B53" s="4">
         <f>January!B53+February!B53+March!B53+April!B53+May!B53+June!B53+July!B53+August!B53+September!B53+October!B53+November!B53+December!B53</f>
-        <v>262</v>
+        <v>281</v>
       </c>
       <c r="C53" s="4">
         <f>January!C53+February!C53+March!C53+April!C53+May!C53+June!C53+July!C53+August!C53+September!C53+October!C53+November!C53+December!C53</f>
-        <v>1986</v>
+        <v>2261</v>
       </c>
       <c r="D53" s="4">
         <f>January!D53+February!D53+March!D53+April!D53+May!D53+June!D53+July!D53+August!D53+September!D53+October!D53+November!D53+December!D53</f>
-        <v>-1724</v>
+        <v>-1980</v>
       </c>
       <c r="E53" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6917,7 +6938,7 @@
       </c>
       <c r="G53" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.13 : 1</v>
+        <v>0.12 : 1</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6926,15 +6947,15 @@
       </c>
       <c r="B54" s="10">
         <f>January!B54+February!B54+March!B54+April!B54+May!B54+June!B54+July!B54+August!B54+September!B54+October!B54+November!B54+December!B54</f>
-        <v>3104</v>
+        <v>3447</v>
       </c>
       <c r="C54" s="10">
         <f>January!C54+February!C54+March!C54+April!C54+May!C54+June!C54+July!C54+August!C54+September!C54+October!C54+November!C54+December!C54</f>
-        <v>1646</v>
+        <v>1846</v>
       </c>
       <c r="D54" s="10">
         <f>January!D54+February!D54+March!D54+April!D54+May!D54+June!D54+July!D54+August!D54+September!D54+October!D54+November!D54+December!D54</f>
-        <v>1458</v>
+        <v>1601</v>
       </c>
       <c r="E54" s="32" t="str">
         <f t="shared" si="3"/>
@@ -6946,7 +6967,7 @@
       </c>
       <c r="G54" s="11" t="str">
         <f t="shared" si="5"/>
-        <v>1.89 : 1</v>
+        <v>1.87 : 1</v>
       </c>
     </row>
   </sheetData>
@@ -14124,7 +14145,7 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A42" activeCellId="1" sqref="A40:G40 A42:G42"/>
       <selection pane="topRight" activeCell="A42" activeCellId="1" sqref="A40:G40 A42:G42"/>
@@ -15321,7 +15342,7 @@
       <selection activeCell="A42" activeCellId="1" sqref="A40:G40 A42:G42"/>
       <selection pane="topRight" activeCell="A42" activeCellId="1" sqref="A40:G40 A42:G42"/>
       <selection pane="bottomLeft" activeCell="A42" activeCellId="1" sqref="A40:G40 A42:G42"/>
-      <selection pane="bottomRight" activeCell="A42" activeCellId="1" sqref="A40:G40 A42:G42"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15361,108 +15382,204 @@
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="28"/>
+      <c r="B2" s="18">
+        <v>1577</v>
+      </c>
+      <c r="C2" s="18">
+        <v>1345</v>
+      </c>
+      <c r="D2" s="18">
+        <v>232</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F2" s="28"/>
-      <c r="G2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="29"/>
+      <c r="B3" s="21">
+        <v>670</v>
+      </c>
+      <c r="C3" s="21">
+        <v>351</v>
+      </c>
+      <c r="D3" s="21">
+        <v>319</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F3" s="29"/>
-      <c r="G3" s="5"/>
+      <c r="G3" s="5" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
+      <c r="B4" s="18">
+        <v>1174</v>
+      </c>
+      <c r="C4" s="18">
+        <v>1349</v>
+      </c>
+      <c r="D4" s="18">
+        <v>-175</v>
+      </c>
       <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="3"/>
+      <c r="F4" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
+      <c r="B5" s="21">
+        <v>24</v>
+      </c>
+      <c r="C5" s="21">
+        <v>97</v>
+      </c>
+      <c r="D5" s="21">
+        <v>-73</v>
+      </c>
       <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="5"/>
+      <c r="F5" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
+      <c r="B6" s="18">
+        <v>1190</v>
+      </c>
+      <c r="C6" s="18">
+        <v>1195</v>
+      </c>
+      <c r="D6" s="18">
+        <v>-5</v>
+      </c>
       <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="3"/>
+      <c r="F6" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="29"/>
+      <c r="B7" s="21">
+        <v>224</v>
+      </c>
+      <c r="C7" s="21">
+        <v>172</v>
+      </c>
+      <c r="D7" s="21">
+        <v>52</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F7" s="29"/>
-      <c r="G7" s="5"/>
+      <c r="G7" s="5" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="28"/>
+      <c r="B8" s="18">
+        <v>177</v>
+      </c>
+      <c r="C8" s="18">
+        <v>163</v>
+      </c>
+      <c r="D8" s="18">
+        <v>14</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F8" s="28"/>
-      <c r="G8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="29"/>
+      <c r="B9" s="21">
+        <v>88</v>
+      </c>
+      <c r="C9" s="21">
+        <v>60</v>
+      </c>
+      <c r="D9" s="21">
+        <v>28</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F9" s="29"/>
-      <c r="G9" s="5"/>
+      <c r="G9" s="5" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
+      <c r="B10" s="18">
+        <v>1</v>
+      </c>
+      <c r="C10" s="18">
+        <v>36</v>
+      </c>
+      <c r="D10" s="18">
+        <v>-35</v>
+      </c>
       <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="3"/>
+      <c r="F10" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
+      <c r="B11" s="21">
+        <v>0</v>
+      </c>
+      <c r="C11" s="21">
+        <v>0</v>
+      </c>
+      <c r="D11" s="21">
+        <v>0</v>
+      </c>
       <c r="E11" s="29"/>
       <c r="F11" s="29"/>
       <c r="G11" s="5"/>
@@ -15471,163 +15588,307 @@
       <c r="A12" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
+      <c r="B12" s="41">
+        <v>22</v>
+      </c>
+      <c r="C12" s="41">
+        <v>22</v>
+      </c>
+      <c r="D12" s="41">
+        <v>0</v>
+      </c>
       <c r="E12" s="35"/>
       <c r="F12" s="35"/>
-      <c r="G12" s="36"/>
+      <c r="G12" s="36" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="30"/>
+      <c r="B13" s="23">
+        <v>94</v>
+      </c>
+      <c r="C13" s="23">
+        <v>85</v>
+      </c>
+      <c r="D13" s="23">
+        <v>9</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>60</v>
+      </c>
       <c r="F13" s="30"/>
-      <c r="G13" s="7"/>
+      <c r="G13" s="7" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
+      <c r="B14" s="41">
+        <v>217</v>
+      </c>
+      <c r="C14" s="41">
+        <v>299</v>
+      </c>
+      <c r="D14" s="41">
+        <v>-82</v>
+      </c>
       <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="36"/>
+      <c r="F14" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="36" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
+      <c r="B15" s="23">
+        <v>59</v>
+      </c>
+      <c r="C15" s="23">
+        <v>117</v>
+      </c>
+      <c r="D15" s="23">
+        <v>-58</v>
+      </c>
       <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="7"/>
+      <c r="F15" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="B16" s="18">
+        <v>82</v>
+      </c>
+      <c r="C16" s="18">
+        <v>187</v>
+      </c>
+      <c r="D16" s="18">
+        <v>-105</v>
+      </c>
       <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="3"/>
+      <c r="F16" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="29"/>
+      <c r="B17" s="21">
+        <v>617</v>
+      </c>
+      <c r="C17" s="21">
+        <v>516</v>
+      </c>
+      <c r="D17" s="21">
+        <v>101</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F17" s="29"/>
-      <c r="G17" s="5"/>
+      <c r="G17" s="5" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
+      <c r="B18" s="18">
+        <v>81</v>
+      </c>
+      <c r="C18" s="18">
+        <v>108</v>
+      </c>
+      <c r="D18" s="18">
+        <v>-27</v>
+      </c>
       <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="3"/>
+      <c r="F18" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="29"/>
+      <c r="B19" s="21">
+        <v>619</v>
+      </c>
+      <c r="C19" s="21">
+        <v>466</v>
+      </c>
+      <c r="D19" s="21">
+        <v>153</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F19" s="29"/>
-      <c r="G19" s="5"/>
+      <c r="G19" s="5" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+      <c r="B20" s="18">
+        <v>16</v>
+      </c>
+      <c r="C20" s="18">
+        <v>55</v>
+      </c>
+      <c r="D20" s="18">
+        <v>-39</v>
+      </c>
       <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="3"/>
+      <c r="F20" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="29"/>
+      <c r="B21" s="21">
+        <v>525</v>
+      </c>
+      <c r="C21" s="21">
+        <v>379</v>
+      </c>
+      <c r="D21" s="21">
+        <v>146</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F21" s="29"/>
-      <c r="G21" s="5"/>
+      <c r="G21" s="5" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="B22" s="18">
+        <v>62</v>
+      </c>
+      <c r="C22" s="18">
+        <v>255</v>
+      </c>
+      <c r="D22" s="18">
+        <v>-193</v>
+      </c>
       <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="3"/>
+      <c r="F22" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="29"/>
+      <c r="B23" s="21">
+        <v>770</v>
+      </c>
+      <c r="C23" s="21">
+        <v>714</v>
+      </c>
+      <c r="D23" s="21">
+        <v>56</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F23" s="29"/>
-      <c r="G23" s="5"/>
+      <c r="G23" s="5" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="28"/>
+      <c r="B24" s="18">
+        <v>1706</v>
+      </c>
+      <c r="C24" s="18">
+        <v>1152</v>
+      </c>
+      <c r="D24" s="18">
+        <v>554</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F24" s="28"/>
-      <c r="G24" s="3"/>
+      <c r="G24" s="3" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
+      <c r="B25" s="21">
+        <v>145</v>
+      </c>
+      <c r="C25" s="21">
+        <v>405</v>
+      </c>
+      <c r="D25" s="21">
+        <v>-260</v>
+      </c>
       <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="5"/>
+      <c r="F25" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
+      <c r="B26" s="18">
+        <v>0</v>
+      </c>
+      <c r="C26" s="18">
+        <v>0</v>
+      </c>
+      <c r="D26" s="18">
+        <v>0</v>
+      </c>
       <c r="E26" s="28"/>
       <c r="F26" s="28"/>
       <c r="G26" s="3"/>
@@ -15636,309 +15897,589 @@
       <c r="A27" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="29"/>
+      <c r="B27" s="21">
+        <v>266</v>
+      </c>
+      <c r="C27" s="21">
+        <v>179</v>
+      </c>
+      <c r="D27" s="21">
+        <v>87</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F27" s="29"/>
-      <c r="G27" s="5"/>
+      <c r="G27" s="5" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="28"/>
+      <c r="B28" s="18">
+        <v>119</v>
+      </c>
+      <c r="C28" s="18">
+        <v>87</v>
+      </c>
+      <c r="D28" s="18">
+        <v>32</v>
+      </c>
+      <c r="E28" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F28" s="28"/>
-      <c r="G28" s="3"/>
+      <c r="G28" s="3" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="29"/>
+      <c r="B29" s="21">
+        <v>570</v>
+      </c>
+      <c r="C29" s="21">
+        <v>496</v>
+      </c>
+      <c r="D29" s="21">
+        <v>74</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F29" s="29"/>
-      <c r="G29" s="5"/>
+      <c r="G29" s="5" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
+      <c r="B30" s="18">
+        <v>22</v>
+      </c>
+      <c r="C30" s="18">
+        <v>28</v>
+      </c>
+      <c r="D30" s="18">
+        <v>-6</v>
+      </c>
       <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="3"/>
+      <c r="F30" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
+      <c r="B31" s="21">
+        <v>94</v>
+      </c>
+      <c r="C31" s="21">
+        <v>324</v>
+      </c>
+      <c r="D31" s="21">
+        <v>-230</v>
+      </c>
       <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="5"/>
+      <c r="F31" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="B32" s="18">
+        <v>408</v>
+      </c>
+      <c r="C32" s="18">
+        <v>596</v>
+      </c>
+      <c r="D32" s="18">
+        <v>-188</v>
+      </c>
       <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="3"/>
+      <c r="F32" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="29"/>
+      <c r="B33" s="21">
+        <v>442</v>
+      </c>
+      <c r="C33" s="21">
+        <v>369</v>
+      </c>
+      <c r="D33" s="21">
+        <v>73</v>
+      </c>
+      <c r="E33" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F33" s="29"/>
-      <c r="G33" s="5"/>
+      <c r="G33" s="5" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="28"/>
+      <c r="B34" s="18">
+        <v>172</v>
+      </c>
+      <c r="C34" s="18">
+        <v>121</v>
+      </c>
+      <c r="D34" s="18">
+        <v>51</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F34" s="28"/>
-      <c r="G34" s="3"/>
+      <c r="G34" s="3" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="29"/>
+      <c r="B35" s="21">
+        <v>1531</v>
+      </c>
+      <c r="C35" s="21">
+        <v>1359</v>
+      </c>
+      <c r="D35" s="21">
+        <v>172</v>
+      </c>
+      <c r="E35" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F35" s="29"/>
-      <c r="G35" s="5"/>
+      <c r="G35" s="5" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="B36" s="18">
+        <v>169</v>
+      </c>
+      <c r="C36" s="18">
+        <v>610</v>
+      </c>
+      <c r="D36" s="18">
+        <v>-441</v>
+      </c>
       <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="3"/>
+      <c r="F36" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="29"/>
+      <c r="B37" s="21">
+        <v>480</v>
+      </c>
+      <c r="C37" s="21">
+        <v>382</v>
+      </c>
+      <c r="D37" s="21">
+        <v>98</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F37" s="29"/>
-      <c r="G37" s="5"/>
+      <c r="G37" s="5" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
+      <c r="B38" s="18">
+        <v>29</v>
+      </c>
+      <c r="C38" s="18">
+        <v>229</v>
+      </c>
+      <c r="D38" s="18">
+        <v>-200</v>
+      </c>
       <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="3"/>
+      <c r="F38" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="B39" s="21"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
+        <v>44</v>
+      </c>
+      <c r="B39" s="21">
+        <v>91</v>
+      </c>
+      <c r="C39" s="21">
+        <v>118</v>
+      </c>
+      <c r="D39" s="21">
+        <v>-27</v>
+      </c>
       <c r="E39" s="29"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="5"/>
+      <c r="F39" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="B40" s="42"/>
-      <c r="C40" s="42"/>
-      <c r="D40" s="42"/>
+        <v>45</v>
+      </c>
+      <c r="B40" s="42">
+        <v>41</v>
+      </c>
+      <c r="C40" s="42">
+        <v>74</v>
+      </c>
+      <c r="D40" s="42">
+        <v>-33</v>
+      </c>
       <c r="E40" s="39"/>
-      <c r="F40" s="39"/>
-      <c r="G40" s="40"/>
+      <c r="F40" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="G40" s="40" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
+        <v>46</v>
+      </c>
+      <c r="B41" s="25">
+        <v>14</v>
+      </c>
+      <c r="C41" s="25">
+        <v>28</v>
+      </c>
+      <c r="D41" s="25">
+        <v>-14</v>
+      </c>
       <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="9"/>
+      <c r="F41" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" s="42"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="42"/>
+        <v>47</v>
+      </c>
+      <c r="B42" s="42">
+        <v>11</v>
+      </c>
+      <c r="C42" s="42">
+        <v>23</v>
+      </c>
+      <c r="D42" s="42">
+        <v>-12</v>
+      </c>
       <c r="E42" s="39"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="40"/>
+      <c r="F42" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="G42" s="40" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
+        <v>48</v>
+      </c>
+      <c r="B43" s="25">
+        <v>91</v>
+      </c>
+      <c r="C43" s="25">
+        <v>112</v>
+      </c>
+      <c r="D43" s="25">
+        <v>-21</v>
+      </c>
       <c r="E43" s="31"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="9"/>
+      <c r="F43" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
+      <c r="B44" s="18">
+        <v>100</v>
+      </c>
+      <c r="C44" s="18">
+        <v>189</v>
+      </c>
+      <c r="D44" s="18">
+        <v>-89</v>
+      </c>
       <c r="E44" s="28"/>
-      <c r="F44" s="28"/>
-      <c r="G44" s="3"/>
+      <c r="F44" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="21"/>
-      <c r="C45" s="21"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="29"/>
+      <c r="B45" s="21">
+        <v>583</v>
+      </c>
+      <c r="C45" s="21">
+        <v>529</v>
+      </c>
+      <c r="D45" s="21">
+        <v>54</v>
+      </c>
+      <c r="E45" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F45" s="29"/>
-      <c r="G45" s="5"/>
+      <c r="G45" s="5" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="28"/>
+      <c r="B46" s="18">
+        <v>965</v>
+      </c>
+      <c r="C46" s="18">
+        <v>709</v>
+      </c>
+      <c r="D46" s="18">
+        <v>256</v>
+      </c>
+      <c r="E46" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F46" s="28"/>
-      <c r="G46" s="3"/>
+      <c r="G46" s="3" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="21"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
+      <c r="B47" s="21">
+        <v>235</v>
+      </c>
+      <c r="C47" s="21">
+        <v>596</v>
+      </c>
+      <c r="D47" s="21">
+        <v>-361</v>
+      </c>
       <c r="E47" s="29"/>
-      <c r="F47" s="29"/>
-      <c r="G47" s="5"/>
+      <c r="F47" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="28"/>
+      <c r="B48" s="18">
+        <v>450</v>
+      </c>
+      <c r="C48" s="18">
+        <v>198</v>
+      </c>
+      <c r="D48" s="18">
+        <v>252</v>
+      </c>
+      <c r="E48" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F48" s="28"/>
-      <c r="G48" s="3"/>
+      <c r="G48" s="3" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="21"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="29"/>
+      <c r="B49" s="21">
+        <v>869</v>
+      </c>
+      <c r="C49" s="21">
+        <v>713</v>
+      </c>
+      <c r="D49" s="21">
+        <v>156</v>
+      </c>
+      <c r="E49" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F49" s="29"/>
-      <c r="G49" s="5"/>
+      <c r="G49" s="5" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="18"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
+      <c r="B50" s="18">
+        <v>95</v>
+      </c>
+      <c r="C50" s="18">
+        <v>167</v>
+      </c>
+      <c r="D50" s="18">
+        <v>-72</v>
+      </c>
       <c r="E50" s="28"/>
-      <c r="F50" s="28"/>
-      <c r="G50" s="3"/>
+      <c r="F50" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="21"/>
-      <c r="C51" s="21"/>
-      <c r="D51" s="21"/>
+      <c r="B51" s="21">
+        <v>317</v>
+      </c>
+      <c r="C51" s="21">
+        <v>470</v>
+      </c>
+      <c r="D51" s="21">
+        <v>-153</v>
+      </c>
       <c r="E51" s="29"/>
-      <c r="F51" s="29"/>
-      <c r="G51" s="5"/>
+      <c r="F51" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="18"/>
-      <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="28"/>
+      <c r="B52" s="18">
+        <v>260</v>
+      </c>
+      <c r="C52" s="18">
+        <v>217</v>
+      </c>
+      <c r="D52" s="18">
+        <v>43</v>
+      </c>
+      <c r="E52" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F52" s="28"/>
-      <c r="G52" s="3"/>
+      <c r="G52" s="3" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="21"/>
-      <c r="C53" s="21"/>
-      <c r="D53" s="21"/>
+      <c r="B53" s="21">
+        <v>19</v>
+      </c>
+      <c r="C53" s="21">
+        <v>275</v>
+      </c>
+      <c r="D53" s="21">
+        <v>-256</v>
+      </c>
       <c r="E53" s="29"/>
-      <c r="F53" s="29"/>
-      <c r="G53" s="5"/>
+      <c r="F53" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="B54" s="27"/>
-      <c r="C54" s="27"/>
-      <c r="D54" s="27"/>
-      <c r="E54" s="32"/>
+      <c r="B54" s="27">
+        <v>343</v>
+      </c>
+      <c r="C54" s="27">
+        <v>200</v>
+      </c>
+      <c r="D54" s="27">
+        <v>143</v>
+      </c>
+      <c r="E54" s="32" t="s">
+        <v>60</v>
+      </c>
       <c r="F54" s="32"/>
-      <c r="G54" s="11"/>
+      <c r="G54" s="11" t="s">
+        <v>247</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G54" xr:uid="{00000000-0009-0000-0000-000009000000}"/>

</xml_diff>

<commit_message>
Update last 4 files
</commit_message>
<xml_diff>
--- a/statistics_files/2025/2025_99_g_net_borrower_lender.xlsx
+++ b/statistics_files/2025/2025_99_g_net_borrower_lender.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\github\next_statistics\statistics_files\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09807FBD-0A2A-4655-A8DB-5DB5BC19E211}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D109EF0-DD27-44ED-AD94-1849426106FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="673" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1692" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1794" uniqueCount="253">
   <si>
     <t>NET</t>
   </si>
@@ -799,6 +799,21 @@
   </si>
   <si>
     <t>1.72 : 1</t>
+  </si>
+  <si>
+    <t>1.38 : 1</t>
+  </si>
+  <si>
+    <t>1.67 : 1</t>
+  </si>
+  <si>
+    <t>0.08 : 1</t>
+  </si>
+  <si>
+    <t>0.85 : 1</t>
+  </si>
+  <si>
+    <t>2.57 : 1</t>
   </si>
 </sst>
 </file>
@@ -3390,7 +3405,7 @@
       <selection activeCell="A42" activeCellId="1" sqref="A40:G40 A42:G42"/>
       <selection pane="topRight" activeCell="A42" activeCellId="1" sqref="A40:G40 A42:G42"/>
       <selection pane="bottomLeft" activeCell="A42" activeCellId="1" sqref="A40:G40 A42:G42"/>
-      <selection pane="bottomRight" activeCell="A42" activeCellId="1" sqref="A40:G40 A42:G42"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3430,108 +3445,204 @@
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="28"/>
+      <c r="B2" s="18">
+        <v>1655</v>
+      </c>
+      <c r="C2" s="18">
+        <v>1331</v>
+      </c>
+      <c r="D2" s="18">
+        <v>324</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F2" s="28"/>
-      <c r="G2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="29"/>
+      <c r="B3" s="21">
+        <v>570</v>
+      </c>
+      <c r="C3" s="21">
+        <v>391</v>
+      </c>
+      <c r="D3" s="21">
+        <v>179</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F3" s="29"/>
-      <c r="G3" s="5"/>
+      <c r="G3" s="5" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
+      <c r="B4" s="18">
+        <v>1051</v>
+      </c>
+      <c r="C4" s="18">
+        <v>1299</v>
+      </c>
+      <c r="D4" s="18">
+        <v>-248</v>
+      </c>
       <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="3"/>
+      <c r="F4" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
+      <c r="B5" s="21">
+        <v>31</v>
+      </c>
+      <c r="C5" s="21">
+        <v>114</v>
+      </c>
+      <c r="D5" s="21">
+        <v>-83</v>
+      </c>
       <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="5"/>
+      <c r="F5" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="28"/>
+      <c r="B6" s="18">
+        <v>1320</v>
+      </c>
+      <c r="C6" s="18">
+        <v>1243</v>
+      </c>
+      <c r="D6" s="18">
+        <v>77</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F6" s="28"/>
-      <c r="G6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="29"/>
+      <c r="B7" s="21">
+        <v>214</v>
+      </c>
+      <c r="C7" s="21">
+        <v>198</v>
+      </c>
+      <c r="D7" s="21">
+        <v>16</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F7" s="29"/>
-      <c r="G7" s="5"/>
+      <c r="G7" s="5" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="28"/>
+      <c r="B8" s="18">
+        <v>182</v>
+      </c>
+      <c r="C8" s="18">
+        <v>177</v>
+      </c>
+      <c r="D8" s="18">
+        <v>5</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F8" s="28"/>
-      <c r="G8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="29"/>
+      <c r="B9" s="21">
+        <v>84</v>
+      </c>
+      <c r="C9" s="21">
+        <v>63</v>
+      </c>
+      <c r="D9" s="21">
+        <v>21</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F9" s="29"/>
-      <c r="G9" s="5"/>
+      <c r="G9" s="5" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
+      <c r="B10" s="18">
+        <v>1</v>
+      </c>
+      <c r="C10" s="18">
+        <v>47</v>
+      </c>
+      <c r="D10" s="18">
+        <v>-46</v>
+      </c>
       <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="3"/>
+      <c r="F10" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
+      <c r="B11" s="21">
+        <v>0</v>
+      </c>
+      <c r="C11" s="21">
+        <v>0</v>
+      </c>
+      <c r="D11" s="21">
+        <v>0</v>
+      </c>
       <c r="E11" s="29"/>
       <c r="F11" s="29"/>
       <c r="G11" s="5"/>
@@ -3540,163 +3651,309 @@
       <c r="A12" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="35"/>
+      <c r="B12" s="41">
+        <v>26</v>
+      </c>
+      <c r="C12" s="41">
+        <v>16</v>
+      </c>
+      <c r="D12" s="41">
+        <v>10</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>60</v>
+      </c>
       <c r="F12" s="35"/>
-      <c r="G12" s="36"/>
+      <c r="G12" s="36" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
+      <c r="B13" s="23">
+        <v>68</v>
+      </c>
+      <c r="C13" s="23">
+        <v>82</v>
+      </c>
+      <c r="D13" s="23">
+        <v>-14</v>
+      </c>
       <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="7"/>
+      <c r="F13" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
+      <c r="B14" s="41">
+        <v>219</v>
+      </c>
+      <c r="C14" s="41">
+        <v>325</v>
+      </c>
+      <c r="D14" s="41">
+        <v>-106</v>
+      </c>
       <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="36"/>
+      <c r="F14" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="36" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
+      <c r="B15" s="23">
+        <v>85</v>
+      </c>
+      <c r="C15" s="23">
+        <v>160</v>
+      </c>
+      <c r="D15" s="23">
+        <v>-75</v>
+      </c>
       <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="7"/>
+      <c r="F15" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="B16" s="18">
+        <v>56</v>
+      </c>
+      <c r="C16" s="18">
+        <v>181</v>
+      </c>
+      <c r="D16" s="18">
+        <v>-125</v>
+      </c>
       <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="3"/>
+      <c r="F16" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="29"/>
+      <c r="B17" s="21">
+        <v>638</v>
+      </c>
+      <c r="C17" s="21">
+        <v>461</v>
+      </c>
+      <c r="D17" s="21">
+        <v>177</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F17" s="29"/>
-      <c r="G17" s="5"/>
+      <c r="G17" s="5" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
+      <c r="B18" s="18">
+        <v>109</v>
+      </c>
+      <c r="C18" s="18">
+        <v>132</v>
+      </c>
+      <c r="D18" s="18">
+        <v>-23</v>
+      </c>
       <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="3"/>
+      <c r="F18" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="29"/>
+      <c r="B19" s="21">
+        <v>505</v>
+      </c>
+      <c r="C19" s="21">
+        <v>493</v>
+      </c>
+      <c r="D19" s="21">
+        <v>12</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F19" s="29"/>
-      <c r="G19" s="5"/>
+      <c r="G19" s="5" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+      <c r="B20" s="18">
+        <v>5</v>
+      </c>
+      <c r="C20" s="18">
+        <v>54</v>
+      </c>
+      <c r="D20" s="18">
+        <v>-49</v>
+      </c>
       <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="3"/>
+      <c r="F20" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="29"/>
+      <c r="B21" s="21">
+        <v>562</v>
+      </c>
+      <c r="C21" s="21">
+        <v>465</v>
+      </c>
+      <c r="D21" s="21">
+        <v>97</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F21" s="29"/>
-      <c r="G21" s="5"/>
+      <c r="G21" s="5" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="B22" s="18">
+        <v>74</v>
+      </c>
+      <c r="C22" s="18">
+        <v>239</v>
+      </c>
+      <c r="D22" s="18">
+        <v>-165</v>
+      </c>
       <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="3"/>
+      <c r="F22" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
+      <c r="B23" s="21">
+        <v>725</v>
+      </c>
+      <c r="C23" s="21">
+        <v>752</v>
+      </c>
+      <c r="D23" s="21">
+        <v>-27</v>
+      </c>
       <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="5"/>
+      <c r="F23" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="28"/>
+      <c r="B24" s="18">
+        <v>2075</v>
+      </c>
+      <c r="C24" s="18">
+        <v>1246</v>
+      </c>
+      <c r="D24" s="18">
+        <v>829</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F24" s="28"/>
-      <c r="G24" s="3"/>
+      <c r="G24" s="3" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
+      <c r="B25" s="21">
+        <v>119</v>
+      </c>
+      <c r="C25" s="21">
+        <v>384</v>
+      </c>
+      <c r="D25" s="21">
+        <v>-265</v>
+      </c>
       <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="5"/>
+      <c r="F25" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
+      <c r="B26" s="18">
+        <v>0</v>
+      </c>
+      <c r="C26" s="18">
+        <v>0</v>
+      </c>
+      <c r="D26" s="18">
+        <v>0</v>
+      </c>
       <c r="E26" s="28"/>
       <c r="F26" s="28"/>
       <c r="G26" s="3"/>
@@ -3705,309 +3962,589 @@
       <c r="A27" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
+      <c r="B27" s="21">
+        <v>218</v>
+      </c>
+      <c r="C27" s="21">
+        <v>222</v>
+      </c>
+      <c r="D27" s="21">
+        <v>-4</v>
+      </c>
       <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="5"/>
+      <c r="F27" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="28"/>
+      <c r="B28" s="18">
+        <v>180</v>
+      </c>
+      <c r="C28" s="18">
+        <v>92</v>
+      </c>
+      <c r="D28" s="18">
+        <v>88</v>
+      </c>
+      <c r="E28" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F28" s="28"/>
-      <c r="G28" s="3"/>
+      <c r="G28" s="3" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="29"/>
+      <c r="B29" s="21">
+        <v>646</v>
+      </c>
+      <c r="C29" s="21">
+        <v>540</v>
+      </c>
+      <c r="D29" s="21">
+        <v>106</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F29" s="29"/>
-      <c r="G29" s="5"/>
+      <c r="G29" s="5" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
+      <c r="B30" s="18">
+        <v>26</v>
+      </c>
+      <c r="C30" s="18">
+        <v>38</v>
+      </c>
+      <c r="D30" s="18">
+        <v>-12</v>
+      </c>
       <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="3"/>
+      <c r="F30" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
+      <c r="B31" s="21">
+        <v>66</v>
+      </c>
+      <c r="C31" s="21">
+        <v>244</v>
+      </c>
+      <c r="D31" s="21">
+        <v>-178</v>
+      </c>
       <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="5"/>
+      <c r="F31" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="B32" s="18">
+        <v>547</v>
+      </c>
+      <c r="C32" s="18">
+        <v>609</v>
+      </c>
+      <c r="D32" s="18">
+        <v>-62</v>
+      </c>
       <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="3"/>
+      <c r="F32" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="29"/>
+      <c r="B33" s="21">
+        <v>394</v>
+      </c>
+      <c r="C33" s="21">
+        <v>384</v>
+      </c>
+      <c r="D33" s="21">
+        <v>10</v>
+      </c>
+      <c r="E33" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F33" s="29"/>
-      <c r="G33" s="5"/>
+      <c r="G33" s="5" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="28"/>
+      <c r="B34" s="18">
+        <v>190</v>
+      </c>
+      <c r="C34" s="18">
+        <v>165</v>
+      </c>
+      <c r="D34" s="18">
+        <v>25</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F34" s="28"/>
-      <c r="G34" s="3"/>
+      <c r="G34" s="3" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
+      <c r="B35" s="21">
+        <v>1106</v>
+      </c>
+      <c r="C35" s="21">
+        <v>1491</v>
+      </c>
+      <c r="D35" s="21">
+        <v>-385</v>
+      </c>
       <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="5"/>
+      <c r="F35" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="B36" s="18">
+        <v>142</v>
+      </c>
+      <c r="C36" s="18">
+        <v>630</v>
+      </c>
+      <c r="D36" s="18">
+        <v>-488</v>
+      </c>
       <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="3"/>
+      <c r="F36" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="29"/>
+      <c r="B37" s="21">
+        <v>565</v>
+      </c>
+      <c r="C37" s="21">
+        <v>411</v>
+      </c>
+      <c r="D37" s="21">
+        <v>154</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F37" s="29"/>
-      <c r="G37" s="5"/>
+      <c r="G37" s="5" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
+      <c r="B38" s="18">
+        <v>21</v>
+      </c>
+      <c r="C38" s="18">
+        <v>260</v>
+      </c>
+      <c r="D38" s="18">
+        <v>-239</v>
+      </c>
       <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="3"/>
+      <c r="F38" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="B39" s="21"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
+      <c r="B39" s="21">
+        <v>30</v>
+      </c>
+      <c r="C39" s="21">
+        <v>78</v>
+      </c>
+      <c r="D39" s="21">
+        <v>-48</v>
+      </c>
       <c r="E39" s="29"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="5"/>
+      <c r="F39" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="42"/>
-      <c r="C40" s="42"/>
-      <c r="D40" s="42"/>
+      <c r="B40" s="42">
+        <v>72</v>
+      </c>
+      <c r="C40" s="42">
+        <v>89</v>
+      </c>
+      <c r="D40" s="42">
+        <v>-17</v>
+      </c>
       <c r="E40" s="39"/>
-      <c r="F40" s="39"/>
-      <c r="G40" s="40"/>
+      <c r="F40" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="G40" s="40" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
+      <c r="B41" s="25">
+        <v>22</v>
+      </c>
+      <c r="C41" s="25">
+        <v>27</v>
+      </c>
+      <c r="D41" s="25">
+        <v>-5</v>
+      </c>
       <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="9"/>
+      <c r="F41" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="B42" s="42"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="42"/>
+      <c r="B42" s="42">
+        <v>10</v>
+      </c>
+      <c r="C42" s="42">
+        <v>35</v>
+      </c>
+      <c r="D42" s="42">
+        <v>-25</v>
+      </c>
       <c r="E42" s="39"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="40"/>
+      <c r="F42" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="G42" s="40" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
+      <c r="B43" s="25">
+        <v>106</v>
+      </c>
+      <c r="C43" s="25">
+        <v>124</v>
+      </c>
+      <c r="D43" s="25">
+        <v>-18</v>
+      </c>
       <c r="E43" s="31"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="9"/>
+      <c r="F43" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
+      <c r="B44" s="18">
+        <v>74</v>
+      </c>
+      <c r="C44" s="18">
+        <v>202</v>
+      </c>
+      <c r="D44" s="18">
+        <v>-128</v>
+      </c>
       <c r="E44" s="28"/>
-      <c r="F44" s="28"/>
-      <c r="G44" s="3"/>
+      <c r="F44" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="21"/>
-      <c r="C45" s="21"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="29"/>
+      <c r="B45" s="21">
+        <v>652</v>
+      </c>
+      <c r="C45" s="21">
+        <v>568</v>
+      </c>
+      <c r="D45" s="21">
+        <v>84</v>
+      </c>
+      <c r="E45" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F45" s="29"/>
-      <c r="G45" s="5"/>
+      <c r="G45" s="5" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="28"/>
+      <c r="B46" s="18">
+        <v>973</v>
+      </c>
+      <c r="C46" s="18">
+        <v>693</v>
+      </c>
+      <c r="D46" s="18">
+        <v>280</v>
+      </c>
+      <c r="E46" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F46" s="28"/>
-      <c r="G46" s="3"/>
+      <c r="G46" s="3" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="21"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
+      <c r="B47" s="21">
+        <v>278</v>
+      </c>
+      <c r="C47" s="21">
+        <v>713</v>
+      </c>
+      <c r="D47" s="21">
+        <v>-435</v>
+      </c>
       <c r="E47" s="29"/>
-      <c r="F47" s="29"/>
-      <c r="G47" s="5"/>
+      <c r="F47" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="28"/>
+      <c r="B48" s="18">
+        <v>452</v>
+      </c>
+      <c r="C48" s="18">
+        <v>220</v>
+      </c>
+      <c r="D48" s="18">
+        <v>232</v>
+      </c>
+      <c r="E48" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F48" s="28"/>
-      <c r="G48" s="3"/>
+      <c r="G48" s="3" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="21"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="29"/>
+      <c r="B49" s="21">
+        <v>1011</v>
+      </c>
+      <c r="C49" s="21">
+        <v>597</v>
+      </c>
+      <c r="D49" s="21">
+        <v>414</v>
+      </c>
+      <c r="E49" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F49" s="29"/>
-      <c r="G49" s="5"/>
+      <c r="G49" s="5" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="18"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
+      <c r="B50" s="18">
+        <v>150</v>
+      </c>
+      <c r="C50" s="18">
+        <v>196</v>
+      </c>
+      <c r="D50" s="18">
+        <v>-46</v>
+      </c>
       <c r="E50" s="28"/>
-      <c r="F50" s="28"/>
-      <c r="G50" s="3"/>
+      <c r="F50" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="21"/>
-      <c r="C51" s="21"/>
-      <c r="D51" s="21"/>
+      <c r="B51" s="21">
+        <v>318</v>
+      </c>
+      <c r="C51" s="21">
+        <v>403</v>
+      </c>
+      <c r="D51" s="21">
+        <v>-85</v>
+      </c>
       <c r="E51" s="29"/>
-      <c r="F51" s="29"/>
-      <c r="G51" s="5"/>
+      <c r="F51" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="18"/>
-      <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="28"/>
+      <c r="B52" s="18">
+        <v>327</v>
+      </c>
+      <c r="C52" s="18">
+        <v>212</v>
+      </c>
+      <c r="D52" s="18">
+        <v>115</v>
+      </c>
+      <c r="E52" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F52" s="28"/>
-      <c r="G52" s="3"/>
+      <c r="G52" s="3" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="21"/>
-      <c r="C53" s="21"/>
-      <c r="D53" s="21"/>
+      <c r="B53" s="21">
+        <v>34</v>
+      </c>
+      <c r="C53" s="21">
+        <v>215</v>
+      </c>
+      <c r="D53" s="21">
+        <v>-181</v>
+      </c>
       <c r="E53" s="29"/>
-      <c r="F53" s="29"/>
-      <c r="G53" s="5"/>
+      <c r="F53" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="B54" s="27"/>
-      <c r="C54" s="27"/>
-      <c r="D54" s="27"/>
-      <c r="E54" s="32"/>
+      <c r="B54" s="27">
+        <v>535</v>
+      </c>
+      <c r="C54" s="27">
+        <v>208</v>
+      </c>
+      <c r="D54" s="27">
+        <v>327</v>
+      </c>
+      <c r="E54" s="32" t="s">
+        <v>60</v>
+      </c>
       <c r="F54" s="32"/>
-      <c r="G54" s="11"/>
+      <c r="G54" s="11" t="s">
+        <v>252</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G54" xr:uid="{00000000-0009-0000-0000-00000A000000}"/>
@@ -5439,15 +5976,15 @@
       </c>
       <c r="B2" s="2">
         <f>January!B2+February!B2+March!B2+April!B2+May!B2+June!B2+July!B2+August!B2+September!B2+October!B2+November!B2+December!B2</f>
-        <v>13621</v>
+        <v>15276</v>
       </c>
       <c r="C2" s="2">
         <f>January!C2+February!C2+March!C2+April!C2+May!C2+June!C2+July!C2+August!C2+September!C2+October!C2+November!C2+December!C2</f>
-        <v>11327</v>
+        <v>12658</v>
       </c>
       <c r="D2" s="2">
         <f>January!D2+February!D2+March!D2+April!D2+May!D2+June!D2+July!D2+August!D2+September!D2+October!D2+November!D2+December!D2</f>
-        <v>2294</v>
+        <v>2618</v>
       </c>
       <c r="E2" s="28" t="str">
         <f t="shared" ref="E2:E33" si="0">IF(D2 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -5459,7 +5996,7 @@
       </c>
       <c r="G2" s="3" t="str">
         <f t="shared" ref="G2:G33" si="2">IF(ISERROR(ROUND(B2/C2,2)&amp;" : 1"), "", ROUND(B2/C2,2)&amp;" : 1")</f>
-        <v>1.2 : 1</v>
+        <v>1.21 : 1</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5468,15 +6005,15 @@
       </c>
       <c r="B3" s="4">
         <f>January!B3+February!B3+March!B3+April!B3+May!B3+June!B3+July!B3+August!B3+September!B3+October!B3+November!B3+December!B3</f>
-        <v>5808</v>
+        <v>6378</v>
       </c>
       <c r="C3" s="4">
         <f>January!C3+February!C3+March!C3+April!C3+May!C3+June!C3+July!C3+August!C3+September!C3+October!C3+November!C3+December!C3</f>
-        <v>3293</v>
+        <v>3684</v>
       </c>
       <c r="D3" s="4">
         <f>January!D3+February!D3+March!D3+April!D3+May!D3+June!D3+July!D3+August!D3+September!D3+October!D3+November!D3+December!D3</f>
-        <v>2515</v>
+        <v>2694</v>
       </c>
       <c r="E3" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5488,7 +6025,7 @@
       </c>
       <c r="G3" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.76 : 1</v>
+        <v>1.73 : 1</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5497,27 +6034,27 @@
       </c>
       <c r="B4" s="2">
         <f>January!B4+February!B4+March!B4+April!B4+May!B4+June!B4+July!B4+August!B4+September!B4+October!B4+November!B4+December!B4</f>
-        <v>10341</v>
+        <v>11392</v>
       </c>
       <c r="C4" s="2">
         <f>January!C4+February!C4+March!C4+April!C4+May!C4+June!C4+July!C4+August!C4+September!C4+October!C4+November!C4+December!C4</f>
-        <v>10314</v>
+        <v>11613</v>
       </c>
       <c r="D4" s="2">
         <f>January!D4+February!D4+March!D4+April!D4+May!D4+June!D4+July!D4+August!D4+September!D4+October!D4+November!D4+December!D4</f>
-        <v>27</v>
+        <v>-221</v>
       </c>
       <c r="E4" s="28" t="str">
         <f t="shared" si="0"/>
-        <v>We borrowed more than we lent this year</v>
+        <v/>
       </c>
       <c r="F4" s="28" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>We lent more than we borrowed this year</v>
       </c>
       <c r="G4" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1 : 1</v>
+        <v>0.98 : 1</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5526,15 +6063,15 @@
       </c>
       <c r="B5" s="4">
         <f>January!B5+February!B5+March!B5+April!B5+May!B5+June!B5+July!B5+August!B5+September!B5+October!B5+November!B5+December!B5</f>
-        <v>290</v>
+        <v>321</v>
       </c>
       <c r="C5" s="4">
         <f>January!C5+February!C5+March!C5+April!C5+May!C5+June!C5+July!C5+August!C5+September!C5+October!C5+November!C5+December!C5</f>
-        <v>1119</v>
+        <v>1233</v>
       </c>
       <c r="D5" s="4">
         <f>January!D5+February!D5+March!D5+April!D5+May!D5+June!D5+July!D5+August!D5+September!D5+October!D5+November!D5+December!D5</f>
-        <v>-829</v>
+        <v>-912</v>
       </c>
       <c r="E5" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5555,15 +6092,15 @@
       </c>
       <c r="B6" s="2">
         <f>January!B6+February!B6+March!B6+April!B6+May!B6+June!B6+July!B6+August!B6+September!B6+October!B6+November!B6+December!B6</f>
-        <v>9497</v>
+        <v>10817</v>
       </c>
       <c r="C6" s="2">
         <f>January!C6+February!C6+March!C6+April!C6+May!C6+June!C6+July!C6+August!C6+September!C6+October!C6+November!C6+December!C6</f>
-        <v>10783</v>
+        <v>12026</v>
       </c>
       <c r="D6" s="2">
         <f>January!D6+February!D6+March!D6+April!D6+May!D6+June!D6+July!D6+August!D6+September!D6+October!D6+November!D6+December!D6</f>
-        <v>-1286</v>
+        <v>-1209</v>
       </c>
       <c r="E6" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5575,7 +6112,7 @@
       </c>
       <c r="G6" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.88 : 1</v>
+        <v>0.9 : 1</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5584,15 +6121,15 @@
       </c>
       <c r="B7" s="4">
         <f>January!B7+February!B7+March!B7+April!B7+May!B7+June!B7+July!B7+August!B7+September!B7+October!B7+November!B7+December!B7</f>
-        <v>2034</v>
+        <v>2248</v>
       </c>
       <c r="C7" s="4">
         <f>January!C7+February!C7+March!C7+April!C7+May!C7+June!C7+July!C7+August!C7+September!C7+October!C7+November!C7+December!C7</f>
-        <v>1515</v>
+        <v>1713</v>
       </c>
       <c r="D7" s="4">
         <f>January!D7+February!D7+March!D7+April!D7+May!D7+June!D7+July!D7+August!D7+September!D7+October!D7+November!D7+December!D7</f>
-        <v>519</v>
+        <v>535</v>
       </c>
       <c r="E7" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5604,7 +6141,7 @@
       </c>
       <c r="G7" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.34 : 1</v>
+        <v>1.31 : 1</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5613,15 +6150,15 @@
       </c>
       <c r="B8" s="2">
         <f>January!B8+February!B8+March!B8+April!B8+May!B8+June!B8+July!B8+August!B8+September!B8+October!B8+November!B8+December!B8</f>
-        <v>1363</v>
+        <v>1545</v>
       </c>
       <c r="C8" s="2">
         <f>January!C8+February!C8+March!C8+April!C8+May!C8+June!C8+July!C8+August!C8+September!C8+October!C8+November!C8+December!C8</f>
-        <v>1564</v>
+        <v>1741</v>
       </c>
       <c r="D8" s="2">
         <f>January!D8+February!D8+March!D8+April!D8+May!D8+June!D8+July!D8+August!D8+September!D8+October!D8+November!D8+December!D8</f>
-        <v>-201</v>
+        <v>-196</v>
       </c>
       <c r="E8" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5633,7 +6170,7 @@
       </c>
       <c r="G8" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.87 : 1</v>
+        <v>0.89 : 1</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5642,15 +6179,15 @@
       </c>
       <c r="B9" s="4">
         <f>January!B9+February!B9+March!B9+April!B9+May!B9+June!B9+July!B9+August!B9+September!B9+October!B9+November!B9+December!B9</f>
-        <v>507</v>
+        <v>591</v>
       </c>
       <c r="C9" s="4">
         <f>January!C9+February!C9+March!C9+April!C9+May!C9+June!C9+July!C9+August!C9+September!C9+October!C9+November!C9+December!C9</f>
-        <v>604</v>
+        <v>667</v>
       </c>
       <c r="D9" s="4">
         <f>January!D9+February!D9+March!D9+April!D9+May!D9+June!D9+July!D9+August!D9+September!D9+October!D9+November!D9+December!D9</f>
-        <v>-97</v>
+        <v>-76</v>
       </c>
       <c r="E9" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5662,7 +6199,7 @@
       </c>
       <c r="G9" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.84 : 1</v>
+        <v>0.89 : 1</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5671,15 +6208,15 @@
       </c>
       <c r="B10" s="2">
         <f>January!B10+February!B10+March!B10+April!B10+May!B10+June!B10+July!B10+August!B10+September!B10+October!B10+November!B10+December!B10</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C10" s="2">
         <f>January!C10+February!C10+March!C10+April!C10+May!C10+June!C10+July!C10+August!C10+September!C10+October!C10+November!C10+December!C10</f>
-        <v>351</v>
+        <v>398</v>
       </c>
       <c r="D10" s="2">
         <f>January!D10+February!D10+March!D10+April!D10+May!D10+June!D10+July!D10+August!D10+September!D10+October!D10+November!D10+December!D10</f>
-        <v>-347</v>
+        <v>-393</v>
       </c>
       <c r="E10" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5729,15 +6266,15 @@
       </c>
       <c r="B12" s="34">
         <f>January!B12+February!B12+March!B12+April!B12+May!B12+June!B12+July!B12+August!B12+September!B12+October!B12+November!B12+December!B12</f>
-        <v>268</v>
+        <v>294</v>
       </c>
       <c r="C12" s="34">
         <f>January!C12+February!C12+March!C12+April!C12+May!C12+June!C12+July!C12+August!C12+September!C12+October!C12+November!C12+December!C12</f>
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="D12" s="34">
         <f>January!D12+February!D12+March!D12+April!D12+May!D12+June!D12+July!D12+August!D12+September!D12+October!D12+November!D12+December!D12</f>
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="E12" s="35" t="str">
         <f t="shared" si="0"/>
@@ -5749,7 +6286,7 @@
       </c>
       <c r="G12" s="36" t="str">
         <f t="shared" si="2"/>
-        <v>1.9 : 1</v>
+        <v>1.87 : 1</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5758,15 +6295,15 @@
       </c>
       <c r="B13" s="6">
         <f>January!B13+February!B13+March!B13+April!B13+May!B13+June!B13+July!B13+August!B13+September!B13+October!B13+November!B13+December!B13</f>
-        <v>744</v>
+        <v>812</v>
       </c>
       <c r="C13" s="6">
         <f>January!C13+February!C13+March!C13+April!C13+May!C13+June!C13+July!C13+August!C13+September!C13+October!C13+November!C13+December!C13</f>
-        <v>672</v>
+        <v>754</v>
       </c>
       <c r="D13" s="6">
         <f>January!D13+February!D13+March!D13+April!D13+May!D13+June!D13+July!D13+August!D13+September!D13+October!D13+November!D13+December!D13</f>
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="E13" s="30" t="str">
         <f t="shared" si="0"/>
@@ -5778,7 +6315,7 @@
       </c>
       <c r="G13" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>1.11 : 1</v>
+        <v>1.08 : 1</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5787,15 +6324,15 @@
       </c>
       <c r="B14" s="34">
         <f>January!B14+February!B14+March!B14+April!B14+May!B14+June!B14+July!B14+August!B14+September!B14+October!B14+November!B14+December!B14</f>
-        <v>1611</v>
+        <v>1830</v>
       </c>
       <c r="C14" s="34">
         <f>January!C14+February!C14+March!C14+April!C14+May!C14+June!C14+July!C14+August!C14+September!C14+October!C14+November!C14+December!C14</f>
-        <v>2070</v>
+        <v>2395</v>
       </c>
       <c r="D14" s="34">
         <f>January!D14+February!D14+March!D14+April!D14+May!D14+June!D14+July!D14+August!D14+September!D14+October!D14+November!D14+December!D14</f>
-        <v>-459</v>
+        <v>-565</v>
       </c>
       <c r="E14" s="35" t="str">
         <f t="shared" si="0"/>
@@ -5807,7 +6344,7 @@
       </c>
       <c r="G14" s="36" t="str">
         <f t="shared" si="2"/>
-        <v>0.78 : 1</v>
+        <v>0.76 : 1</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5816,15 +6353,15 @@
       </c>
       <c r="B15" s="6">
         <f>January!B15+February!B15+March!B15+April!B15+May!B15+June!B15+July!B15+August!B15+September!B15+October!B15+November!B15+December!B15</f>
-        <v>531</v>
+        <v>616</v>
       </c>
       <c r="C15" s="6">
         <f>January!C15+February!C15+March!C15+April!C15+May!C15+June!C15+July!C15+August!C15+September!C15+October!C15+November!C15+December!C15</f>
-        <v>1321</v>
+        <v>1481</v>
       </c>
       <c r="D15" s="6">
         <f>January!D15+February!D15+March!D15+April!D15+May!D15+June!D15+July!D15+August!D15+September!D15+October!D15+November!D15+December!D15</f>
-        <v>-790</v>
+        <v>-865</v>
       </c>
       <c r="E15" s="30" t="str">
         <f t="shared" si="0"/>
@@ -5836,7 +6373,7 @@
       </c>
       <c r="G15" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0.4 : 1</v>
+        <v>0.42 : 1</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5845,15 +6382,15 @@
       </c>
       <c r="B16" s="2">
         <f>January!B16+February!B16+March!B16+April!B16+May!B16+June!B16+July!B16+August!B16+September!B16+October!B16+November!B16+December!B16</f>
-        <v>635</v>
+        <v>691</v>
       </c>
       <c r="C16" s="2">
         <f>January!C16+February!C16+March!C16+April!C16+May!C16+June!C16+July!C16+August!C16+September!C16+October!C16+November!C16+December!C16</f>
-        <v>1545</v>
+        <v>1726</v>
       </c>
       <c r="D16" s="2">
         <f>January!D16+February!D16+March!D16+April!D16+May!D16+June!D16+July!D16+August!D16+September!D16+October!D16+November!D16+December!D16</f>
-        <v>-910</v>
+        <v>-1035</v>
       </c>
       <c r="E16" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5865,7 +6402,7 @@
       </c>
       <c r="G16" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.41 : 1</v>
+        <v>0.4 : 1</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5874,15 +6411,15 @@
       </c>
       <c r="B17" s="4">
         <f>January!B17+February!B17+March!B17+April!B17+May!B17+June!B17+July!B17+August!B17+September!B17+October!B17+November!B17+December!B17</f>
-        <v>5648</v>
+        <v>6286</v>
       </c>
       <c r="C17" s="4">
         <f>January!C17+February!C17+March!C17+April!C17+May!C17+June!C17+July!C17+August!C17+September!C17+October!C17+November!C17+December!C17</f>
-        <v>4179</v>
+        <v>4640</v>
       </c>
       <c r="D17" s="4">
         <f>January!D17+February!D17+March!D17+April!D17+May!D17+June!D17+July!D17+August!D17+September!D17+October!D17+November!D17+December!D17</f>
-        <v>1469</v>
+        <v>1646</v>
       </c>
       <c r="E17" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5903,15 +6440,15 @@
       </c>
       <c r="B18" s="2">
         <f>January!B18+February!B18+March!B18+April!B18+May!B18+June!B18+July!B18+August!B18+September!B18+October!B18+November!B18+December!B18</f>
-        <v>413</v>
+        <v>522</v>
       </c>
       <c r="C18" s="2">
         <f>January!C18+February!C18+March!C18+April!C18+May!C18+June!C18+July!C18+August!C18+September!C18+October!C18+November!C18+December!C18</f>
-        <v>819</v>
+        <v>951</v>
       </c>
       <c r="D18" s="2">
         <f>January!D18+February!D18+March!D18+April!D18+May!D18+June!D18+July!D18+August!D18+September!D18+October!D18+November!D18+December!D18</f>
-        <v>-406</v>
+        <v>-429</v>
       </c>
       <c r="E18" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5923,7 +6460,7 @@
       </c>
       <c r="G18" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.5 : 1</v>
+        <v>0.55 : 1</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5932,15 +6469,15 @@
       </c>
       <c r="B19" s="4">
         <f>January!B19+February!B19+March!B19+April!B19+May!B19+June!B19+July!B19+August!B19+September!B19+October!B19+November!B19+December!B19</f>
-        <v>4107</v>
+        <v>4612</v>
       </c>
       <c r="C19" s="4">
         <f>January!C19+February!C19+March!C19+April!C19+May!C19+June!C19+July!C19+August!C19+September!C19+October!C19+November!C19+December!C19</f>
-        <v>3900</v>
+        <v>4393</v>
       </c>
       <c r="D19" s="4">
         <f>January!D19+February!D19+March!D19+April!D19+May!D19+June!D19+July!D19+August!D19+September!D19+October!D19+November!D19+December!D19</f>
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="E19" s="29" t="str">
         <f t="shared" si="0"/>
@@ -5961,15 +6498,15 @@
       </c>
       <c r="B20" s="2">
         <f>January!B20+February!B20+March!B20+April!B20+May!B20+June!B20+July!B20+August!B20+September!B20+October!B20+November!B20+December!B20</f>
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="C20" s="2">
         <f>January!C20+February!C20+March!C20+April!C20+May!C20+June!C20+July!C20+August!C20+September!C20+October!C20+November!C20+December!C20</f>
-        <v>486</v>
+        <v>540</v>
       </c>
       <c r="D20" s="2">
         <f>January!D20+February!D20+March!D20+April!D20+May!D20+June!D20+July!D20+August!D20+September!D20+October!D20+November!D20+December!D20</f>
-        <v>-303</v>
+        <v>-352</v>
       </c>
       <c r="E20" s="28" t="str">
         <f t="shared" si="0"/>
@@ -5981,7 +6518,7 @@
       </c>
       <c r="G20" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.38 : 1</v>
+        <v>0.35 : 1</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5990,15 +6527,15 @@
       </c>
       <c r="B21" s="4">
         <f>January!B21+February!B21+March!B21+April!B21+May!B21+June!B21+July!B21+August!B21+September!B21+October!B21+November!B21+December!B21</f>
-        <v>4481</v>
+        <v>5043</v>
       </c>
       <c r="C21" s="4">
         <f>January!C21+February!C21+March!C21+April!C21+May!C21+June!C21+July!C21+August!C21+September!C21+October!C21+November!C21+December!C21</f>
-        <v>3024</v>
+        <v>3489</v>
       </c>
       <c r="D21" s="4">
         <f>January!D21+February!D21+March!D21+April!D21+May!D21+June!D21+July!D21+August!D21+September!D21+October!D21+November!D21+December!D21</f>
-        <v>1457</v>
+        <v>1554</v>
       </c>
       <c r="E21" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6010,7 +6547,7 @@
       </c>
       <c r="G21" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.48 : 1</v>
+        <v>1.45 : 1</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6019,15 +6556,15 @@
       </c>
       <c r="B22" s="2">
         <f>January!B22+February!B22+March!B22+April!B22+May!B22+June!B22+July!B22+August!B22+September!B22+October!B22+November!B22+December!B22</f>
-        <v>600</v>
+        <v>674</v>
       </c>
       <c r="C22" s="2">
         <f>January!C22+February!C22+March!C22+April!C22+May!C22+June!C22+July!C22+August!C22+September!C22+October!C22+November!C22+December!C22</f>
-        <v>2283</v>
+        <v>2522</v>
       </c>
       <c r="D22" s="2">
         <f>January!D22+February!D22+March!D22+April!D22+May!D22+June!D22+July!D22+August!D22+September!D22+October!D22+November!D22+December!D22</f>
-        <v>-1683</v>
+        <v>-1848</v>
       </c>
       <c r="E22" s="28" t="str">
         <f t="shared" si="0"/>
@@ -6039,7 +6576,7 @@
       </c>
       <c r="G22" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.26 : 1</v>
+        <v>0.27 : 1</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6048,15 +6585,15 @@
       </c>
       <c r="B23" s="4">
         <f>January!B23+February!B23+March!B23+April!B23+May!B23+June!B23+July!B23+August!B23+September!B23+October!B23+November!B23+December!B23</f>
-        <v>5700</v>
+        <v>6425</v>
       </c>
       <c r="C23" s="4">
         <f>January!C23+February!C23+March!C23+April!C23+May!C23+June!C23+July!C23+August!C23+September!C23+October!C23+November!C23+December!C23</f>
-        <v>4999</v>
+        <v>5751</v>
       </c>
       <c r="D23" s="4">
         <f>January!D23+February!D23+March!D23+April!D23+May!D23+June!D23+July!D23+August!D23+September!D23+October!D23+November!D23+December!D23</f>
-        <v>701</v>
+        <v>674</v>
       </c>
       <c r="E23" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6068,7 +6605,7 @@
       </c>
       <c r="G23" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.14 : 1</v>
+        <v>1.12 : 1</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6077,15 +6614,15 @@
       </c>
       <c r="B24" s="2">
         <f>January!B24+February!B24+March!B24+April!B24+May!B24+June!B24+July!B24+August!B24+September!B24+October!B24+November!B24+December!B24</f>
-        <v>14127</v>
+        <v>16202</v>
       </c>
       <c r="C24" s="2">
         <f>January!C24+February!C24+March!C24+April!C24+May!C24+June!C24+July!C24+August!C24+September!C24+October!C24+November!C24+December!C24</f>
-        <v>10197</v>
+        <v>11443</v>
       </c>
       <c r="D24" s="2">
         <f>January!D24+February!D24+March!D24+April!D24+May!D24+June!D24+July!D24+August!D24+September!D24+October!D24+November!D24+December!D24</f>
-        <v>3930</v>
+        <v>4759</v>
       </c>
       <c r="E24" s="28" t="str">
         <f t="shared" si="0"/>
@@ -6097,7 +6634,7 @@
       </c>
       <c r="G24" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.39 : 1</v>
+        <v>1.42 : 1</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6106,15 +6643,15 @@
       </c>
       <c r="B25" s="4">
         <f>January!B25+February!B25+March!B25+April!B25+May!B25+June!B25+July!B25+August!B25+September!B25+October!B25+November!B25+December!B25</f>
-        <v>1357</v>
+        <v>1476</v>
       </c>
       <c r="C25" s="4">
         <f>January!C25+February!C25+March!C25+April!C25+May!C25+June!C25+July!C25+August!C25+September!C25+October!C25+November!C25+December!C25</f>
-        <v>3923</v>
+        <v>4307</v>
       </c>
       <c r="D25" s="4">
         <f>January!D25+February!D25+March!D25+April!D25+May!D25+June!D25+July!D25+August!D25+September!D25+October!D25+November!D25+December!D25</f>
-        <v>-2566</v>
+        <v>-2831</v>
       </c>
       <c r="E25" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6126,7 +6663,7 @@
       </c>
       <c r="G25" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.35 : 1</v>
+        <v>0.34 : 1</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6164,15 +6701,15 @@
       </c>
       <c r="B27" s="4">
         <f>January!B27+February!B27+March!B27+April!B27+May!B27+June!B27+July!B27+August!B27+September!B27+October!B27+November!B27+December!B27</f>
-        <v>1882</v>
+        <v>2100</v>
       </c>
       <c r="C27" s="4">
         <f>January!C27+February!C27+March!C27+April!C27+May!C27+June!C27+July!C27+August!C27+September!C27+October!C27+November!C27+December!C27</f>
-        <v>1496</v>
+        <v>1718</v>
       </c>
       <c r="D27" s="4">
         <f>January!D27+February!D27+March!D27+April!D27+May!D27+June!D27+July!D27+August!D27+September!D27+October!D27+November!D27+December!D27</f>
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="E27" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6184,7 +6721,7 @@
       </c>
       <c r="G27" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.26 : 1</v>
+        <v>1.22 : 1</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6193,15 +6730,15 @@
       </c>
       <c r="B28" s="2">
         <f>January!B28+February!B28+March!B28+April!B28+May!B28+June!B28+July!B28+August!B28+September!B28+October!B28+November!B28+December!B28</f>
-        <v>1077</v>
+        <v>1257</v>
       </c>
       <c r="C28" s="2">
         <f>January!C28+February!C28+March!C28+April!C28+May!C28+June!C28+July!C28+August!C28+September!C28+October!C28+November!C28+December!C28</f>
-        <v>988</v>
+        <v>1080</v>
       </c>
       <c r="D28" s="2">
         <f>January!D28+February!D28+March!D28+April!D28+May!D28+June!D28+July!D28+August!D28+September!D28+October!D28+November!D28+December!D28</f>
-        <v>89</v>
+        <v>177</v>
       </c>
       <c r="E28" s="28" t="str">
         <f t="shared" si="0"/>
@@ -6213,7 +6750,7 @@
       </c>
       <c r="G28" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.09 : 1</v>
+        <v>1.16 : 1</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6222,15 +6759,15 @@
       </c>
       <c r="B29" s="4">
         <f>January!B29+February!B29+March!B29+April!B29+May!B29+June!B29+July!B29+August!B29+September!B29+October!B29+November!B29+December!B29</f>
-        <v>5804</v>
+        <v>6450</v>
       </c>
       <c r="C29" s="4">
         <f>January!C29+February!C29+March!C29+April!C29+May!C29+June!C29+July!C29+August!C29+September!C29+October!C29+November!C29+December!C29</f>
-        <v>4174</v>
+        <v>4714</v>
       </c>
       <c r="D29" s="4">
         <f>January!D29+February!D29+March!D29+April!D29+May!D29+June!D29+July!D29+August!D29+September!D29+October!D29+November!D29+December!D29</f>
-        <v>1630</v>
+        <v>1736</v>
       </c>
       <c r="E29" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6242,7 +6779,7 @@
       </c>
       <c r="G29" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.39 : 1</v>
+        <v>1.37 : 1</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6251,15 +6788,15 @@
       </c>
       <c r="B30" s="2">
         <f>January!B30+February!B30+March!B30+April!B30+May!B30+June!B30+July!B30+August!B30+September!B30+October!B30+November!B30+December!B30</f>
-        <v>307</v>
+        <v>333</v>
       </c>
       <c r="C30" s="2">
         <f>January!C30+February!C30+March!C30+April!C30+May!C30+June!C30+July!C30+August!C30+September!C30+October!C30+November!C30+December!C30</f>
-        <v>226</v>
+        <v>264</v>
       </c>
       <c r="D30" s="2">
         <f>January!D30+February!D30+March!D30+April!D30+May!D30+June!D30+July!D30+August!D30+September!D30+October!D30+November!D30+December!D30</f>
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="E30" s="28" t="str">
         <f t="shared" si="0"/>
@@ -6271,7 +6808,7 @@
       </c>
       <c r="G30" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.36 : 1</v>
+        <v>1.26 : 1</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6280,15 +6817,15 @@
       </c>
       <c r="B31" s="4">
         <f>January!B31+February!B31+March!B31+April!B31+May!B31+June!B31+July!B31+August!B31+September!B31+October!B31+November!B31+December!B31</f>
-        <v>634</v>
+        <v>700</v>
       </c>
       <c r="C31" s="4">
         <f>January!C31+February!C31+March!C31+April!C31+May!C31+June!C31+July!C31+August!C31+September!C31+October!C31+November!C31+December!C31</f>
-        <v>2317</v>
+        <v>2561</v>
       </c>
       <c r="D31" s="4">
         <f>January!D31+February!D31+March!D31+April!D31+May!D31+June!D31+July!D31+August!D31+September!D31+October!D31+November!D31+December!D31</f>
-        <v>-1683</v>
+        <v>-1861</v>
       </c>
       <c r="E31" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6309,15 +6846,15 @@
       </c>
       <c r="B32" s="2">
         <f>January!B32+February!B32+March!B32+April!B32+May!B32+June!B32+July!B32+August!B32+September!B32+October!B32+November!B32+December!B32</f>
-        <v>3696</v>
+        <v>4243</v>
       </c>
       <c r="C32" s="2">
         <f>January!C32+February!C32+March!C32+April!C32+May!C32+June!C32+July!C32+August!C32+September!C32+October!C32+November!C32+December!C32</f>
-        <v>5034</v>
+        <v>5643</v>
       </c>
       <c r="D32" s="2">
         <f>January!D32+February!D32+March!D32+April!D32+May!D32+June!D32+July!D32+August!D32+September!D32+October!D32+November!D32+December!D32</f>
-        <v>-1338</v>
+        <v>-1400</v>
       </c>
       <c r="E32" s="28" t="str">
         <f t="shared" si="0"/>
@@ -6329,7 +6866,7 @@
       </c>
       <c r="G32" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.73 : 1</v>
+        <v>0.75 : 1</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6338,15 +6875,15 @@
       </c>
       <c r="B33" s="4">
         <f>January!B33+February!B33+March!B33+April!B33+May!B33+June!B33+July!B33+August!B33+September!B33+October!B33+November!B33+December!B33</f>
-        <v>3904</v>
+        <v>4298</v>
       </c>
       <c r="C33" s="4">
         <f>January!C33+February!C33+March!C33+April!C33+May!C33+June!C33+July!C33+August!C33+September!C33+October!C33+November!C33+December!C33</f>
-        <v>3855</v>
+        <v>4239</v>
       </c>
       <c r="D33" s="4">
         <f>January!D33+February!D33+March!D33+April!D33+May!D33+June!D33+July!D33+August!D33+September!D33+October!D33+November!D33+December!D33</f>
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="E33" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6367,15 +6904,15 @@
       </c>
       <c r="B34" s="2">
         <f>January!B34+February!B34+March!B34+April!B34+May!B34+June!B34+July!B34+August!B34+September!B34+October!B34+November!B34+December!B34</f>
-        <v>1744</v>
+        <v>1934</v>
       </c>
       <c r="C34" s="2">
         <f>January!C34+February!C34+March!C34+April!C34+May!C34+June!C34+July!C34+August!C34+September!C34+October!C34+November!C34+December!C34</f>
-        <v>1327</v>
+        <v>1492</v>
       </c>
       <c r="D34" s="2">
         <f>January!D34+February!D34+March!D34+April!D34+May!D34+June!D34+July!D34+August!D34+September!D34+October!D34+November!D34+December!D34</f>
-        <v>417</v>
+        <v>442</v>
       </c>
       <c r="E34" s="28" t="str">
         <f t="shared" ref="E34:E54" si="3">IF(D34 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -6387,7 +6924,7 @@
       </c>
       <c r="G34" s="3" t="str">
         <f t="shared" ref="G34:G54" si="5">IF(ISERROR(ROUND(B34/C34,2)&amp;" : 1"), "", ROUND(B34/C34,2)&amp;" : 1")</f>
-        <v>1.31 : 1</v>
+        <v>1.3 : 1</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6396,15 +6933,15 @@
       </c>
       <c r="B35" s="4">
         <f>January!B35+February!B35+March!B35+April!B35+May!B35+June!B35+July!B35+August!B35+September!B35+October!B35+November!B35+December!B35</f>
-        <v>9076</v>
+        <v>10182</v>
       </c>
       <c r="C35" s="4">
         <f>January!C35+February!C35+March!C35+April!C35+May!C35+June!C35+July!C35+August!C35+September!C35+October!C35+November!C35+December!C35</f>
-        <v>11692</v>
+        <v>13183</v>
       </c>
       <c r="D35" s="4">
         <f>January!D35+February!D35+March!D35+April!D35+May!D35+June!D35+July!D35+August!D35+September!D35+October!D35+November!D35+December!D35</f>
-        <v>-2616</v>
+        <v>-3001</v>
       </c>
       <c r="E35" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6416,7 +6953,7 @@
       </c>
       <c r="G35" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.78 : 1</v>
+        <v>0.77 : 1</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6425,15 +6962,15 @@
       </c>
       <c r="B36" s="2">
         <f>January!B36+February!B36+March!B36+April!B36+May!B36+June!B36+July!B36+August!B36+September!B36+October!B36+November!B36+December!B36</f>
-        <v>1437</v>
+        <v>1579</v>
       </c>
       <c r="C36" s="2">
         <f>January!C36+February!C36+March!C36+April!C36+May!C36+June!C36+July!C36+August!C36+September!C36+October!C36+November!C36+December!C36</f>
-        <v>4747</v>
+        <v>5377</v>
       </c>
       <c r="D36" s="2">
         <f>January!D36+February!D36+March!D36+April!D36+May!D36+June!D36+July!D36+August!D36+September!D36+October!D36+November!D36+December!D36</f>
-        <v>-3310</v>
+        <v>-3798</v>
       </c>
       <c r="E36" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6445,7 +6982,7 @@
       </c>
       <c r="G36" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.3 : 1</v>
+        <v>0.29 : 1</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6454,15 +6991,15 @@
       </c>
       <c r="B37" s="4">
         <f>January!B37+February!B37+March!B37+April!B37+May!B37+June!B37+July!B37+August!B37+September!B37+October!B37+November!B37+December!B37</f>
-        <v>4638</v>
+        <v>5203</v>
       </c>
       <c r="C37" s="4">
         <f>January!C37+February!C37+March!C37+April!C37+May!C37+June!C37+July!C37+August!C37+September!C37+October!C37+November!C37+December!C37</f>
-        <v>2751</v>
+        <v>3162</v>
       </c>
       <c r="D37" s="4">
         <f>January!D37+February!D37+March!D37+April!D37+May!D37+June!D37+July!D37+August!D37+September!D37+October!D37+November!D37+December!D37</f>
-        <v>1887</v>
+        <v>2041</v>
       </c>
       <c r="E37" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6474,7 +7011,7 @@
       </c>
       <c r="G37" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>1.69 : 1</v>
+        <v>1.65 : 1</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6483,15 +7020,15 @@
       </c>
       <c r="B38" s="2">
         <f>January!B38+February!B38+March!B38+April!B38+May!B38+June!B38+July!B38+August!B38+September!B38+October!B38+November!B38+December!B38</f>
-        <v>225</v>
+        <v>246</v>
       </c>
       <c r="C38" s="2">
         <f>January!C38+February!C38+March!C38+April!C38+May!C38+June!C38+July!C38+August!C38+September!C38+October!C38+November!C38+December!C38</f>
-        <v>1584</v>
+        <v>1844</v>
       </c>
       <c r="D38" s="2">
         <f>January!D38+February!D38+March!D38+April!D38+May!D38+June!D38+July!D38+August!D38+September!D38+October!D38+November!D38+December!D38</f>
-        <v>-1359</v>
+        <v>-1598</v>
       </c>
       <c r="E38" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6503,7 +7040,7 @@
       </c>
       <c r="G38" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.14 : 1</v>
+        <v>0.13 : 1</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6512,15 +7049,15 @@
       </c>
       <c r="B39" s="4">
         <f>January!B39+February!B39+March!B39+April!B39+May!B39+June!B39+July!B39+August!B39+September!B39+October!B39+November!B39+December!B39</f>
-        <v>306</v>
+        <v>336</v>
       </c>
       <c r="C39" s="4">
         <f>January!C39+February!C39+March!C39+April!C39+May!C39+June!C39+July!C39+August!C39+September!C39+October!C39+November!C39+December!C39</f>
-        <v>632</v>
+        <v>710</v>
       </c>
       <c r="D39" s="4">
         <f>January!D39+February!D39+March!D39+April!D39+May!D39+June!D39+July!D39+August!D39+September!D39+October!D39+November!D39+December!D39</f>
-        <v>-326</v>
+        <v>-374</v>
       </c>
       <c r="E39" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6532,7 +7069,7 @@
       </c>
       <c r="G39" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.48 : 1</v>
+        <v>0.47 : 1</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6541,15 +7078,15 @@
       </c>
       <c r="B40" s="38">
         <f>January!B40+February!B40+March!B40+April!B40+May!B40+June!B40+July!B40+August!B40+September!B40+October!B40+November!B40+December!B40</f>
-        <v>265</v>
+        <v>337</v>
       </c>
       <c r="C40" s="38">
         <f>January!C40+February!C40+March!C40+April!C40+May!C40+June!C40+July!C40+August!C40+September!C40+October!C40+November!C40+December!C40</f>
-        <v>498</v>
+        <v>587</v>
       </c>
       <c r="D40" s="38">
         <f>January!D40+February!D40+March!D40+April!D40+May!D40+June!D40+July!D40+August!D40+September!D40+October!D40+November!D40+December!D40</f>
-        <v>-233</v>
+        <v>-250</v>
       </c>
       <c r="E40" s="39" t="str">
         <f t="shared" si="3"/>
@@ -6561,7 +7098,7 @@
       </c>
       <c r="G40" s="40" t="str">
         <f t="shared" si="5"/>
-        <v>0.53 : 1</v>
+        <v>0.57 : 1</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6570,15 +7107,15 @@
       </c>
       <c r="B41" s="8">
         <f>January!B41+February!B41+March!B41+April!B41+May!B41+June!B41+July!B41+August!B41+September!B41+October!B41+November!B41+December!B41</f>
-        <v>251</v>
+        <v>273</v>
       </c>
       <c r="C41" s="8">
         <f>January!C41+February!C41+March!C41+April!C41+May!C41+June!C41+July!C41+August!C41+September!C41+October!C41+November!C41+December!C41</f>
-        <v>281</v>
+        <v>308</v>
       </c>
       <c r="D41" s="8">
         <f>January!D41+February!D41+March!D41+April!D41+May!D41+June!D41+July!D41+August!D41+September!D41+October!D41+November!D41+December!D41</f>
-        <v>-30</v>
+        <v>-35</v>
       </c>
       <c r="E41" s="31" t="str">
         <f t="shared" si="3"/>
@@ -6599,15 +7136,15 @@
       </c>
       <c r="B42" s="38">
         <f>January!B42+February!B42+March!B42+April!B42+May!B42+June!B42+July!B42+August!B42+September!B42+October!B42+November!B42+December!B42</f>
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C42" s="38">
         <f>January!C42+February!C42+March!C42+April!C42+May!C42+June!C42+July!C42+August!C42+September!C42+October!C42+November!C42+December!C42</f>
-        <v>239</v>
+        <v>274</v>
       </c>
       <c r="D42" s="38">
         <f>January!D42+February!D42+March!D42+April!D42+May!D42+June!D42+July!D42+August!D42+September!D42+October!D42+November!D42+December!D42</f>
-        <v>-190</v>
+        <v>-215</v>
       </c>
       <c r="E42" s="39" t="str">
         <f t="shared" si="3"/>
@@ -6619,7 +7156,7 @@
       </c>
       <c r="G42" s="40" t="str">
         <f t="shared" si="5"/>
-        <v>0.21 : 1</v>
+        <v>0.22 : 1</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6628,15 +7165,15 @@
       </c>
       <c r="B43" s="8">
         <f>January!B43+February!B43+March!B43+April!B43+May!B43+June!B43+July!B43+August!B43+September!B43+October!B43+November!B43+December!B43</f>
-        <v>542</v>
+        <v>648</v>
       </c>
       <c r="C43" s="8">
         <f>January!C43+February!C43+March!C43+April!C43+May!C43+June!C43+July!C43+August!C43+September!C43+October!C43+November!C43+December!C43</f>
-        <v>712</v>
+        <v>836</v>
       </c>
       <c r="D43" s="8">
         <f>January!D43+February!D43+March!D43+April!D43+May!D43+June!D43+July!D43+August!D43+September!D43+October!D43+November!D43+December!D43</f>
-        <v>-170</v>
+        <v>-188</v>
       </c>
       <c r="E43" s="31" t="str">
         <f t="shared" si="3"/>
@@ -6648,7 +7185,7 @@
       </c>
       <c r="G43" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0.76 : 1</v>
+        <v>0.78 : 1</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6657,15 +7194,15 @@
       </c>
       <c r="B44" s="2">
         <f>January!B44+February!B44+March!B44+April!B44+May!B44+June!B44+July!B44+August!B44+September!B44+October!B44+November!B44+December!B44</f>
-        <v>551</v>
+        <v>625</v>
       </c>
       <c r="C44" s="2">
         <f>January!C44+February!C44+March!C44+April!C44+May!C44+June!C44+July!C44+August!C44+September!C44+October!C44+November!C44+December!C44</f>
-        <v>1796</v>
+        <v>1998</v>
       </c>
       <c r="D44" s="2">
         <f>January!D44+February!D44+March!D44+April!D44+May!D44+June!D44+July!D44+August!D44+September!D44+October!D44+November!D44+December!D44</f>
-        <v>-1245</v>
+        <v>-1373</v>
       </c>
       <c r="E44" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6686,27 +7223,27 @@
       </c>
       <c r="B45" s="4">
         <f>January!B45+February!B45+March!B45+April!B45+May!B45+June!B45+July!B45+August!B45+September!B45+October!B45+November!B45+December!B45</f>
-        <v>4946</v>
+        <v>5598</v>
       </c>
       <c r="C45" s="4">
         <f>January!C45+February!C45+March!C45+April!C45+May!C45+June!C45+July!C45+August!C45+September!C45+October!C45+November!C45+December!C45</f>
-        <v>4975</v>
+        <v>5543</v>
       </c>
       <c r="D45" s="4">
         <f>January!D45+February!D45+March!D45+April!D45+May!D45+June!D45+July!D45+August!D45+September!D45+October!D45+November!D45+December!D45</f>
-        <v>-29</v>
+        <v>55</v>
       </c>
       <c r="E45" s="29" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>We borrowed more than we lent this year</v>
       </c>
       <c r="F45" s="29" t="str">
         <f t="shared" si="4"/>
-        <v>We lent more than we borrowed this year</v>
+        <v/>
       </c>
       <c r="G45" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.99 : 1</v>
+        <v>1.01 : 1</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6715,15 +7252,15 @@
       </c>
       <c r="B46" s="2">
         <f>January!B46+February!B46+March!B46+April!B46+May!B46+June!B46+July!B46+August!B46+September!B46+October!B46+November!B46+December!B46</f>
-        <v>9260</v>
+        <v>10233</v>
       </c>
       <c r="C46" s="2">
         <f>January!C46+February!C46+March!C46+April!C46+May!C46+June!C46+July!C46+August!C46+September!C46+October!C46+November!C46+December!C46</f>
-        <v>5983</v>
+        <v>6676</v>
       </c>
       <c r="D46" s="2">
         <f>January!D46+February!D46+March!D46+April!D46+May!D46+June!D46+July!D46+August!D46+September!D46+October!D46+November!D46+December!D46</f>
-        <v>3277</v>
+        <v>3557</v>
       </c>
       <c r="E46" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6735,7 +7272,7 @@
       </c>
       <c r="G46" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>1.55 : 1</v>
+        <v>1.53 : 1</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6744,15 +7281,15 @@
       </c>
       <c r="B47" s="4">
         <f>January!B47+February!B47+March!B47+April!B47+May!B47+June!B47+July!B47+August!B47+September!B47+October!B47+November!B47+December!B47</f>
-        <v>1883</v>
+        <v>2161</v>
       </c>
       <c r="C47" s="4">
         <f>January!C47+February!C47+March!C47+April!C47+May!C47+June!C47+July!C47+August!C47+September!C47+October!C47+November!C47+December!C47</f>
-        <v>5505</v>
+        <v>6218</v>
       </c>
       <c r="D47" s="4">
         <f>January!D47+February!D47+March!D47+April!D47+May!D47+June!D47+July!D47+August!D47+September!D47+October!D47+November!D47+December!D47</f>
-        <v>-3622</v>
+        <v>-4057</v>
       </c>
       <c r="E47" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6764,7 +7301,7 @@
       </c>
       <c r="G47" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.34 : 1</v>
+        <v>0.35 : 1</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6773,15 +7310,15 @@
       </c>
       <c r="B48" s="2">
         <f>January!B48+February!B48+March!B48+April!B48+May!B48+June!B48+July!B48+August!B48+September!B48+October!B48+November!B48+December!B48</f>
-        <v>5544</v>
+        <v>5996</v>
       </c>
       <c r="C48" s="2">
         <f>January!C48+February!C48+March!C48+April!C48+May!C48+June!C48+July!C48+August!C48+September!C48+October!C48+November!C48+December!C48</f>
-        <v>2004</v>
+        <v>2224</v>
       </c>
       <c r="D48" s="2">
         <f>January!D48+February!D48+March!D48+April!D48+May!D48+June!D48+July!D48+August!D48+September!D48+October!D48+November!D48+December!D48</f>
-        <v>3540</v>
+        <v>3772</v>
       </c>
       <c r="E48" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6793,7 +7330,7 @@
       </c>
       <c r="G48" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>2.77 : 1</v>
+        <v>2.7 : 1</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6802,15 +7339,15 @@
       </c>
       <c r="B49" s="4">
         <f>January!B49+February!B49+March!B49+April!B49+May!B49+June!B49+July!B49+August!B49+September!B49+October!B49+November!B49+December!B49</f>
-        <v>7919</v>
+        <v>8930</v>
       </c>
       <c r="C49" s="4">
         <f>January!C49+February!C49+March!C49+April!C49+May!C49+June!C49+July!C49+August!C49+September!C49+October!C49+November!C49+December!C49</f>
-        <v>5376</v>
+        <v>5973</v>
       </c>
       <c r="D49" s="4">
         <f>January!D49+February!D49+March!D49+April!D49+May!D49+June!D49+July!D49+August!D49+September!D49+October!D49+November!D49+December!D49</f>
-        <v>2543</v>
+        <v>2957</v>
       </c>
       <c r="E49" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6822,7 +7359,7 @@
       </c>
       <c r="G49" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>1.47 : 1</v>
+        <v>1.5 : 1</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6831,27 +7368,27 @@
       </c>
       <c r="B50" s="2">
         <f>January!B50+February!B50+March!B50+April!B50+May!B50+June!B50+July!B50+August!B50+September!B50+October!B50+November!B50+December!B50</f>
-        <v>1488</v>
+        <v>1638</v>
       </c>
       <c r="C50" s="2">
         <f>January!C50+February!C50+March!C50+April!C50+May!C50+June!C50+July!C50+August!C50+September!C50+October!C50+November!C50+December!C50</f>
-        <v>1457</v>
+        <v>1653</v>
       </c>
       <c r="D50" s="2">
         <f>January!D50+February!D50+March!D50+April!D50+May!D50+June!D50+July!D50+August!D50+September!D50+October!D50+November!D50+December!D50</f>
-        <v>31</v>
+        <v>-15</v>
       </c>
       <c r="E50" s="28" t="str">
         <f t="shared" si="3"/>
-        <v>We borrowed more than we lent this year</v>
+        <v/>
       </c>
       <c r="F50" s="28" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>We lent more than we borrowed this year</v>
       </c>
       <c r="G50" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>1.02 : 1</v>
+        <v>0.99 : 1</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6860,15 +7397,15 @@
       </c>
       <c r="B51" s="4">
         <f>January!B51+February!B51+March!B51+April!B51+May!B51+June!B51+July!B51+August!B51+September!B51+October!B51+November!B51+December!B51</f>
-        <v>3145</v>
+        <v>3463</v>
       </c>
       <c r="C51" s="4">
         <f>January!C51+February!C51+March!C51+April!C51+May!C51+June!C51+July!C51+August!C51+September!C51+October!C51+November!C51+December!C51</f>
-        <v>3470</v>
+        <v>3873</v>
       </c>
       <c r="D51" s="4">
         <f>January!D51+February!D51+March!D51+April!D51+May!D51+June!D51+July!D51+August!D51+September!D51+October!D51+November!D51+December!D51</f>
-        <v>-325</v>
+        <v>-410</v>
       </c>
       <c r="E51" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6880,7 +7417,7 @@
       </c>
       <c r="G51" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.91 : 1</v>
+        <v>0.89 : 1</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6889,15 +7426,15 @@
       </c>
       <c r="B52" s="2">
         <f>January!B52+February!B52+March!B52+April!B52+May!B52+June!B52+July!B52+August!B52+September!B52+October!B52+November!B52+December!B52</f>
-        <v>1406</v>
+        <v>1733</v>
       </c>
       <c r="C52" s="2">
         <f>January!C52+February!C52+March!C52+April!C52+May!C52+June!C52+July!C52+August!C52+September!C52+October!C52+November!C52+December!C52</f>
-        <v>1933</v>
+        <v>2145</v>
       </c>
       <c r="D52" s="2">
         <f>January!D52+February!D52+March!D52+April!D52+May!D52+June!D52+July!D52+August!D52+September!D52+October!D52+November!D52+December!D52</f>
-        <v>-527</v>
+        <v>-412</v>
       </c>
       <c r="E52" s="28" t="str">
         <f t="shared" si="3"/>
@@ -6909,7 +7446,7 @@
       </c>
       <c r="G52" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.73 : 1</v>
+        <v>0.81 : 1</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6918,15 +7455,15 @@
       </c>
       <c r="B53" s="4">
         <f>January!B53+February!B53+March!B53+April!B53+May!B53+June!B53+July!B53+August!B53+September!B53+October!B53+November!B53+December!B53</f>
-        <v>281</v>
+        <v>315</v>
       </c>
       <c r="C53" s="4">
         <f>January!C53+February!C53+March!C53+April!C53+May!C53+June!C53+July!C53+August!C53+September!C53+October!C53+November!C53+December!C53</f>
-        <v>2261</v>
+        <v>2476</v>
       </c>
       <c r="D53" s="4">
         <f>January!D53+February!D53+March!D53+April!D53+May!D53+June!D53+July!D53+August!D53+September!D53+October!D53+November!D53+December!D53</f>
-        <v>-1980</v>
+        <v>-2161</v>
       </c>
       <c r="E53" s="29" t="str">
         <f t="shared" si="3"/>
@@ -6938,7 +7475,7 @@
       </c>
       <c r="G53" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.12 : 1</v>
+        <v>0.13 : 1</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6947,15 +7484,15 @@
       </c>
       <c r="B54" s="10">
         <f>January!B54+February!B54+March!B54+April!B54+May!B54+June!B54+July!B54+August!B54+September!B54+October!B54+November!B54+December!B54</f>
-        <v>3447</v>
+        <v>3982</v>
       </c>
       <c r="C54" s="10">
         <f>January!C54+February!C54+March!C54+April!C54+May!C54+June!C54+July!C54+August!C54+September!C54+October!C54+November!C54+December!C54</f>
-        <v>1846</v>
+        <v>2054</v>
       </c>
       <c r="D54" s="10">
         <f>January!D54+February!D54+March!D54+April!D54+May!D54+June!D54+July!D54+August!D54+September!D54+October!D54+November!D54+December!D54</f>
-        <v>1601</v>
+        <v>1928</v>
       </c>
       <c r="E54" s="32" t="str">
         <f t="shared" si="3"/>
@@ -6967,7 +7504,7 @@
       </c>
       <c r="G54" s="11" t="str">
         <f t="shared" si="5"/>
-        <v>1.87 : 1</v>
+        <v>1.94 : 1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All files updated for December 2025
</commit_message>
<xml_diff>
--- a/statistics_files/2025/2025_99_g_net_borrower_lender.xlsx
+++ b/statistics_files/2025/2025_99_g_net_borrower_lender.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\github\next_statistics\statistics_files\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681D1664-94E3-4CE2-9BBA-68F2011D3D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB73C961-9B0D-4800-A77B-297245E36596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="673" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="673" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="January" sheetId="2" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1895" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1997" uniqueCount="267">
   <si>
     <t>NET</t>
   </si>
@@ -844,6 +844,27 @@
   </si>
   <si>
     <t>2.18 : 1</t>
+  </si>
+  <si>
+    <t>1.25 : 1</t>
+  </si>
+  <si>
+    <t>1.83 : 1</t>
+  </si>
+  <si>
+    <t>3.19 : 1</t>
+  </si>
+  <si>
+    <t>0.62 : 1</t>
+  </si>
+  <si>
+    <t>2.22 : 1</t>
+  </si>
+  <si>
+    <t>2.23 : 1</t>
+  </si>
+  <si>
+    <t>1.99 : 1</t>
   </si>
 </sst>
 </file>
@@ -2237,7 +2258,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B40" sqref="B40"/>
       <selection pane="topRight" activeCell="B40" sqref="B40"/>
@@ -5811,11 +5832,11 @@
   <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="A3" sqref="A3"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A42" activeCellId="1" sqref="A40:G40 A42:G42"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5855,108 +5876,204 @@
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="28"/>
+      <c r="B2" s="18">
+        <v>1209</v>
+      </c>
+      <c r="C2" s="18">
+        <v>1094</v>
+      </c>
+      <c r="D2" s="18">
+        <v>115</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F2" s="28"/>
-      <c r="G2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="29"/>
+      <c r="B3" s="21">
+        <v>506</v>
+      </c>
+      <c r="C3" s="21">
+        <v>280</v>
+      </c>
+      <c r="D3" s="21">
+        <v>226</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F3" s="29"/>
-      <c r="G3" s="5"/>
+      <c r="G3" s="5" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
+      <c r="B4" s="18">
+        <v>1065</v>
+      </c>
+      <c r="C4" s="18">
+        <v>1147</v>
+      </c>
+      <c r="D4" s="18">
+        <v>-82</v>
+      </c>
       <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="3"/>
+      <c r="F4" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
+      <c r="B5" s="21">
+        <v>55</v>
+      </c>
+      <c r="C5" s="21">
+        <v>167</v>
+      </c>
+      <c r="D5" s="21">
+        <v>-112</v>
+      </c>
       <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="5"/>
+      <c r="F5" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
+      <c r="B6" s="18">
+        <v>907</v>
+      </c>
+      <c r="C6" s="18">
+        <v>1044</v>
+      </c>
+      <c r="D6" s="18">
+        <v>-137</v>
+      </c>
       <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="3"/>
+      <c r="F6" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="29"/>
+      <c r="B7" s="21">
+        <v>190</v>
+      </c>
+      <c r="C7" s="21">
+        <v>146</v>
+      </c>
+      <c r="D7" s="21">
+        <v>44</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F7" s="29"/>
-      <c r="G7" s="5"/>
+      <c r="G7" s="5" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
+      <c r="B8" s="18">
+        <v>76</v>
+      </c>
+      <c r="C8" s="18">
+        <v>146</v>
+      </c>
+      <c r="D8" s="18">
+        <v>-70</v>
+      </c>
       <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="3"/>
+      <c r="F8" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="29"/>
+      <c r="B9" s="21">
+        <v>82</v>
+      </c>
+      <c r="C9" s="21">
+        <v>60</v>
+      </c>
+      <c r="D9" s="21">
+        <v>22</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F9" s="29"/>
-      <c r="G9" s="5"/>
+      <c r="G9" s="5" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
+      <c r="B10" s="18">
+        <v>0</v>
+      </c>
+      <c r="C10" s="18">
+        <v>32</v>
+      </c>
+      <c r="D10" s="18">
+        <v>-32</v>
+      </c>
       <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="3"/>
+      <c r="F10" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
+      <c r="B11" s="21">
+        <v>0</v>
+      </c>
+      <c r="C11" s="21">
+        <v>0</v>
+      </c>
+      <c r="D11" s="21">
+        <v>0</v>
+      </c>
       <c r="E11" s="29"/>
       <c r="F11" s="29"/>
       <c r="G11" s="5"/>
@@ -5965,163 +6082,309 @@
       <c r="A12" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
+      <c r="B12" s="41">
+        <v>4</v>
+      </c>
+      <c r="C12" s="41">
+        <v>24</v>
+      </c>
+      <c r="D12" s="41">
+        <v>-20</v>
+      </c>
       <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="36"/>
+      <c r="F12" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="36" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="30"/>
+      <c r="B13" s="23">
+        <v>55</v>
+      </c>
+      <c r="C13" s="23">
+        <v>44</v>
+      </c>
+      <c r="D13" s="23">
+        <v>11</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>60</v>
+      </c>
       <c r="F13" s="30"/>
-      <c r="G13" s="7"/>
+      <c r="G13" s="7" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
+      <c r="B14" s="41">
+        <v>120</v>
+      </c>
+      <c r="C14" s="41">
+        <v>244</v>
+      </c>
+      <c r="D14" s="41">
+        <v>-124</v>
+      </c>
       <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="36"/>
+      <c r="F14" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="36" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
+      <c r="B15" s="23">
+        <v>70</v>
+      </c>
+      <c r="C15" s="23">
+        <v>127</v>
+      </c>
+      <c r="D15" s="23">
+        <v>-57</v>
+      </c>
       <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="7"/>
+      <c r="F15" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="B16" s="18">
+        <v>56</v>
+      </c>
+      <c r="C16" s="18">
+        <v>173</v>
+      </c>
+      <c r="D16" s="18">
+        <v>-117</v>
+      </c>
       <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="3"/>
+      <c r="F16" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="29"/>
+      <c r="B17" s="21">
+        <v>630</v>
+      </c>
+      <c r="C17" s="21">
+        <v>344</v>
+      </c>
+      <c r="D17" s="21">
+        <v>286</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F17" s="29"/>
-      <c r="G17" s="5"/>
+      <c r="G17" s="5" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="28"/>
+      <c r="B18" s="18">
+        <v>99</v>
+      </c>
+      <c r="C18" s="18">
+        <v>70</v>
+      </c>
+      <c r="D18" s="18">
+        <v>29</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F18" s="28"/>
-      <c r="G18" s="3"/>
+      <c r="G18" s="3" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
+      <c r="B19" s="21">
+        <v>407</v>
+      </c>
+      <c r="C19" s="21">
+        <v>410</v>
+      </c>
+      <c r="D19" s="21">
+        <v>-3</v>
+      </c>
       <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="5"/>
+      <c r="F19" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+      <c r="B20" s="18">
+        <v>2</v>
+      </c>
+      <c r="C20" s="18">
+        <v>37</v>
+      </c>
+      <c r="D20" s="18">
+        <v>-35</v>
+      </c>
       <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="3"/>
+      <c r="F20" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="29"/>
+      <c r="B21" s="21">
+        <v>416</v>
+      </c>
+      <c r="C21" s="21">
+        <v>332</v>
+      </c>
+      <c r="D21" s="21">
+        <v>84</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F21" s="29"/>
-      <c r="G21" s="5"/>
+      <c r="G21" s="5" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="B22" s="18">
+        <v>82</v>
+      </c>
+      <c r="C22" s="18">
+        <v>236</v>
+      </c>
+      <c r="D22" s="18">
+        <v>-154</v>
+      </c>
       <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="3"/>
+      <c r="F22" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
+      <c r="B23" s="21">
+        <v>614</v>
+      </c>
+      <c r="C23" s="21">
+        <v>634</v>
+      </c>
+      <c r="D23" s="21">
+        <v>-20</v>
+      </c>
       <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="5"/>
+      <c r="F23" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="28"/>
+      <c r="B24" s="18">
+        <v>1640</v>
+      </c>
+      <c r="C24" s="18">
+        <v>1236</v>
+      </c>
+      <c r="D24" s="18">
+        <v>404</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F24" s="28"/>
-      <c r="G24" s="3"/>
+      <c r="G24" s="3" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
+      <c r="B25" s="21">
+        <v>138</v>
+      </c>
+      <c r="C25" s="21">
+        <v>321</v>
+      </c>
+      <c r="D25" s="21">
+        <v>-183</v>
+      </c>
       <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="5"/>
+      <c r="F25" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
+      <c r="B26" s="18">
+        <v>0</v>
+      </c>
+      <c r="C26" s="18">
+        <v>0</v>
+      </c>
+      <c r="D26" s="18">
+        <v>0</v>
+      </c>
       <c r="E26" s="28"/>
       <c r="F26" s="28"/>
       <c r="G26" s="3"/>
@@ -6130,309 +6393,589 @@
       <c r="A27" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
+      <c r="B27" s="21">
+        <v>177</v>
+      </c>
+      <c r="C27" s="21">
+        <v>189</v>
+      </c>
+      <c r="D27" s="21">
+        <v>-12</v>
+      </c>
       <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="5"/>
+      <c r="F27" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
+      <c r="B28" s="18">
+        <v>91</v>
+      </c>
+      <c r="C28" s="18">
+        <v>92</v>
+      </c>
+      <c r="D28" s="18">
+        <v>-1</v>
+      </c>
       <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="3"/>
+      <c r="F28" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="29"/>
+      <c r="B29" s="21">
+        <v>671</v>
+      </c>
+      <c r="C29" s="21">
+        <v>488</v>
+      </c>
+      <c r="D29" s="21">
+        <v>183</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F29" s="29"/>
-      <c r="G29" s="5"/>
+      <c r="G29" s="5" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="28"/>
+      <c r="B30" s="18">
+        <v>51</v>
+      </c>
+      <c r="C30" s="18">
+        <v>16</v>
+      </c>
+      <c r="D30" s="18">
+        <v>35</v>
+      </c>
+      <c r="E30" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F30" s="28"/>
-      <c r="G30" s="3"/>
+      <c r="G30" s="3" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
+      <c r="B31" s="21">
+        <v>67</v>
+      </c>
+      <c r="C31" s="21">
+        <v>234</v>
+      </c>
+      <c r="D31" s="21">
+        <v>-167</v>
+      </c>
       <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="5"/>
+      <c r="F31" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="B32" s="18">
+        <v>471</v>
+      </c>
+      <c r="C32" s="18">
+        <v>499</v>
+      </c>
+      <c r="D32" s="18">
+        <v>-28</v>
+      </c>
       <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="3"/>
+      <c r="F32" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="29"/>
+      <c r="B33" s="21">
+        <v>314</v>
+      </c>
+      <c r="C33" s="21">
+        <v>277</v>
+      </c>
+      <c r="D33" s="21">
+        <v>37</v>
+      </c>
+      <c r="E33" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F33" s="29"/>
-      <c r="G33" s="5"/>
+      <c r="G33" s="5" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="28"/>
+      <c r="B34" s="18">
+        <v>154</v>
+      </c>
+      <c r="C34" s="18">
+        <v>84</v>
+      </c>
+      <c r="D34" s="18">
+        <v>70</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F34" s="28"/>
-      <c r="G34" s="3"/>
+      <c r="G34" s="3" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
+      <c r="B35" s="21">
+        <v>940</v>
+      </c>
+      <c r="C35" s="21">
+        <v>1226</v>
+      </c>
+      <c r="D35" s="21">
+        <v>-286</v>
+      </c>
       <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="5"/>
+      <c r="F35" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="B36" s="18">
+        <v>136</v>
+      </c>
+      <c r="C36" s="18">
+        <v>566</v>
+      </c>
+      <c r="D36" s="18">
+        <v>-430</v>
+      </c>
       <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="3"/>
+      <c r="F36" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="29"/>
+      <c r="B37" s="21">
+        <v>426</v>
+      </c>
+      <c r="C37" s="21">
+        <v>363</v>
+      </c>
+      <c r="D37" s="21">
+        <v>63</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F37" s="29"/>
-      <c r="G37" s="5"/>
+      <c r="G37" s="5" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
+      <c r="B38" s="18">
+        <v>18</v>
+      </c>
+      <c r="C38" s="18">
+        <v>115</v>
+      </c>
+      <c r="D38" s="18">
+        <v>-97</v>
+      </c>
       <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="3"/>
+      <c r="F38" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="B39" s="21"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
+        <v>44</v>
+      </c>
+      <c r="B39" s="21">
+        <v>11</v>
+      </c>
+      <c r="C39" s="21">
+        <v>44</v>
+      </c>
+      <c r="D39" s="21">
+        <v>-33</v>
+      </c>
       <c r="E39" s="29"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="5"/>
+      <c r="F39" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="B40" s="42"/>
-      <c r="C40" s="42"/>
-      <c r="D40" s="42"/>
+        <v>45</v>
+      </c>
+      <c r="B40" s="42">
+        <v>68</v>
+      </c>
+      <c r="C40" s="42">
+        <v>110</v>
+      </c>
+      <c r="D40" s="42">
+        <v>-42</v>
+      </c>
       <c r="E40" s="39"/>
-      <c r="F40" s="39"/>
-      <c r="G40" s="40"/>
+      <c r="F40" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="G40" s="40" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
+        <v>46</v>
+      </c>
+      <c r="B41" s="25">
+        <v>6</v>
+      </c>
+      <c r="C41" s="25">
+        <v>13</v>
+      </c>
+      <c r="D41" s="25">
+        <v>-7</v>
+      </c>
       <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="9"/>
+      <c r="F41" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" s="42"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="42"/>
+        <v>47</v>
+      </c>
+      <c r="B42" s="42">
+        <v>12</v>
+      </c>
+      <c r="C42" s="42">
+        <v>45</v>
+      </c>
+      <c r="D42" s="42">
+        <v>-33</v>
+      </c>
       <c r="E42" s="39"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="40"/>
+      <c r="F42" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="G42" s="40" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="31"/>
+        <v>48</v>
+      </c>
+      <c r="B43" s="25">
+        <v>139</v>
+      </c>
+      <c r="C43" s="25">
+        <v>79</v>
+      </c>
+      <c r="D43" s="25">
+        <v>60</v>
+      </c>
+      <c r="E43" s="31" t="s">
+        <v>60</v>
+      </c>
       <c r="F43" s="31"/>
-      <c r="G43" s="9"/>
+      <c r="G43" s="9" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
+      <c r="B44" s="18">
+        <v>50</v>
+      </c>
+      <c r="C44" s="18">
+        <v>151</v>
+      </c>
+      <c r="D44" s="18">
+        <v>-101</v>
+      </c>
       <c r="E44" s="28"/>
-      <c r="F44" s="28"/>
-      <c r="G44" s="3"/>
+      <c r="F44" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="21"/>
-      <c r="C45" s="21"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="29"/>
+      <c r="B45" s="21">
+        <v>458</v>
+      </c>
+      <c r="C45" s="21">
+        <v>446</v>
+      </c>
+      <c r="D45" s="21">
+        <v>12</v>
+      </c>
+      <c r="E45" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F45" s="29"/>
-      <c r="G45" s="5"/>
+      <c r="G45" s="5" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="28"/>
+      <c r="B46" s="18">
+        <v>935</v>
+      </c>
+      <c r="C46" s="18">
+        <v>642</v>
+      </c>
+      <c r="D46" s="18">
+        <v>293</v>
+      </c>
+      <c r="E46" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F46" s="28"/>
-      <c r="G46" s="3"/>
+      <c r="G46" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="21"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
+      <c r="B47" s="21">
+        <v>221</v>
+      </c>
+      <c r="C47" s="21">
+        <v>590</v>
+      </c>
+      <c r="D47" s="21">
+        <v>-369</v>
+      </c>
       <c r="E47" s="29"/>
-      <c r="F47" s="29"/>
-      <c r="G47" s="5"/>
+      <c r="F47" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="28"/>
+      <c r="B48" s="18">
+        <v>500</v>
+      </c>
+      <c r="C48" s="18">
+        <v>225</v>
+      </c>
+      <c r="D48" s="18">
+        <v>275</v>
+      </c>
+      <c r="E48" s="28" t="s">
+        <v>60</v>
+      </c>
       <c r="F48" s="28"/>
-      <c r="G48" s="3"/>
+      <c r="G48" s="3" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="21"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="29"/>
+      <c r="B49" s="21">
+        <v>774</v>
+      </c>
+      <c r="C49" s="21">
+        <v>518</v>
+      </c>
+      <c r="D49" s="21">
+        <v>256</v>
+      </c>
+      <c r="E49" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F49" s="29"/>
-      <c r="G49" s="5"/>
+      <c r="G49" s="5" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="18"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
+      <c r="B50" s="18">
+        <v>98</v>
+      </c>
+      <c r="C50" s="18">
+        <v>137</v>
+      </c>
+      <c r="D50" s="18">
+        <v>-39</v>
+      </c>
       <c r="E50" s="28"/>
-      <c r="F50" s="28"/>
-      <c r="G50" s="3"/>
+      <c r="F50" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="21"/>
-      <c r="C51" s="21"/>
-      <c r="D51" s="21"/>
-      <c r="E51" s="29"/>
+      <c r="B51" s="21">
+        <v>734</v>
+      </c>
+      <c r="C51" s="21">
+        <v>329</v>
+      </c>
+      <c r="D51" s="21">
+        <v>405</v>
+      </c>
+      <c r="E51" s="29" t="s">
+        <v>60</v>
+      </c>
       <c r="F51" s="29"/>
-      <c r="G51" s="5"/>
+      <c r="G51" s="5" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="18"/>
-      <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
+      <c r="B52" s="18">
+        <v>92</v>
+      </c>
+      <c r="C52" s="18">
+        <v>166</v>
+      </c>
+      <c r="D52" s="18">
+        <v>-74</v>
+      </c>
       <c r="E52" s="28"/>
-      <c r="F52" s="28"/>
-      <c r="G52" s="3"/>
+      <c r="F52" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="21"/>
-      <c r="C53" s="21"/>
-      <c r="D53" s="21"/>
+      <c r="B53" s="21">
+        <v>54</v>
+      </c>
+      <c r="C53" s="21">
+        <v>280</v>
+      </c>
+      <c r="D53" s="21">
+        <v>-226</v>
+      </c>
       <c r="E53" s="29"/>
-      <c r="F53" s="29"/>
-      <c r="G53" s="5"/>
+      <c r="F53" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="B54" s="27"/>
-      <c r="C54" s="27"/>
-      <c r="D54" s="27"/>
-      <c r="E54" s="32"/>
+      <c r="B54" s="27">
+        <v>364</v>
+      </c>
+      <c r="C54" s="27">
+        <v>183</v>
+      </c>
+      <c r="D54" s="27">
+        <v>181</v>
+      </c>
+      <c r="E54" s="32" t="s">
+        <v>60</v>
+      </c>
       <c r="F54" s="32"/>
-      <c r="G54" s="11"/>
+      <c r="G54" s="11" t="s">
+        <v>266</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G54" xr:uid="{00000000-0009-0000-0000-00000C000000}"/>
@@ -6480,7 +7023,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A40" sqref="A40"/>
       <selection pane="topRight" activeCell="A40" sqref="A40"/>
@@ -6526,15 +7069,15 @@
       </c>
       <c r="B2" s="2">
         <f>January!B2+February!B2+March!B2+April!B2+May!B2+June!B2+July!B2+August!B2+September!B2+October!B2+November!B2+December!B2</f>
-        <v>16452</v>
+        <v>17661</v>
       </c>
       <c r="C2" s="2">
         <f>January!C2+February!C2+March!C2+April!C2+May!C2+June!C2+July!C2+August!C2+September!C2+October!C2+November!C2+December!C2</f>
-        <v>13751</v>
+        <v>14845</v>
       </c>
       <c r="D2" s="2">
         <f>January!D2+February!D2+March!D2+April!D2+May!D2+June!D2+July!D2+August!D2+September!D2+October!D2+November!D2+December!D2</f>
-        <v>2701</v>
+        <v>2816</v>
       </c>
       <c r="E2" s="28" t="str">
         <f t="shared" ref="E2:E33" si="0">IF(D2 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -6546,7 +7089,7 @@
       </c>
       <c r="G2" s="3" t="str">
         <f t="shared" ref="G2:G33" si="2">IF(ISERROR(ROUND(B2/C2,2)&amp;" : 1"), "", ROUND(B2/C2,2)&amp;" : 1")</f>
-        <v>1.2 : 1</v>
+        <v>1.19 : 1</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6555,15 +7098,15 @@
       </c>
       <c r="B3" s="4">
         <f>January!B3+February!B3+March!B3+April!B3+May!B3+June!B3+July!B3+August!B3+September!B3+October!B3+November!B3+December!B3</f>
-        <v>6945</v>
+        <v>7451</v>
       </c>
       <c r="C3" s="4">
         <f>January!C3+February!C3+March!C3+April!C3+May!C3+June!C3+July!C3+August!C3+September!C3+October!C3+November!C3+December!C3</f>
-        <v>3947</v>
+        <v>4227</v>
       </c>
       <c r="D3" s="4">
         <f>January!D3+February!D3+March!D3+April!D3+May!D3+June!D3+July!D3+August!D3+September!D3+October!D3+November!D3+December!D3</f>
-        <v>2998</v>
+        <v>3224</v>
       </c>
       <c r="E3" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6584,15 +7127,15 @@
       </c>
       <c r="B4" s="2">
         <f>January!B4+February!B4+March!B4+April!B4+May!B4+June!B4+July!B4+August!B4+September!B4+October!B4+November!B4+December!B4</f>
-        <v>12309</v>
+        <v>13374</v>
       </c>
       <c r="C4" s="2">
         <f>January!C4+February!C4+March!C4+April!C4+May!C4+June!C4+July!C4+August!C4+September!C4+October!C4+November!C4+December!C4</f>
-        <v>12753</v>
+        <v>13900</v>
       </c>
       <c r="D4" s="2">
         <f>January!D4+February!D4+March!D4+April!D4+May!D4+June!D4+July!D4+August!D4+September!D4+October!D4+November!D4+December!D4</f>
-        <v>-444</v>
+        <v>-526</v>
       </c>
       <c r="E4" s="28" t="str">
         <f t="shared" si="0"/>
@@ -6604,7 +7147,7 @@
       </c>
       <c r="G4" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.97 : 1</v>
+        <v>0.96 : 1</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6613,15 +7156,15 @@
       </c>
       <c r="B5" s="4">
         <f>January!B5+February!B5+March!B5+April!B5+May!B5+June!B5+July!B5+August!B5+September!B5+October!B5+November!B5+December!B5</f>
-        <v>355</v>
+        <v>410</v>
       </c>
       <c r="C5" s="4">
         <f>January!C5+February!C5+March!C5+April!C5+May!C5+June!C5+July!C5+August!C5+September!C5+October!C5+November!C5+December!C5</f>
-        <v>1333</v>
+        <v>1500</v>
       </c>
       <c r="D5" s="4">
         <f>January!D5+February!D5+March!D5+April!D5+May!D5+June!D5+July!D5+August!D5+September!D5+October!D5+November!D5+December!D5</f>
-        <v>-978</v>
+        <v>-1090</v>
       </c>
       <c r="E5" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6642,15 +7185,15 @@
       </c>
       <c r="B6" s="2">
         <f>January!B6+February!B6+March!B6+April!B6+May!B6+June!B6+July!B6+August!B6+September!B6+October!B6+November!B6+December!B6</f>
-        <v>11798</v>
+        <v>12705</v>
       </c>
       <c r="C6" s="2">
         <f>January!C6+February!C6+March!C6+April!C6+May!C6+June!C6+July!C6+August!C6+September!C6+October!C6+November!C6+December!C6</f>
-        <v>13086</v>
+        <v>14130</v>
       </c>
       <c r="D6" s="2">
         <f>January!D6+February!D6+March!D6+April!D6+May!D6+June!D6+July!D6+August!D6+September!D6+October!D6+November!D6+December!D6</f>
-        <v>-1288</v>
+        <v>-1425</v>
       </c>
       <c r="E6" s="28" t="str">
         <f t="shared" si="0"/>
@@ -6671,15 +7214,15 @@
       </c>
       <c r="B7" s="4">
         <f>January!B7+February!B7+March!B7+April!B7+May!B7+June!B7+July!B7+August!B7+September!B7+October!B7+November!B7+December!B7</f>
-        <v>2407</v>
+        <v>2597</v>
       </c>
       <c r="C7" s="4">
         <f>January!C7+February!C7+March!C7+April!C7+May!C7+June!C7+July!C7+August!C7+September!C7+October!C7+November!C7+December!C7</f>
-        <v>1875</v>
+        <v>2021</v>
       </c>
       <c r="D7" s="4">
         <f>January!D7+February!D7+March!D7+April!D7+May!D7+June!D7+July!D7+August!D7+September!D7+October!D7+November!D7+December!D7</f>
-        <v>532</v>
+        <v>576</v>
       </c>
       <c r="E7" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6691,7 +7234,7 @@
       </c>
       <c r="G7" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.28 : 1</v>
+        <v>1.29 : 1</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6700,15 +7243,15 @@
       </c>
       <c r="B8" s="2">
         <f>January!B8+February!B8+March!B8+April!B8+May!B8+June!B8+July!B8+August!B8+September!B8+October!B8+November!B8+December!B8</f>
-        <v>1696</v>
+        <v>1772</v>
       </c>
       <c r="C8" s="2">
         <f>January!C8+February!C8+March!C8+April!C8+May!C8+June!C8+July!C8+August!C8+September!C8+October!C8+November!C8+December!C8</f>
-        <v>1915</v>
+        <v>2061</v>
       </c>
       <c r="D8" s="2">
         <f>January!D8+February!D8+March!D8+April!D8+May!D8+June!D8+July!D8+August!D8+September!D8+October!D8+November!D8+December!D8</f>
-        <v>-219</v>
+        <v>-289</v>
       </c>
       <c r="E8" s="28" t="str">
         <f t="shared" si="0"/>
@@ -6720,7 +7263,7 @@
       </c>
       <c r="G8" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.89 : 1</v>
+        <v>0.86 : 1</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6729,15 +7272,15 @@
       </c>
       <c r="B9" s="4">
         <f>January!B9+February!B9+March!B9+April!B9+May!B9+June!B9+July!B9+August!B9+September!B9+October!B9+November!B9+December!B9</f>
-        <v>676</v>
+        <v>758</v>
       </c>
       <c r="C9" s="4">
         <f>January!C9+February!C9+March!C9+April!C9+May!C9+June!C9+July!C9+August!C9+September!C9+October!C9+November!C9+December!C9</f>
-        <v>736</v>
+        <v>796</v>
       </c>
       <c r="D9" s="4">
         <f>January!D9+February!D9+March!D9+April!D9+May!D9+June!D9+July!D9+August!D9+September!D9+October!D9+November!D9+December!D9</f>
-        <v>-60</v>
+        <v>-38</v>
       </c>
       <c r="E9" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6749,7 +7292,7 @@
       </c>
       <c r="G9" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>0.92 : 1</v>
+        <v>0.95 : 1</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6762,11 +7305,11 @@
       </c>
       <c r="C10" s="2">
         <f>January!C10+February!C10+March!C10+April!C10+May!C10+June!C10+July!C10+August!C10+September!C10+October!C10+November!C10+December!C10</f>
-        <v>427</v>
+        <v>459</v>
       </c>
       <c r="D10" s="2">
         <f>January!D10+February!D10+March!D10+April!D10+May!D10+June!D10+July!D10+August!D10+September!D10+October!D10+November!D10+December!D10</f>
-        <v>-422</v>
+        <v>-454</v>
       </c>
       <c r="E10" s="28" t="str">
         <f t="shared" si="0"/>
@@ -6816,15 +7359,15 @@
       </c>
       <c r="B12" s="34">
         <f>January!B12+February!B12+March!B12+April!B12+May!B12+June!B12+July!B12+August!B12+September!B12+October!B12+November!B12+December!B12</f>
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="C12" s="34">
         <f>January!C12+February!C12+March!C12+April!C12+May!C12+June!C12+July!C12+August!C12+September!C12+October!C12+November!C12+December!C12</f>
-        <v>176</v>
+        <v>200</v>
       </c>
       <c r="D12" s="34">
         <f>January!D12+February!D12+March!D12+April!D12+May!D12+June!D12+July!D12+August!D12+September!D12+October!D12+November!D12+December!D12</f>
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="E12" s="35" t="str">
         <f t="shared" si="0"/>
@@ -6836,7 +7379,7 @@
       </c>
       <c r="G12" s="36" t="str">
         <f t="shared" si="2"/>
-        <v>1.69 : 1</v>
+        <v>1.51 : 1</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6845,15 +7388,15 @@
       </c>
       <c r="B13" s="6">
         <f>January!B13+February!B13+March!B13+April!B13+May!B13+June!B13+July!B13+August!B13+September!B13+October!B13+November!B13+December!B13</f>
-        <v>860</v>
+        <v>915</v>
       </c>
       <c r="C13" s="6">
         <f>January!C13+February!C13+March!C13+April!C13+May!C13+June!C13+July!C13+August!C13+September!C13+October!C13+November!C13+December!C13</f>
-        <v>802</v>
+        <v>846</v>
       </c>
       <c r="D13" s="6">
         <f>January!D13+February!D13+March!D13+April!D13+May!D13+June!D13+July!D13+August!D13+September!D13+October!D13+November!D13+December!D13</f>
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="E13" s="30" t="str">
         <f t="shared" si="0"/>
@@ -6865,7 +7408,7 @@
       </c>
       <c r="G13" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>1.07 : 1</v>
+        <v>1.08 : 1</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6874,15 +7417,15 @@
       </c>
       <c r="B14" s="34">
         <f>January!B14+February!B14+March!B14+April!B14+May!B14+June!B14+July!B14+August!B14+September!B14+October!B14+November!B14+December!B14</f>
-        <v>2034</v>
+        <v>2154</v>
       </c>
       <c r="C14" s="34">
         <f>January!C14+February!C14+March!C14+April!C14+May!C14+June!C14+July!C14+August!C14+September!C14+October!C14+November!C14+December!C14</f>
-        <v>2651</v>
+        <v>2895</v>
       </c>
       <c r="D14" s="34">
         <f>January!D14+February!D14+March!D14+April!D14+May!D14+June!D14+July!D14+August!D14+September!D14+October!D14+November!D14+December!D14</f>
-        <v>-617</v>
+        <v>-741</v>
       </c>
       <c r="E14" s="35" t="str">
         <f t="shared" si="0"/>
@@ -6894,7 +7437,7 @@
       </c>
       <c r="G14" s="36" t="str">
         <f t="shared" si="2"/>
-        <v>0.77 : 1</v>
+        <v>0.74 : 1</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6903,15 +7446,15 @@
       </c>
       <c r="B15" s="6">
         <f>January!B15+February!B15+March!B15+April!B15+May!B15+June!B15+July!B15+August!B15+September!B15+October!B15+November!B15+December!B15</f>
-        <v>659</v>
+        <v>729</v>
       </c>
       <c r="C15" s="6">
         <f>January!C15+February!C15+March!C15+April!C15+May!C15+June!C15+July!C15+August!C15+September!C15+October!C15+November!C15+December!C15</f>
-        <v>1572</v>
+        <v>1699</v>
       </c>
       <c r="D15" s="6">
         <f>January!D15+February!D15+March!D15+April!D15+May!D15+June!D15+July!D15+August!D15+September!D15+October!D15+November!D15+December!D15</f>
-        <v>-913</v>
+        <v>-970</v>
       </c>
       <c r="E15" s="30" t="str">
         <f t="shared" si="0"/>
@@ -6923,7 +7466,7 @@
       </c>
       <c r="G15" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>0.42 : 1</v>
+        <v>0.43 : 1</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6932,15 +7475,15 @@
       </c>
       <c r="B16" s="2">
         <f>January!B16+February!B16+March!B16+April!B16+May!B16+June!B16+July!B16+August!B16+September!B16+October!B16+November!B16+December!B16</f>
-        <v>749</v>
+        <v>805</v>
       </c>
       <c r="C16" s="2">
         <f>January!C16+February!C16+March!C16+April!C16+May!C16+June!C16+July!C16+August!C16+September!C16+October!C16+November!C16+December!C16</f>
-        <v>1848</v>
+        <v>2021</v>
       </c>
       <c r="D16" s="2">
         <f>January!D16+February!D16+March!D16+April!D16+May!D16+June!D16+July!D16+August!D16+September!D16+October!D16+November!D16+December!D16</f>
-        <v>-1099</v>
+        <v>-1216</v>
       </c>
       <c r="E16" s="28" t="str">
         <f t="shared" si="0"/>
@@ -6952,7 +7495,7 @@
       </c>
       <c r="G16" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.41 : 1</v>
+        <v>0.4 : 1</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6961,15 +7504,15 @@
       </c>
       <c r="B17" s="4">
         <f>January!B17+February!B17+March!B17+April!B17+May!B17+June!B17+July!B17+August!B17+September!B17+October!B17+November!B17+December!B17</f>
-        <v>6818</v>
+        <v>7448</v>
       </c>
       <c r="C17" s="4">
         <f>January!C17+February!C17+March!C17+April!C17+May!C17+June!C17+July!C17+August!C17+September!C17+October!C17+November!C17+December!C17</f>
-        <v>5021</v>
+        <v>5365</v>
       </c>
       <c r="D17" s="4">
         <f>January!D17+February!D17+March!D17+April!D17+May!D17+June!D17+July!D17+August!D17+September!D17+October!D17+November!D17+December!D17</f>
-        <v>1797</v>
+        <v>2083</v>
       </c>
       <c r="E17" s="29" t="str">
         <f t="shared" si="0"/>
@@ -6981,7 +7524,7 @@
       </c>
       <c r="G17" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.36 : 1</v>
+        <v>1.39 : 1</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6990,15 +7533,15 @@
       </c>
       <c r="B18" s="2">
         <f>January!B18+February!B18+March!B18+April!B18+May!B18+June!B18+July!B18+August!B18+September!B18+October!B18+November!B18+December!B18</f>
-        <v>641</v>
+        <v>740</v>
       </c>
       <c r="C18" s="2">
         <f>January!C18+February!C18+March!C18+April!C18+May!C18+June!C18+July!C18+August!C18+September!C18+October!C18+November!C18+December!C18</f>
-        <v>1042</v>
+        <v>1112</v>
       </c>
       <c r="D18" s="2">
         <f>January!D18+February!D18+March!D18+April!D18+May!D18+June!D18+July!D18+August!D18+September!D18+October!D18+November!D18+December!D18</f>
-        <v>-401</v>
+        <v>-372</v>
       </c>
       <c r="E18" s="28" t="str">
         <f t="shared" si="0"/>
@@ -7010,7 +7553,7 @@
       </c>
       <c r="G18" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.62 : 1</v>
+        <v>0.67 : 1</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7019,15 +7562,15 @@
       </c>
       <c r="B19" s="4">
         <f>January!B19+February!B19+March!B19+April!B19+May!B19+June!B19+July!B19+August!B19+September!B19+October!B19+November!B19+December!B19</f>
-        <v>5090</v>
+        <v>5497</v>
       </c>
       <c r="C19" s="4">
         <f>January!C19+February!C19+March!C19+April!C19+May!C19+June!C19+July!C19+August!C19+September!C19+October!C19+November!C19+December!C19</f>
-        <v>4713</v>
+        <v>5123</v>
       </c>
       <c r="D19" s="4">
         <f>January!D19+February!D19+March!D19+April!D19+May!D19+June!D19+July!D19+August!D19+September!D19+October!D19+November!D19+December!D19</f>
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="E19" s="29" t="str">
         <f t="shared" si="0"/>
@@ -7039,7 +7582,7 @@
       </c>
       <c r="G19" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.08 : 1</v>
+        <v>1.07 : 1</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7048,15 +7591,15 @@
       </c>
       <c r="B20" s="2">
         <f>January!B20+February!B20+March!B20+April!B20+May!B20+June!B20+July!B20+August!B20+September!B20+October!B20+November!B20+December!B20</f>
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C20" s="2">
         <f>January!C20+February!C20+March!C20+April!C20+May!C20+June!C20+July!C20+August!C20+September!C20+October!C20+November!C20+December!C20</f>
-        <v>581</v>
+        <v>618</v>
       </c>
       <c r="D20" s="2">
         <f>January!D20+February!D20+March!D20+April!D20+May!D20+June!D20+July!D20+August!D20+September!D20+October!D20+November!D20+December!D20</f>
-        <v>-390</v>
+        <v>-425</v>
       </c>
       <c r="E20" s="28" t="str">
         <f t="shared" si="0"/>
@@ -7068,7 +7611,7 @@
       </c>
       <c r="G20" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.33 : 1</v>
+        <v>0.31 : 1</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7077,15 +7620,15 @@
       </c>
       <c r="B21" s="4">
         <f>January!B21+February!B21+March!B21+April!B21+May!B21+June!B21+July!B21+August!B21+September!B21+October!B21+November!B21+December!B21</f>
-        <v>5479</v>
+        <v>5895</v>
       </c>
       <c r="C21" s="4">
         <f>January!C21+February!C21+March!C21+April!C21+May!C21+June!C21+July!C21+August!C21+September!C21+October!C21+November!C21+December!C21</f>
-        <v>3836</v>
+        <v>4168</v>
       </c>
       <c r="D21" s="4">
         <f>January!D21+February!D21+March!D21+April!D21+May!D21+June!D21+July!D21+August!D21+September!D21+October!D21+November!D21+December!D21</f>
-        <v>1643</v>
+        <v>1727</v>
       </c>
       <c r="E21" s="29" t="str">
         <f t="shared" si="0"/>
@@ -7097,7 +7640,7 @@
       </c>
       <c r="G21" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.43 : 1</v>
+        <v>1.41 : 1</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7106,15 +7649,15 @@
       </c>
       <c r="B22" s="2">
         <f>January!B22+February!B22+March!B22+April!B22+May!B22+June!B22+July!B22+August!B22+September!B22+October!B22+November!B22+December!B22</f>
-        <v>750</v>
+        <v>832</v>
       </c>
       <c r="C22" s="2">
         <f>January!C22+February!C22+March!C22+April!C22+May!C22+June!C22+July!C22+August!C22+September!C22+October!C22+November!C22+December!C22</f>
-        <v>2730</v>
+        <v>2966</v>
       </c>
       <c r="D22" s="2">
         <f>January!D22+February!D22+March!D22+April!D22+May!D22+June!D22+July!D22+August!D22+September!D22+October!D22+November!D22+December!D22</f>
-        <v>-1980</v>
+        <v>-2134</v>
       </c>
       <c r="E22" s="28" t="str">
         <f t="shared" si="0"/>
@@ -7126,7 +7669,7 @@
       </c>
       <c r="G22" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.27 : 1</v>
+        <v>0.28 : 1</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7135,15 +7678,15 @@
       </c>
       <c r="B23" s="4">
         <f>January!B23+February!B23+March!B23+April!B23+May!B23+June!B23+July!B23+August!B23+September!B23+October!B23+November!B23+December!B23</f>
-        <v>6944</v>
+        <v>7558</v>
       </c>
       <c r="C23" s="4">
         <f>January!C23+February!C23+March!C23+April!C23+May!C23+June!C23+July!C23+August!C23+September!C23+October!C23+November!C23+December!C23</f>
-        <v>6432</v>
+        <v>7066</v>
       </c>
       <c r="D23" s="4">
         <f>January!D23+February!D23+March!D23+April!D23+May!D23+June!D23+July!D23+August!D23+September!D23+October!D23+November!D23+December!D23</f>
-        <v>512</v>
+        <v>492</v>
       </c>
       <c r="E23" s="29" t="str">
         <f t="shared" si="0"/>
@@ -7155,7 +7698,7 @@
       </c>
       <c r="G23" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.08 : 1</v>
+        <v>1.07 : 1</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7164,15 +7707,15 @@
       </c>
       <c r="B24" s="2">
         <f>January!B24+February!B24+March!B24+April!B24+May!B24+June!B24+July!B24+August!B24+September!B24+October!B24+November!B24+December!B24</f>
-        <v>17947</v>
+        <v>19587</v>
       </c>
       <c r="C24" s="2">
         <f>January!C24+February!C24+March!C24+April!C24+May!C24+June!C24+July!C24+August!C24+September!C24+October!C24+November!C24+December!C24</f>
-        <v>12470</v>
+        <v>13706</v>
       </c>
       <c r="D24" s="2">
         <f>January!D24+February!D24+March!D24+April!D24+May!D24+June!D24+July!D24+August!D24+September!D24+October!D24+November!D24+December!D24</f>
-        <v>5477</v>
+        <v>5881</v>
       </c>
       <c r="E24" s="28" t="str">
         <f t="shared" si="0"/>
@@ -7184,7 +7727,7 @@
       </c>
       <c r="G24" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.44 : 1</v>
+        <v>1.43 : 1</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7193,15 +7736,15 @@
       </c>
       <c r="B25" s="4">
         <f>January!B25+February!B25+March!B25+April!B25+May!B25+June!B25+July!B25+August!B25+September!B25+October!B25+November!B25+December!B25</f>
-        <v>1597</v>
+        <v>1735</v>
       </c>
       <c r="C25" s="4">
         <f>January!C25+February!C25+March!C25+April!C25+May!C25+June!C25+July!C25+August!C25+September!C25+October!C25+November!C25+December!C25</f>
-        <v>4614</v>
+        <v>4935</v>
       </c>
       <c r="D25" s="4">
         <f>January!D25+February!D25+March!D25+April!D25+May!D25+June!D25+July!D25+August!D25+September!D25+October!D25+November!D25+December!D25</f>
-        <v>-3017</v>
+        <v>-3200</v>
       </c>
       <c r="E25" s="29" t="str">
         <f t="shared" si="0"/>
@@ -7251,15 +7794,15 @@
       </c>
       <c r="B27" s="4">
         <f>January!B27+February!B27+March!B27+April!B27+May!B27+June!B27+July!B27+August!B27+September!B27+October!B27+November!B27+December!B27</f>
-        <v>2273</v>
+        <v>2450</v>
       </c>
       <c r="C27" s="4">
         <f>January!C27+February!C27+March!C27+April!C27+May!C27+June!C27+July!C27+August!C27+September!C27+October!C27+November!C27+December!C27</f>
-        <v>1880</v>
+        <v>2069</v>
       </c>
       <c r="D27" s="4">
         <f>January!D27+February!D27+March!D27+April!D27+May!D27+June!D27+July!D27+August!D27+September!D27+October!D27+November!D27+December!D27</f>
-        <v>393</v>
+        <v>381</v>
       </c>
       <c r="E27" s="29" t="str">
         <f t="shared" si="0"/>
@@ -7271,7 +7814,7 @@
       </c>
       <c r="G27" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.21 : 1</v>
+        <v>1.18 : 1</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7280,15 +7823,15 @@
       </c>
       <c r="B28" s="2">
         <f>January!B28+February!B28+March!B28+April!B28+May!B28+June!B28+July!B28+August!B28+September!B28+October!B28+November!B28+December!B28</f>
-        <v>1369</v>
+        <v>1460</v>
       </c>
       <c r="C28" s="2">
         <f>January!C28+February!C28+March!C28+April!C28+May!C28+June!C28+July!C28+August!C28+September!C28+October!C28+November!C28+December!C28</f>
-        <v>1159</v>
+        <v>1251</v>
       </c>
       <c r="D28" s="2">
         <f>January!D28+February!D28+March!D28+April!D28+May!D28+June!D28+July!D28+August!D28+September!D28+October!D28+November!D28+December!D28</f>
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E28" s="28" t="str">
         <f t="shared" si="0"/>
@@ -7300,7 +7843,7 @@
       </c>
       <c r="G28" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.18 : 1</v>
+        <v>1.17 : 1</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7309,15 +7852,15 @@
       </c>
       <c r="B29" s="4">
         <f>January!B29+February!B29+March!B29+April!B29+May!B29+June!B29+July!B29+August!B29+September!B29+October!B29+November!B29+December!B29</f>
-        <v>7160</v>
+        <v>7831</v>
       </c>
       <c r="C29" s="4">
         <f>January!C29+February!C29+March!C29+April!C29+May!C29+June!C29+July!C29+August!C29+September!C29+October!C29+November!C29+December!C29</f>
-        <v>5143</v>
+        <v>5631</v>
       </c>
       <c r="D29" s="4">
         <f>January!D29+February!D29+March!D29+April!D29+May!D29+June!D29+July!D29+August!D29+September!D29+October!D29+November!D29+December!D29</f>
-        <v>2017</v>
+        <v>2200</v>
       </c>
       <c r="E29" s="29" t="str">
         <f t="shared" si="0"/>
@@ -7338,15 +7881,15 @@
       </c>
       <c r="B30" s="2">
         <f>January!B30+February!B30+March!B30+April!B30+May!B30+June!B30+July!B30+August!B30+September!B30+October!B30+November!B30+December!B30</f>
-        <v>380</v>
+        <v>431</v>
       </c>
       <c r="C30" s="2">
         <f>January!C30+February!C30+March!C30+April!C30+May!C30+June!C30+July!C30+August!C30+September!C30+October!C30+November!C30+December!C30</f>
-        <v>288</v>
+        <v>304</v>
       </c>
       <c r="D30" s="2">
         <f>January!D30+February!D30+March!D30+April!D30+May!D30+June!D30+July!D30+August!D30+September!D30+October!D30+November!D30+December!D30</f>
-        <v>92</v>
+        <v>127</v>
       </c>
       <c r="E30" s="28" t="str">
         <f t="shared" si="0"/>
@@ -7358,7 +7901,7 @@
       </c>
       <c r="G30" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>1.32 : 1</v>
+        <v>1.42 : 1</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7367,15 +7910,15 @@
       </c>
       <c r="B31" s="4">
         <f>January!B31+February!B31+March!B31+April!B31+May!B31+June!B31+July!B31+August!B31+September!B31+October!B31+November!B31+December!B31</f>
-        <v>775</v>
+        <v>842</v>
       </c>
       <c r="C31" s="4">
         <f>January!C31+February!C31+March!C31+April!C31+May!C31+June!C31+July!C31+August!C31+September!C31+October!C31+November!C31+December!C31</f>
-        <v>2749</v>
+        <v>2983</v>
       </c>
       <c r="D31" s="4">
         <f>January!D31+February!D31+March!D31+April!D31+May!D31+June!D31+July!D31+August!D31+September!D31+October!D31+November!D31+December!D31</f>
-        <v>-1974</v>
+        <v>-2141</v>
       </c>
       <c r="E31" s="29" t="str">
         <f t="shared" si="0"/>
@@ -7396,15 +7939,15 @@
       </c>
       <c r="B32" s="2">
         <f>January!B32+February!B32+March!B32+April!B32+May!B32+June!B32+July!B32+August!B32+September!B32+October!B32+November!B32+December!B32</f>
-        <v>4666</v>
+        <v>5137</v>
       </c>
       <c r="C32" s="2">
         <f>January!C32+February!C32+March!C32+April!C32+May!C32+June!C32+July!C32+August!C32+September!C32+October!C32+November!C32+December!C32</f>
-        <v>6115</v>
+        <v>6614</v>
       </c>
       <c r="D32" s="2">
         <f>January!D32+February!D32+March!D32+April!D32+May!D32+June!D32+July!D32+August!D32+September!D32+October!D32+November!D32+December!D32</f>
-        <v>-1449</v>
+        <v>-1477</v>
       </c>
       <c r="E32" s="28" t="str">
         <f t="shared" si="0"/>
@@ -7416,7 +7959,7 @@
       </c>
       <c r="G32" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>0.76 : 1</v>
+        <v>0.78 : 1</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7425,15 +7968,15 @@
       </c>
       <c r="B33" s="4">
         <f>January!B33+February!B33+March!B33+April!B33+May!B33+June!B33+July!B33+August!B33+September!B33+October!B33+November!B33+December!B33</f>
-        <v>4617</v>
+        <v>4931</v>
       </c>
       <c r="C33" s="4">
         <f>January!C33+February!C33+March!C33+April!C33+May!C33+June!C33+July!C33+August!C33+September!C33+October!C33+November!C33+December!C33</f>
-        <v>4525</v>
+        <v>4802</v>
       </c>
       <c r="D33" s="4">
         <f>January!D33+February!D33+March!D33+April!D33+May!D33+June!D33+July!D33+August!D33+September!D33+October!D33+November!D33+December!D33</f>
-        <v>92</v>
+        <v>129</v>
       </c>
       <c r="E33" s="29" t="str">
         <f t="shared" si="0"/>
@@ -7445,7 +7988,7 @@
       </c>
       <c r="G33" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>1.02 : 1</v>
+        <v>1.03 : 1</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7454,15 +7997,15 @@
       </c>
       <c r="B34" s="2">
         <f>January!B34+February!B34+March!B34+April!B34+May!B34+June!B34+July!B34+August!B34+September!B34+October!B34+November!B34+December!B34</f>
-        <v>2041</v>
+        <v>2195</v>
       </c>
       <c r="C34" s="2">
         <f>January!C34+February!C34+March!C34+April!C34+May!C34+June!C34+July!C34+August!C34+September!C34+October!C34+November!C34+December!C34</f>
-        <v>1611</v>
+        <v>1695</v>
       </c>
       <c r="D34" s="2">
         <f>January!D34+February!D34+March!D34+April!D34+May!D34+June!D34+July!D34+August!D34+September!D34+October!D34+November!D34+December!D34</f>
-        <v>430</v>
+        <v>500</v>
       </c>
       <c r="E34" s="28" t="str">
         <f t="shared" ref="E34:E54" si="3">IF(D34 &gt; 0, "We borrowed more than we lent this year", "")</f>
@@ -7474,7 +8017,7 @@
       </c>
       <c r="G34" s="3" t="str">
         <f t="shared" ref="G34:G54" si="5">IF(ISERROR(ROUND(B34/C34,2)&amp;" : 1"), "", ROUND(B34/C34,2)&amp;" : 1")</f>
-        <v>1.27 : 1</v>
+        <v>1.29 : 1</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7483,15 +8026,15 @@
       </c>
       <c r="B35" s="4">
         <f>January!B35+February!B35+March!B35+April!B35+May!B35+June!B35+July!B35+August!B35+September!B35+October!B35+November!B35+December!B35</f>
-        <v>11007</v>
+        <v>11947</v>
       </c>
       <c r="C35" s="4">
         <f>January!C35+February!C35+March!C35+April!C35+May!C35+June!C35+July!C35+August!C35+September!C35+October!C35+November!C35+December!C35</f>
-        <v>14343</v>
+        <v>15569</v>
       </c>
       <c r="D35" s="4">
         <f>January!D35+February!D35+March!D35+April!D35+May!D35+June!D35+July!D35+August!D35+September!D35+October!D35+November!D35+December!D35</f>
-        <v>-3336</v>
+        <v>-3622</v>
       </c>
       <c r="E35" s="29" t="str">
         <f t="shared" si="3"/>
@@ -7512,15 +8055,15 @@
       </c>
       <c r="B36" s="2">
         <f>January!B36+February!B36+March!B36+April!B36+May!B36+June!B36+July!B36+August!B36+September!B36+October!B36+November!B36+December!B36</f>
-        <v>1700</v>
+        <v>1836</v>
       </c>
       <c r="C36" s="2">
         <f>January!C36+February!C36+March!C36+April!C36+May!C36+June!C36+July!C36+August!C36+September!C36+October!C36+November!C36+December!C36</f>
-        <v>5832</v>
+        <v>6398</v>
       </c>
       <c r="D36" s="2">
         <f>January!D36+February!D36+March!D36+April!D36+May!D36+June!D36+July!D36+August!D36+September!D36+October!D36+November!D36+December!D36</f>
-        <v>-4132</v>
+        <v>-4562</v>
       </c>
       <c r="E36" s="28" t="str">
         <f t="shared" si="3"/>
@@ -7541,15 +8084,15 @@
       </c>
       <c r="B37" s="4">
         <f>January!B37+February!B37+March!B37+April!B37+May!B37+June!B37+July!B37+August!B37+September!B37+October!B37+November!B37+December!B37</f>
-        <v>5654</v>
+        <v>6080</v>
       </c>
       <c r="C37" s="4">
         <f>January!C37+February!C37+March!C37+April!C37+May!C37+June!C37+July!C37+August!C37+September!C37+October!C37+November!C37+December!C37</f>
-        <v>3475</v>
+        <v>3838</v>
       </c>
       <c r="D37" s="4">
         <f>January!D37+February!D37+March!D37+April!D37+May!D37+June!D37+July!D37+August!D37+September!D37+October!D37+November!D37+December!D37</f>
-        <v>2179</v>
+        <v>2242</v>
       </c>
       <c r="E37" s="29" t="str">
         <f t="shared" si="3"/>
@@ -7561,7 +8104,7 @@
       </c>
       <c r="G37" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>1.63 : 1</v>
+        <v>1.58 : 1</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7570,15 +8113,15 @@
       </c>
       <c r="B38" s="2">
         <f>January!B38+February!B38+March!B38+April!B38+May!B38+June!B38+July!B38+August!B38+September!B38+October!B38+November!B38+December!B38</f>
-        <v>267</v>
+        <v>285</v>
       </c>
       <c r="C38" s="2">
         <f>January!C38+February!C38+March!C38+April!C38+May!C38+June!C38+July!C38+August!C38+September!C38+October!C38+November!C38+December!C38</f>
-        <v>1985</v>
+        <v>2100</v>
       </c>
       <c r="D38" s="2">
         <f>January!D38+February!D38+March!D38+April!D38+May!D38+June!D38+July!D38+August!D38+September!D38+October!D38+November!D38+December!D38</f>
-        <v>-1718</v>
+        <v>-1815</v>
       </c>
       <c r="E38" s="28" t="str">
         <f t="shared" si="3"/>
@@ -7590,7 +8133,7 @@
       </c>
       <c r="G38" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.13 : 1</v>
+        <v>0.14 : 1</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7599,15 +8142,15 @@
       </c>
       <c r="B39" s="4">
         <f>January!B39+February!B39+March!B39+April!B39+May!B39+June!B39+July!B39+August!B39+September!B39+October!B39+November!B39+December!B39</f>
-        <v>353</v>
+        <v>364</v>
       </c>
       <c r="C39" s="4">
         <f>January!C39+February!C39+March!C39+April!C39+May!C39+June!C39+July!C39+August!C39+September!C39+October!C39+November!C39+December!C39</f>
-        <v>778</v>
+        <v>822</v>
       </c>
       <c r="D39" s="4">
         <f>January!D39+February!D39+March!D39+April!D39+May!D39+June!D39+July!D39+August!D39+September!D39+October!D39+November!D39+December!D39</f>
-        <v>-425</v>
+        <v>-458</v>
       </c>
       <c r="E39" s="29" t="str">
         <f t="shared" si="3"/>
@@ -7619,7 +8162,7 @@
       </c>
       <c r="G39" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.45 : 1</v>
+        <v>0.44 : 1</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7628,15 +8171,15 @@
       </c>
       <c r="B40" s="38">
         <f>January!B40+February!B40+March!B40+April!B40+May!B40+June!B40+July!B40+August!B40+September!B40+October!B40+November!B40+December!B40</f>
-        <v>417</v>
+        <v>485</v>
       </c>
       <c r="C40" s="38">
         <f>January!C40+February!C40+March!C40+April!C40+May!C40+June!C40+July!C40+August!C40+September!C40+October!C40+November!C40+December!C40</f>
-        <v>708</v>
+        <v>818</v>
       </c>
       <c r="D40" s="38">
         <f>January!D40+February!D40+March!D40+April!D40+May!D40+June!D40+July!D40+August!D40+September!D40+October!D40+November!D40+December!D40</f>
-        <v>-291</v>
+        <v>-333</v>
       </c>
       <c r="E40" s="39" t="str">
         <f t="shared" si="3"/>
@@ -7657,15 +8200,15 @@
       </c>
       <c r="B41" s="8">
         <f>January!B41+February!B41+March!B41+April!B41+May!B41+June!B41+July!B41+August!B41+September!B41+October!B41+November!B41+December!B41</f>
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="C41" s="8">
         <f>January!C41+February!C41+March!C41+April!C41+May!C41+June!C41+July!C41+August!C41+September!C41+October!C41+November!C41+December!C41</f>
-        <v>327</v>
+        <v>340</v>
       </c>
       <c r="D41" s="8">
         <f>January!D41+February!D41+March!D41+April!D41+May!D41+June!D41+July!D41+August!D41+September!D41+October!D41+November!D41+December!D41</f>
-        <v>-39</v>
+        <v>-46</v>
       </c>
       <c r="E41" s="31" t="str">
         <f t="shared" si="3"/>
@@ -7677,7 +8220,7 @@
       </c>
       <c r="G41" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0.88 : 1</v>
+        <v>0.86 : 1</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7686,15 +8229,15 @@
       </c>
       <c r="B42" s="38">
         <f>January!B42+February!B42+March!B42+April!B42+May!B42+June!B42+July!B42+August!B42+September!B42+October!B42+November!B42+December!B42</f>
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="C42" s="38">
         <f>January!C42+February!C42+March!C42+April!C42+May!C42+June!C42+July!C42+August!C42+September!C42+October!C42+November!C42+December!C42</f>
-        <v>314</v>
+        <v>359</v>
       </c>
       <c r="D42" s="38">
         <f>January!D42+February!D42+March!D42+April!D42+May!D42+June!D42+July!D42+August!D42+September!D42+October!D42+November!D42+December!D42</f>
-        <v>-232</v>
+        <v>-265</v>
       </c>
       <c r="E42" s="39" t="str">
         <f t="shared" si="3"/>
@@ -7715,15 +8258,15 @@
       </c>
       <c r="B43" s="8">
         <f>January!B43+February!B43+March!B43+April!B43+May!B43+June!B43+July!B43+August!B43+September!B43+October!B43+November!B43+December!B43</f>
-        <v>770</v>
+        <v>909</v>
       </c>
       <c r="C43" s="8">
         <f>January!C43+February!C43+March!C43+April!C43+May!C43+June!C43+July!C43+August!C43+September!C43+October!C43+November!C43+December!C43</f>
-        <v>932</v>
+        <v>1011</v>
       </c>
       <c r="D43" s="8">
         <f>January!D43+February!D43+March!D43+April!D43+May!D43+June!D43+July!D43+August!D43+September!D43+October!D43+November!D43+December!D43</f>
-        <v>-162</v>
+        <v>-102</v>
       </c>
       <c r="E43" s="31" t="str">
         <f t="shared" si="3"/>
@@ -7735,7 +8278,7 @@
       </c>
       <c r="G43" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>0.83 : 1</v>
+        <v>0.9 : 1</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7744,15 +8287,15 @@
       </c>
       <c r="B44" s="2">
         <f>January!B44+February!B44+March!B44+April!B44+May!B44+June!B44+July!B44+August!B44+September!B44+October!B44+November!B44+December!B44</f>
-        <v>666</v>
+        <v>716</v>
       </c>
       <c r="C44" s="2">
         <f>January!C44+February!C44+March!C44+April!C44+May!C44+June!C44+July!C44+August!C44+September!C44+October!C44+November!C44+December!C44</f>
-        <v>2158</v>
+        <v>2309</v>
       </c>
       <c r="D44" s="2">
         <f>January!D44+February!D44+March!D44+April!D44+May!D44+June!D44+July!D44+August!D44+September!D44+October!D44+November!D44+December!D44</f>
-        <v>-1492</v>
+        <v>-1593</v>
       </c>
       <c r="E44" s="28" t="str">
         <f t="shared" si="3"/>
@@ -7773,15 +8316,15 @@
       </c>
       <c r="B45" s="4">
         <f>January!B45+February!B45+March!B45+April!B45+May!B45+June!B45+July!B45+August!B45+September!B45+October!B45+November!B45+December!B45</f>
-        <v>6119</v>
+        <v>6577</v>
       </c>
       <c r="C45" s="4">
         <f>January!C45+February!C45+March!C45+April!C45+May!C45+June!C45+July!C45+August!C45+September!C45+October!C45+November!C45+December!C45</f>
-        <v>6077</v>
+        <v>6523</v>
       </c>
       <c r="D45" s="4">
         <f>January!D45+February!D45+March!D45+April!D45+May!D45+June!D45+July!D45+August!D45+September!D45+October!D45+November!D45+December!D45</f>
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E45" s="29" t="str">
         <f t="shared" si="3"/>
@@ -7802,15 +8345,15 @@
       </c>
       <c r="B46" s="2">
         <f>January!B46+February!B46+March!B46+April!B46+May!B46+June!B46+July!B46+August!B46+September!B46+October!B46+November!B46+December!B46</f>
-        <v>10984</v>
+        <v>11919</v>
       </c>
       <c r="C46" s="2">
         <f>January!C46+February!C46+March!C46+April!C46+May!C46+June!C46+July!C46+August!C46+September!C46+October!C46+November!C46+December!C46</f>
-        <v>7263</v>
+        <v>7905</v>
       </c>
       <c r="D46" s="2">
         <f>January!D46+February!D46+March!D46+April!D46+May!D46+June!D46+July!D46+August!D46+September!D46+October!D46+November!D46+December!D46</f>
-        <v>3721</v>
+        <v>4014</v>
       </c>
       <c r="E46" s="28" t="str">
         <f t="shared" si="3"/>
@@ -7831,15 +8374,15 @@
       </c>
       <c r="B47" s="4">
         <f>January!B47+February!B47+March!B47+April!B47+May!B47+June!B47+July!B47+August!B47+September!B47+October!B47+November!B47+December!B47</f>
-        <v>2335</v>
+        <v>2556</v>
       </c>
       <c r="C47" s="4">
         <f>January!C47+February!C47+March!C47+April!C47+May!C47+June!C47+July!C47+August!C47+September!C47+October!C47+November!C47+December!C47</f>
-        <v>6784</v>
+        <v>7374</v>
       </c>
       <c r="D47" s="4">
         <f>January!D47+February!D47+March!D47+April!D47+May!D47+June!D47+July!D47+August!D47+September!D47+October!D47+November!D47+December!D47</f>
-        <v>-4449</v>
+        <v>-4818</v>
       </c>
       <c r="E47" s="29" t="str">
         <f t="shared" si="3"/>
@@ -7851,7 +8394,7 @@
       </c>
       <c r="G47" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.34 : 1</v>
+        <v>0.35 : 1</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7860,15 +8403,15 @@
       </c>
       <c r="B48" s="2">
         <f>January!B48+February!B48+March!B48+April!B48+May!B48+June!B48+July!B48+August!B48+September!B48+October!B48+November!B48+December!B48</f>
-        <v>6354</v>
+        <v>6854</v>
       </c>
       <c r="C48" s="2">
         <f>January!C48+February!C48+March!C48+April!C48+May!C48+June!C48+July!C48+August!C48+September!C48+October!C48+November!C48+December!C48</f>
-        <v>2400</v>
+        <v>2625</v>
       </c>
       <c r="D48" s="2">
         <f>January!D48+February!D48+March!D48+April!D48+May!D48+June!D48+July!D48+August!D48+September!D48+October!D48+November!D48+December!D48</f>
-        <v>3954</v>
+        <v>4229</v>
       </c>
       <c r="E48" s="28" t="str">
         <f t="shared" si="3"/>
@@ -7880,7 +8423,7 @@
       </c>
       <c r="G48" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>2.65 : 1</v>
+        <v>2.61 : 1</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7889,15 +8432,15 @@
       </c>
       <c r="B49" s="4">
         <f>January!B49+February!B49+March!B49+April!B49+May!B49+June!B49+July!B49+August!B49+September!B49+October!B49+November!B49+December!B49</f>
-        <v>9827</v>
+        <v>10601</v>
       </c>
       <c r="C49" s="4">
         <f>January!C49+February!C49+March!C49+April!C49+May!C49+June!C49+July!C49+August!C49+September!C49+October!C49+November!C49+December!C49</f>
-        <v>6482</v>
+        <v>7000</v>
       </c>
       <c r="D49" s="4">
         <f>January!D49+February!D49+March!D49+April!D49+May!D49+June!D49+July!D49+August!D49+September!D49+October!D49+November!D49+December!D49</f>
-        <v>3345</v>
+        <v>3601</v>
       </c>
       <c r="E49" s="29" t="str">
         <f t="shared" si="3"/>
@@ -7909,7 +8452,7 @@
       </c>
       <c r="G49" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>1.52 : 1</v>
+        <v>1.51 : 1</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7918,15 +8461,15 @@
       </c>
       <c r="B50" s="2">
         <f>January!B50+February!B50+March!B50+April!B50+May!B50+June!B50+July!B50+August!B50+September!B50+October!B50+November!B50+December!B50</f>
-        <v>1722</v>
+        <v>1820</v>
       </c>
       <c r="C50" s="2">
         <f>January!C50+February!C50+March!C50+April!C50+May!C50+June!C50+July!C50+August!C50+September!C50+October!C50+November!C50+December!C50</f>
-        <v>1815</v>
+        <v>1952</v>
       </c>
       <c r="D50" s="2">
         <f>January!D50+February!D50+March!D50+April!D50+May!D50+June!D50+July!D50+August!D50+September!D50+October!D50+November!D50+December!D50</f>
-        <v>-93</v>
+        <v>-132</v>
       </c>
       <c r="E50" s="28" t="str">
         <f t="shared" si="3"/>
@@ -7938,7 +8481,7 @@
       </c>
       <c r="G50" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.95 : 1</v>
+        <v>0.93 : 1</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7947,15 +8490,15 @@
       </c>
       <c r="B51" s="4">
         <f>January!B51+February!B51+March!B51+April!B51+May!B51+June!B51+July!B51+August!B51+September!B51+October!B51+November!B51+December!B51</f>
-        <v>3806</v>
+        <v>4540</v>
       </c>
       <c r="C51" s="4">
         <f>January!C51+February!C51+March!C51+April!C51+May!C51+June!C51+July!C51+August!C51+September!C51+October!C51+November!C51+December!C51</f>
-        <v>4284</v>
+        <v>4613</v>
       </c>
       <c r="D51" s="4">
         <f>January!D51+February!D51+March!D51+April!D51+May!D51+June!D51+July!D51+August!D51+September!D51+October!D51+November!D51+December!D51</f>
-        <v>-478</v>
+        <v>-73</v>
       </c>
       <c r="E51" s="29" t="str">
         <f t="shared" si="3"/>
@@ -7967,7 +8510,7 @@
       </c>
       <c r="G51" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.89 : 1</v>
+        <v>0.98 : 1</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7976,15 +8519,15 @@
       </c>
       <c r="B52" s="2">
         <f>January!B52+February!B52+March!B52+April!B52+May!B52+June!B52+July!B52+August!B52+September!B52+October!B52+November!B52+December!B52</f>
-        <v>1870</v>
+        <v>1962</v>
       </c>
       <c r="C52" s="2">
         <f>January!C52+February!C52+March!C52+April!C52+May!C52+June!C52+July!C52+August!C52+September!C52+October!C52+November!C52+December!C52</f>
-        <v>2318</v>
+        <v>2484</v>
       </c>
       <c r="D52" s="2">
         <f>January!D52+February!D52+March!D52+April!D52+May!D52+June!D52+July!D52+August!D52+September!D52+October!D52+November!D52+December!D52</f>
-        <v>-448</v>
+        <v>-522</v>
       </c>
       <c r="E52" s="28" t="str">
         <f t="shared" si="3"/>
@@ -7996,7 +8539,7 @@
       </c>
       <c r="G52" s="3" t="str">
         <f t="shared" si="5"/>
-        <v>0.81 : 1</v>
+        <v>0.79 : 1</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -8005,15 +8548,15 @@
       </c>
       <c r="B53" s="4">
         <f>January!B53+February!B53+March!B53+April!B53+May!B53+June!B53+July!B53+August!B53+September!B53+October!B53+November!B53+December!B53</f>
-        <v>330</v>
+        <v>384</v>
       </c>
       <c r="C53" s="4">
         <f>January!C53+February!C53+March!C53+April!C53+May!C53+June!C53+July!C53+August!C53+September!C53+October!C53+November!C53+December!C53</f>
-        <v>2648</v>
+        <v>2928</v>
       </c>
       <c r="D53" s="4">
         <f>January!D53+February!D53+March!D53+April!D53+May!D53+June!D53+July!D53+August!D53+September!D53+October!D53+November!D53+December!D53</f>
-        <v>-2318</v>
+        <v>-2544</v>
       </c>
       <c r="E53" s="29" t="str">
         <f t="shared" si="3"/>
@@ -8025,7 +8568,7 @@
       </c>
       <c r="G53" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>0.12 : 1</v>
+        <v>0.13 : 1</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -8034,15 +8577,15 @@
       </c>
       <c r="B54" s="10">
         <f>January!B54+February!B54+March!B54+April!B54+May!B54+June!B54+July!B54+August!B54+September!B54+October!B54+November!B54+December!B54</f>
-        <v>4415</v>
+        <v>4779</v>
       </c>
       <c r="C54" s="10">
         <f>January!C54+February!C54+March!C54+April!C54+May!C54+June!C54+July!C54+August!C54+September!C54+October!C54+November!C54+December!C54</f>
-        <v>2253</v>
+        <v>2436</v>
       </c>
       <c r="D54" s="10">
         <f>January!D54+February!D54+March!D54+April!D54+May!D54+June!D54+July!D54+August!D54+September!D54+October!D54+November!D54+December!D54</f>
-        <v>2162</v>
+        <v>2343</v>
       </c>
       <c r="E54" s="32" t="str">
         <f t="shared" si="3"/>

</xml_diff>